<commit_message>
cheers is now IT; began outlining what edge is and how it affects games. Continued work on defining game eqs
</commit_message>
<xml_diff>
--- a/plans/baseball stats.xlsx
+++ b/plans/baseball stats.xlsx
@@ -13,8 +13,9 @@
   </bookViews>
   <sheets>
     <sheet name="iterative" sheetId="2" r:id="rId1"/>
-    <sheet name="run speed" sheetId="3" r:id="rId2"/>
-    <sheet name="pitch outcomes" sheetId="1" r:id="rId3"/>
+    <sheet name="gauss" sheetId="5" r:id="rId2"/>
+    <sheet name="run speed" sheetId="3" r:id="rId3"/>
+    <sheet name="pitch outcomes" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="dratings">iterative!$B$2:$L$2</definedName>
@@ -180,12 +181,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="P5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Kayla McGiffen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+MLB FP is 0.985 average, with a minimum around 0.95</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="120">
   <si>
     <t>Ball</t>
   </si>
@@ -220,9 +245,6 @@
     <t>defense</t>
   </si>
   <si>
-    <t>Column17</t>
-  </si>
-  <si>
     <t>base leadoff</t>
   </si>
   <si>
@@ -412,21 +434,6 @@
     <t>pickoff time</t>
   </si>
   <si>
-    <t>Column18</t>
-  </si>
-  <si>
-    <t>Column19</t>
-  </si>
-  <si>
-    <t>Column20</t>
-  </si>
-  <si>
-    <t>Column21</t>
-  </si>
-  <si>
-    <t>Column22</t>
-  </si>
-  <si>
     <t>Column23</t>
   </si>
   <si>
@@ -475,23 +482,104 @@
     <t>pickoff evade time</t>
   </si>
   <si>
-    <t>Picked off?</t>
-  </si>
-  <si>
     <t>stdv:</t>
   </si>
   <si>
-    <t>evade + 2 stdv?</t>
-  </si>
-  <si>
-    <t>evade + 3 stdv?</t>
+    <t>awe factor:</t>
+  </si>
+  <si>
+    <t>force factor:</t>
+  </si>
+  <si>
+    <t>timing factor:</t>
+  </si>
+  <si>
+    <t>speed factor:</t>
+  </si>
+  <si>
+    <t>stdv</t>
+  </si>
+  <si>
+    <t>mean:</t>
+  </si>
+  <si>
+    <t>pickoff probability</t>
+  </si>
+  <si>
+    <t>bravery factor:</t>
+  </si>
+  <si>
+    <t>strat factor:</t>
+  </si>
+  <si>
+    <t>const:</t>
+  </si>
+  <si>
+    <t>INVERTER BOX:</t>
+  </si>
+  <si>
+    <t>probability</t>
+  </si>
+  <si>
+    <t>z score</t>
+  </si>
+  <si>
+    <t>stdev:</t>
+  </si>
+  <si>
+    <t>x:</t>
+  </si>
+  <si>
+    <t>GUASS CRUNCHER</t>
+  </si>
+  <si>
+    <t>DOUBLE GAUSS CRUNCHER</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>prob:</t>
+  </si>
+  <si>
+    <t>targets:</t>
+  </si>
+  <si>
+    <t>diff:</t>
+  </si>
+  <si>
+    <t>fielding fuzzer:</t>
+  </si>
+  <si>
+    <t>Fielding Odds</t>
+  </si>
+  <si>
+    <t>pickoff worth it?</t>
+  </si>
+  <si>
+    <t>Error %</t>
+  </si>
+  <si>
+    <t>Blatant steal time</t>
+  </si>
+  <si>
+    <t>Response speed</t>
+  </si>
+  <si>
+    <t>reaction factor</t>
+  </si>
+  <si>
+    <t>blatant steal probability</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -504,6 +592,20 @@
       <color rgb="FF252C2F"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
@@ -532,7 +634,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -541,7 +643,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -559,12 +672,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -572,25 +703,277 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="7" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="10" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="10" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="7" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="22">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="0.0%"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -632,19 +1015,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -6107,66 +6478,72 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A5:AF21" totalsRowShown="0" headerRowDxfId="14">
-  <autoFilter ref="A5:AF21"/>
-  <tableColumns count="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A5:AD21" totalsRowShown="0" headerRowDxfId="19">
+  <autoFilter ref="A5:AD21"/>
+  <tableColumns count="30">
     <tableColumn id="1" name="Rep #">
       <calculatedColumnFormula>ROW()-ROW(home)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="offense" dataDxfId="17">
+    <tableColumn id="2" name="offense" dataDxfId="21">
       <calculatedColumnFormula>INDEX(oratings, 1, 1+MOD(Table3[[#This Row],[Rep '#]]-1, COUNT(oratings)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="defense" dataDxfId="16">
+    <tableColumn id="3" name="defense" dataDxfId="20">
       <calculatedColumnFormula>INDEX(dratings, 1, MOD(FLOOR( (Table3[[#This Row],[Rep '#]]-1) / COUNT(oratings), 1), COUNT(dratings))+1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="base leadoff" dataDxfId="15">
-      <calculatedColumnFormula>Table3[[#This Row],[offense]]*0.1+0.05</calculatedColumnFormula>
+    <tableColumn id="4" name="base leadoff" dataDxfId="12">
+      <calculatedColumnFormula>Table3[[#This Row],[offense]]*$D$25+0.05</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="leadoff modifier" dataDxfId="13">
-      <calculatedColumnFormula>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*0.1</calculatedColumnFormula>
+    <tableColumn id="5" name="leadoff modifier" dataDxfId="11">
+      <calculatedColumnFormula>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*$E$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="total leadoff (ft)" dataDxfId="12">
-      <calculatedColumnFormula>Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90</calculatedColumnFormula>
+    <tableColumn id="6" name="total leadoff (ft)" dataDxfId="10">
+      <calculatedColumnFormula>MAX(Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90, 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="pickoff manuver (s)" dataDxfId="11">
+    <tableColumn id="7" name="pickoff manuver (s)" dataDxfId="18">
       <calculatedColumnFormula>1.1 - Table3[[#This Row],[defense]]*0.1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="throw speed (s/ft)" dataDxfId="10">
+    <tableColumn id="8" name="throw speed (s/ft)" dataDxfId="17">
       <calculatedColumnFormula xml:space="preserve"> 0.01 - 0.0025 *  Table3[[#This Row],[defense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="32" name="throw speed (mph)" dataDxfId="7">
+    <tableColumn id="32" name="throw speed (mph)" dataDxfId="15">
       <calculatedColumnFormula>1 / Table3[[#This Row],[throw speed (s/ft)]] * ((60 * 60)/5280)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="pickoff time" dataDxfId="9">
+    <tableColumn id="9" name="pickoff time" dataDxfId="16">
       <calculatedColumnFormula>Table3[[#This Row],[pickoff manuver (s)]]+60*Table3[[#This Row],[throw speed (s/ft)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="runner reaction" dataDxfId="8">
-      <calculatedColumnFormula>1-0.1*Table3[[#This Row],[offense]]</calculatedColumnFormula>
+    <tableColumn id="10" name="runner reaction" dataDxfId="9">
+      <calculatedColumnFormula>$K$27-$K$25*Table3[[#This Row],[offense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="runner speed (s/ft)" dataDxfId="5">
-      <calculatedColumnFormula>0.05 - Table3[[#This Row],[offense]]*0.015</calculatedColumnFormula>
+    <tableColumn id="11" name="runner speed (s/ft)" dataDxfId="3">
+      <calculatedColumnFormula>0.05 - Table3[[#This Row],[offense]]*$L$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="runner speed (mph)" dataDxfId="6">
+    <tableColumn id="12" name="runner speed (mph)" dataDxfId="14">
       <calculatedColumnFormula>1 / Table3[[#This Row],[runner speed (s/ft)]] * ((60 * 60)/5280)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="pickoff evade time" dataDxfId="4">
+    <tableColumn id="13" name="pickoff evade time" dataDxfId="13">
       <calculatedColumnFormula>Table3[[#This Row],[runner reaction]]+Table3[[#This Row],[runner speed (s/ft)]]*Table3[[#This Row],[total leadoff (ft)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Picked off?" dataDxfId="3">
-      <calculatedColumnFormula>Table3[[#This Row],[pickoff evade time]]&gt;Table3[[#This Row],[pickoff time]]</calculatedColumnFormula>
+    <tableColumn id="14" name="pickoff probability" dataDxfId="7" dataCellStyle="Percent">
+      <calculatedColumnFormula>1 - _xlfn.NORM.DIST(Table3[[#This Row],[pickoff time]], Table3[[#This Row],[pickoff evade time]], $O$4, TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="evade + 2 stdv?" dataDxfId="2">
-      <calculatedColumnFormula>Table3[[#This Row],[pickoff evade time]]+2*$P$4 &gt; Table3[[#This Row],[pickoff time]]</calculatedColumnFormula>
+    <tableColumn id="17" name="Fielding Odds" dataDxfId="6" dataCellStyle="Percent">
+      <calculatedColumnFormula>_xlfn.NORM.DIST(Table3[[#This Row],[defense]], $P$25, $P$26, TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="evade + 3 stdv?" dataDxfId="1">
-      <calculatedColumnFormula>Table3[[#This Row],[pickoff evade time]]+3*$P$4 &gt; Table3[[#This Row],[pickoff time]]</calculatedColumnFormula>
+    <tableColumn id="18" name="pickoff worth it?" dataDxfId="5">
+      <calculatedColumnFormula>Table3[[#This Row],[pickoff probability]] &gt; 1-Table3[[#This Row],[Fielding Odds]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="Column17"/>
-    <tableColumn id="18" name="Column18"/>
-    <tableColumn id="19" name="Column19"/>
-    <tableColumn id="20" name="Column20"/>
-    <tableColumn id="21" name="Column21"/>
-    <tableColumn id="22" name="Column22"/>
+    <tableColumn id="19" name="Error %" dataDxfId="4" dataCellStyle="Percent">
+      <calculatedColumnFormula>1-Table3[[#This Row],[Fielding Odds]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="20" name="Blatant steal time" dataDxfId="2">
+      <calculatedColumnFormula>(90-Table3[[#This Row],[total leadoff (ft)]])*Table3[[#This Row],[runner speed (s/ft)]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="21" name="Response speed" dataDxfId="0">
+      <calculatedColumnFormula>$T$25*(2-Table3[[#This Row],[defense]]) + Table3[[#This Row],[pickoff time]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="22" name="blatant steal probability" dataDxfId="1" dataCellStyle="Percent">
+      <calculatedColumnFormula>_xlfn.NORM.DIST(Table3[[#This Row],[Response speed]], Table3[[#This Row],[Blatant steal time]], $U$4, TRUE)</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="23" name="Column23"/>
     <tableColumn id="24" name="Column24"/>
     <tableColumn id="25" name="Column25"/>
@@ -6444,15 +6821,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF21"/>
+  <dimension ref="A1:AD27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="U24" sqref="U24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -6469,7 +6846,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -6486,7 +6863,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -6494,16 +6871,22 @@
         <f>COUNT(oratings)*COUNT(dratings)</f>
         <v>16</v>
       </c>
-      <c r="P3" t="s">
-        <v>97</v>
+      <c r="O3" t="s">
+        <v>90</v>
+      </c>
+      <c r="U3" t="s">
+        <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="P4">
-        <v>0.15</v>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="O4">
+        <v>0.2</v>
+      </c>
+      <c r="U4">
+        <v>0.6</v>
       </c>
     </row>
-    <row r="5" spans="1:32" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -6514,1216 +6897,1537 @@
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="G5" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="J5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="V5" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="S5" s="2" t="s">
+      <c r="W5" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="T5" s="2" t="s">
+      <c r="X5" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="U5" s="2" t="s">
+      <c r="Y5" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="V5" s="2" t="s">
+      <c r="Z5" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="W5" s="2" t="s">
+      <c r="AA5" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="X5" s="2" t="s">
+      <c r="AB5" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="Y5" s="2" t="s">
+      <c r="AC5" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Z5" s="2" t="s">
+      <c r="AD5" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="AA5" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AB5" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="AC5" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="AD5" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AE5" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AF5" s="2" t="s">
-        <v>88</v>
-      </c>
     </row>
-    <row r="6" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+    <row r="6" spans="1:30" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="28">
         <f>ROW()-ROW(home)</f>
         <v>1</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="29">
         <f>INDEX(oratings, 1, 1+MOD(Table3[[#This Row],[Rep '#]]-1, COUNT(oratings)))</f>
         <v>0.1</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="29">
         <f>INDEX(dratings, 1, MOD(FLOOR( (Table3[[#This Row],[Rep '#]]-1) / COUNT(oratings), 1), COUNT(dratings))+1)</f>
         <v>0.1</v>
       </c>
-      <c r="D6" s="3">
-        <f>Table3[[#This Row],[offense]]*0.1+0.05</f>
+      <c r="D6" s="29">
+        <f>Table3[[#This Row],[offense]]*$D$25+0.05</f>
         <v>6.0000000000000005E-2</v>
       </c>
-      <c r="E6" s="3">
-        <f>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*0.1</f>
+      <c r="E6" s="29">
+        <f>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*$E$25</f>
         <v>-1.2E-2</v>
       </c>
-      <c r="F6" s="3">
-        <f>Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90</f>
+      <c r="F6" s="29">
+        <f>MAX(Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90, 0)</f>
         <v>5.4648000000000003</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="29">
         <f>1.1 - Table3[[#This Row],[defense]]*0.1</f>
         <v>1.0900000000000001</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="29">
         <f xml:space="preserve"> 0.01 - 0.0025 *  Table3[[#This Row],[defense]]</f>
         <v>9.75E-3</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="29">
         <f>1 / Table3[[#This Row],[throw speed (s/ft)]] * ((60 * 60)/5280)</f>
         <v>69.930069930069934</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="29">
         <f>Table3[[#This Row],[pickoff manuver (s)]]+60*Table3[[#This Row],[throw speed (s/ft)]]</f>
         <v>1.675</v>
       </c>
-      <c r="K6" s="3">
-        <f>1-0.1*Table3[[#This Row],[offense]]</f>
-        <v>0.99</v>
-      </c>
-      <c r="L6" s="3">
-        <f>0.05 - Table3[[#This Row],[offense]]*0.015</f>
-        <v>4.8500000000000001E-2</v>
-      </c>
-      <c r="M6" s="3">
+      <c r="K6" s="29">
+        <f>$K$27-$K$25*Table3[[#This Row],[offense]]</f>
+        <v>0.88</v>
+      </c>
+      <c r="L6" s="29">
+        <f>0.05 - Table3[[#This Row],[offense]]*$L$25</f>
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="M6" s="29">
         <f>1 / Table3[[#This Row],[runner speed (s/ft)]] * ((60 * 60)/5280)</f>
-        <v>14.058106841611993</v>
-      </c>
-      <c r="N6" s="3">
+        <v>13.914656771799628</v>
+      </c>
+      <c r="N6" s="29">
         <f>Table3[[#This Row],[runner reaction]]+Table3[[#This Row],[runner speed (s/ft)]]*Table3[[#This Row],[total leadoff (ft)]]</f>
-        <v>1.2550428</v>
-      </c>
-      <c r="O6" s="3" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]&gt;Table3[[#This Row],[pickoff time]]</f>
+        <v>1.1477752000000001</v>
+      </c>
+      <c r="O6" s="30">
+        <f>1 - _xlfn.NORM.DIST(Table3[[#This Row],[pickoff time]], Table3[[#This Row],[pickoff evade time]], $O$4, TRUE)</f>
+        <v>4.1929540286620437E-3</v>
+      </c>
+      <c r="P6" s="48">
+        <f>_xlfn.NORM.DIST(Table3[[#This Row],[defense]], $P$25, $P$26, TRUE)</f>
+        <v>0.96588837667724492</v>
+      </c>
+      <c r="Q6" s="29" t="b">
+        <f>Table3[[#This Row],[pickoff probability]] &gt; 1-Table3[[#This Row],[Fielding Odds]]</f>
         <v>0</v>
       </c>
-      <c r="P6" s="3" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]+2*$P$4 &gt; Table3[[#This Row],[pickoff time]]</f>
-        <v>0</v>
-      </c>
-      <c r="Q6" s="3" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]+3*$P$4 &gt; Table3[[#This Row],[pickoff time]]</f>
-        <v>1</v>
+      <c r="R6" s="48">
+        <f>1-Table3[[#This Row],[Fielding Odds]]</f>
+        <v>3.411162332275508E-2</v>
+      </c>
+      <c r="S6" s="29">
+        <f>(90-Table3[[#This Row],[total leadoff (ft)]])*Table3[[#This Row],[runner speed (s/ft)]]</f>
+        <v>4.1422248000000002</v>
+      </c>
+      <c r="T6" s="29">
+        <f>$T$25*(2-Table3[[#This Row],[defense]]) + Table3[[#This Row],[pickoff time]]</f>
+        <v>2.0550000000000002</v>
+      </c>
+      <c r="U6" s="48">
+        <f>_xlfn.NORM.DIST(Table3[[#This Row],[Response speed]], Table3[[#This Row],[Blatant steal time]], $U$4, TRUE)</f>
+        <v>2.5191863061619241E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <f>ROW()-ROW(home)</f>
         <v>2</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <f>INDEX(oratings, 1, 1+MOD(Table3[[#This Row],[Rep '#]]-1, COUNT(oratings)))</f>
         <v>0.5</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <f>INDEX(dratings, 1, MOD(FLOOR( (Table3[[#This Row],[Rep '#]]-1) / COUNT(oratings), 1), COUNT(dratings))+1)</f>
         <v>0.1</v>
       </c>
-      <c r="D7">
-        <f>Table3[[#This Row],[offense]]*0.1+0.05</f>
+      <c r="D7" s="3">
+        <f>Table3[[#This Row],[offense]]*$D$25+0.05</f>
         <v>0.1</v>
       </c>
-      <c r="E7">
-        <f>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*0.1</f>
+      <c r="E7" s="3">
+        <f>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*$E$25</f>
         <v>-0.06</v>
       </c>
-      <c r="F7">
-        <f>Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90</f>
+      <c r="F7" s="3">
+        <f>MAX(Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90, 0)</f>
         <v>9.5400000000000009</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="3">
         <f>1.1 - Table3[[#This Row],[defense]]*0.1</f>
         <v>1.0900000000000001</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="3">
         <f xml:space="preserve"> 0.01 - 0.0025 *  Table3[[#This Row],[defense]]</f>
         <v>9.75E-3</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="3">
         <f>1 / Table3[[#This Row],[throw speed (s/ft)]] * ((60 * 60)/5280)</f>
         <v>69.930069930069934</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="3">
         <f>Table3[[#This Row],[pickoff manuver (s)]]+60*Table3[[#This Row],[throw speed (s/ft)]]</f>
         <v>1.675</v>
       </c>
-      <c r="K7">
-        <f>1-0.1*Table3[[#This Row],[offense]]</f>
-        <v>0.95</v>
-      </c>
-      <c r="L7">
-        <f>0.05 - Table3[[#This Row],[offense]]*0.015</f>
-        <v>4.2500000000000003E-2</v>
-      </c>
-      <c r="M7">
+      <c r="K7" s="3">
+        <f>$K$27-$K$25*Table3[[#This Row],[offense]]</f>
+        <v>0.8</v>
+      </c>
+      <c r="L7" s="3">
+        <f>0.05 - Table3[[#This Row],[offense]]*$L$25</f>
+        <v>4.5000000000000005E-2</v>
+      </c>
+      <c r="M7" s="3">
         <f>1 / Table3[[#This Row],[runner speed (s/ft)]] * ((60 * 60)/5280)</f>
-        <v>16.042780748663098</v>
-      </c>
-      <c r="N7">
+        <v>15.151515151515147</v>
+      </c>
+      <c r="N7" s="3">
         <f>Table3[[#This Row],[runner reaction]]+Table3[[#This Row],[runner speed (s/ft)]]*Table3[[#This Row],[total leadoff (ft)]]</f>
-        <v>1.35545</v>
-      </c>
-      <c r="O7" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]&gt;Table3[[#This Row],[pickoff time]]</f>
+        <v>1.2293000000000001</v>
+      </c>
+      <c r="O7" s="7">
+        <f>1 - _xlfn.NORM.DIST(Table3[[#This Row],[pickoff time]], Table3[[#This Row],[pickoff evade time]], $O$4, TRUE)</f>
+        <v>1.2923595669015353E-2</v>
+      </c>
+      <c r="P7" s="49">
+        <f>_xlfn.NORM.DIST(Table3[[#This Row],[defense]], $P$25, $P$26, TRUE)</f>
+        <v>0.96588837667724492</v>
+      </c>
+      <c r="Q7" s="3" t="b">
+        <f>Table3[[#This Row],[pickoff probability]] &gt; 1-Table3[[#This Row],[Fielding Odds]]</f>
         <v>0</v>
       </c>
-      <c r="P7" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]+2*$P$4 &gt; Table3[[#This Row],[pickoff time]]</f>
-        <v>0</v>
-      </c>
-      <c r="Q7" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]+3*$P$4 &gt; Table3[[#This Row],[pickoff time]]</f>
-        <v>1</v>
+      <c r="R7" s="49">
+        <f>1-Table3[[#This Row],[Fielding Odds]]</f>
+        <v>3.411162332275508E-2</v>
+      </c>
+      <c r="S7" s="3">
+        <f>(90-Table3[[#This Row],[total leadoff (ft)]])*Table3[[#This Row],[runner speed (s/ft)]]</f>
+        <v>3.6207000000000003</v>
+      </c>
+      <c r="T7" s="3">
+        <f>$T$25*(2-Table3[[#This Row],[defense]]) + Table3[[#This Row],[pickoff time]]</f>
+        <v>2.0550000000000002</v>
+      </c>
+      <c r="U7" s="49">
+        <f>_xlfn.NORM.DIST(Table3[[#This Row],[Response speed]], Table3[[#This Row],[Blatant steal time]], $U$4, TRUE)</f>
+        <v>4.5337323029872069E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
         <f>ROW()-ROW(home)</f>
         <v>3</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="4">
         <f>INDEX(oratings, 1, 1+MOD(Table3[[#This Row],[Rep '#]]-1, COUNT(oratings)))</f>
         <v>1</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="4">
         <f>INDEX(dratings, 1, MOD(FLOOR( (Table3[[#This Row],[Rep '#]]-1) / COUNT(oratings), 1), COUNT(dratings))+1)</f>
         <v>0.1</v>
       </c>
-      <c r="D8">
-        <f>Table3[[#This Row],[offense]]*0.1+0.05</f>
+      <c r="D8" s="4">
+        <f>Table3[[#This Row],[offense]]*$D$25+0.05</f>
         <v>0.15000000000000002</v>
       </c>
-      <c r="E8">
-        <f>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*0.1</f>
+      <c r="E8" s="4">
+        <f>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*$E$25</f>
         <v>-0.12</v>
       </c>
-      <c r="F8">
-        <f>Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90</f>
+      <c r="F8" s="4">
+        <f>MAX(Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90, 0)</f>
         <v>15.120000000000003</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="4">
         <f>1.1 - Table3[[#This Row],[defense]]*0.1</f>
         <v>1.0900000000000001</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="4">
         <f xml:space="preserve"> 0.01 - 0.0025 *  Table3[[#This Row],[defense]]</f>
         <v>9.75E-3</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="4">
         <f>1 / Table3[[#This Row],[throw speed (s/ft)]] * ((60 * 60)/5280)</f>
         <v>69.930069930069934</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="4">
         <f>Table3[[#This Row],[pickoff manuver (s)]]+60*Table3[[#This Row],[throw speed (s/ft)]]</f>
         <v>1.675</v>
       </c>
-      <c r="K8">
-        <f>1-0.1*Table3[[#This Row],[offense]]</f>
-        <v>0.9</v>
-      </c>
-      <c r="L8">
-        <f>0.05 - Table3[[#This Row],[offense]]*0.015</f>
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="M8">
+      <c r="K8" s="4">
+        <f>$K$27-$K$25*Table3[[#This Row],[offense]]</f>
+        <v>0.7</v>
+      </c>
+      <c r="L8" s="4">
+        <f>0.05 - Table3[[#This Row],[offense]]*$L$25</f>
+        <v>0.04</v>
+      </c>
+      <c r="M8" s="4">
         <f>1 / Table3[[#This Row],[runner speed (s/ft)]] * ((60 * 60)/5280)</f>
-        <v>19.480519480519479</v>
-      </c>
-      <c r="N8">
+        <v>17.045454545454543</v>
+      </c>
+      <c r="N8" s="4">
         <f>Table3[[#This Row],[runner reaction]]+Table3[[#This Row],[runner speed (s/ft)]]*Table3[[#This Row],[total leadoff (ft)]]</f>
-        <v>1.4292000000000002</v>
-      </c>
-      <c r="O8" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]&gt;Table3[[#This Row],[pickoff time]]</f>
+        <v>1.3048000000000002</v>
+      </c>
+      <c r="O8" s="10">
+        <f>1 - _xlfn.NORM.DIST(Table3[[#This Row],[pickoff time]], Table3[[#This Row],[pickoff evade time]], $O$4, TRUE)</f>
+        <v>3.208477655219244E-2</v>
+      </c>
+      <c r="P8" s="50">
+        <f>_xlfn.NORM.DIST(Table3[[#This Row],[defense]], $P$25, $P$26, TRUE)</f>
+        <v>0.96588837667724492</v>
+      </c>
+      <c r="Q8" s="4" t="b">
+        <f>Table3[[#This Row],[pickoff probability]] &gt; 1-Table3[[#This Row],[Fielding Odds]]</f>
         <v>0</v>
       </c>
-      <c r="P8" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]+2*$P$4 &gt; Table3[[#This Row],[pickoff time]]</f>
-        <v>1</v>
-      </c>
-      <c r="Q8" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]+3*$P$4 &gt; Table3[[#This Row],[pickoff time]]</f>
-        <v>1</v>
+      <c r="R8" s="50">
+        <f>1-Table3[[#This Row],[Fielding Odds]]</f>
+        <v>3.411162332275508E-2</v>
+      </c>
+      <c r="S8" s="4">
+        <f>(90-Table3[[#This Row],[total leadoff (ft)]])*Table3[[#This Row],[runner speed (s/ft)]]</f>
+        <v>2.9952000000000001</v>
+      </c>
+      <c r="T8" s="4">
+        <f>$T$25*(2-Table3[[#This Row],[defense]]) + Table3[[#This Row],[pickoff time]]</f>
+        <v>2.0550000000000002</v>
+      </c>
+      <c r="U8" s="50">
+        <f>_xlfn.NORM.DIST(Table3[[#This Row],[Response speed]], Table3[[#This Row],[Blatant steal time]], $U$4, TRUE)</f>
+        <v>5.8557345807363756E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
         <f>ROW()-ROW(home)</f>
         <v>4</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <f>INDEX(oratings, 1, 1+MOD(Table3[[#This Row],[Rep '#]]-1, COUNT(oratings)))</f>
         <v>2</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <f>INDEX(dratings, 1, MOD(FLOOR( (Table3[[#This Row],[Rep '#]]-1) / COUNT(oratings), 1), COUNT(dratings))+1)</f>
         <v>0.1</v>
       </c>
-      <c r="D9">
-        <f>Table3[[#This Row],[offense]]*0.1+0.05</f>
+      <c r="D9" s="3">
+        <f>Table3[[#This Row],[offense]]*$D$25+0.05</f>
         <v>0.25</v>
       </c>
-      <c r="E9">
-        <f>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*0.1</f>
+      <c r="E9" s="3">
+        <f>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*$E$25</f>
         <v>-0.24</v>
       </c>
-      <c r="F9">
-        <f>Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90</f>
+      <c r="F9" s="3">
+        <f>MAX(Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90, 0)</f>
         <v>27.9</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="3">
         <f>1.1 - Table3[[#This Row],[defense]]*0.1</f>
         <v>1.0900000000000001</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="3">
         <f xml:space="preserve"> 0.01 - 0.0025 *  Table3[[#This Row],[defense]]</f>
         <v>9.75E-3</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="3">
         <f>1 / Table3[[#This Row],[throw speed (s/ft)]] * ((60 * 60)/5280)</f>
         <v>69.930069930069934</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="3">
         <f>Table3[[#This Row],[pickoff manuver (s)]]+60*Table3[[#This Row],[throw speed (s/ft)]]</f>
         <v>1.675</v>
       </c>
-      <c r="K9">
-        <f>1-0.1*Table3[[#This Row],[offense]]</f>
-        <v>0.8</v>
-      </c>
-      <c r="L9">
-        <f>0.05 - Table3[[#This Row],[offense]]*0.015</f>
-        <v>2.0000000000000004E-2</v>
-      </c>
-      <c r="M9">
+      <c r="K9" s="3">
+        <f>$K$27-$K$25*Table3[[#This Row],[offense]]</f>
+        <v>0.5</v>
+      </c>
+      <c r="L9" s="3">
+        <f>0.05 - Table3[[#This Row],[offense]]*$L$25</f>
+        <v>3.0000000000000002E-2</v>
+      </c>
+      <c r="M9" s="3">
         <f>1 / Table3[[#This Row],[runner speed (s/ft)]] * ((60 * 60)/5280)</f>
-        <v>34.090909090909086</v>
-      </c>
-      <c r="N9">
+        <v>22.727272727272723</v>
+      </c>
+      <c r="N9" s="3">
         <f>Table3[[#This Row],[runner reaction]]+Table3[[#This Row],[runner speed (s/ft)]]*Table3[[#This Row],[total leadoff (ft)]]</f>
-        <v>1.3580000000000001</v>
-      </c>
-      <c r="O9" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]&gt;Table3[[#This Row],[pickoff time]]</f>
-        <v>0</v>
-      </c>
-      <c r="P9" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]+2*$P$4 &gt; Table3[[#This Row],[pickoff time]]</f>
-        <v>0</v>
-      </c>
-      <c r="Q9" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]+3*$P$4 &gt; Table3[[#This Row],[pickoff time]]</f>
+        <v>1.3370000000000002</v>
+      </c>
+      <c r="O9" s="7">
+        <f>1 - _xlfn.NORM.DIST(Table3[[#This Row],[pickoff time]], Table3[[#This Row],[pickoff evade time]], $O$4, TRUE)</f>
+        <v>4.5513977321549826E-2</v>
+      </c>
+      <c r="P9" s="49">
+        <f>_xlfn.NORM.DIST(Table3[[#This Row],[defense]], $P$25, $P$26, TRUE)</f>
+        <v>0.96588837667724492</v>
+      </c>
+      <c r="Q9" s="3" t="b">
+        <f>Table3[[#This Row],[pickoff probability]] &gt; 1-Table3[[#This Row],[Fielding Odds]]</f>
         <v>1</v>
       </c>
+      <c r="R9" s="49">
+        <f>1-Table3[[#This Row],[Fielding Odds]]</f>
+        <v>3.411162332275508E-2</v>
+      </c>
+      <c r="S9" s="3">
+        <f>(90-Table3[[#This Row],[total leadoff (ft)]])*Table3[[#This Row],[runner speed (s/ft)]]</f>
+        <v>1.8630000000000002</v>
+      </c>
+      <c r="T9" s="3">
+        <f>$T$25*(2-Table3[[#This Row],[defense]]) + Table3[[#This Row],[pickoff time]]</f>
+        <v>2.0550000000000002</v>
+      </c>
+      <c r="U9" s="49">
+        <f>_xlfn.NORM.DIST(Table3[[#This Row],[Response speed]], Table3[[#This Row],[Blatant steal time]], $U$4, TRUE)</f>
+        <v>0.62551583472332006</v>
+      </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:30" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
         <f>ROW()-ROW(home)</f>
         <v>5</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="13">
         <f>INDEX(oratings, 1, 1+MOD(Table3[[#This Row],[Rep '#]]-1, COUNT(oratings)))</f>
         <v>0.1</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="13">
         <f>INDEX(dratings, 1, MOD(FLOOR( (Table3[[#This Row],[Rep '#]]-1) / COUNT(oratings), 1), COUNT(dratings))+1)</f>
         <v>0.5</v>
       </c>
-      <c r="D10">
-        <f>Table3[[#This Row],[offense]]*0.1+0.05</f>
+      <c r="D10" s="13">
+        <f>Table3[[#This Row],[offense]]*$D$25+0.05</f>
         <v>6.0000000000000005E-2</v>
       </c>
-      <c r="E10">
-        <f>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*0.1</f>
+      <c r="E10" s="13">
+        <f>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*$E$25</f>
         <v>0</v>
       </c>
-      <c r="F10">
-        <f>Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90</f>
+      <c r="F10" s="13">
+        <f>MAX(Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90, 0)</f>
         <v>5.4</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="13">
         <f>1.1 - Table3[[#This Row],[defense]]*0.1</f>
         <v>1.05</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="13">
         <f xml:space="preserve"> 0.01 - 0.0025 *  Table3[[#This Row],[defense]]</f>
         <v>8.7500000000000008E-3</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="13">
         <f>1 / Table3[[#This Row],[throw speed (s/ft)]] * ((60 * 60)/5280)</f>
         <v>77.922077922077918</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="13">
         <f>Table3[[#This Row],[pickoff manuver (s)]]+60*Table3[[#This Row],[throw speed (s/ft)]]</f>
         <v>1.5750000000000002</v>
       </c>
-      <c r="K10">
-        <f>1-0.1*Table3[[#This Row],[offense]]</f>
-        <v>0.99</v>
-      </c>
-      <c r="L10">
-        <f>0.05 - Table3[[#This Row],[offense]]*0.015</f>
-        <v>4.8500000000000001E-2</v>
-      </c>
-      <c r="M10">
+      <c r="K10" s="13">
+        <f>$K$27-$K$25*Table3[[#This Row],[offense]]</f>
+        <v>0.88</v>
+      </c>
+      <c r="L10" s="13">
+        <f>0.05 - Table3[[#This Row],[offense]]*$L$25</f>
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="M10" s="13">
         <f>1 / Table3[[#This Row],[runner speed (s/ft)]] * ((60 * 60)/5280)</f>
-        <v>14.058106841611993</v>
-      </c>
-      <c r="N10">
+        <v>13.914656771799628</v>
+      </c>
+      <c r="N10" s="13">
         <f>Table3[[#This Row],[runner reaction]]+Table3[[#This Row],[runner speed (s/ft)]]*Table3[[#This Row],[total leadoff (ft)]]</f>
-        <v>1.2519</v>
-      </c>
-      <c r="O10" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]&gt;Table3[[#This Row],[pickoff time]]</f>
+        <v>1.1446000000000001</v>
+      </c>
+      <c r="O10" s="14">
+        <f>1 - _xlfn.NORM.DIST(Table3[[#This Row],[pickoff time]], Table3[[#This Row],[pickoff evade time]], $O$4, TRUE)</f>
+        <v>1.5698677182155896E-2</v>
+      </c>
+      <c r="P10" s="51">
+        <f>_xlfn.NORM.DIST(Table3[[#This Row],[defense]], $P$25, $P$26, TRUE)</f>
+        <v>0.98024442661121902</v>
+      </c>
+      <c r="Q10" s="13" t="b">
+        <f>Table3[[#This Row],[pickoff probability]] &gt; 1-Table3[[#This Row],[Fielding Odds]]</f>
         <v>0</v>
       </c>
-      <c r="P10" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]+2*$P$4 &gt; Table3[[#This Row],[pickoff time]]</f>
-        <v>0</v>
-      </c>
-      <c r="Q10" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]+3*$P$4 &gt; Table3[[#This Row],[pickoff time]]</f>
-        <v>1</v>
+      <c r="R10" s="51">
+        <f>1-Table3[[#This Row],[Fielding Odds]]</f>
+        <v>1.9755573388780978E-2</v>
+      </c>
+      <c r="S10" s="13">
+        <f>(90-Table3[[#This Row],[total leadoff (ft)]])*Table3[[#This Row],[runner speed (s/ft)]]</f>
+        <v>4.1453999999999995</v>
+      </c>
+      <c r="T10" s="13">
+        <f>$T$25*(2-Table3[[#This Row],[defense]]) + Table3[[#This Row],[pickoff time]]</f>
+        <v>1.8750000000000002</v>
+      </c>
+      <c r="U10" s="51">
+        <f>_xlfn.NORM.DIST(Table3[[#This Row],[Response speed]], Table3[[#This Row],[Blatant steal time]], $U$4, TRUE)</f>
+        <v>7.7163911324126927E-5</v>
       </c>
     </row>
-    <row r="11" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+    <row r="11" spans="1:30" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="25">
         <f>ROW()-ROW(home)</f>
         <v>6</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="26">
         <f>INDEX(oratings, 1, 1+MOD(Table3[[#This Row],[Rep '#]]-1, COUNT(oratings)))</f>
         <v>0.5</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="26">
         <f>INDEX(dratings, 1, MOD(FLOOR( (Table3[[#This Row],[Rep '#]]-1) / COUNT(oratings), 1), COUNT(dratings))+1)</f>
         <v>0.5</v>
       </c>
-      <c r="D11" s="4">
-        <f>Table3[[#This Row],[offense]]*0.1+0.05</f>
+      <c r="D11" s="26">
+        <f>Table3[[#This Row],[offense]]*$D$25+0.05</f>
         <v>0.1</v>
       </c>
-      <c r="E11" s="4">
-        <f>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*0.1</f>
+      <c r="E11" s="26">
+        <f>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*$E$25</f>
         <v>0</v>
       </c>
-      <c r="F11" s="4">
-        <f>Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90</f>
+      <c r="F11" s="26">
+        <f>MAX(Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90, 0)</f>
         <v>9</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="26">
         <f>1.1 - Table3[[#This Row],[defense]]*0.1</f>
         <v>1.05</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="26">
         <f xml:space="preserve"> 0.01 - 0.0025 *  Table3[[#This Row],[defense]]</f>
         <v>8.7500000000000008E-3</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="26">
         <f>1 / Table3[[#This Row],[throw speed (s/ft)]] * ((60 * 60)/5280)</f>
         <v>77.922077922077918</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11" s="26">
         <f>Table3[[#This Row],[pickoff manuver (s)]]+60*Table3[[#This Row],[throw speed (s/ft)]]</f>
         <v>1.5750000000000002</v>
       </c>
-      <c r="K11" s="4">
-        <f>1-0.1*Table3[[#This Row],[offense]]</f>
-        <v>0.95</v>
-      </c>
-      <c r="L11" s="4">
-        <f>0.05 - Table3[[#This Row],[offense]]*0.015</f>
-        <v>4.2500000000000003E-2</v>
-      </c>
-      <c r="M11" s="4">
+      <c r="K11" s="26">
+        <f>$K$27-$K$25*Table3[[#This Row],[offense]]</f>
+        <v>0.8</v>
+      </c>
+      <c r="L11" s="26">
+        <f>0.05 - Table3[[#This Row],[offense]]*$L$25</f>
+        <v>4.5000000000000005E-2</v>
+      </c>
+      <c r="M11" s="26">
         <f>1 / Table3[[#This Row],[runner speed (s/ft)]] * ((60 * 60)/5280)</f>
-        <v>16.042780748663098</v>
-      </c>
-      <c r="N11" s="4">
+        <v>15.151515151515147</v>
+      </c>
+      <c r="N11" s="26">
         <f>Table3[[#This Row],[runner reaction]]+Table3[[#This Row],[runner speed (s/ft)]]*Table3[[#This Row],[total leadoff (ft)]]</f>
-        <v>1.3325</v>
-      </c>
-      <c r="O11" s="4" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]&gt;Table3[[#This Row],[pickoff time]]</f>
-        <v>0</v>
-      </c>
-      <c r="P11" s="4" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]+2*$P$4 &gt; Table3[[#This Row],[pickoff time]]</f>
+        <v>1.2050000000000001</v>
+      </c>
+      <c r="O11" s="27">
+        <f>1 - _xlfn.NORM.DIST(Table3[[#This Row],[pickoff time]], Table3[[#This Row],[pickoff evade time]], $O$4, TRUE)</f>
+        <v>3.215677479561363E-2</v>
+      </c>
+      <c r="P11" s="52">
+        <f>_xlfn.NORM.DIST(Table3[[#This Row],[defense]], $P$25, $P$26, TRUE)</f>
+        <v>0.98024442661121902</v>
+      </c>
+      <c r="Q11" s="26" t="b">
+        <f>Table3[[#This Row],[pickoff probability]] &gt; 1-Table3[[#This Row],[Fielding Odds]]</f>
         <v>1</v>
       </c>
-      <c r="Q11" s="4" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]+3*$P$4 &gt; Table3[[#This Row],[pickoff time]]</f>
-        <v>1</v>
+      <c r="R11" s="52">
+        <f>1-Table3[[#This Row],[Fielding Odds]]</f>
+        <v>1.9755573388780978E-2</v>
+      </c>
+      <c r="S11" s="26">
+        <f>(90-Table3[[#This Row],[total leadoff (ft)]])*Table3[[#This Row],[runner speed (s/ft)]]</f>
+        <v>3.6450000000000005</v>
+      </c>
+      <c r="T11" s="26">
+        <f>$T$25*(2-Table3[[#This Row],[defense]]) + Table3[[#This Row],[pickoff time]]</f>
+        <v>1.8750000000000002</v>
+      </c>
+      <c r="U11" s="52">
+        <f>_xlfn.NORM.DIST(Table3[[#This Row],[Response speed]], Table3[[#This Row],[Blatant steal time]], $U$4, TRUE)</f>
+        <v>1.5888696473648632E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" spans="1:30" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="13">
         <f>ROW()-ROW(home)</f>
         <v>7</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="13">
         <f>INDEX(oratings, 1, 1+MOD(Table3[[#This Row],[Rep '#]]-1, COUNT(oratings)))</f>
         <v>1</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="13">
         <f>INDEX(dratings, 1, MOD(FLOOR( (Table3[[#This Row],[Rep '#]]-1) / COUNT(oratings), 1), COUNT(dratings))+1)</f>
         <v>0.5</v>
       </c>
-      <c r="D12">
-        <f>Table3[[#This Row],[offense]]*0.1+0.05</f>
+      <c r="D12" s="13">
+        <f>Table3[[#This Row],[offense]]*$D$25+0.05</f>
         <v>0.15000000000000002</v>
       </c>
-      <c r="E12">
-        <f>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*0.1</f>
+      <c r="E12" s="13">
+        <f>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*$E$25</f>
         <v>0</v>
       </c>
-      <c r="F12">
-        <f>Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90</f>
+      <c r="F12" s="13">
+        <f>MAX(Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90, 0)</f>
         <v>13.500000000000002</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="13">
         <f>1.1 - Table3[[#This Row],[defense]]*0.1</f>
         <v>1.05</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="13">
         <f xml:space="preserve"> 0.01 - 0.0025 *  Table3[[#This Row],[defense]]</f>
         <v>8.7500000000000008E-3</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="13">
         <f>1 / Table3[[#This Row],[throw speed (s/ft)]] * ((60 * 60)/5280)</f>
         <v>77.922077922077918</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="13">
         <f>Table3[[#This Row],[pickoff manuver (s)]]+60*Table3[[#This Row],[throw speed (s/ft)]]</f>
         <v>1.5750000000000002</v>
       </c>
-      <c r="K12">
-        <f>1-0.1*Table3[[#This Row],[offense]]</f>
-        <v>0.9</v>
-      </c>
-      <c r="L12">
-        <f>0.05 - Table3[[#This Row],[offense]]*0.015</f>
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="M12">
+      <c r="K12" s="13">
+        <f>$K$27-$K$25*Table3[[#This Row],[offense]]</f>
+        <v>0.7</v>
+      </c>
+      <c r="L12" s="13">
+        <f>0.05 - Table3[[#This Row],[offense]]*$L$25</f>
+        <v>0.04</v>
+      </c>
+      <c r="M12" s="13">
         <f>1 / Table3[[#This Row],[runner speed (s/ft)]] * ((60 * 60)/5280)</f>
-        <v>19.480519480519479</v>
-      </c>
-      <c r="N12">
+        <v>17.045454545454543</v>
+      </c>
+      <c r="N12" s="13">
         <f>Table3[[#This Row],[runner reaction]]+Table3[[#This Row],[runner speed (s/ft)]]*Table3[[#This Row],[total leadoff (ft)]]</f>
-        <v>1.3725000000000001</v>
-      </c>
-      <c r="O12" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]&gt;Table3[[#This Row],[pickoff time]]</f>
-        <v>0</v>
-      </c>
-      <c r="P12" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]+2*$P$4 &gt; Table3[[#This Row],[pickoff time]]</f>
+        <v>1.24</v>
+      </c>
+      <c r="O12" s="14">
+        <f>1 - _xlfn.NORM.DIST(Table3[[#This Row],[pickoff time]], Table3[[#This Row],[pickoff evade time]], $O$4, TRUE)</f>
+        <v>4.6967115830745643E-2</v>
+      </c>
+      <c r="P12" s="51">
+        <f>_xlfn.NORM.DIST(Table3[[#This Row],[defense]], $P$25, $P$26, TRUE)</f>
+        <v>0.98024442661121902</v>
+      </c>
+      <c r="Q12" s="13" t="b">
+        <f>Table3[[#This Row],[pickoff probability]] &gt; 1-Table3[[#This Row],[Fielding Odds]]</f>
         <v>1</v>
       </c>
-      <c r="Q12" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]+3*$P$4 &gt; Table3[[#This Row],[pickoff time]]</f>
-        <v>1</v>
+      <c r="R12" s="51">
+        <f>1-Table3[[#This Row],[Fielding Odds]]</f>
+        <v>1.9755573388780978E-2</v>
+      </c>
+      <c r="S12" s="13">
+        <f>(90-Table3[[#This Row],[total leadoff (ft)]])*Table3[[#This Row],[runner speed (s/ft)]]</f>
+        <v>3.06</v>
+      </c>
+      <c r="T12" s="13">
+        <f>$T$25*(2-Table3[[#This Row],[defense]]) + Table3[[#This Row],[pickoff time]]</f>
+        <v>1.8750000000000002</v>
+      </c>
+      <c r="U12" s="51">
+        <f>_xlfn.NORM.DIST(Table3[[#This Row],[Response speed]], Table3[[#This Row],[Blatant steal time]], $U$4, TRUE)</f>
+        <v>2.4134074004724768E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="13" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
         <f>ROW()-ROW(home)</f>
         <v>8</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="5">
         <f>INDEX(oratings, 1, 1+MOD(Table3[[#This Row],[Rep '#]]-1, COUNT(oratings)))</f>
         <v>2</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="5">
         <f>INDEX(dratings, 1, MOD(FLOOR( (Table3[[#This Row],[Rep '#]]-1) / COUNT(oratings), 1), COUNT(dratings))+1)</f>
         <v>0.5</v>
       </c>
-      <c r="D13">
-        <f>Table3[[#This Row],[offense]]*0.1+0.05</f>
+      <c r="D13" s="5">
+        <f>Table3[[#This Row],[offense]]*$D$25+0.05</f>
         <v>0.25</v>
       </c>
-      <c r="E13">
-        <f>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*0.1</f>
+      <c r="E13" s="5">
+        <f>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*$E$25</f>
         <v>0</v>
       </c>
-      <c r="F13">
-        <f>Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90</f>
+      <c r="F13" s="5">
+        <f>MAX(Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90, 0)</f>
         <v>22.5</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="5">
         <f>1.1 - Table3[[#This Row],[defense]]*0.1</f>
         <v>1.05</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="5">
         <f xml:space="preserve"> 0.01 - 0.0025 *  Table3[[#This Row],[defense]]</f>
         <v>8.7500000000000008E-3</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="5">
         <f>1 / Table3[[#This Row],[throw speed (s/ft)]] * ((60 * 60)/5280)</f>
         <v>77.922077922077918</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="5">
         <f>Table3[[#This Row],[pickoff manuver (s)]]+60*Table3[[#This Row],[throw speed (s/ft)]]</f>
         <v>1.5750000000000002</v>
       </c>
-      <c r="K13">
-        <f>1-0.1*Table3[[#This Row],[offense]]</f>
-        <v>0.8</v>
-      </c>
-      <c r="L13">
-        <f>0.05 - Table3[[#This Row],[offense]]*0.015</f>
-        <v>2.0000000000000004E-2</v>
-      </c>
-      <c r="M13">
+      <c r="K13" s="5">
+        <f>$K$27-$K$25*Table3[[#This Row],[offense]]</f>
+        <v>0.5</v>
+      </c>
+      <c r="L13" s="5">
+        <f>0.05 - Table3[[#This Row],[offense]]*$L$25</f>
+        <v>3.0000000000000002E-2</v>
+      </c>
+      <c r="M13" s="5">
         <f>1 / Table3[[#This Row],[runner speed (s/ft)]] * ((60 * 60)/5280)</f>
-        <v>34.090909090909086</v>
-      </c>
-      <c r="N13">
+        <v>22.727272727272723</v>
+      </c>
+      <c r="N13" s="5">
         <f>Table3[[#This Row],[runner reaction]]+Table3[[#This Row],[runner speed (s/ft)]]*Table3[[#This Row],[total leadoff (ft)]]</f>
-        <v>1.25</v>
-      </c>
-      <c r="O13" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]&gt;Table3[[#This Row],[pickoff time]]</f>
-        <v>0</v>
-      </c>
-      <c r="P13" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]+2*$P$4 &gt; Table3[[#This Row],[pickoff time]]</f>
-        <v>0</v>
-      </c>
-      <c r="Q13" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]+3*$P$4 &gt; Table3[[#This Row],[pickoff time]]</f>
+        <v>1.175</v>
+      </c>
+      <c r="O13" s="8">
+        <f>1 - _xlfn.NORM.DIST(Table3[[#This Row],[pickoff time]], Table3[[#This Row],[pickoff evade time]], $O$4, TRUE)</f>
+        <v>2.2750131948179209E-2</v>
+      </c>
+      <c r="P13" s="53">
+        <f>_xlfn.NORM.DIST(Table3[[#This Row],[defense]], $P$25, $P$26, TRUE)</f>
+        <v>0.98024442661121902</v>
+      </c>
+      <c r="Q13" s="5" t="b">
+        <f>Table3[[#This Row],[pickoff probability]] &gt; 1-Table3[[#This Row],[Fielding Odds]]</f>
         <v>1</v>
       </c>
+      <c r="R13" s="53">
+        <f>1-Table3[[#This Row],[Fielding Odds]]</f>
+        <v>1.9755573388780978E-2</v>
+      </c>
+      <c r="S13" s="5">
+        <f>(90-Table3[[#This Row],[total leadoff (ft)]])*Table3[[#This Row],[runner speed (s/ft)]]</f>
+        <v>2.0250000000000004</v>
+      </c>
+      <c r="T13" s="5">
+        <f>$T$25*(2-Table3[[#This Row],[defense]]) + Table3[[#This Row],[pickoff time]]</f>
+        <v>1.8750000000000002</v>
+      </c>
+      <c r="U13" s="53">
+        <f>_xlfn.NORM.DIST(Table3[[#This Row],[Response speed]], Table3[[#This Row],[Blatant steal time]], $U$4, TRUE)</f>
+        <v>0.40129367431707619</v>
+      </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="14" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="17">
         <f>ROW()-ROW(home)</f>
         <v>9</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="17">
         <f>INDEX(oratings, 1, 1+MOD(Table3[[#This Row],[Rep '#]]-1, COUNT(oratings)))</f>
         <v>0.1</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="17">
         <f>INDEX(dratings, 1, MOD(FLOOR( (Table3[[#This Row],[Rep '#]]-1) / COUNT(oratings), 1), COUNT(dratings))+1)</f>
         <v>1</v>
       </c>
-      <c r="D14">
-        <f>Table3[[#This Row],[offense]]*0.1+0.05</f>
+      <c r="D14" s="17">
+        <f>Table3[[#This Row],[offense]]*$D$25+0.05</f>
         <v>6.0000000000000005E-2</v>
       </c>
-      <c r="E14">
-        <f>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*0.1</f>
+      <c r="E14" s="17">
+        <f>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*$E$25</f>
         <v>1.5000000000000003E-2</v>
       </c>
-      <c r="F14">
-        <f>Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90</f>
+      <c r="F14" s="17">
+        <f>MAX(Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90, 0)</f>
         <v>5.3190000000000008</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="17">
         <f>1.1 - Table3[[#This Row],[defense]]*0.1</f>
         <v>1</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="17">
         <f xml:space="preserve"> 0.01 - 0.0025 *  Table3[[#This Row],[defense]]</f>
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="17">
         <f>1 / Table3[[#This Row],[throw speed (s/ft)]] * ((60 * 60)/5280)</f>
         <v>90.909090909090907</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="17">
         <f>Table3[[#This Row],[pickoff manuver (s)]]+60*Table3[[#This Row],[throw speed (s/ft)]]</f>
         <v>1.45</v>
       </c>
-      <c r="K14">
-        <f>1-0.1*Table3[[#This Row],[offense]]</f>
-        <v>0.99</v>
-      </c>
-      <c r="L14">
-        <f>0.05 - Table3[[#This Row],[offense]]*0.015</f>
-        <v>4.8500000000000001E-2</v>
-      </c>
-      <c r="M14">
+      <c r="K14" s="17">
+        <f>$K$27-$K$25*Table3[[#This Row],[offense]]</f>
+        <v>0.88</v>
+      </c>
+      <c r="L14" s="17">
+        <f>0.05 - Table3[[#This Row],[offense]]*$L$25</f>
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="M14" s="17">
         <f>1 / Table3[[#This Row],[runner speed (s/ft)]] * ((60 * 60)/5280)</f>
-        <v>14.058106841611993</v>
-      </c>
-      <c r="N14">
+        <v>13.914656771799628</v>
+      </c>
+      <c r="N14" s="17">
         <f>Table3[[#This Row],[runner reaction]]+Table3[[#This Row],[runner speed (s/ft)]]*Table3[[#This Row],[total leadoff (ft)]]</f>
-        <v>1.2479715</v>
-      </c>
-      <c r="O14" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]&gt;Table3[[#This Row],[pickoff time]]</f>
-        <v>0</v>
-      </c>
-      <c r="P14" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]+2*$P$4 &gt; Table3[[#This Row],[pickoff time]]</f>
+        <v>1.140631</v>
+      </c>
+      <c r="O14" s="18">
+        <f>1 - _xlfn.NORM.DIST(Table3[[#This Row],[pickoff time]], Table3[[#This Row],[pickoff evade time]], $O$4, TRUE)</f>
+        <v>6.0950313073531937E-2</v>
+      </c>
+      <c r="P14" s="54">
+        <f>_xlfn.NORM.DIST(Table3[[#This Row],[defense]], $P$25, $P$26, TRUE)</f>
+        <v>0.99068720985629855</v>
+      </c>
+      <c r="Q14" s="17" t="b">
+        <f>Table3[[#This Row],[pickoff probability]] &gt; 1-Table3[[#This Row],[Fielding Odds]]</f>
         <v>1</v>
       </c>
-      <c r="Q14" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]+3*$P$4 &gt; Table3[[#This Row],[pickoff time]]</f>
-        <v>1</v>
+      <c r="R14" s="54">
+        <f>1-Table3[[#This Row],[Fielding Odds]]</f>
+        <v>9.3127901437014549E-3</v>
+      </c>
+      <c r="S14" s="17">
+        <f>(90-Table3[[#This Row],[total leadoff (ft)]])*Table3[[#This Row],[runner speed (s/ft)]]</f>
+        <v>4.1493690000000001</v>
+      </c>
+      <c r="T14" s="17">
+        <f>$T$25*(2-Table3[[#This Row],[defense]]) + Table3[[#This Row],[pickoff time]]</f>
+        <v>1.65</v>
+      </c>
+      <c r="U14" s="54">
+        <f>_xlfn.NORM.DIST(Table3[[#This Row],[Response speed]], Table3[[#This Row],[Blatant steal time]], $U$4, TRUE)</f>
+        <v>1.5525717333822399E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="15" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
         <f>ROW()-ROW(home)</f>
         <v>10</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="6">
         <f>INDEX(oratings, 1, 1+MOD(Table3[[#This Row],[Rep '#]]-1, COUNT(oratings)))</f>
         <v>0.5</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="6">
         <f>INDEX(dratings, 1, MOD(FLOOR( (Table3[[#This Row],[Rep '#]]-1) / COUNT(oratings), 1), COUNT(dratings))+1)</f>
         <v>1</v>
       </c>
-      <c r="D15">
-        <f>Table3[[#This Row],[offense]]*0.1+0.05</f>
+      <c r="D15" s="6">
+        <f>Table3[[#This Row],[offense]]*$D$25+0.05</f>
         <v>0.1</v>
       </c>
-      <c r="E15">
-        <f>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*0.1</f>
+      <c r="E15" s="6">
+        <f>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*$E$25</f>
         <v>7.5000000000000011E-2</v>
       </c>
-      <c r="F15">
-        <f>Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90</f>
+      <c r="F15" s="6">
+        <f>MAX(Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90, 0)</f>
         <v>8.3250000000000011</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="6">
         <f>1.1 - Table3[[#This Row],[defense]]*0.1</f>
         <v>1</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="6">
         <f xml:space="preserve"> 0.01 - 0.0025 *  Table3[[#This Row],[defense]]</f>
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="6">
         <f>1 / Table3[[#This Row],[throw speed (s/ft)]] * ((60 * 60)/5280)</f>
         <v>90.909090909090907</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="6">
         <f>Table3[[#This Row],[pickoff manuver (s)]]+60*Table3[[#This Row],[throw speed (s/ft)]]</f>
         <v>1.45</v>
       </c>
-      <c r="K15">
-        <f>1-0.1*Table3[[#This Row],[offense]]</f>
-        <v>0.95</v>
-      </c>
-      <c r="L15">
-        <f>0.05 - Table3[[#This Row],[offense]]*0.015</f>
-        <v>4.2500000000000003E-2</v>
-      </c>
-      <c r="M15">
+      <c r="K15" s="6">
+        <f>$K$27-$K$25*Table3[[#This Row],[offense]]</f>
+        <v>0.8</v>
+      </c>
+      <c r="L15" s="6">
+        <f>0.05 - Table3[[#This Row],[offense]]*$L$25</f>
+        <v>4.5000000000000005E-2</v>
+      </c>
+      <c r="M15" s="6">
         <f>1 / Table3[[#This Row],[runner speed (s/ft)]] * ((60 * 60)/5280)</f>
-        <v>16.042780748663098</v>
-      </c>
-      <c r="N15">
+        <v>15.151515151515147</v>
+      </c>
+      <c r="N15" s="6">
         <f>Table3[[#This Row],[runner reaction]]+Table3[[#This Row],[runner speed (s/ft)]]*Table3[[#This Row],[total leadoff (ft)]]</f>
-        <v>1.3038125</v>
-      </c>
-      <c r="O15" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]&gt;Table3[[#This Row],[pickoff time]]</f>
-        <v>0</v>
-      </c>
-      <c r="P15" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]+2*$P$4 &gt; Table3[[#This Row],[pickoff time]]</f>
+        <v>1.1746250000000003</v>
+      </c>
+      <c r="O15" s="9">
+        <f>1 - _xlfn.NORM.DIST(Table3[[#This Row],[pickoff time]], Table3[[#This Row],[pickoff evade time]], $O$4, TRUE)</f>
+        <v>8.4275448865239744E-2</v>
+      </c>
+      <c r="P15" s="55">
+        <f>_xlfn.NORM.DIST(Table3[[#This Row],[defense]], $P$25, $P$26, TRUE)</f>
+        <v>0.99068720985629855</v>
+      </c>
+      <c r="Q15" s="6" t="b">
+        <f>Table3[[#This Row],[pickoff probability]] &gt; 1-Table3[[#This Row],[Fielding Odds]]</f>
         <v>1</v>
       </c>
-      <c r="Q15" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]+3*$P$4 &gt; Table3[[#This Row],[pickoff time]]</f>
-        <v>1</v>
+      <c r="R15" s="55">
+        <f>1-Table3[[#This Row],[Fielding Odds]]</f>
+        <v>9.3127901437014549E-3</v>
+      </c>
+      <c r="S15" s="6">
+        <f>(90-Table3[[#This Row],[total leadoff (ft)]])*Table3[[#This Row],[runner speed (s/ft)]]</f>
+        <v>3.6753750000000003</v>
+      </c>
+      <c r="T15" s="6">
+        <f>$T$25*(2-Table3[[#This Row],[defense]]) + Table3[[#This Row],[pickoff time]]</f>
+        <v>1.65</v>
+      </c>
+      <c r="U15" s="55">
+        <f>_xlfn.NORM.DIST(Table3[[#This Row],[Response speed]], Table3[[#This Row],[Blatant steal time]], $U$4, TRUE)</f>
+        <v>3.682411384506767E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+    <row r="16" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="22">
         <f>ROW()-ROW(home)</f>
         <v>11</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="23">
         <f>INDEX(oratings, 1, 1+MOD(Table3[[#This Row],[Rep '#]]-1, COUNT(oratings)))</f>
         <v>1</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="23">
         <f>INDEX(dratings, 1, MOD(FLOOR( (Table3[[#This Row],[Rep '#]]-1) / COUNT(oratings), 1), COUNT(dratings))+1)</f>
         <v>1</v>
       </c>
-      <c r="D16" s="5">
-        <f>Table3[[#This Row],[offense]]*0.1+0.05</f>
+      <c r="D16" s="23">
+        <f>Table3[[#This Row],[offense]]*$D$25+0.05</f>
         <v>0.15000000000000002</v>
       </c>
-      <c r="E16" s="5">
-        <f>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*0.1</f>
+      <c r="E16" s="23">
+        <f>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*$E$25</f>
         <v>0.15000000000000002</v>
       </c>
-      <c r="F16" s="5">
-        <f>Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90</f>
+      <c r="F16" s="23">
+        <f>MAX(Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90, 0)</f>
         <v>11.475</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16" s="23">
         <f>1.1 - Table3[[#This Row],[defense]]*0.1</f>
         <v>1</v>
       </c>
-      <c r="H16" s="5">
+      <c r="H16" s="23">
         <f xml:space="preserve"> 0.01 - 0.0025 *  Table3[[#This Row],[defense]]</f>
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="I16" s="5">
+      <c r="I16" s="23">
         <f>1 / Table3[[#This Row],[throw speed (s/ft)]] * ((60 * 60)/5280)</f>
         <v>90.909090909090907</v>
       </c>
-      <c r="J16" s="5">
+      <c r="J16" s="23">
         <f>Table3[[#This Row],[pickoff manuver (s)]]+60*Table3[[#This Row],[throw speed (s/ft)]]</f>
         <v>1.45</v>
       </c>
-      <c r="K16" s="5">
-        <f>1-0.1*Table3[[#This Row],[offense]]</f>
-        <v>0.9</v>
-      </c>
-      <c r="L16" s="5">
-        <f>0.05 - Table3[[#This Row],[offense]]*0.015</f>
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="M16" s="5">
+      <c r="K16" s="23">
+        <f>$K$27-$K$25*Table3[[#This Row],[offense]]</f>
+        <v>0.7</v>
+      </c>
+      <c r="L16" s="23">
+        <f>0.05 - Table3[[#This Row],[offense]]*$L$25</f>
+        <v>0.04</v>
+      </c>
+      <c r="M16" s="23">
         <f>1 / Table3[[#This Row],[runner speed (s/ft)]] * ((60 * 60)/5280)</f>
-        <v>19.480519480519479</v>
-      </c>
-      <c r="N16" s="5">
+        <v>17.045454545454543</v>
+      </c>
+      <c r="N16" s="23">
         <f>Table3[[#This Row],[runner reaction]]+Table3[[#This Row],[runner speed (s/ft)]]*Table3[[#This Row],[total leadoff (ft)]]</f>
-        <v>1.301625</v>
-      </c>
-      <c r="O16" s="5" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]&gt;Table3[[#This Row],[pickoff time]]</f>
-        <v>0</v>
-      </c>
-      <c r="P16" s="5" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]+2*$P$4 &gt; Table3[[#This Row],[pickoff time]]</f>
+        <v>1.159</v>
+      </c>
+      <c r="O16" s="24">
+        <f>1 - _xlfn.NORM.DIST(Table3[[#This Row],[pickoff time]], Table3[[#This Row],[pickoff evade time]], $O$4, TRUE)</f>
+        <v>7.2834630749186058E-2</v>
+      </c>
+      <c r="P16" s="56">
+        <f>_xlfn.NORM.DIST(Table3[[#This Row],[defense]], $P$25, $P$26, TRUE)</f>
+        <v>0.99068720985629855</v>
+      </c>
+      <c r="Q16" s="23" t="b">
+        <f>Table3[[#This Row],[pickoff probability]] &gt; 1-Table3[[#This Row],[Fielding Odds]]</f>
         <v>1</v>
       </c>
-      <c r="Q16" s="5" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]+3*$P$4 &gt; Table3[[#This Row],[pickoff time]]</f>
-        <v>1</v>
+      <c r="R16" s="56">
+        <f>1-Table3[[#This Row],[Fielding Odds]]</f>
+        <v>9.3127901437014549E-3</v>
+      </c>
+      <c r="S16" s="23">
+        <f>(90-Table3[[#This Row],[total leadoff (ft)]])*Table3[[#This Row],[runner speed (s/ft)]]</f>
+        <v>3.1410000000000005</v>
+      </c>
+      <c r="T16" s="23">
+        <f>$T$25*(2-Table3[[#This Row],[defense]]) + Table3[[#This Row],[pickoff time]]</f>
+        <v>1.65</v>
+      </c>
+      <c r="U16" s="56">
+        <f>_xlfn.NORM.DIST(Table3[[#This Row],[Response speed]], Table3[[#This Row],[Blatant steal time]], $U$4, TRUE)</f>
+        <v>6.4775717318678221E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="17" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
         <f>ROW()-ROW(home)</f>
         <v>12</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="6">
         <f>INDEX(oratings, 1, 1+MOD(Table3[[#This Row],[Rep '#]]-1, COUNT(oratings)))</f>
         <v>2</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="6">
         <f>INDEX(dratings, 1, MOD(FLOOR( (Table3[[#This Row],[Rep '#]]-1) / COUNT(oratings), 1), COUNT(dratings))+1)</f>
         <v>1</v>
       </c>
-      <c r="D17">
-        <f>Table3[[#This Row],[offense]]*0.1+0.05</f>
+      <c r="D17" s="6">
+        <f>Table3[[#This Row],[offense]]*$D$25+0.05</f>
         <v>0.25</v>
       </c>
-      <c r="E17">
-        <f>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*0.1</f>
+      <c r="E17" s="6">
+        <f>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*$E$25</f>
         <v>0.30000000000000004</v>
       </c>
-      <c r="F17">
-        <f>Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90</f>
+      <c r="F17" s="6">
+        <f>MAX(Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90, 0)</f>
         <v>15.749999999999998</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="6">
         <f>1.1 - Table3[[#This Row],[defense]]*0.1</f>
         <v>1</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="6">
         <f xml:space="preserve"> 0.01 - 0.0025 *  Table3[[#This Row],[defense]]</f>
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="6">
         <f>1 / Table3[[#This Row],[throw speed (s/ft)]] * ((60 * 60)/5280)</f>
         <v>90.909090909090907</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="6">
         <f>Table3[[#This Row],[pickoff manuver (s)]]+60*Table3[[#This Row],[throw speed (s/ft)]]</f>
         <v>1.45</v>
       </c>
-      <c r="K17">
-        <f>1-0.1*Table3[[#This Row],[offense]]</f>
-        <v>0.8</v>
-      </c>
-      <c r="L17">
-        <f>0.05 - Table3[[#This Row],[offense]]*0.015</f>
-        <v>2.0000000000000004E-2</v>
-      </c>
-      <c r="M17">
+      <c r="K17" s="6">
+        <f>$K$27-$K$25*Table3[[#This Row],[offense]]</f>
+        <v>0.5</v>
+      </c>
+      <c r="L17" s="6">
+        <f>0.05 - Table3[[#This Row],[offense]]*$L$25</f>
+        <v>3.0000000000000002E-2</v>
+      </c>
+      <c r="M17" s="6">
         <f>1 / Table3[[#This Row],[runner speed (s/ft)]] * ((60 * 60)/5280)</f>
-        <v>34.090909090909086</v>
-      </c>
-      <c r="N17">
+        <v>22.727272727272723</v>
+      </c>
+      <c r="N17" s="6">
         <f>Table3[[#This Row],[runner reaction]]+Table3[[#This Row],[runner speed (s/ft)]]*Table3[[#This Row],[total leadoff (ft)]]</f>
-        <v>1.115</v>
-      </c>
-      <c r="O17" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]&gt;Table3[[#This Row],[pickoff time]]</f>
+        <v>0.97249999999999992</v>
+      </c>
+      <c r="O17" s="9">
+        <f>1 - _xlfn.NORM.DIST(Table3[[#This Row],[pickoff time]], Table3[[#This Row],[pickoff evade time]], $O$4, TRUE)</f>
+        <v>8.4817013785601914E-3</v>
+      </c>
+      <c r="P17" s="55">
+        <f>_xlfn.NORM.DIST(Table3[[#This Row],[defense]], $P$25, $P$26, TRUE)</f>
+        <v>0.99068720985629855</v>
+      </c>
+      <c r="Q17" s="6" t="b">
+        <f>Table3[[#This Row],[pickoff probability]] &gt; 1-Table3[[#This Row],[Fielding Odds]]</f>
         <v>0</v>
       </c>
-      <c r="P17" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]+2*$P$4 &gt; Table3[[#This Row],[pickoff time]]</f>
-        <v>0</v>
-      </c>
-      <c r="Q17" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]+3*$P$4 &gt; Table3[[#This Row],[pickoff time]]</f>
-        <v>1</v>
+      <c r="R17" s="55">
+        <f>1-Table3[[#This Row],[Fielding Odds]]</f>
+        <v>9.3127901437014549E-3</v>
+      </c>
+      <c r="S17" s="6">
+        <f>(90-Table3[[#This Row],[total leadoff (ft)]])*Table3[[#This Row],[runner speed (s/ft)]]</f>
+        <v>2.2275</v>
+      </c>
+      <c r="T17" s="6">
+        <f>$T$25*(2-Table3[[#This Row],[defense]]) + Table3[[#This Row],[pickoff time]]</f>
+        <v>1.65</v>
+      </c>
+      <c r="U17" s="55">
+        <f>_xlfn.NORM.DIST(Table3[[#This Row],[Response speed]], Table3[[#This Row],[Blatant steal time]], $U$4, TRUE)</f>
+        <v>0.16789925159767624</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="18" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15">
         <f>ROW()-ROW(home)</f>
         <v>13</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="15">
         <f>INDEX(oratings, 1, 1+MOD(Table3[[#This Row],[Rep '#]]-1, COUNT(oratings)))</f>
         <v>0.1</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="15">
         <f>INDEX(dratings, 1, MOD(FLOOR( (Table3[[#This Row],[Rep '#]]-1) / COUNT(oratings), 1), COUNT(dratings))+1)</f>
         <v>2</v>
       </c>
-      <c r="D18">
-        <f>Table3[[#This Row],[offense]]*0.1+0.05</f>
+      <c r="D18" s="15">
+        <f>Table3[[#This Row],[offense]]*$D$25+0.05</f>
         <v>6.0000000000000005E-2</v>
       </c>
-      <c r="E18">
-        <f>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*0.1</f>
+      <c r="E18" s="15">
+        <f>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*$E$25</f>
         <v>4.5000000000000005E-2</v>
       </c>
-      <c r="F18">
-        <f>Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90</f>
+      <c r="F18" s="15">
+        <f>MAX(Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90, 0)</f>
         <v>5.157</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="15">
         <f>1.1 - Table3[[#This Row],[defense]]*0.1</f>
         <v>0.90000000000000013</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="15">
         <f xml:space="preserve"> 0.01 - 0.0025 *  Table3[[#This Row],[defense]]</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="15">
         <f>1 / Table3[[#This Row],[throw speed (s/ft)]] * ((60 * 60)/5280)</f>
         <v>136.36363636363635</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="15">
         <f>Table3[[#This Row],[pickoff manuver (s)]]+60*Table3[[#This Row],[throw speed (s/ft)]]</f>
         <v>1.2000000000000002</v>
       </c>
-      <c r="K18">
-        <f>1-0.1*Table3[[#This Row],[offense]]</f>
-        <v>0.99</v>
-      </c>
-      <c r="L18">
-        <f>0.05 - Table3[[#This Row],[offense]]*0.015</f>
-        <v>4.8500000000000001E-2</v>
-      </c>
-      <c r="M18">
+      <c r="K18" s="15">
+        <f>$K$27-$K$25*Table3[[#This Row],[offense]]</f>
+        <v>0.88</v>
+      </c>
+      <c r="L18" s="15">
+        <f>0.05 - Table3[[#This Row],[offense]]*$L$25</f>
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="M18" s="15">
         <f>1 / Table3[[#This Row],[runner speed (s/ft)]] * ((60 * 60)/5280)</f>
-        <v>14.058106841611993</v>
-      </c>
-      <c r="N18">
+        <v>13.914656771799628</v>
+      </c>
+      <c r="N18" s="15">
         <f>Table3[[#This Row],[runner reaction]]+Table3[[#This Row],[runner speed (s/ft)]]*Table3[[#This Row],[total leadoff (ft)]]</f>
-        <v>1.2401145</v>
-      </c>
-      <c r="O18" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]&gt;Table3[[#This Row],[pickoff time]]</f>
+        <v>1.1326929999999999</v>
+      </c>
+      <c r="O18" s="16">
+        <f>1 - _xlfn.NORM.DIST(Table3[[#This Row],[pickoff time]], Table3[[#This Row],[pickoff evade time]], $O$4, TRUE)</f>
+        <v>0.36823373145283722</v>
+      </c>
+      <c r="P18" s="57">
+        <f>_xlfn.NORM.DIST(Table3[[#This Row],[defense]], $P$25, $P$26, TRUE)</f>
+        <v>0.99836515899365319</v>
+      </c>
+      <c r="Q18" s="15" t="b">
+        <f>Table3[[#This Row],[pickoff probability]] &gt; 1-Table3[[#This Row],[Fielding Odds]]</f>
         <v>1</v>
       </c>
-      <c r="P18" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]+2*$P$4 &gt; Table3[[#This Row],[pickoff time]]</f>
-        <v>1</v>
-      </c>
-      <c r="Q18" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]+3*$P$4 &gt; Table3[[#This Row],[pickoff time]]</f>
-        <v>1</v>
+      <c r="R18" s="57">
+        <f>1-Table3[[#This Row],[Fielding Odds]]</f>
+        <v>1.63484100634681E-3</v>
+      </c>
+      <c r="S18" s="15">
+        <f>(90-Table3[[#This Row],[total leadoff (ft)]])*Table3[[#This Row],[runner speed (s/ft)]]</f>
+        <v>4.1573070000000003</v>
+      </c>
+      <c r="T18" s="15">
+        <f>$T$25*(2-Table3[[#This Row],[defense]]) + Table3[[#This Row],[pickoff time]]</f>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="U18" s="57">
+        <f>_xlfn.NORM.DIST(Table3[[#This Row],[Response speed]], Table3[[#This Row],[Blatant steal time]], $U$4, TRUE)</f>
+        <v>4.1358582187294249E-7</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="19" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="11">
         <f>ROW()-ROW(home)</f>
         <v>14</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="11">
         <f>INDEX(oratings, 1, 1+MOD(Table3[[#This Row],[Rep '#]]-1, COUNT(oratings)))</f>
         <v>0.5</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="11">
         <f>INDEX(dratings, 1, MOD(FLOOR( (Table3[[#This Row],[Rep '#]]-1) / COUNT(oratings), 1), COUNT(dratings))+1)</f>
         <v>2</v>
       </c>
-      <c r="D19">
-        <f>Table3[[#This Row],[offense]]*0.1+0.05</f>
+      <c r="D19" s="11">
+        <f>Table3[[#This Row],[offense]]*$D$25+0.05</f>
         <v>0.1</v>
       </c>
-      <c r="E19">
-        <f>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*0.1</f>
+      <c r="E19" s="11">
+        <f>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*$E$25</f>
         <v>0.22500000000000001</v>
       </c>
-      <c r="F19">
-        <f>Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90</f>
+      <c r="F19" s="11">
+        <f>MAX(Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90, 0)</f>
         <v>6.9750000000000014</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="11">
         <f>1.1 - Table3[[#This Row],[defense]]*0.1</f>
         <v>0.90000000000000013</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="11">
         <f xml:space="preserve"> 0.01 - 0.0025 *  Table3[[#This Row],[defense]]</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="11">
         <f>1 / Table3[[#This Row],[throw speed (s/ft)]] * ((60 * 60)/5280)</f>
         <v>136.36363636363635</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="11">
         <f>Table3[[#This Row],[pickoff manuver (s)]]+60*Table3[[#This Row],[throw speed (s/ft)]]</f>
         <v>1.2000000000000002</v>
       </c>
-      <c r="K19">
-        <f>1-0.1*Table3[[#This Row],[offense]]</f>
-        <v>0.95</v>
-      </c>
-      <c r="L19">
-        <f>0.05 - Table3[[#This Row],[offense]]*0.015</f>
-        <v>4.2500000000000003E-2</v>
-      </c>
-      <c r="M19">
+      <c r="K19" s="11">
+        <f>$K$27-$K$25*Table3[[#This Row],[offense]]</f>
+        <v>0.8</v>
+      </c>
+      <c r="L19" s="11">
+        <f>0.05 - Table3[[#This Row],[offense]]*$L$25</f>
+        <v>4.5000000000000005E-2</v>
+      </c>
+      <c r="M19" s="11">
         <f>1 / Table3[[#This Row],[runner speed (s/ft)]] * ((60 * 60)/5280)</f>
-        <v>16.042780748663098</v>
-      </c>
-      <c r="N19">
+        <v>15.151515151515147</v>
+      </c>
+      <c r="N19" s="11">
         <f>Table3[[#This Row],[runner reaction]]+Table3[[#This Row],[runner speed (s/ft)]]*Table3[[#This Row],[total leadoff (ft)]]</f>
-        <v>1.2464375000000001</v>
-      </c>
-      <c r="O19" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]&gt;Table3[[#This Row],[pickoff time]]</f>
+        <v>1.1138750000000002</v>
+      </c>
+      <c r="O19" s="12">
+        <f>1 - _xlfn.NORM.DIST(Table3[[#This Row],[pickoff time]], Table3[[#This Row],[pickoff evade time]], $O$4, TRUE)</f>
+        <v>0.33337053015354379</v>
+      </c>
+      <c r="P19" s="58">
+        <f>_xlfn.NORM.DIST(Table3[[#This Row],[defense]], $P$25, $P$26, TRUE)</f>
+        <v>0.99836515899365319</v>
+      </c>
+      <c r="Q19" s="11" t="b">
+        <f>Table3[[#This Row],[pickoff probability]] &gt; 1-Table3[[#This Row],[Fielding Odds]]</f>
         <v>1</v>
       </c>
-      <c r="P19" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]+2*$P$4 &gt; Table3[[#This Row],[pickoff time]]</f>
-        <v>1</v>
-      </c>
-      <c r="Q19" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]+3*$P$4 &gt; Table3[[#This Row],[pickoff time]]</f>
-        <v>1</v>
+      <c r="R19" s="58">
+        <f>1-Table3[[#This Row],[Fielding Odds]]</f>
+        <v>1.63484100634681E-3</v>
+      </c>
+      <c r="S19" s="11">
+        <f>(90-Table3[[#This Row],[total leadoff (ft)]])*Table3[[#This Row],[runner speed (s/ft)]]</f>
+        <v>3.7361250000000008</v>
+      </c>
+      <c r="T19" s="11">
+        <f>$T$25*(2-Table3[[#This Row],[defense]]) + Table3[[#This Row],[pickoff time]]</f>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="U19" s="58">
+        <f>_xlfn.NORM.DIST(Table3[[#This Row],[Response speed]], Table3[[#This Row],[Blatant steal time]], $U$4, TRUE)</f>
+        <v>1.1847960716990601E-5</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="20" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="15">
         <f>ROW()-ROW(home)</f>
         <v>15</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="15">
         <f>INDEX(oratings, 1, 1+MOD(Table3[[#This Row],[Rep '#]]-1, COUNT(oratings)))</f>
         <v>1</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="15">
         <f>INDEX(dratings, 1, MOD(FLOOR( (Table3[[#This Row],[Rep '#]]-1) / COUNT(oratings), 1), COUNT(dratings))+1)</f>
         <v>2</v>
       </c>
-      <c r="D20">
-        <f>Table3[[#This Row],[offense]]*0.1+0.05</f>
+      <c r="D20" s="15">
+        <f>Table3[[#This Row],[offense]]*$D$25+0.05</f>
         <v>0.15000000000000002</v>
       </c>
-      <c r="E20">
-        <f>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*0.1</f>
+      <c r="E20" s="15">
+        <f>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*$E$25</f>
         <v>0.45</v>
       </c>
-      <c r="F20">
-        <f>Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90</f>
+      <c r="F20" s="15">
+        <f>MAX(Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90, 0)</f>
         <v>7.4250000000000016</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="15">
         <f>1.1 - Table3[[#This Row],[defense]]*0.1</f>
         <v>0.90000000000000013</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="15">
         <f xml:space="preserve"> 0.01 - 0.0025 *  Table3[[#This Row],[defense]]</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="15">
         <f>1 / Table3[[#This Row],[throw speed (s/ft)]] * ((60 * 60)/5280)</f>
         <v>136.36363636363635</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="15">
         <f>Table3[[#This Row],[pickoff manuver (s)]]+60*Table3[[#This Row],[throw speed (s/ft)]]</f>
         <v>1.2000000000000002</v>
       </c>
-      <c r="K20">
-        <f>1-0.1*Table3[[#This Row],[offense]]</f>
-        <v>0.9</v>
-      </c>
-      <c r="L20">
-        <f>0.05 - Table3[[#This Row],[offense]]*0.015</f>
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="M20">
+      <c r="K20" s="15">
+        <f>$K$27-$K$25*Table3[[#This Row],[offense]]</f>
+        <v>0.7</v>
+      </c>
+      <c r="L20" s="15">
+        <f>0.05 - Table3[[#This Row],[offense]]*$L$25</f>
+        <v>0.04</v>
+      </c>
+      <c r="M20" s="15">
         <f>1 / Table3[[#This Row],[runner speed (s/ft)]] * ((60 * 60)/5280)</f>
-        <v>19.480519480519479</v>
-      </c>
-      <c r="N20">
+        <v>17.045454545454543</v>
+      </c>
+      <c r="N20" s="15">
         <f>Table3[[#This Row],[runner reaction]]+Table3[[#This Row],[runner speed (s/ft)]]*Table3[[#This Row],[total leadoff (ft)]]</f>
-        <v>1.159875</v>
-      </c>
-      <c r="O20" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]&gt;Table3[[#This Row],[pickoff time]]</f>
-        <v>0</v>
-      </c>
-      <c r="P20" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]+2*$P$4 &gt; Table3[[#This Row],[pickoff time]]</f>
+        <v>0.99700000000000011</v>
+      </c>
+      <c r="O20" s="16">
+        <f>1 - _xlfn.NORM.DIST(Table3[[#This Row],[pickoff time]], Table3[[#This Row],[pickoff evade time]], $O$4, TRUE)</f>
+        <v>0.15505291375244945</v>
+      </c>
+      <c r="P20" s="57">
+        <f>_xlfn.NORM.DIST(Table3[[#This Row],[defense]], $P$25, $P$26, TRUE)</f>
+        <v>0.99836515899365319</v>
+      </c>
+      <c r="Q20" s="15" t="b">
+        <f>Table3[[#This Row],[pickoff probability]] &gt; 1-Table3[[#This Row],[Fielding Odds]]</f>
         <v>1</v>
       </c>
-      <c r="Q20" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]+3*$P$4 &gt; Table3[[#This Row],[pickoff time]]</f>
-        <v>1</v>
+      <c r="R20" s="57">
+        <f>1-Table3[[#This Row],[Fielding Odds]]</f>
+        <v>1.63484100634681E-3</v>
+      </c>
+      <c r="S20" s="15">
+        <f>(90-Table3[[#This Row],[total leadoff (ft)]])*Table3[[#This Row],[runner speed (s/ft)]]</f>
+        <v>3.3030000000000004</v>
+      </c>
+      <c r="T20" s="15">
+        <f>$T$25*(2-Table3[[#This Row],[defense]]) + Table3[[#This Row],[pickoff time]]</f>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="U20" s="57">
+        <f>_xlfn.NORM.DIST(Table3[[#This Row],[Response speed]], Table3[[#This Row],[Blatant steal time]], $U$4, TRUE)</f>
+        <v>2.2830364162715008E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
+    <row r="21" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="19">
         <f>ROW()-ROW(home)</f>
         <v>16</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="20">
         <f>INDEX(oratings, 1, 1+MOD(Table3[[#This Row],[Rep '#]]-1, COUNT(oratings)))</f>
         <v>2</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="20">
         <f>INDEX(dratings, 1, MOD(FLOOR( (Table3[[#This Row],[Rep '#]]-1) / COUNT(oratings), 1), COUNT(dratings))+1)</f>
         <v>2</v>
       </c>
-      <c r="D21" s="6">
-        <f>Table3[[#This Row],[offense]]*0.1+0.05</f>
+      <c r="D21" s="20">
+        <f>Table3[[#This Row],[offense]]*$D$25+0.05</f>
         <v>0.25</v>
       </c>
-      <c r="E21" s="6">
-        <f>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*0.1</f>
+      <c r="E21" s="20">
+        <f>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*$E$25</f>
         <v>0.9</v>
       </c>
-      <c r="F21" s="6">
-        <f>Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90</f>
+      <c r="F21" s="20">
+        <f>MAX(Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90, 0)</f>
         <v>2.2499999999999996</v>
       </c>
-      <c r="G21" s="6">
+      <c r="G21" s="20">
         <f>1.1 - Table3[[#This Row],[defense]]*0.1</f>
         <v>0.90000000000000013</v>
       </c>
-      <c r="H21" s="6">
+      <c r="H21" s="20">
         <f xml:space="preserve"> 0.01 - 0.0025 *  Table3[[#This Row],[defense]]</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="I21" s="6">
+      <c r="I21" s="20">
         <f>1 / Table3[[#This Row],[throw speed (s/ft)]] * ((60 * 60)/5280)</f>
         <v>136.36363636363635</v>
       </c>
-      <c r="J21" s="6">
+      <c r="J21" s="20">
         <f>Table3[[#This Row],[pickoff manuver (s)]]+60*Table3[[#This Row],[throw speed (s/ft)]]</f>
         <v>1.2000000000000002</v>
       </c>
-      <c r="K21" s="6">
-        <f>1-0.1*Table3[[#This Row],[offense]]</f>
-        <v>0.8</v>
-      </c>
-      <c r="L21" s="6">
-        <f>0.05 - Table3[[#This Row],[offense]]*0.015</f>
-        <v>2.0000000000000004E-2</v>
-      </c>
-      <c r="M21" s="6">
+      <c r="K21" s="20">
+        <f>$K$27-$K$25*Table3[[#This Row],[offense]]</f>
+        <v>0.5</v>
+      </c>
+      <c r="L21" s="20">
+        <f>0.05 - Table3[[#This Row],[offense]]*$L$25</f>
+        <v>3.0000000000000002E-2</v>
+      </c>
+      <c r="M21" s="20">
         <f>1 / Table3[[#This Row],[runner speed (s/ft)]] * ((60 * 60)/5280)</f>
-        <v>34.090909090909086</v>
-      </c>
-      <c r="N21" s="6">
+        <v>22.727272727272723</v>
+      </c>
+      <c r="N21" s="20">
         <f>Table3[[#This Row],[runner reaction]]+Table3[[#This Row],[runner speed (s/ft)]]*Table3[[#This Row],[total leadoff (ft)]]</f>
-        <v>0.84500000000000008</v>
-      </c>
-      <c r="O21" s="6" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]&gt;Table3[[#This Row],[pickoff time]]</f>
+        <v>0.5675</v>
+      </c>
+      <c r="O21" s="21">
+        <f>1 - _xlfn.NORM.DIST(Table3[[#This Row],[pickoff time]], Table3[[#This Row],[pickoff evade time]], $O$4, TRUE)</f>
+        <v>7.8210367804876224E-4</v>
+      </c>
+      <c r="P21" s="59">
+        <f>_xlfn.NORM.DIST(Table3[[#This Row],[defense]], $P$25, $P$26, TRUE)</f>
+        <v>0.99836515899365319</v>
+      </c>
+      <c r="Q21" s="20" t="b">
+        <f>Table3[[#This Row],[pickoff probability]] &gt; 1-Table3[[#This Row],[Fielding Odds]]</f>
         <v>0</v>
       </c>
-      <c r="P21" s="6" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]+2*$P$4 &gt; Table3[[#This Row],[pickoff time]]</f>
-        <v>0</v>
-      </c>
-      <c r="Q21" s="6" t="b">
-        <f>Table3[[#This Row],[pickoff evade time]]+3*$P$4 &gt; Table3[[#This Row],[pickoff time]]</f>
-        <v>1</v>
+      <c r="R21" s="59">
+        <f>1-Table3[[#This Row],[Fielding Odds]]</f>
+        <v>1.63484100634681E-3</v>
+      </c>
+      <c r="S21" s="20">
+        <f>(90-Table3[[#This Row],[total leadoff (ft)]])*Table3[[#This Row],[runner speed (s/ft)]]</f>
+        <v>2.6325000000000003</v>
+      </c>
+      <c r="T21" s="20">
+        <f>$T$25*(2-Table3[[#This Row],[defense]]) + Table3[[#This Row],[pickoff time]]</f>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="U21" s="59">
+        <f>_xlfn.NORM.DIST(Table3[[#This Row],[Response speed]], Table3[[#This Row],[Blatant steal time]], $U$4, TRUE)</f>
+        <v>8.4817013785601532E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>98</v>
+      </c>
+      <c r="E24" t="s">
+        <v>99</v>
+      </c>
+      <c r="G24" t="s">
+        <v>91</v>
+      </c>
+      <c r="H24" t="s">
+        <v>92</v>
+      </c>
+      <c r="K24" t="s">
+        <v>93</v>
+      </c>
+      <c r="L24" t="s">
+        <v>94</v>
+      </c>
+      <c r="P24" t="s">
+        <v>112</v>
+      </c>
+      <c r="T24" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>0.1</v>
+      </c>
+      <c r="E25">
+        <v>0.1</v>
+      </c>
+      <c r="G25">
+        <v>0.1</v>
+      </c>
+      <c r="H25">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="K25">
+        <v>0.2</v>
+      </c>
+      <c r="L25">
+        <v>0.01</v>
+      </c>
+      <c r="O25" t="s">
+        <v>96</v>
+      </c>
+      <c r="P25">
+        <v>-3</v>
+      </c>
+      <c r="T25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="K26" t="s">
+        <v>100</v>
+      </c>
+      <c r="O26" t="s">
+        <v>104</v>
+      </c>
+      <c r="P26">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="K27">
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="O6:Q21">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="O6:O21">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7738,6 +8442,248 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:S9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T19" sqref="T19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="3:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="38"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="37"/>
+      <c r="R3" s="37"/>
+      <c r="S3" s="38"/>
+    </row>
+    <row r="4" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C4" s="31"/>
+      <c r="D4" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="E4" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="F4" s="32"/>
+      <c r="G4" s="33"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="M4" s="39">
+        <v>-3</v>
+      </c>
+      <c r="N4" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="O4" s="39">
+        <v>1.7</v>
+      </c>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="32"/>
+      <c r="R4" s="32"/>
+      <c r="S4" s="33"/>
+    </row>
+    <row r="5" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C5" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="39">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="E5" s="32">
+        <f>_xlfn.NORM.S.INV(D5)</f>
+        <v>2.1700903775845601</v>
+      </c>
+      <c r="F5" s="32"/>
+      <c r="G5" s="33"/>
+      <c r="K5" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="L5" s="32">
+        <v>0</v>
+      </c>
+      <c r="M5" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="N5" s="32">
+        <v>0.25</v>
+      </c>
+      <c r="O5" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="P5" s="32">
+        <v>0.8</v>
+      </c>
+      <c r="Q5" s="32">
+        <v>1</v>
+      </c>
+      <c r="R5" s="32">
+        <v>1.5</v>
+      </c>
+      <c r="S5" s="33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="31"/>
+      <c r="D6" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" s="39">
+        <v>1</v>
+      </c>
+      <c r="F6" s="32"/>
+      <c r="G6" s="33"/>
+      <c r="K6" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="L6" s="44">
+        <f>_xlfn.NORM.DIST(L5, $M$4, $O$4, TRUE)</f>
+        <v>0.96119339527114878</v>
+      </c>
+      <c r="M6" s="44">
+        <f>_xlfn.NORM.DIST(M5, $M$4, $O$4, TRUE)</f>
+        <v>0.96588837667724492</v>
+      </c>
+      <c r="N6" s="44">
+        <f>_xlfn.NORM.DIST(N5, $M$4, $O$4, TRUE)</f>
+        <v>0.97204680967698576</v>
+      </c>
+      <c r="O6" s="44">
+        <f>_xlfn.NORM.DIST(O5, $M$4, $O$4, TRUE)</f>
+        <v>0.98024442661121902</v>
+      </c>
+      <c r="P6" s="44">
+        <f>_xlfn.NORM.DIST(P5, $M$4, $O$4, TRUE)</f>
+        <v>0.98730097700023178</v>
+      </c>
+      <c r="Q6" s="44">
+        <f>_xlfn.NORM.DIST(Q5, $M$4, $O$4, TRUE)</f>
+        <v>0.99068720985629855</v>
+      </c>
+      <c r="R6" s="44">
+        <f>_xlfn.NORM.DIST(R5, $M$4, $O$4, TRUE)</f>
+        <v>0.99594023860462444</v>
+      </c>
+      <c r="S6" s="45">
+        <f>_xlfn.NORM.DIST(S5, $M$4, $O$4, TRUE)</f>
+        <v>0.99836515899365319</v>
+      </c>
+    </row>
+    <row r="7" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="31"/>
+      <c r="D7" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="E7" s="39">
+        <v>0.7</v>
+      </c>
+      <c r="F7" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="G7" s="40">
+        <v>0.36477409900000002</v>
+      </c>
+      <c r="K7" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="L7" s="39"/>
+      <c r="M7" s="39">
+        <v>0.95</v>
+      </c>
+      <c r="N7" s="39"/>
+      <c r="O7" s="39">
+        <v>0.97</v>
+      </c>
+      <c r="P7" s="39"/>
+      <c r="Q7" s="39">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="R7" s="39"/>
+      <c r="S7" s="40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="34"/>
+      <c r="D8" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" s="41">
+        <f>(E6-E7)/E5</f>
+        <v>0.13824309028728929</v>
+      </c>
+      <c r="F8" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="G8" s="42">
+        <f>-E5*G7 + E6</f>
+        <v>0.20840723776802228</v>
+      </c>
+      <c r="K8" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="L8" s="46" t="str">
+        <f>IF(ISBLANK(L7), "", L6-L7)</f>
+        <v/>
+      </c>
+      <c r="M8" s="46">
+        <f>IF(ISBLANK(M7), "", M6-M7)</f>
+        <v>1.5888376677244964E-2</v>
+      </c>
+      <c r="N8" s="46" t="str">
+        <f t="shared" ref="N8:S8" si="0">IF(ISBLANK(N7), "", N6-N7)</f>
+        <v/>
+      </c>
+      <c r="O8" s="46">
+        <f t="shared" si="0"/>
+        <v>1.0244426611219049E-2</v>
+      </c>
+      <c r="P8" s="46" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Q8" s="46">
+        <f t="shared" si="0"/>
+        <v>5.6872098562985585E-3</v>
+      </c>
+      <c r="R8" s="46" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="S8" s="47">
+        <f t="shared" si="0"/>
+        <v>-1.63484100634681E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="3:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB18"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -7748,88 +8694,88 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>24</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>25</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>26</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>27</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>28</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>29</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>30</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>31</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>32</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>33</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>34</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>35</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>36</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>37</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>38</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>39</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>40</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>41</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>42</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>43</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>44</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>45</v>
       </c>
-      <c r="Y1" t="s">
-        <v>46</v>
-      </c>
       <c r="Z1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB1" t="s">
         <v>71</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
@@ -7918,16 +8864,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
       </c>
       <c r="F3">
         <v>41</v>
@@ -8007,16 +8953,16 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
       </c>
       <c r="F4">
         <v>34</v>
@@ -8096,16 +9042,16 @@
         <v>30</v>
       </c>
       <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
         <v>47</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" t="s">
-        <v>16</v>
       </c>
       <c r="F5">
         <v>27</v>
@@ -8185,16 +9131,16 @@
         <v>69</v>
       </c>
       <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
         <v>49</v>
       </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>50</v>
-      </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F6">
         <v>30</v>
@@ -8274,16 +9220,16 @@
         <v>124</v>
       </c>
       <c r="B7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
         <v>51</v>
       </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" t="s">
-        <v>52</v>
-      </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F7">
         <v>25</v>
@@ -8363,16 +9309,16 @@
         <v>338</v>
       </c>
       <c r="B8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" t="s">
         <v>53</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>54</v>
       </c>
-      <c r="D8" t="s">
-        <v>55</v>
-      </c>
       <c r="E8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8">
         <v>26</v>
@@ -8452,16 +9398,16 @@
         <v>388</v>
       </c>
       <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
         <v>56</v>
       </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>57</v>
-      </c>
-      <c r="E9" t="s">
-        <v>58</v>
       </c>
       <c r="F9">
         <v>29</v>
@@ -8541,16 +9487,16 @@
         <v>465</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F10">
         <v>26</v>
@@ -8630,16 +9576,16 @@
         <v>510</v>
       </c>
       <c r="B11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" t="s">
         <v>60</v>
       </c>
-      <c r="C11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D11" t="s">
-        <v>61</v>
-      </c>
       <c r="E11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F11">
         <v>37</v>
@@ -8719,16 +9665,16 @@
         <v>468</v>
       </c>
       <c r="B12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" t="s">
         <v>62</v>
       </c>
-      <c r="C12" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>63</v>
-      </c>
-      <c r="E12" t="s">
-        <v>64</v>
       </c>
       <c r="F12">
         <v>27</v>
@@ -8808,16 +9754,16 @@
         <v>174</v>
       </c>
       <c r="B13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" t="s">
         <v>66</v>
       </c>
-      <c r="C13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" t="s">
-        <v>67</v>
-      </c>
       <c r="E13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F13">
         <v>25</v>
@@ -8897,16 +9843,16 @@
         <v>218</v>
       </c>
       <c r="B14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" t="s">
         <v>68</v>
-      </c>
-      <c r="C14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" t="s">
-        <v>52</v>
-      </c>
-      <c r="E14" t="s">
-        <v>69</v>
       </c>
       <c r="F14">
         <v>25</v>
@@ -8986,16 +9932,16 @@
         <v>275</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F15">
         <v>27</v>
@@ -9187,7 +10133,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F17"/>
   <sheetViews>

</xml_diff>

<commit_message>
pitch math done for now!
</commit_message>
<xml_diff>
--- a/plans/baseball stats.xlsx
+++ b/plans/baseball stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcgiffenk\Desktop\newpy\xtreemblaseball99\plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24DD4418-24DB-4305-B617-38102F732D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2148204-692F-4848-B8AE-6B54289FC49A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,6 +28,8 @@
     <definedName name="home">Table3[[#Headers],[Rep '#]]</definedName>
     <definedName name="ms">#REF!</definedName>
     <definedName name="oratings">iterative!$B$1:$L$1</definedName>
+    <definedName name="pitchmod">iterative!$AN$25</definedName>
+    <definedName name="pitchstdv">iterative!$AN$27</definedName>
     <definedName name="stratfactor">iterative!$E$26</definedName>
     <definedName name="total">#REF!</definedName>
     <definedName name="values">#REF!</definedName>
@@ -366,7 +368,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="217">
   <si>
     <t>Ball</t>
   </si>
@@ -743,30 +745,6 @@
     <t>HR</t>
   </si>
   <si>
-    <t>Column44</t>
-  </si>
-  <si>
-    <t>Column45</t>
-  </si>
-  <si>
-    <t>Column46</t>
-  </si>
-  <si>
-    <t>Column47</t>
-  </si>
-  <si>
-    <t>Column48</t>
-  </si>
-  <si>
-    <t>Column49</t>
-  </si>
-  <si>
-    <t>Column50</t>
-  </si>
-  <si>
-    <t>Column51</t>
-  </si>
-  <si>
     <t>Column52</t>
   </si>
   <si>
@@ -968,10 +946,7 @@
     <t>first pitch bias</t>
   </si>
   <si>
-    <t>Column1</t>
-  </si>
-  <si>
-    <t>Column2</t>
+    <t>called position</t>
   </si>
   <si>
     <t>calling modifier</t>
@@ -998,7 +973,52 @@
     <t>tanh strike percent</t>
   </si>
   <si>
-    <t>XYZZY - called position</t>
+    <t>called pos 0.2 pitch</t>
+  </si>
+  <si>
+    <t>called pos 2 pitch</t>
+  </si>
+  <si>
+    <t>pitch spread modifier</t>
+  </si>
+  <si>
+    <t>pitch spread max stdev</t>
+  </si>
+  <si>
+    <t>the pitch</t>
+  </si>
+  <si>
+    <t>location +1 stdv</t>
+  </si>
+  <si>
+    <t>difficulty</t>
+  </si>
+  <si>
+    <t>min dist to sz 1stdv</t>
+  </si>
+  <si>
+    <t>max dist to sz 1stdv</t>
+  </si>
+  <si>
+    <t>min obscurity</t>
+  </si>
+  <si>
+    <t>max base obsc</t>
+  </si>
+  <si>
+    <t>obsc den factor</t>
+  </si>
+  <si>
+    <t>max obscurity2</t>
+  </si>
+  <si>
+    <t>trickiness factor</t>
+  </si>
+  <si>
+    <t>location -1  stdv</t>
+  </si>
+  <si>
+    <t>ave obscurity</t>
   </si>
 </sst>
 </file>
@@ -1443,7 +1463,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1564,25 +1584,65 @@
     <xf numFmtId="9" fontId="0" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="7" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="10" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="43">
+  <dxfs count="50">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1590,10 +1650,16 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
       <font>
@@ -1614,16 +1680,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1773,9 +1829,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -7283,139 +7336,159 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A6:BE22" totalsRowShown="0" headerRowDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A6:BE22" totalsRowShown="0" headerRowDxfId="49">
   <autoFilter ref="A6:BE22" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="57">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Rep #">
       <calculatedColumnFormula>ROW()-ROW(home)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="offense" dataDxfId="41">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="offense" dataDxfId="48">
       <calculatedColumnFormula>INDEX(oratings, 1, 1+MOD(Table3[[#This Row],[Rep '#]]-1, COUNT(oratings)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="defense" dataDxfId="40">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="defense" dataDxfId="47">
       <calculatedColumnFormula>INDEX(dratings, 1, MOD(FLOOR( (Table3[[#This Row],[Rep '#]]-1) / COUNT(oratings), 1), COUNT(dratings))+1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="base leadoff" dataDxfId="39">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="base leadoff" dataDxfId="46">
       <calculatedColumnFormula>Table3[[#This Row],[offense]]*$D$26+0.05</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="leadoff modifier" dataDxfId="38">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="leadoff modifier" dataDxfId="8">
       <calculatedColumnFormula>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*$E$26</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="total leadoff (ft)" dataDxfId="37">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="total leadoff (ft)" dataDxfId="45">
       <calculatedColumnFormula>MAX(Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90, 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="pickoff manuver (s)" dataDxfId="36">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="pickoff manuver (s)" dataDxfId="44">
       <calculatedColumnFormula>1.1 - Table3[[#This Row],[defense]]*0.1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="throw speed (s/ft)" dataDxfId="35">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="throw speed (s/ft)" dataDxfId="43">
       <calculatedColumnFormula xml:space="preserve"> 0.01 - 0.0025 *  Table3[[#This Row],[defense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="throw speed (mph)" dataDxfId="34">
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="throw speed (mph)" dataDxfId="42">
       <calculatedColumnFormula>1 / Table3[[#This Row],[throw speed (s/ft)]] * ((60 * 60)/5280)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="pickoff time" dataDxfId="33">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="pickoff time" dataDxfId="41">
       <calculatedColumnFormula>Table3[[#This Row],[pickoff manuver (s)]]+60*Table3[[#This Row],[throw speed (s/ft)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="runner reaction" dataDxfId="32">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="runner reaction" dataDxfId="40">
       <calculatedColumnFormula>$K$28-$K$26*Table3[[#This Row],[offense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="runner speed (s/ft)" dataDxfId="31">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="runner speed (s/ft)" dataDxfId="39">
       <calculatedColumnFormula>0.05 - Table3[[#This Row],[offense]]*$L$26</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="runner speed (mph)" dataDxfId="30">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="runner speed (mph)" dataDxfId="38">
       <calculatedColumnFormula>1 / Table3[[#This Row],[runner speed (s/ft)]] * ((60 * 60)/5280)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="pickoff evade time" dataDxfId="29">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="pickoff evade time" dataDxfId="37">
       <calculatedColumnFormula>Table3[[#This Row],[runner reaction]]+Table3[[#This Row],[runner speed (s/ft)]]*Table3[[#This Row],[total leadoff (ft)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="pickoff probability" dataDxfId="28" dataCellStyle="Percent">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="pickoff probability" dataDxfId="36" dataCellStyle="Percent">
       <calculatedColumnFormula>1 - _xlfn.NORM.DIST(Table3[[#This Row],[pickoff time]], Table3[[#This Row],[pickoff evade time]], $O$4, TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Fielding Odds" dataDxfId="27" dataCellStyle="Percent">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Fielding Odds" dataDxfId="35" dataCellStyle="Percent">
       <calculatedColumnFormula>_xlfn.NORM.DIST(Table3[[#This Row],[defense]], $P$26, $P$27, TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="pickoff worth it?" dataDxfId="26">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="pickoff worth it?" dataDxfId="34">
       <calculatedColumnFormula>Table3[[#This Row],[pickoff probability]] &gt; 1-Table3[[#This Row],[Fielding Odds]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Error %" dataDxfId="25" dataCellStyle="Percent">
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Error %" dataDxfId="33" dataCellStyle="Percent">
       <calculatedColumnFormula>1-Table3[[#This Row],[Fielding Odds]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Blatant steal time" dataDxfId="24">
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Blatant steal time" dataDxfId="32">
       <calculatedColumnFormula>(90-Table3[[#This Row],[total leadoff (ft)]])*Table3[[#This Row],[runner speed (s/ft)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Response speed" dataDxfId="23">
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Response speed" dataDxfId="31">
       <calculatedColumnFormula>$T$26*(2-Table3[[#This Row],[defense]]) + Table3[[#This Row],[pickoff time]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="blatant steal probability" dataDxfId="22" dataCellStyle="Percent">
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="blatant steal probability" dataDxfId="30" dataCellStyle="Percent">
       <calculatedColumnFormula>_xlfn.NORM.DIST(Table3[[#This Row],[Response speed]], Table3[[#This Row],[Blatant steal time]], $U$4, TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="defense fear" dataDxfId="21">
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="defense fear" dataDxfId="29">
       <calculatedColumnFormula>Table3[[#This Row],[defense]]+Table3[[#This Row],[defense]]*Table3[[#This Row],[offense]]*$E$26</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="ball factor" dataDxfId="20">
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="ball factor" dataDxfId="28">
       <calculatedColumnFormula>(1-$W$32)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="desperation" dataDxfId="19" dataCellStyle="Percent">
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="desperation" dataDxfId="27" dataCellStyle="Percent">
       <calculatedColumnFormula>Table3[[#This Row],[ball factor]]/$X$32*(1-$X$34)+$X$34</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="player control" dataDxfId="18">
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="player control" dataDxfId="26">
       <calculatedColumnFormula>Table3[[#This Row],[offense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="ideal steer" dataDxfId="17">
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="ideal steer" dataDxfId="25">
       <calculatedColumnFormula>$AA$33</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="scaled control" dataDxfId="16">
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="scaled control" dataDxfId="24">
       <calculatedColumnFormula>IF(Table3[[#This Row],[player control]]&gt;1,Table3[[#This Row],[player control]]*$AA$41+$AA$40,Table3[[#This Row],[player control]]*$AA$39+$AA$38)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="unmod foul percent 3rd" dataDxfId="15" dataCellStyle="Percent">
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="unmod foul percent 3rd" dataDxfId="23" dataCellStyle="Percent">
       <calculatedColumnFormula>_xlfn.NORM.DIST(-1,Table3[[#This Row],[ideal steer]],($AB$25-Table3[[#This Row],[scaled control]])*$AB$27,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="unmod foul percent 1st" dataDxfId="14" dataCellStyle="Percent">
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="unmod foul percent 1st" dataDxfId="22" dataCellStyle="Percent">
       <calculatedColumnFormula>1-_xlfn.NORM.DIST(1,Table3[[#This Row],[ideal steer]],($AB$25-Table3[[#This Row],[scaled control]])*$AB$27,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="total unmod foul percent" dataDxfId="13" dataCellStyle="Percent">
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="total unmod foul percent" dataDxfId="21" dataCellStyle="Percent">
       <calculatedColumnFormula>1-(1-Table3[[#This Row],[unmod foul percent 3rd]])*(1-Table3[[#This Row],[unmod foul percent 1st]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="unmod dead center foul%" dataDxfId="12" dataCellStyle="Percent">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="unmod dead center foul%" dataDxfId="20" dataCellStyle="Percent">
       <calculatedColumnFormula>1-((1-_xlfn.NORM.DIST(-1,0,($AB$25-Table3[[#This Row],[scaled control]])*$AB$27,TRUE))*_xlfn.NORM.DIST(1,0,($AB$25-Table3[[#This Row],[scaled control]])*$AB$27,TRUE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="count" dataDxfId="11">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="count" dataDxfId="19">
       <calculatedColumnFormula>$AF$34*$AF$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="hitter discipline bias" dataDxfId="10">
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="hitter discipline bias" dataDxfId="18">
       <calculatedColumnFormula>$AG$25*($AG$34*Table3[[#This Row],[offense]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="bases loaded" dataDxfId="9">
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="bases loaded" dataDxfId="17">
       <calculatedColumnFormula>$AH$25*$AH$34</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="number of outs" dataDxfId="8">
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="number of outs" dataDxfId="16">
       <calculatedColumnFormula>$AI$34*$AI$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="current hitter vs next hitter" dataDxfId="7">
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="current hitter vs next hitter" dataDxfId="15">
       <calculatedColumnFormula>$AJ$25*(Table3[[#This Row],[offense]]-$AJ$27)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="calling modifier" dataDxfId="5">
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="calling modifier" dataDxfId="14">
       <calculatedColumnFormula array="1">SUM(Table3[[#This Row],[count]:[current hitter vs next hitter]]*MIN(1, Table3[[#This Row],[defense]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="sigmoid strike percent" dataDxfId="4" dataCellStyle="Percent">
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="sigmoid strike percent" dataDxfId="13" dataCellStyle="Percent">
       <calculatedColumnFormula>$AL$25-(Table3[[#This Row],[calling modifier]]/(ABS(Table3[[#This Row],[calling modifier]])+$AL$29)*$AL$27)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="tanh strike percent" dataDxfId="2" dataCellStyle="Percent">
+    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="tanh strike percent" dataDxfId="12" dataCellStyle="Percent">
       <calculatedColumnFormula>$AL$25-$AL$27*TANH(Table3[[#This Row],[calling modifier]]/$AM$29)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="XYZZY - called position" dataDxfId="0" dataCellStyle="Percent">
-      <calculatedColumnFormula>1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*(0.4*(3-Table3[[#This Row],[defense]]))</calculatedColumnFormula>
+    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="called position" dataDxfId="11" dataCellStyle="Percent">
+      <calculatedColumnFormula>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-Table3[[#This Row],[defense]])))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="Column1" dataDxfId="1"/>
-    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="Column2" dataDxfId="3"/>
-    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="Column44"/>
-    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="Column45"/>
-    <tableColumn id="45" xr3:uid="{00000000-0010-0000-0000-00002D000000}" name="Column46"/>
-    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="Column47"/>
-    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="Column48"/>
-    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="Column49"/>
-    <tableColumn id="49" xr3:uid="{00000000-0010-0000-0000-000031000000}" name="Column50"/>
-    <tableColumn id="50" xr3:uid="{00000000-0010-0000-0000-000032000000}" name="Column51"/>
+    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="called pos 0.2 pitch" dataDxfId="10">
+      <calculatedColumnFormula>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-0.2)))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="called pos 2 pitch" dataDxfId="9">
+      <calculatedColumnFormula>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-2)))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="location -1  stdv" dataDxfId="5">
+      <calculatedColumnFormula>Table3[[#This Row],[called position]]-pitchmod*(pitchstdv-Table3[[#This Row],[defense]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="location +1 stdv" dataDxfId="6">
+      <calculatedColumnFormula>ABS(Table3[[#This Row],[called position]]+pitchmod*(pitchstdv-Table3[[#This Row],[defense]]))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="45" xr3:uid="{00000000-0010-0000-0000-00002D000000}" name="difficulty" dataDxfId="7">
+      <calculatedColumnFormula>Table3[[#This Row],[defense]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="min dist to sz 1stdv" dataDxfId="2">
+      <calculatedColumnFormula>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;1, Table3[[#This Row],[location +1 stdv]]&gt;1),0, MIN(Table3[[#This Row],[location -1  stdv]]+1, 1-Table3[[#This Row],[location +1 stdv]]))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="max dist to sz 1stdv" dataDxfId="1">
+      <calculatedColumnFormula>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;0, Table3[[#This Row],[location +1 stdv]]&gt;0),1, MAX(1-ABS(Table3[[#This Row],[location -1  stdv]]), Table3[[#This Row],[location +1 stdv]]-1))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="ave obscurity" dataDxfId="0">
+      <calculatedColumnFormula>1/(ABS(Table3[[#This Row],[called position]]-1)+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="49" xr3:uid="{00000000-0010-0000-0000-000031000000}" name="max obscurity2" dataDxfId="3">
+      <calculatedColumnFormula>1/(Table3[[#This Row],[min dist to sz 1stdv]]+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="50" xr3:uid="{00000000-0010-0000-0000-000032000000}" name="min obscurity">
+      <calculatedColumnFormula>1/(Table3[[#This Row],[max dist to sz 1stdv]]+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="Column52"/>
     <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="Column53"/>
     <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="Column54"/>
@@ -7693,8 +7766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BE41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD4" workbookViewId="0">
-      <selection activeCell="AJ34" sqref="AJ34"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AR31" sqref="AR31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7758,12 +7831,12 @@
     </row>
     <row r="5" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A5" s="73" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B5" s="74"/>
       <c r="C5" s="75"/>
       <c r="D5" s="73" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="E5" s="74"/>
       <c r="F5" s="74"/>
@@ -7780,17 +7853,17 @@
       <c r="Q5" s="74"/>
       <c r="R5" s="75"/>
       <c r="S5" s="73" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="T5" s="74"/>
       <c r="U5" s="74"/>
       <c r="V5" s="75"/>
       <c r="W5" s="73" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="X5" s="75"/>
       <c r="Y5" s="73" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="Z5" s="74"/>
       <c r="AA5" s="74"/>
@@ -7798,8 +7871,21 @@
       <c r="AC5" s="74"/>
       <c r="AD5" s="74"/>
       <c r="AE5" s="75"/>
-      <c r="AF5" t="s">
-        <v>182</v>
+      <c r="AF5" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="AG5" s="74"/>
+      <c r="AH5" s="74"/>
+      <c r="AI5" s="74"/>
+      <c r="AJ5" s="74"/>
+      <c r="AK5" s="74"/>
+      <c r="AL5" s="74"/>
+      <c r="AM5" s="74"/>
+      <c r="AN5" s="75"/>
+      <c r="AO5" s="73"/>
+      <c r="AP5" s="75"/>
+      <c r="AQ5" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:57" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -7870,109 +7956,109 @@
         <v>111</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="X6" s="2" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="Y6" s="2" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="Z6" s="78" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="AA6" s="78" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB6" s="78" t="s">
+        <v>169</v>
+      </c>
+      <c r="AC6" s="78" t="s">
         <v>170</v>
       </c>
-      <c r="AB6" s="78" t="s">
-        <v>177</v>
-      </c>
-      <c r="AC6" s="78" t="s">
-        <v>178</v>
-      </c>
       <c r="AD6" s="78" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="AE6" s="78" t="s">
+        <v>172</v>
+      </c>
+      <c r="AF6" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AG6" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="AH6" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="AF6" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="AG6" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="AH6" s="2" t="s">
-        <v>188</v>
-      </c>
       <c r="AI6" s="2" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="AJ6" s="2" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="AK6" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="AL6" s="78" t="s">
+        <v>195</v>
+      </c>
+      <c r="AM6" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="AN6" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="AO6" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="AP6" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="AL6" s="78" t="s">
-        <v>204</v>
-      </c>
-      <c r="AM6" s="2" t="s">
+      <c r="AQ6" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="AR6" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="AS6" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="AT6" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="AU6" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="AN6" s="2" t="s">
+      <c r="AV6" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="AW6" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="AX6" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="AO6" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="AP6" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="AQ6" s="2" t="s">
+      <c r="AY6" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="AR6" s="2" t="s">
+      <c r="AZ6" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="AS6" s="2" t="s">
+      <c r="BA6" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="AT6" s="2" t="s">
+      <c r="BB6" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="AU6" s="2" t="s">
+      <c r="BC6" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="AV6" s="2" t="s">
+      <c r="BD6" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="AW6" s="2" t="s">
+      <c r="BE6" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="AX6" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="AY6" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="AZ6" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="BA6" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="BB6" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="BC6" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="BD6" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="BE6" s="2" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:57" s="29" customFormat="1" x14ac:dyDescent="0.25">
@@ -7993,12 +8079,12 @@
         <v>6.0000000000000005E-2</v>
       </c>
       <c r="E7" s="29">
-        <f>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*$E$26</f>
-        <v>-1.2E-2</v>
+        <f>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*$E$26</f>
+        <v>-0.12</v>
       </c>
       <c r="F7" s="29">
         <f>MAX(Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90, 0)</f>
-        <v>5.4648000000000003</v>
+        <v>6.0480000000000009</v>
       </c>
       <c r="G7" s="29">
         <f>1.1 - Table3[[#This Row],[defense]]*0.1</f>
@@ -8030,11 +8116,11 @@
       </c>
       <c r="N7" s="29">
         <f>Table3[[#This Row],[runner reaction]]+Table3[[#This Row],[runner speed (s/ft)]]*Table3[[#This Row],[total leadoff (ft)]]</f>
-        <v>1.1477752000000001</v>
+        <v>1.1763520000000001</v>
       </c>
       <c r="O7" s="30">
         <f>1 - _xlfn.NORM.DIST(Table3[[#This Row],[pickoff time]], Table3[[#This Row],[pickoff evade time]], $O$4, TRUE)</f>
-        <v>4.1929540286620437E-3</v>
+        <v>6.3291626390171718E-3</v>
       </c>
       <c r="P7" s="48">
         <f>_xlfn.NORM.DIST(Table3[[#This Row],[defense]], $P$26, $P$27, TRUE)</f>
@@ -8050,7 +8136,7 @@
       </c>
       <c r="S7" s="29">
         <f>(90-Table3[[#This Row],[total leadoff (ft)]])*Table3[[#This Row],[runner speed (s/ft)]]</f>
-        <v>4.1422248000000002</v>
+        <v>4.1136480000000004</v>
       </c>
       <c r="T7" s="29">
         <f>$T$26*(2-Table3[[#This Row],[defense]]) + Table3[[#This Row],[pickoff time]]</f>
@@ -8058,7 +8144,7 @@
       </c>
       <c r="U7" s="48">
         <f>_xlfn.NORM.DIST(Table3[[#This Row],[Response speed]], Table3[[#This Row],[Blatant steal time]], $U$4, TRUE)</f>
-        <v>2.5191863061619241E-4</v>
+        <v>3.005916388905331E-4</v>
       </c>
       <c r="V7" s="29">
         <f>Table3[[#This Row],[defense]]+Table3[[#This Row],[defense]]*Table3[[#This Row],[offense]]*$E$26</f>
@@ -8102,7 +8188,7 @@
       </c>
       <c r="AF7" s="29">
         <f>$AF$34*$AF$25</f>
-        <v>-13.333333333333332</v>
+        <v>-20</v>
       </c>
       <c r="AG7" s="29">
         <f>$AG$25*($AG$34*Table3[[#This Row],[offense]])</f>
@@ -8122,19 +8208,59 @@
       </c>
       <c r="AK7" s="29" cm="1">
         <f t="array" ref="AK7">SUM(Table3[[#This Row],[count]:[current hitter vs next hitter]]*MIN(1, Table3[[#This Row],[defense]]))</f>
-        <v>-1.4233333333333333</v>
+        <v>-2.09</v>
       </c>
       <c r="AL7" s="80">
         <f>$AL$25-(Table3[[#This Row],[calling modifier]]/(ABS(Table3[[#This Row],[calling modifier]])+$AL$29)*$AL$27)</f>
-        <v>0.62657538509413413</v>
+        <v>0.63784517881394298</v>
       </c>
       <c r="AM7" s="104">
         <f>$AL$25-$AL$27*TANH(Table3[[#This Row],[calling modifier]]/$AM$29)</f>
-        <v>0.62841870550493606</v>
+        <v>0.64164850622224268</v>
       </c>
       <c r="AN7" s="116">
-        <f>1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*(0.4*(3-Table3[[#This Row],[defense]]))</f>
-        <v>0.61990494808770902</v>
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-Table3[[#This Row],[defense]])))</f>
+        <v>0.57907233656026214</v>
+      </c>
+      <c r="AO7" s="117">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-0.2)))</f>
+        <v>0.59358708357542556</v>
+      </c>
+      <c r="AP7" s="117">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-2)))</f>
+        <v>0.85485252984836624</v>
+      </c>
+      <c r="AQ7" s="117">
+        <f>Table3[[#This Row],[called position]]-pitchmod*(pitchstdv-Table3[[#This Row],[defense]])</f>
+        <v>-0.58092766343973778</v>
+      </c>
+      <c r="AR7" s="117">
+        <f>ABS(Table3[[#This Row],[called position]]+pitchmod*(pitchstdv-Table3[[#This Row],[defense]]))</f>
+        <v>1.7390723365602621</v>
+      </c>
+      <c r="AS7" s="29">
+        <f>Table3[[#This Row],[defense]]</f>
+        <v>0.1</v>
+      </c>
+      <c r="AT7" s="117">
+        <f>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;1, Table3[[#This Row],[location +1 stdv]]&gt;1),0, MIN(Table3[[#This Row],[location -1  stdv]]+1, 1-Table3[[#This Row],[location +1 stdv]]))</f>
+        <v>0</v>
+      </c>
+      <c r="AU7" s="117">
+        <f>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;0, Table3[[#This Row],[location +1 stdv]]&gt;0),1, MAX(1-ABS(Table3[[#This Row],[location -1  stdv]]), Table3[[#This Row],[location +1 stdv]]-1))</f>
+        <v>1</v>
+      </c>
+      <c r="AV7" s="117">
+        <f>1/(ABS(Table3[[#This Row],[called position]]-1)+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>2.1196523244645893</v>
+      </c>
+      <c r="AW7" s="117">
+        <f>1/(Table3[[#This Row],[min dist to sz 1stdv]]+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="AX7" s="117">
+        <f>1/(Table3[[#This Row],[max dist to sz 1stdv]]+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>1.1090909090909091</v>
       </c>
     </row>
     <row r="8" spans="1:57" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -8264,7 +8390,7 @@
       </c>
       <c r="AF8" s="3">
         <f>$AF$34*$AF$25</f>
-        <v>-13.333333333333332</v>
+        <v>-20</v>
       </c>
       <c r="AG8" s="3">
         <f>$AG$25*($AG$34*Table3[[#This Row],[offense]])</f>
@@ -8284,19 +8410,59 @@
       </c>
       <c r="AK8" s="3" cm="1">
         <f t="array" ref="AK8">SUM(Table3[[#This Row],[count]:[current hitter vs next hitter]]*MIN(1, Table3[[#This Row],[defense]]))</f>
-        <v>-1.3833333333333333</v>
+        <v>-2.0499999999999998</v>
       </c>
       <c r="AL8" s="82">
         <f>$AL$25-(Table3[[#This Row],[calling modifier]]/(ABS(Table3[[#This Row],[calling modifier]])+$AL$29)*$AL$27)</f>
-        <v>0.62587685113016367</v>
+        <v>0.63718820861678005</v>
       </c>
       <c r="AM8" s="105">
         <f>$AL$25-$AL$27*TANH(Table3[[#This Row],[calling modifier]]/$AM$29)</f>
-        <v>0.62762263156352605</v>
-      </c>
-      <c r="AN8" s="117">
-        <f>1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*(0.4*(3-Table3[[#This Row],[defense]]))</f>
-        <v>0.62234650135700387</v>
+        <v>0.64085701544587359</v>
+      </c>
+      <c r="AN8" s="118">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-Table3[[#This Row],[defense]])))</f>
+        <v>0.58152941922290857</v>
+      </c>
+      <c r="AO8" s="119">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-0.2)))</f>
+        <v>0.59595943924970474</v>
+      </c>
+      <c r="AP8" s="119">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-2)))</f>
+        <v>0.85569979973203736</v>
+      </c>
+      <c r="AQ8" s="119">
+        <f>Table3[[#This Row],[called position]]-pitchmod*(pitchstdv-Table3[[#This Row],[defense]])</f>
+        <v>-0.57847058077709135</v>
+      </c>
+      <c r="AR8" s="119">
+        <f>ABS(Table3[[#This Row],[called position]]+pitchmod*(pitchstdv-Table3[[#This Row],[defense]]))</f>
+        <v>1.7415294192229085</v>
+      </c>
+      <c r="AS8" s="3">
+        <f>Table3[[#This Row],[defense]]</f>
+        <v>0.1</v>
+      </c>
+      <c r="AT8" s="119">
+        <f>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;1, Table3[[#This Row],[location +1 stdv]]&gt;1),0, MIN(Table3[[#This Row],[location -1  stdv]]+1, 1-Table3[[#This Row],[location +1 stdv]]))</f>
+        <v>0</v>
+      </c>
+      <c r="AU8" s="119">
+        <f>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;0, Table3[[#This Row],[location +1 stdv]]&gt;0),1, MAX(1-ABS(Table3[[#This Row],[location -1  stdv]]), Table3[[#This Row],[location +1 stdv]]-1))</f>
+        <v>1</v>
+      </c>
+      <c r="AV8" s="119">
+        <f>1/(ABS(Table3[[#This Row],[called position]]-1)+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>2.1287497441054133</v>
+      </c>
+      <c r="AW8" s="119">
+        <f>1/(Table3[[#This Row],[min dist to sz 1stdv]]+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="AX8" s="119">
+        <f>1/(Table3[[#This Row],[max dist to sz 1stdv]]+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>1.1090909090909091</v>
       </c>
     </row>
     <row r="9" spans="1:57" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -8426,7 +8592,7 @@
       </c>
       <c r="AF9" s="4">
         <f>$AF$34*$AF$25</f>
-        <v>-13.333333333333332</v>
+        <v>-20</v>
       </c>
       <c r="AG9" s="4">
         <f>$AG$25*($AG$34*Table3[[#This Row],[offense]])</f>
@@ -8446,19 +8612,59 @@
       </c>
       <c r="AK9" s="4" cm="1">
         <f t="array" ref="AK9">SUM(Table3[[#This Row],[count]:[current hitter vs next hitter]]*MIN(1, Table3[[#This Row],[defense]]))</f>
-        <v>-1.3333333333333333</v>
+        <v>-2</v>
       </c>
       <c r="AL9" s="84">
         <f>$AL$25-(Table3[[#This Row],[calling modifier]]/(ABS(Table3[[#This Row],[calling modifier]])+$AL$29)*$AL$27)</f>
-        <v>0.625</v>
+        <v>0.63636363636363635</v>
       </c>
       <c r="AM9" s="106">
         <f>$AL$25-$AL$27*TANH(Table3[[#This Row],[calling modifier]]/$AM$29)</f>
-        <v>0.62662723060090497</v>
-      </c>
-      <c r="AN9" s="118">
-        <f>1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*(0.4*(3-Table3[[#This Row],[defense]]))</f>
-        <v>0.62539703849887918</v>
+        <v>0.63986719784998236</v>
+      </c>
+      <c r="AN9" s="120">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-Table3[[#This Row],[defense]])))</f>
+        <v>0.58459954379728118</v>
+      </c>
+      <c r="AO9" s="121">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-0.2)))</f>
+        <v>0.59892369745944385</v>
+      </c>
+      <c r="AP9" s="121">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-2)))</f>
+        <v>0.8567584633783728</v>
+      </c>
+      <c r="AQ9" s="121">
+        <f>Table3[[#This Row],[called position]]-pitchmod*(pitchstdv-Table3[[#This Row],[defense]])</f>
+        <v>-0.57540045620271874</v>
+      </c>
+      <c r="AR9" s="121">
+        <f>ABS(Table3[[#This Row],[called position]]+pitchmod*(pitchstdv-Table3[[#This Row],[defense]]))</f>
+        <v>1.744599543797281</v>
+      </c>
+      <c r="AS9" s="4">
+        <f>Table3[[#This Row],[defense]]</f>
+        <v>0.1</v>
+      </c>
+      <c r="AT9" s="121">
+        <f>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;1, Table3[[#This Row],[location +1 stdv]]&gt;1),0, MIN(Table3[[#This Row],[location -1  stdv]]+1, 1-Table3[[#This Row],[location +1 stdv]]))</f>
+        <v>0</v>
+      </c>
+      <c r="AU9" s="121">
+        <f>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;0, Table3[[#This Row],[location +1 stdv]]&gt;0),1, MAX(1-ABS(Table3[[#This Row],[location -1  stdv]]), Table3[[#This Row],[location +1 stdv]]-1))</f>
+        <v>1</v>
+      </c>
+      <c r="AV9" s="121">
+        <f>1/(ABS(Table3[[#This Row],[called position]]-1)+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>2.1402388724442205</v>
+      </c>
+      <c r="AW9" s="121">
+        <f>1/(Table3[[#This Row],[min dist to sz 1stdv]]+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="AX9" s="121">
+        <f>1/(Table3[[#This Row],[max dist to sz 1stdv]]+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>1.1090909090909091</v>
       </c>
     </row>
     <row r="10" spans="1:57" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -8588,7 +8794,7 @@
       </c>
       <c r="AF10" s="3">
         <f>$AF$34*$AF$25</f>
-        <v>-13.333333333333332</v>
+        <v>-20</v>
       </c>
       <c r="AG10" s="3">
         <f>$AG$25*($AG$34*Table3[[#This Row],[offense]])</f>
@@ -8608,19 +8814,59 @@
       </c>
       <c r="AK10" s="3" cm="1">
         <f t="array" ref="AK10">SUM(Table3[[#This Row],[count]:[current hitter vs next hitter]]*MIN(1, Table3[[#This Row],[defense]]))</f>
-        <v>-1.2333333333333332</v>
+        <v>-1.9</v>
       </c>
       <c r="AL10" s="82">
         <f>$AL$25-(Table3[[#This Row],[calling modifier]]/(ABS(Table3[[#This Row],[calling modifier]])+$AL$29)*$AL$27)</f>
-        <v>0.62323390894819464</v>
+        <v>0.63470319634703198</v>
       </c>
       <c r="AM10" s="105">
         <f>$AL$25-$AL$27*TANH(Table3[[#This Row],[calling modifier]]/$AM$29)</f>
-        <v>0.62463544687063488</v>
-      </c>
-      <c r="AN10" s="117">
-        <f>1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*(0.4*(3-Table3[[#This Row],[defense]]))</f>
-        <v>0.63149337535819994</v>
+        <v>0.63788609451447142</v>
+      </c>
+      <c r="AN10" s="118">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-Table3[[#This Row],[defense]])))</f>
+        <v>0.59073564174578364</v>
+      </c>
+      <c r="AO10" s="119">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-0.2)))</f>
+        <v>0.60484820582351528</v>
+      </c>
+      <c r="AP10" s="119">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-2)))</f>
+        <v>0.85887435922268396</v>
+      </c>
+      <c r="AQ10" s="119">
+        <f>Table3[[#This Row],[called position]]-pitchmod*(pitchstdv-Table3[[#This Row],[defense]])</f>
+        <v>-0.56926435825421629</v>
+      </c>
+      <c r="AR10" s="119">
+        <f>ABS(Table3[[#This Row],[called position]]+pitchmod*(pitchstdv-Table3[[#This Row],[defense]]))</f>
+        <v>1.7507356417457836</v>
+      </c>
+      <c r="AS10" s="3">
+        <f>Table3[[#This Row],[defense]]</f>
+        <v>0.1</v>
+      </c>
+      <c r="AT10" s="119">
+        <f>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;1, Table3[[#This Row],[location +1 stdv]]&gt;1),0, MIN(Table3[[#This Row],[location -1  stdv]]+1, 1-Table3[[#This Row],[location +1 stdv]]))</f>
+        <v>0</v>
+      </c>
+      <c r="AU10" s="119">
+        <f>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;0, Table3[[#This Row],[location +1 stdv]]&gt;0),1, MAX(1-ABS(Table3[[#This Row],[location -1  stdv]]), Table3[[#This Row],[location +1 stdv]]-1))</f>
+        <v>1</v>
+      </c>
+      <c r="AV10" s="119">
+        <f>1/(ABS(Table3[[#This Row],[called position]]-1)+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>2.1636167027829121</v>
+      </c>
+      <c r="AW10" s="119">
+        <f>1/(Table3[[#This Row],[min dist to sz 1stdv]]+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="AX10" s="119">
+        <f>1/(Table3[[#This Row],[max dist to sz 1stdv]]+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>1.1090909090909091</v>
       </c>
     </row>
     <row r="11" spans="1:57" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -8750,7 +8996,7 @@
       </c>
       <c r="AF11" s="13">
         <f>$AF$34*$AF$25</f>
-        <v>-13.333333333333332</v>
+        <v>-20</v>
       </c>
       <c r="AG11" s="13">
         <f>$AG$25*($AG$34*Table3[[#This Row],[offense]])</f>
@@ -8770,19 +9016,59 @@
       </c>
       <c r="AK11" s="13" cm="1">
         <f t="array" ref="AK11">SUM(Table3[[#This Row],[count]:[current hitter vs next hitter]]*MIN(1, Table3[[#This Row],[defense]]))</f>
-        <v>-7.1166666666666663</v>
+        <v>-10.45</v>
       </c>
       <c r="AL11" s="86">
         <f>$AL$25-(Table3[[#This Row],[calling modifier]]/(ABS(Table3[[#This Row],[calling modifier]])+$AL$29)*$AL$27)</f>
-        <v>0.70497848801475105</v>
+        <v>0.73727422003284071</v>
       </c>
       <c r="AM11" s="107">
         <f>$AL$25-$AL$27*TANH(Table3[[#This Row],[calling modifier]]/$AM$29)</f>
-        <v>0.73661546205694517</v>
-      </c>
-      <c r="AN11" s="119">
-        <f>1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*(0.4*(3-Table3[[#This Row],[defense]]))</f>
-        <v>0.36705425848964723</v>
+        <v>0.79185088533575021</v>
+      </c>
+      <c r="AN11" s="122">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-Table3[[#This Row],[defense]])))</f>
+        <v>0.18713982377703142</v>
+      </c>
+      <c r="AO11" s="123">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-0.2)))</f>
+        <v>8.9596602630275246E-2</v>
+      </c>
+      <c r="AP11" s="123">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-2)))</f>
+        <v>0.67485592951081252</v>
+      </c>
+      <c r="AQ11" s="123">
+        <f>Table3[[#This Row],[called position]]-pitchmod*(pitchstdv-Table3[[#This Row],[defense]])</f>
+        <v>-0.81286017622296858</v>
+      </c>
+      <c r="AR11" s="123">
+        <f>ABS(Table3[[#This Row],[called position]]+pitchmod*(pitchstdv-Table3[[#This Row],[defense]]))</f>
+        <v>1.1871398237770314</v>
+      </c>
+      <c r="AS11" s="13">
+        <f>Table3[[#This Row],[defense]]</f>
+        <v>0.5</v>
+      </c>
+      <c r="AT11" s="123">
+        <f>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;1, Table3[[#This Row],[location +1 stdv]]&gt;1),0, MIN(Table3[[#This Row],[location -1  stdv]]+1, 1-Table3[[#This Row],[location +1 stdv]]))</f>
+        <v>0</v>
+      </c>
+      <c r="AU11" s="123">
+        <f>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;0, Table3[[#This Row],[location +1 stdv]]&gt;0),1, MAX(1-ABS(Table3[[#This Row],[location -1  stdv]]), Table3[[#This Row],[location +1 stdv]]-1))</f>
+        <v>1</v>
+      </c>
+      <c r="AV11" s="123">
+        <f>1/(ABS(Table3[[#This Row],[called position]]-1)+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>2.0954580187050982</v>
+      </c>
+      <c r="AW11" s="123">
+        <f>1/(Table3[[#This Row],[min dist to sz 1stdv]]+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>11</v>
+      </c>
+      <c r="AX11" s="123">
+        <f>1/(Table3[[#This Row],[max dist to sz 1stdv]]+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>1.9090909090909092</v>
       </c>
     </row>
     <row r="12" spans="1:57" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -8912,7 +9198,7 @@
       </c>
       <c r="AF12" s="26">
         <f>$AF$34*$AF$25</f>
-        <v>-13.333333333333332</v>
+        <v>-20</v>
       </c>
       <c r="AG12" s="26">
         <f>$AG$25*($AG$34*Table3[[#This Row],[offense]])</f>
@@ -8932,19 +9218,59 @@
       </c>
       <c r="AK12" s="26" cm="1">
         <f t="array" ref="AK12">SUM(Table3[[#This Row],[count]:[current hitter vs next hitter]]*MIN(1, Table3[[#This Row],[defense]]))</f>
-        <v>-6.9166666666666661</v>
+        <v>-10.25</v>
       </c>
       <c r="AL12" s="88">
         <f>$AL$25-(Table3[[#This Row],[calling modifier]]/(ABS(Table3[[#This Row],[calling modifier]])+$AL$29)*$AL$27)</f>
-        <v>0.70278637770897834</v>
+        <v>0.73553719008264462</v>
       </c>
       <c r="AM12" s="108">
         <f>$AL$25-$AL$27*TANH(Table3[[#This Row],[calling modifier]]/$AM$29)</f>
-        <v>0.73307006594966906</v>
-      </c>
-      <c r="AN12" s="120">
-        <f>1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*(0.4*(3-Table3[[#This Row],[defense]]))</f>
-        <v>0.37787529009365672</v>
+        <v>0.78875631514171873</v>
+      </c>
+      <c r="AN12" s="124">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-Table3[[#This Row],[defense]])))</f>
+        <v>0.19788660926907975</v>
+      </c>
+      <c r="AO12" s="125">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-0.2)))</f>
+        <v>0.10163300238136941</v>
+      </c>
+      <c r="AP12" s="125">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-2)))</f>
+        <v>0.6791546437076319</v>
+      </c>
+      <c r="AQ12" s="125">
+        <f>Table3[[#This Row],[called position]]-pitchmod*(pitchstdv-Table3[[#This Row],[defense]])</f>
+        <v>-0.80211339073092025</v>
+      </c>
+      <c r="AR12" s="125">
+        <f>ABS(Table3[[#This Row],[called position]]+pitchmod*(pitchstdv-Table3[[#This Row],[defense]]))</f>
+        <v>1.1978866092690796</v>
+      </c>
+      <c r="AS12" s="26">
+        <f>Table3[[#This Row],[defense]]</f>
+        <v>0.5</v>
+      </c>
+      <c r="AT12" s="125">
+        <f>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;1, Table3[[#This Row],[location +1 stdv]]&gt;1),0, MIN(Table3[[#This Row],[location -1  stdv]]+1, 1-Table3[[#This Row],[location +1 stdv]]))</f>
+        <v>0</v>
+      </c>
+      <c r="AU12" s="125">
+        <f>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;0, Table3[[#This Row],[location +1 stdv]]&gt;0),1, MAX(1-ABS(Table3[[#This Row],[location -1  stdv]]), Table3[[#This Row],[location +1 stdv]]-1))</f>
+        <v>1</v>
+      </c>
+      <c r="AV12" s="125">
+        <f>1/(ABS(Table3[[#This Row],[called position]]-1)+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>2.1085080991756135</v>
+      </c>
+      <c r="AW12" s="125">
+        <f>1/(Table3[[#This Row],[min dist to sz 1stdv]]+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>11</v>
+      </c>
+      <c r="AX12" s="125">
+        <f>1/(Table3[[#This Row],[max dist to sz 1stdv]]+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>1.9090909090909092</v>
       </c>
     </row>
     <row r="13" spans="1:57" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -9074,7 +9400,7 @@
       </c>
       <c r="AF13" s="13">
         <f>$AF$34*$AF$25</f>
-        <v>-13.333333333333332</v>
+        <v>-20</v>
       </c>
       <c r="AG13" s="13">
         <f>$AG$25*($AG$34*Table3[[#This Row],[offense]])</f>
@@ -9094,19 +9420,59 @@
       </c>
       <c r="AK13" s="13" cm="1">
         <f t="array" ref="AK13">SUM(Table3[[#This Row],[count]:[current hitter vs next hitter]]*MIN(1, Table3[[#This Row],[defense]]))</f>
-        <v>-6.6666666666666661</v>
+        <v>-10</v>
       </c>
       <c r="AL13" s="86">
         <f>$AL$25-(Table3[[#This Row],[calling modifier]]/(ABS(Table3[[#This Row],[calling modifier]])+$AL$29)*$AL$27)</f>
-        <v>0.7</v>
+        <v>0.73333333333333328</v>
       </c>
       <c r="AM13" s="107">
         <f>$AL$25-$AL$27*TANH(Table3[[#This Row],[calling modifier]]/$AM$29)</f>
-        <v>0.72860509501265369</v>
-      </c>
-      <c r="AN13" s="119">
-        <f>1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*(0.4*(3-Table3[[#This Row],[defense]]))</f>
-        <v>0.39140030994856834</v>
+        <v>0.78484686290400396</v>
+      </c>
+      <c r="AN13" s="122">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-Table3[[#This Row],[defense]])))</f>
+        <v>0.21133233970562049</v>
+      </c>
+      <c r="AO13" s="123">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-0.2)))</f>
+        <v>0.11669222047029504</v>
+      </c>
+      <c r="AP13" s="123">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-2)))</f>
+        <v>0.68453293588224817</v>
+      </c>
+      <c r="AQ13" s="123">
+        <f>Table3[[#This Row],[called position]]-pitchmod*(pitchstdv-Table3[[#This Row],[defense]])</f>
+        <v>-0.78866766029437951</v>
+      </c>
+      <c r="AR13" s="123">
+        <f>ABS(Table3[[#This Row],[called position]]+pitchmod*(pitchstdv-Table3[[#This Row],[defense]]))</f>
+        <v>1.2113323397056206</v>
+      </c>
+      <c r="AS13" s="13">
+        <f>Table3[[#This Row],[defense]]</f>
+        <v>0.5</v>
+      </c>
+      <c r="AT13" s="123">
+        <f>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;1, Table3[[#This Row],[location +1 stdv]]&gt;1),0, MIN(Table3[[#This Row],[location -1  stdv]]+1, 1-Table3[[#This Row],[location +1 stdv]]))</f>
+        <v>0</v>
+      </c>
+      <c r="AU13" s="123">
+        <f>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;0, Table3[[#This Row],[location +1 stdv]]&gt;0),1, MAX(1-ABS(Table3[[#This Row],[location -1  stdv]]), Table3[[#This Row],[location +1 stdv]]-1))</f>
+        <v>1</v>
+      </c>
+      <c r="AV13" s="123">
+        <f>1/(ABS(Table3[[#This Row],[called position]]-1)+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>2.1252800621423993</v>
+      </c>
+      <c r="AW13" s="123">
+        <f>1/(Table3[[#This Row],[min dist to sz 1stdv]]+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>11</v>
+      </c>
+      <c r="AX13" s="123">
+        <f>1/(Table3[[#This Row],[max dist to sz 1stdv]]+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>1.9090909090909092</v>
       </c>
     </row>
     <row r="14" spans="1:57" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -9236,7 +9602,7 @@
       </c>
       <c r="AF14" s="5">
         <f>$AF$34*$AF$25</f>
-        <v>-13.333333333333332</v>
+        <v>-20</v>
       </c>
       <c r="AG14" s="5">
         <f>$AG$25*($AG$34*Table3[[#This Row],[offense]])</f>
@@ -9256,19 +9622,59 @@
       </c>
       <c r="AK14" s="5" cm="1">
         <f t="array" ref="AK14">SUM(Table3[[#This Row],[count]:[current hitter vs next hitter]]*MIN(1, Table3[[#This Row],[defense]]))</f>
-        <v>-6.1666666666666661</v>
+        <v>-9.5</v>
       </c>
       <c r="AL14" s="90">
         <f>$AL$25-(Table3[[#This Row],[calling modifier]]/(ABS(Table3[[#This Row],[calling modifier]])+$AL$29)*$AL$27)</f>
-        <v>0.69426751592356684</v>
+        <v>0.72881355932203384</v>
       </c>
       <c r="AM14" s="109">
         <f>$AL$25-$AL$27*TANH(Table3[[#This Row],[calling modifier]]/$AM$29)</f>
-        <v>0.71956804388093409</v>
-      </c>
-      <c r="AN14" s="121">
-        <f>1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*(0.4*(3-Table3[[#This Row],[defense]]))</f>
-        <v>0.41844121656117683</v>
+        <v>0.77689214241829041</v>
+      </c>
+      <c r="AN14" s="126">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-Table3[[#This Row],[defense]])))</f>
+        <v>0.23826086830924254</v>
+      </c>
+      <c r="AO14" s="127">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-0.2)))</f>
+        <v>0.14685217250635174</v>
+      </c>
+      <c r="AP14" s="127">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-2)))</f>
+        <v>0.69530434732369706</v>
+      </c>
+      <c r="AQ14" s="127">
+        <f>Table3[[#This Row],[called position]]-pitchmod*(pitchstdv-Table3[[#This Row],[defense]])</f>
+        <v>-0.76173913169075746</v>
+      </c>
+      <c r="AR14" s="127">
+        <f>ABS(Table3[[#This Row],[called position]]+pitchmod*(pitchstdv-Table3[[#This Row],[defense]]))</f>
+        <v>1.2382608683092426</v>
+      </c>
+      <c r="AS14" s="5">
+        <f>Table3[[#This Row],[defense]]</f>
+        <v>0.5</v>
+      </c>
+      <c r="AT14" s="127">
+        <f>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;1, Table3[[#This Row],[location +1 stdv]]&gt;1),0, MIN(Table3[[#This Row],[location -1  stdv]]+1, 1-Table3[[#This Row],[location +1 stdv]]))</f>
+        <v>0</v>
+      </c>
+      <c r="AU14" s="127">
+        <f>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;0, Table3[[#This Row],[location +1 stdv]]&gt;0),1, MAX(1-ABS(Table3[[#This Row],[location -1  stdv]]), Table3[[#This Row],[location +1 stdv]]-1))</f>
+        <v>1</v>
+      </c>
+      <c r="AV14" s="127">
+        <f>1/(ABS(Table3[[#This Row],[called position]]-1)+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>2.160443994272339</v>
+      </c>
+      <c r="AW14" s="127">
+        <f>1/(Table3[[#This Row],[min dist to sz 1stdv]]+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>11</v>
+      </c>
+      <c r="AX14" s="127">
+        <f>1/(Table3[[#This Row],[max dist to sz 1stdv]]+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>1.9090909090909092</v>
       </c>
     </row>
     <row r="15" spans="1:57" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -9398,7 +9804,7 @@
       </c>
       <c r="AF15" s="17">
         <f>$AF$34*$AF$25</f>
-        <v>-13.333333333333332</v>
+        <v>-20</v>
       </c>
       <c r="AG15" s="17">
         <f>$AG$25*($AG$34*Table3[[#This Row],[offense]])</f>
@@ -9418,19 +9824,59 @@
       </c>
       <c r="AK15" s="17" cm="1">
         <f t="array" ref="AK15">SUM(Table3[[#This Row],[count]:[current hitter vs next hitter]]*MIN(1, Table3[[#This Row],[defense]]))</f>
-        <v>-14.233333333333333</v>
+        <v>-20.9</v>
       </c>
       <c r="AL15" s="92">
         <f>$AL$25-(Table3[[#This Row],[calling modifier]]/(ABS(Table3[[#This Row],[calling modifier]])+$AL$29)*$AL$27)</f>
-        <v>0.76630963972736121</v>
+        <v>0.80440097799511001</v>
       </c>
       <c r="AM15" s="110">
         <f>$AL$25-$AL$27*TANH(Table3[[#This Row],[calling modifier]]/$AM$29)</f>
-        <v>0.84468835688869581</v>
-      </c>
-      <c r="AN15" s="122">
-        <f>1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*(0.4*(3-Table3[[#This Row],[defense]]))</f>
-        <v>0.18886795475493934</v>
+        <v>0.91194194050999755</v>
+      </c>
+      <c r="AN15" s="128">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-Table3[[#This Row],[defense]])))</f>
+        <v>0</v>
+      </c>
+      <c r="AO15" s="129">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-0.2)))</f>
+        <v>0</v>
+      </c>
+      <c r="AP15" s="129">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-2)))</f>
+        <v>0.45887572678899413</v>
+      </c>
+      <c r="AQ15" s="129">
+        <f>Table3[[#This Row],[called position]]-pitchmod*(pitchstdv-Table3[[#This Row],[defense]])</f>
+        <v>-0.8</v>
+      </c>
+      <c r="AR15" s="129">
+        <f>ABS(Table3[[#This Row],[called position]]+pitchmod*(pitchstdv-Table3[[#This Row],[defense]]))</f>
+        <v>0.8</v>
+      </c>
+      <c r="AS15" s="17">
+        <f>Table3[[#This Row],[defense]]</f>
+        <v>1</v>
+      </c>
+      <c r="AT15" s="129">
+        <f>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;1, Table3[[#This Row],[location +1 stdv]]&gt;1),0, MIN(Table3[[#This Row],[location -1  stdv]]+1, 1-Table3[[#This Row],[location +1 stdv]]))</f>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="AU15" s="129">
+        <f>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;0, Table3[[#This Row],[location +1 stdv]]&gt;0),1, MAX(1-ABS(Table3[[#This Row],[location -1  stdv]]), Table3[[#This Row],[location +1 stdv]]-1))</f>
+        <v>1</v>
+      </c>
+      <c r="AV15" s="129">
+        <f>1/(ABS(Table3[[#This Row],[called position]]-1)+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>2.9090909090909092</v>
+      </c>
+      <c r="AW15" s="129">
+        <f>1/(Table3[[#This Row],[min dist to sz 1stdv]]+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>5.3333333333333339</v>
+      </c>
+      <c r="AX15" s="129">
+        <f>1/(Table3[[#This Row],[max dist to sz 1stdv]]+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>2.9090909090909092</v>
       </c>
     </row>
     <row r="16" spans="1:57" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -9560,7 +10006,7 @@
       </c>
       <c r="AF16" s="6">
         <f>$AF$34*$AF$25</f>
-        <v>-13.333333333333332</v>
+        <v>-20</v>
       </c>
       <c r="AG16" s="6">
         <f>$AG$25*($AG$34*Table3[[#This Row],[offense]])</f>
@@ -9580,22 +10026,62 @@
       </c>
       <c r="AK16" s="6" cm="1">
         <f t="array" ref="AK16">SUM(Table3[[#This Row],[count]:[current hitter vs next hitter]]*MIN(1, Table3[[#This Row],[defense]]))</f>
-        <v>-13.833333333333332</v>
+        <v>-20.5</v>
       </c>
       <c r="AL16" s="94">
         <f>$AL$25-(Table3[[#This Row],[calling modifier]]/(ABS(Table3[[#This Row],[calling modifier]])+$AL$29)*$AL$27)</f>
-        <v>0.76354679802955661</v>
+        <v>0.80246913580246915</v>
       </c>
       <c r="AM16" s="111">
         <f>$AL$25-$AL$27*TANH(Table3[[#This Row],[calling modifier]]/$AM$29)</f>
-        <v>0.83962065174226819</v>
-      </c>
-      <c r="AN16" s="123">
-        <f>1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*(0.4*(3-Table3[[#This Row],[defense]]))</f>
-        <v>0.20568001103503175</v>
+        <v>0.90875809497616733</v>
+      </c>
+      <c r="AN16" s="130">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-Table3[[#This Row],[defense]])))</f>
+        <v>0</v>
+      </c>
+      <c r="AO16" s="131">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-0.2)))</f>
+        <v>0</v>
+      </c>
+      <c r="AP16" s="131">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-2)))</f>
+        <v>0.46674149492702643</v>
+      </c>
+      <c r="AQ16" s="131">
+        <f>Table3[[#This Row],[called position]]-pitchmod*(pitchstdv-Table3[[#This Row],[defense]])</f>
+        <v>-0.8</v>
+      </c>
+      <c r="AR16" s="131">
+        <f>ABS(Table3[[#This Row],[called position]]+pitchmod*(pitchstdv-Table3[[#This Row],[defense]]))</f>
+        <v>0.8</v>
+      </c>
+      <c r="AS16" s="6">
+        <f>Table3[[#This Row],[defense]]</f>
+        <v>1</v>
+      </c>
+      <c r="AT16" s="131">
+        <f>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;1, Table3[[#This Row],[location +1 stdv]]&gt;1),0, MIN(Table3[[#This Row],[location -1  stdv]]+1, 1-Table3[[#This Row],[location +1 stdv]]))</f>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="AU16" s="131">
+        <f>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;0, Table3[[#This Row],[location +1 stdv]]&gt;0),1, MAX(1-ABS(Table3[[#This Row],[location -1  stdv]]), Table3[[#This Row],[location +1 stdv]]-1))</f>
+        <v>1</v>
+      </c>
+      <c r="AV16" s="131">
+        <f>1/(ABS(Table3[[#This Row],[called position]]-1)+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>2.9090909090909092</v>
+      </c>
+      <c r="AW16" s="131">
+        <f>1/(Table3[[#This Row],[min dist to sz 1stdv]]+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>5.3333333333333339</v>
+      </c>
+      <c r="AX16" s="131">
+        <f>1/(Table3[[#This Row],[max dist to sz 1stdv]]+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>2.9090909090909092</v>
       </c>
     </row>
-    <row r="17" spans="1:40" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:50" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -9722,7 +10208,7 @@
       </c>
       <c r="AF17" s="23">
         <f>$AF$34*$AF$25</f>
-        <v>-13.333333333333332</v>
+        <v>-20</v>
       </c>
       <c r="AG17" s="23">
         <f>$AG$25*($AG$34*Table3[[#This Row],[offense]])</f>
@@ -9742,22 +10228,62 @@
       </c>
       <c r="AK17" s="23" cm="1">
         <f t="array" ref="AK17">SUM(Table3[[#This Row],[count]:[current hitter vs next hitter]]*MIN(1, Table3[[#This Row],[defense]]))</f>
-        <v>-13.333333333333332</v>
+        <v>-20</v>
       </c>
       <c r="AL17" s="96">
         <f>$AL$25-(Table3[[#This Row],[calling modifier]]/(ABS(Table3[[#This Row],[calling modifier]])+$AL$29)*$AL$27)</f>
-        <v>0.76</v>
+        <v>0.8</v>
       </c>
       <c r="AM17" s="112">
         <f>$AL$25-$AL$27*TANH(Table3[[#This Row],[calling modifier]]/$AM$29)</f>
-        <v>0.83311317813916408</v>
-      </c>
-      <c r="AN17" s="124">
-        <f>1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*(0.4*(3-Table3[[#This Row],[defense]]))</f>
-        <v>0.22676736385001672</v>
+        <v>0.90463766238230592</v>
+      </c>
+      <c r="AN17" s="132">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-Table3[[#This Row],[defense]])))</f>
+        <v>0</v>
+      </c>
+      <c r="AO17" s="133">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-0.2)))</f>
+        <v>0</v>
+      </c>
+      <c r="AP17" s="133">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-2)))</f>
+        <v>0.47662466357427224</v>
+      </c>
+      <c r="AQ17" s="133">
+        <f>Table3[[#This Row],[called position]]-pitchmod*(pitchstdv-Table3[[#This Row],[defense]])</f>
+        <v>-0.8</v>
+      </c>
+      <c r="AR17" s="133">
+        <f>ABS(Table3[[#This Row],[called position]]+pitchmod*(pitchstdv-Table3[[#This Row],[defense]]))</f>
+        <v>0.8</v>
+      </c>
+      <c r="AS17" s="23">
+        <f>Table3[[#This Row],[defense]]</f>
+        <v>1</v>
+      </c>
+      <c r="AT17" s="133">
+        <f>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;1, Table3[[#This Row],[location +1 stdv]]&gt;1),0, MIN(Table3[[#This Row],[location -1  stdv]]+1, 1-Table3[[#This Row],[location +1 stdv]]))</f>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="AU17" s="133">
+        <f>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;0, Table3[[#This Row],[location +1 stdv]]&gt;0),1, MAX(1-ABS(Table3[[#This Row],[location -1  stdv]]), Table3[[#This Row],[location +1 stdv]]-1))</f>
+        <v>1</v>
+      </c>
+      <c r="AV17" s="133">
+        <f>1/(ABS(Table3[[#This Row],[called position]]-1)+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>2.9090909090909092</v>
+      </c>
+      <c r="AW17" s="133">
+        <f>1/(Table3[[#This Row],[min dist to sz 1stdv]]+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>5.3333333333333339</v>
+      </c>
+      <c r="AX17" s="133">
+        <f>1/(Table3[[#This Row],[max dist to sz 1stdv]]+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>2.9090909090909092</v>
       </c>
     </row>
-    <row r="18" spans="1:40" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:50" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -9884,7 +10410,7 @@
       </c>
       <c r="AF18" s="6">
         <f>$AF$34*$AF$25</f>
-        <v>-13.333333333333332</v>
+        <v>-20</v>
       </c>
       <c r="AG18" s="6">
         <f>$AG$25*($AG$34*Table3[[#This Row],[offense]])</f>
@@ -9904,22 +10430,62 @@
       </c>
       <c r="AK18" s="6" cm="1">
         <f t="array" ref="AK18">SUM(Table3[[#This Row],[count]:[current hitter vs next hitter]]*MIN(1, Table3[[#This Row],[defense]]))</f>
-        <v>-12.333333333333332</v>
+        <v>-19</v>
       </c>
       <c r="AL18" s="94">
         <f>$AL$25-(Table3[[#This Row],[calling modifier]]/(ABS(Table3[[#This Row],[calling modifier]])+$AL$29)*$AL$27)</f>
-        <v>0.75257731958762886</v>
+        <v>0.79487179487179482</v>
       </c>
       <c r="AM18" s="111">
         <f>$AL$25-$AL$27*TANH(Table3[[#This Row],[calling modifier]]/$AM$29)</f>
-        <v>0.81952116241142281</v>
-      </c>
-      <c r="AN18" s="123">
-        <f>1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*(0.4*(3-Table3[[#This Row],[defense]]))</f>
-        <v>0.26916658321025666</v>
+        <v>0.89591322050960165</v>
+      </c>
+      <c r="AN18" s="130">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-Table3[[#This Row],[defense]])))</f>
+        <v>0</v>
+      </c>
+      <c r="AO18" s="131">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-0.2)))</f>
+        <v>0</v>
+      </c>
+      <c r="AP18" s="131">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-2)))</f>
+        <v>0.496558574279514</v>
+      </c>
+      <c r="AQ18" s="131">
+        <f>Table3[[#This Row],[called position]]-pitchmod*(pitchstdv-Table3[[#This Row],[defense]])</f>
+        <v>-0.8</v>
+      </c>
+      <c r="AR18" s="131">
+        <f>ABS(Table3[[#This Row],[called position]]+pitchmod*(pitchstdv-Table3[[#This Row],[defense]]))</f>
+        <v>0.8</v>
+      </c>
+      <c r="AS18" s="6">
+        <f>Table3[[#This Row],[defense]]</f>
+        <v>1</v>
+      </c>
+      <c r="AT18" s="131">
+        <f>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;1, Table3[[#This Row],[location +1 stdv]]&gt;1),0, MIN(Table3[[#This Row],[location -1  stdv]]+1, 1-Table3[[#This Row],[location +1 stdv]]))</f>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="AU18" s="131">
+        <f>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;0, Table3[[#This Row],[location +1 stdv]]&gt;0),1, MAX(1-ABS(Table3[[#This Row],[location -1  stdv]]), Table3[[#This Row],[location +1 stdv]]-1))</f>
+        <v>1</v>
+      </c>
+      <c r="AV18" s="131">
+        <f>1/(ABS(Table3[[#This Row],[called position]]-1)+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>2.9090909090909092</v>
+      </c>
+      <c r="AW18" s="131">
+        <f>1/(Table3[[#This Row],[min dist to sz 1stdv]]+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>5.3333333333333339</v>
+      </c>
+      <c r="AX18" s="131">
+        <f>1/(Table3[[#This Row],[max dist to sz 1stdv]]+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>2.9090909090909092</v>
       </c>
     </row>
-    <row r="19" spans="1:40" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:50" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -10046,7 +10612,7 @@
       </c>
       <c r="AF19" s="15">
         <f>$AF$34*$AF$25</f>
-        <v>-13.333333333333332</v>
+        <v>-20</v>
       </c>
       <c r="AG19" s="15">
         <f>$AG$25*($AG$34*Table3[[#This Row],[offense]])</f>
@@ -10066,22 +10632,62 @@
       </c>
       <c r="AK19" s="15" cm="1">
         <f t="array" ref="AK19">SUM(Table3[[#This Row],[count]:[current hitter vs next hitter]]*MIN(1, Table3[[#This Row],[defense]]))</f>
-        <v>-14.233333333333333</v>
+        <v>-20.9</v>
       </c>
       <c r="AL19" s="98">
         <f>$AL$25-(Table3[[#This Row],[calling modifier]]/(ABS(Table3[[#This Row],[calling modifier]])+$AL$29)*$AL$27)</f>
-        <v>0.76630963972736121</v>
+        <v>0.80440097799511001</v>
       </c>
       <c r="AM19" s="113">
         <f>$AL$25-$AL$27*TANH(Table3[[#This Row],[calling modifier]]/$AM$29)</f>
-        <v>0.84468835688869581</v>
-      </c>
-      <c r="AN19" s="125">
-        <f>1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*(0.4*(3-Table3[[#This Row],[defense]]))</f>
-        <v>0.59443397737746961</v>
+        <v>0.91194194050999755</v>
+      </c>
+      <c r="AN19" s="134">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-Table3[[#This Row],[defense]])))</f>
+        <v>0.45887572678899413</v>
+      </c>
+      <c r="AO19" s="135">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-0.2)))</f>
+        <v>0</v>
+      </c>
+      <c r="AP19" s="135">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-2)))</f>
+        <v>0.45887572678899413</v>
+      </c>
+      <c r="AQ19" s="135">
+        <f>Table3[[#This Row],[called position]]-pitchmod*(pitchstdv-Table3[[#This Row],[defense]])</f>
+        <v>5.8875726788994109E-2</v>
+      </c>
+      <c r="AR19" s="135">
+        <f>ABS(Table3[[#This Row],[called position]]+pitchmod*(pitchstdv-Table3[[#This Row],[defense]]))</f>
+        <v>0.85887572678899415</v>
+      </c>
+      <c r="AS19" s="15">
+        <f>Table3[[#This Row],[defense]]</f>
+        <v>2</v>
+      </c>
+      <c r="AT19" s="135">
+        <f>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;1, Table3[[#This Row],[location +1 stdv]]&gt;1),0, MIN(Table3[[#This Row],[location -1  stdv]]+1, 1-Table3[[#This Row],[location +1 stdv]]))</f>
+        <v>0.14112427321100585</v>
+      </c>
+      <c r="AU19" s="135">
+        <f>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;0, Table3[[#This Row],[location +1 stdv]]&gt;0),1, MAX(1-ABS(Table3[[#This Row],[location -1  stdv]]), Table3[[#This Row],[location +1 stdv]]-1))</f>
+        <v>0.94112427321100589</v>
+      </c>
+      <c r="AV19" s="135">
+        <f>1/(ABS(Table3[[#This Row],[called position]]-1)+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>5.5597600056407188</v>
+      </c>
+      <c r="AW19" s="135">
+        <f>1/(Table3[[#This Row],[min dist to sz 1stdv]]+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>8.1472390426861274</v>
+      </c>
+      <c r="AX19" s="135">
+        <f>1/(Table3[[#This Row],[max dist to sz 1stdv]]+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>4.9605001302254035</v>
       </c>
     </row>
-    <row r="20" spans="1:40" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:50" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -10208,7 +10814,7 @@
       </c>
       <c r="AF20" s="11">
         <f>$AF$34*$AF$25</f>
-        <v>-13.333333333333332</v>
+        <v>-20</v>
       </c>
       <c r="AG20" s="11">
         <f>$AG$25*($AG$34*Table3[[#This Row],[offense]])</f>
@@ -10228,22 +10834,62 @@
       </c>
       <c r="AK20" s="11" cm="1">
         <f t="array" ref="AK20">SUM(Table3[[#This Row],[count]:[current hitter vs next hitter]]*MIN(1, Table3[[#This Row],[defense]]))</f>
-        <v>-13.833333333333332</v>
+        <v>-20.5</v>
       </c>
       <c r="AL20" s="100">
         <f>$AL$25-(Table3[[#This Row],[calling modifier]]/(ABS(Table3[[#This Row],[calling modifier]])+$AL$29)*$AL$27)</f>
-        <v>0.76354679802955661</v>
+        <v>0.80246913580246915</v>
       </c>
       <c r="AM20" s="114">
         <f>$AL$25-$AL$27*TANH(Table3[[#This Row],[calling modifier]]/$AM$29)</f>
-        <v>0.83962065174226819</v>
-      </c>
-      <c r="AN20" s="126">
-        <f>1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*(0.4*(3-Table3[[#This Row],[defense]]))</f>
-        <v>0.60284000551751582</v>
+        <v>0.90875809497616733</v>
+      </c>
+      <c r="AN20" s="136">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-Table3[[#This Row],[defense]])))</f>
+        <v>0.46674149492702643</v>
+      </c>
+      <c r="AO20" s="137">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-0.2)))</f>
+        <v>0</v>
+      </c>
+      <c r="AP20" s="137">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-2)))</f>
+        <v>0.46674149492702643</v>
+      </c>
+      <c r="AQ20" s="137">
+        <f>Table3[[#This Row],[called position]]-pitchmod*(pitchstdv-Table3[[#This Row],[defense]])</f>
+        <v>6.6741494927026412E-2</v>
+      </c>
+      <c r="AR20" s="137">
+        <f>ABS(Table3[[#This Row],[called position]]+pitchmod*(pitchstdv-Table3[[#This Row],[defense]]))</f>
+        <v>0.86674149492702646</v>
+      </c>
+      <c r="AS20" s="11">
+        <f>Table3[[#This Row],[defense]]</f>
+        <v>2</v>
+      </c>
+      <c r="AT20" s="137">
+        <f>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;1, Table3[[#This Row],[location +1 stdv]]&gt;1),0, MIN(Table3[[#This Row],[location -1  stdv]]+1, 1-Table3[[#This Row],[location +1 stdv]]))</f>
+        <v>0.13325850507297354</v>
+      </c>
+      <c r="AU20" s="137">
+        <f>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;0, Table3[[#This Row],[location +1 stdv]]&gt;0),1, MAX(1-ABS(Table3[[#This Row],[location -1  stdv]]), Table3[[#This Row],[location +1 stdv]]-1))</f>
+        <v>0.93325850507297359</v>
+      </c>
+      <c r="AV20" s="137">
+        <f>1/(ABS(Table3[[#This Row],[called position]]-1)+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>5.5791339429144582</v>
+      </c>
+      <c r="AW20" s="137">
+        <f>1/(Table3[[#This Row],[min dist to sz 1stdv]]+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>8.2870891232332813</v>
+      </c>
+      <c r="AX20" s="137">
+        <f>1/(Table3[[#This Row],[max dist to sz 1stdv]]+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>4.9678120190545885</v>
       </c>
     </row>
-    <row r="21" spans="1:40" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:50" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -10370,7 +11016,7 @@
       </c>
       <c r="AF21" s="15">
         <f>$AF$34*$AF$25</f>
-        <v>-13.333333333333332</v>
+        <v>-20</v>
       </c>
       <c r="AG21" s="15">
         <f>$AG$25*($AG$34*Table3[[#This Row],[offense]])</f>
@@ -10390,22 +11036,62 @@
       </c>
       <c r="AK21" s="15" cm="1">
         <f t="array" ref="AK21">SUM(Table3[[#This Row],[count]:[current hitter vs next hitter]]*MIN(1, Table3[[#This Row],[defense]]))</f>
-        <v>-13.333333333333332</v>
+        <v>-20</v>
       </c>
       <c r="AL21" s="98">
         <f>$AL$25-(Table3[[#This Row],[calling modifier]]/(ABS(Table3[[#This Row],[calling modifier]])+$AL$29)*$AL$27)</f>
-        <v>0.76</v>
+        <v>0.8</v>
       </c>
       <c r="AM21" s="113">
         <f>$AL$25-$AL$27*TANH(Table3[[#This Row],[calling modifier]]/$AM$29)</f>
-        <v>0.83311317813916408</v>
-      </c>
-      <c r="AN21" s="125">
-        <f>1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*(0.4*(3-Table3[[#This Row],[defense]]))</f>
-        <v>0.61338368192500836</v>
+        <v>0.90463766238230592</v>
+      </c>
+      <c r="AN21" s="134">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-Table3[[#This Row],[defense]])))</f>
+        <v>0.47662466357427224</v>
+      </c>
+      <c r="AO21" s="135">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-0.2)))</f>
+        <v>0</v>
+      </c>
+      <c r="AP21" s="135">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-2)))</f>
+        <v>0.47662466357427224</v>
+      </c>
+      <c r="AQ21" s="135">
+        <f>Table3[[#This Row],[called position]]-pitchmod*(pitchstdv-Table3[[#This Row],[defense]])</f>
+        <v>7.6624663574272223E-2</v>
+      </c>
+      <c r="AR21" s="135">
+        <f>ABS(Table3[[#This Row],[called position]]+pitchmod*(pitchstdv-Table3[[#This Row],[defense]]))</f>
+        <v>0.87662466357427227</v>
+      </c>
+      <c r="AS21" s="15">
+        <f>Table3[[#This Row],[defense]]</f>
+        <v>2</v>
+      </c>
+      <c r="AT21" s="135">
+        <f>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;1, Table3[[#This Row],[location +1 stdv]]&gt;1),0, MIN(Table3[[#This Row],[location -1  stdv]]+1, 1-Table3[[#This Row],[location +1 stdv]]))</f>
+        <v>0.12337533642572773</v>
+      </c>
+      <c r="AU21" s="135">
+        <f>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;0, Table3[[#This Row],[location +1 stdv]]&gt;0),1, MAX(1-ABS(Table3[[#This Row],[location -1  stdv]]), Table3[[#This Row],[location +1 stdv]]-1))</f>
+        <v>0.92337533642572778</v>
+      </c>
+      <c r="AV21" s="135">
+        <f>1/(ABS(Table3[[#This Row],[called position]]-1)+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>5.6041699784494847</v>
+      </c>
+      <c r="AW21" s="135">
+        <f>1/(Table3[[#This Row],[min dist to sz 1stdv]]+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>8.4767699782849562</v>
+      </c>
+      <c r="AX21" s="135">
+        <f>1/(Table3[[#This Row],[max dist to sz 1stdv]]+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>4.9771585892353345</v>
       </c>
     </row>
-    <row r="22" spans="1:40" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:50" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -10532,7 +11218,7 @@
       </c>
       <c r="AF22" s="20">
         <f>$AF$34*$AF$25</f>
-        <v>-13.333333333333332</v>
+        <v>-20</v>
       </c>
       <c r="AG22" s="20">
         <f>$AG$25*($AG$34*Table3[[#This Row],[offense]])</f>
@@ -10552,44 +11238,90 @@
       </c>
       <c r="AK22" s="20" cm="1">
         <f t="array" ref="AK22">SUM(Table3[[#This Row],[count]:[current hitter vs next hitter]]*MIN(1, Table3[[#This Row],[defense]]))</f>
-        <v>-12.333333333333332</v>
+        <v>-19</v>
       </c>
       <c r="AL22" s="102">
         <f>$AL$25-(Table3[[#This Row],[calling modifier]]/(ABS(Table3[[#This Row],[calling modifier]])+$AL$29)*$AL$27)</f>
-        <v>0.75257731958762886</v>
+        <v>0.79487179487179482</v>
       </c>
       <c r="AM22" s="115">
         <f>$AL$25-$AL$27*TANH(Table3[[#This Row],[calling modifier]]/$AM$29)</f>
-        <v>0.81952116241142281</v>
-      </c>
-      <c r="AN22" s="127">
-        <f>1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*(0.4*(3-Table3[[#This Row],[defense]]))</f>
-        <v>0.63458329160512839</v>
+        <v>0.89591322050960165</v>
+      </c>
+      <c r="AN22" s="138">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-Table3[[#This Row],[defense]])))</f>
+        <v>0.496558574279514</v>
+      </c>
+      <c r="AO22" s="139">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-0.2)))</f>
+        <v>0</v>
+      </c>
+      <c r="AP22" s="139">
+        <f>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-2)))</f>
+        <v>0.496558574279514</v>
+      </c>
+      <c r="AQ22" s="139">
+        <f>Table3[[#This Row],[called position]]-pitchmod*(pitchstdv-Table3[[#This Row],[defense]])</f>
+        <v>9.6558574279513976E-2</v>
+      </c>
+      <c r="AR22" s="139">
+        <f>ABS(Table3[[#This Row],[called position]]+pitchmod*(pitchstdv-Table3[[#This Row],[defense]]))</f>
+        <v>0.89655857427951402</v>
+      </c>
+      <c r="AS22" s="20">
+        <f>Table3[[#This Row],[defense]]</f>
+        <v>2</v>
+      </c>
+      <c r="AT22" s="139">
+        <f>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;1, Table3[[#This Row],[location +1 stdv]]&gt;1),0, MIN(Table3[[#This Row],[location -1  stdv]]+1, 1-Table3[[#This Row],[location +1 stdv]]))</f>
+        <v>0.10344142572048598</v>
+      </c>
+      <c r="AU22" s="139">
+        <f>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;0, Table3[[#This Row],[location +1 stdv]]&gt;0),1, MAX(1-ABS(Table3[[#This Row],[location -1  stdv]]), Table3[[#This Row],[location +1 stdv]]-1))</f>
+        <v>0.90344142572048602</v>
+      </c>
+      <c r="AV22" s="139">
+        <f>1/(ABS(Table3[[#This Row],[called position]]-1)+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>5.6571616686839796</v>
+      </c>
+      <c r="AW22" s="139">
+        <f>1/(Table3[[#This Row],[min dist to sz 1stdv]]+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>8.9154197403921494</v>
+      </c>
+      <c r="AX22" s="139">
+        <f>1/(Table3[[#This Row],[max dist to sz 1stdv]]+$AV$27)+$AV$30*Table3[[#This Row],[defense]]</f>
+        <v>4.9965703770720697</v>
       </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:50" x14ac:dyDescent="0.25">
       <c r="Y24" s="63" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="Z24" s="64"/>
       <c r="AA24" s="65"/>
       <c r="AB24" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="AF24" s="63" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="AG24" s="103" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="AH24" s="64"/>
       <c r="AI24" s="64"/>
       <c r="AJ24" s="65"/>
       <c r="AL24" t="s">
+        <v>194</v>
+      </c>
+      <c r="AN24" t="s">
         <v>203</v>
       </c>
+      <c r="AV24" t="s">
+        <v>211</v>
+      </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:50" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
         <v>89</v>
       </c>
@@ -10615,19 +11347,19 @@
         <v>109</v>
       </c>
       <c r="W25" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="X25" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="Y25" s="66" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="Z25" s="72" t="s">
         <v>99</v>
       </c>
       <c r="AA25" s="67" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="AB25" s="72">
         <v>4</v>
@@ -10650,8 +11382,14 @@
       <c r="AL25">
         <v>0.6</v>
       </c>
+      <c r="AN25">
+        <v>0.4</v>
+      </c>
+      <c r="AV25">
+        <v>10</v>
+      </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:50" x14ac:dyDescent="0.25">
       <c r="D26">
         <v>0.1</v>
       </c>
@@ -10687,34 +11425,40 @@
       </c>
       <c r="Y26" s="68"/>
       <c r="Z26" s="69" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="AA26" s="70" t="s">
         <v>99</v>
       </c>
       <c r="AB26" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="AF26" s="60" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="AG26" s="60" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="AH26" s="60" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="AI26" s="60" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="AJ26" s="60" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="AL26" t="s">
-        <v>206</v>
+        <v>197</v>
+      </c>
+      <c r="AN26" t="s">
+        <v>204</v>
+      </c>
+      <c r="AV26" t="s">
+        <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:50" x14ac:dyDescent="0.25">
       <c r="K27" t="s">
         <v>91</v>
       </c>
@@ -10725,20 +11469,20 @@
         <v>1.7</v>
       </c>
       <c r="W27" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="Y27" s="76" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="Z27" s="64"/>
       <c r="AA27" s="65" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="AB27">
         <v>0.1</v>
       </c>
       <c r="AF27" s="61">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AG27" s="61">
         <v>1</v>
@@ -10755,8 +11499,15 @@
       <c r="AL27">
         <v>0.4</v>
       </c>
+      <c r="AN27">
+        <v>3</v>
+      </c>
+      <c r="AV27">
+        <f>1/AV25</f>
+        <v>0.1</v>
+      </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:50" x14ac:dyDescent="0.25">
       <c r="K28">
         <v>0.9</v>
       </c>
@@ -10764,7 +11515,7 @@
         <v>0</v>
       </c>
       <c r="Y28" s="71" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="Z28" s="32">
         <v>-0.2</v>
@@ -10774,29 +11525,29 @@
         <v>-0.2</v>
       </c>
       <c r="AF28" s="61" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="AG28" s="61" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="AH28" s="61" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="AI28" s="61"/>
       <c r="AJ28" s="61"/>
       <c r="AL28" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="AM28" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:50" x14ac:dyDescent="0.25">
       <c r="W29" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="Y29" s="71" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="Z29" s="32">
         <v>-0.4</v>
@@ -10823,14 +11574,17 @@
       <c r="AM29">
         <v>20</v>
       </c>
+      <c r="AV29" t="s">
+        <v>214</v>
+      </c>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:50" x14ac:dyDescent="0.25">
       <c r="W30">
         <f xml:space="preserve"> W28/2 - W26/3</f>
         <v>-0.33333333333333331</v>
       </c>
       <c r="Y30" s="71" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="Z30" s="32">
         <v>0</v>
@@ -10840,24 +11594,27 @@
         <v>0</v>
       </c>
       <c r="AF30" s="61" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="AG30" s="61"/>
       <c r="AH30" s="61" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="AI30" s="61"/>
       <c r="AJ30" s="61"/>
+      <c r="AV30">
+        <v>2</v>
+      </c>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:50" x14ac:dyDescent="0.25">
       <c r="W31" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="X31" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="Y31" s="71" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="Z31" s="32">
         <v>0.8</v>
@@ -10876,10 +11633,10 @@
       <c r="AI31" s="61"/>
       <c r="AJ31" s="61"/>
       <c r="AL31" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
     </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:50" x14ac:dyDescent="0.25">
       <c r="W32">
         <f>MAX(0, ((W26+X26)/(3+X26))-(W28/2))</f>
         <v>0.42857142857142855</v>
@@ -10908,10 +11665,10 @@
     </row>
     <row r="33" spans="24:38" x14ac:dyDescent="0.25">
       <c r="X33" t="s">
+        <v>150</v>
+      </c>
+      <c r="Y33" s="68" t="s">
         <v>158</v>
-      </c>
-      <c r="Y33" s="68" t="s">
-        <v>166</v>
       </c>
       <c r="Z33" s="69">
         <v>0.5</v>
@@ -10921,20 +11678,20 @@
         <v>-0.90000000000000013</v>
       </c>
       <c r="AF33" s="61" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="AG33" s="61" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="AH33" s="61" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="AI33" s="61" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="AJ33" s="61"/>
       <c r="AL33" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="34" spans="24:38" x14ac:dyDescent="0.25">
@@ -10943,7 +11700,7 @@
       </c>
       <c r="AF34" s="62">
         <f xml:space="preserve"> IF(SUM(AF27,AF29)=0, AF31,  AF29/2-AF27/3)</f>
-        <v>-0.66666666666666663</v>
+        <v>-1</v>
       </c>
       <c r="AG34" s="62">
         <f>AG27-AG29</f>
@@ -10965,7 +11722,7 @@
     </row>
     <row r="35" spans="24:38" x14ac:dyDescent="0.25">
       <c r="Z35" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="AA35">
         <v>-0.2</v>
@@ -10973,7 +11730,7 @@
     </row>
     <row r="36" spans="24:38" x14ac:dyDescent="0.25">
       <c r="Z36" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="AA36">
         <v>0.4</v>
@@ -10981,7 +11738,7 @@
     </row>
     <row r="37" spans="24:38" x14ac:dyDescent="0.25">
       <c r="Z37" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="AA37">
         <v>2</v>
@@ -10989,7 +11746,7 @@
     </row>
     <row r="38" spans="24:38" x14ac:dyDescent="0.25">
       <c r="Z38" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="AA38">
         <f>AA35</f>
@@ -10998,7 +11755,7 @@
     </row>
     <row r="39" spans="24:38" x14ac:dyDescent="0.25">
       <c r="Z39" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="AA39">
         <f>AA36-AA35</f>
@@ -11007,7 +11764,7 @@
     </row>
     <row r="40" spans="24:38" x14ac:dyDescent="0.25">
       <c r="Z40" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="AA40">
         <f>AA36-AA41</f>
@@ -11016,7 +11773,7 @@
     </row>
     <row r="41" spans="24:38" x14ac:dyDescent="0.25">
       <c r="Z41" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="AA41">
         <f>(AA37-AA36)</f>
@@ -11025,7 +11782,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="O7:O22">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11043,7 +11800,7 @@
   <dimension ref="C2:S9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Finishing some stats planning. Fielding is still an open question, but I think we'll implement what we have first.
</commit_message>
<xml_diff>
--- a/plans/baseball stats.xlsx
+++ b/plans/baseball stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcgiffenk\Desktop\newpy\xtreemblaseball99\plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88607C53-FFE7-4046-96DA-8D1BDE742E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304D5927-64A9-4B4E-9984-8600057850EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1170,21 +1170,6 @@
     <t>ave obscurity</t>
   </si>
   <si>
-    <t>Column90</t>
-  </si>
-  <si>
-    <t>Column91</t>
-  </si>
-  <si>
-    <t>Column92</t>
-  </si>
-  <si>
-    <t>Column93</t>
-  </si>
-  <si>
-    <t>Column94</t>
-  </si>
-  <si>
     <t>Column95</t>
   </si>
   <si>
@@ -1448,6 +1433,21 @@
   </si>
   <si>
     <t>actual distance</t>
+  </si>
+  <si>
+    <t>+1stdv EV</t>
+  </si>
+  <si>
+    <t>+1stdv LA</t>
+  </si>
+  <si>
+    <t>+1stdv flight time</t>
+  </si>
+  <si>
+    <t>+1stdev distance</t>
+  </si>
+  <si>
+    <t>+1stdev delta</t>
   </si>
 </sst>
 </file>
@@ -2102,7 +2102,32 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="77">
+  <dxfs count="82">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="174" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -2120,16 +2145,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -7905,181 +7920,181 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A6:DO22" totalsRowShown="0" headerRowDxfId="76">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A6:DO22" totalsRowShown="0" headerRowDxfId="81">
   <autoFilter ref="A6:DO22" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="119">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Rep #">
       <calculatedColumnFormula>ROW()-ROW(home)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="offense" dataDxfId="75">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="offense" dataDxfId="80">
       <calculatedColumnFormula>INDEX(oratings, 1, 1+MOD(Table3[[#This Row],[Rep '#]]-1, COUNT(oratings)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="defense" dataDxfId="74">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="defense" dataDxfId="79">
       <calculatedColumnFormula>INDEX(dratings, 1, MOD(FLOOR( (Table3[[#This Row],[Rep '#]]-1) / COUNT(oratings), 1), COUNT(dratings))+1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="base leadoff" dataDxfId="73">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="base leadoff" dataDxfId="78">
       <calculatedColumnFormula>Table3[[#This Row],[offense]]*$D$26+0.05</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="leadoff modifier" dataDxfId="35">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="leadoff modifier" dataDxfId="40">
       <calculatedColumnFormula>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*$E$26</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="total leadoff (ft)" dataDxfId="72">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="total leadoff (ft)" dataDxfId="77">
       <calculatedColumnFormula>MAX(Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90, 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="pickoff manuver (s)" dataDxfId="71">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="pickoff manuver (s)" dataDxfId="76">
       <calculatedColumnFormula>1.1 - Table3[[#This Row],[defense]]*0.1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="throw speed (s/ft)" dataDxfId="70">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="throw speed (s/ft)" dataDxfId="75">
       <calculatedColumnFormula xml:space="preserve"> 0.01 - 0.0025 *  Table3[[#This Row],[defense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="throw speed (mph)" dataDxfId="69">
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="throw speed (mph)" dataDxfId="74">
       <calculatedColumnFormula>1 / Table3[[#This Row],[throw speed (s/ft)]] * ((60 * 60)/5280)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="pickoff time" dataDxfId="68">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="pickoff time" dataDxfId="73">
       <calculatedColumnFormula>Table3[[#This Row],[pickoff manuver (s)]]+60*Table3[[#This Row],[throw speed (s/ft)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="runner reaction" dataDxfId="67">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="runner reaction" dataDxfId="72">
       <calculatedColumnFormula>$K$28-$K$26*Table3[[#This Row],[offense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="runner speed (s/ft)" dataDxfId="66">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="runner speed (s/ft)" dataDxfId="71">
       <calculatedColumnFormula>0.05 - Table3[[#This Row],[offense]]*$L$26</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="runner speed (mph)" dataDxfId="65">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="runner speed (mph)" dataDxfId="70">
       <calculatedColumnFormula>1 / Table3[[#This Row],[runner speed (s/ft)]] * ((60 * 60)/5280)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="pickoff evade time" dataDxfId="64">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="pickoff evade time" dataDxfId="69">
       <calculatedColumnFormula>Table3[[#This Row],[runner reaction]]+Table3[[#This Row],[runner speed (s/ft)]]*Table3[[#This Row],[total leadoff (ft)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="pickoff probability" dataDxfId="63" dataCellStyle="Percent">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="pickoff probability" dataDxfId="68" dataCellStyle="Percent">
       <calculatedColumnFormula>1 - _xlfn.NORM.DIST(Table3[[#This Row],[pickoff time]], Table3[[#This Row],[pickoff evade time]], $O$4, TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Fielding Odds" dataDxfId="62" dataCellStyle="Percent">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Fielding Odds" dataDxfId="67" dataCellStyle="Percent">
       <calculatedColumnFormula>_xlfn.NORM.DIST(Table3[[#This Row],[defense]], $P$26, $P$27, TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="pickoff worth it?" dataDxfId="61">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="pickoff worth it?" dataDxfId="66">
       <calculatedColumnFormula>Table3[[#This Row],[pickoff probability]] &gt; 1-Table3[[#This Row],[Fielding Odds]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Error %" dataDxfId="60" dataCellStyle="Percent">
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Error %" dataDxfId="65" dataCellStyle="Percent">
       <calculatedColumnFormula>1-Table3[[#This Row],[Fielding Odds]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Blatant steal time" dataDxfId="59">
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Blatant steal time" dataDxfId="64">
       <calculatedColumnFormula>(90-Table3[[#This Row],[total leadoff (ft)]])*Table3[[#This Row],[runner speed (s/ft)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Response speed" dataDxfId="58">
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Response speed" dataDxfId="63">
       <calculatedColumnFormula>$T$26*(2-Table3[[#This Row],[defense]]) + Table3[[#This Row],[pickoff time]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="blatant steal probability" dataDxfId="57" dataCellStyle="Percent">
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="blatant steal probability" dataDxfId="62" dataCellStyle="Percent">
       <calculatedColumnFormula>_xlfn.NORM.DIST(Table3[[#This Row],[Response speed]], Table3[[#This Row],[Blatant steal time]], $U$4, TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="defense fear" dataDxfId="56">
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="defense fear" dataDxfId="61">
       <calculatedColumnFormula>Table3[[#This Row],[defense]]+Table3[[#This Row],[defense]]*Table3[[#This Row],[offense]]*$E$26</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="ball factor" dataDxfId="55">
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="ball factor" dataDxfId="60">
       <calculatedColumnFormula>(1-$W$32)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="desperation" dataDxfId="54" dataCellStyle="Percent">
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="desperation" dataDxfId="59" dataCellStyle="Percent">
       <calculatedColumnFormula>Table3[[#This Row],[ball factor]]/$X$32*(1-$X$34)+$X$34</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="player control" dataDxfId="53">
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="player control" dataDxfId="58">
       <calculatedColumnFormula>Table3[[#This Row],[offense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="ideal steer" dataDxfId="52">
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="ideal steer" dataDxfId="57">
       <calculatedColumnFormula>$AA$33</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="scaled control" dataDxfId="51">
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="scaled control" dataDxfId="56">
       <calculatedColumnFormula>IF(Table3[[#This Row],[player control]]&gt;1,Table3[[#This Row],[player control]]*$AA$41+$AA$40,Table3[[#This Row],[player control]]*$AA$39+$AA$38)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="unmod foul percent 3rd" dataDxfId="50" dataCellStyle="Percent">
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="unmod foul percent 3rd" dataDxfId="55" dataCellStyle="Percent">
       <calculatedColumnFormula>_xlfn.NORM.DIST(-1,Table3[[#This Row],[ideal steer]],($AB$25-Table3[[#This Row],[scaled control]])*$AB$27,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="unmod foul percent 1st" dataDxfId="49" dataCellStyle="Percent">
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="unmod foul percent 1st" dataDxfId="54" dataCellStyle="Percent">
       <calculatedColumnFormula>1-_xlfn.NORM.DIST(1,Table3[[#This Row],[ideal steer]],($AB$25-Table3[[#This Row],[scaled control]])*$AB$27,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="total unmod foul percent" dataDxfId="48" dataCellStyle="Percent">
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="total unmod foul percent" dataDxfId="53" dataCellStyle="Percent">
       <calculatedColumnFormula>1-(1-Table3[[#This Row],[unmod foul percent 3rd]])*(1-Table3[[#This Row],[unmod foul percent 1st]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="unmod dead center foul%" dataDxfId="47" dataCellStyle="Percent">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="unmod dead center foul%" dataDxfId="52" dataCellStyle="Percent">
       <calculatedColumnFormula>1-((1-_xlfn.NORM.DIST(-1,0,($AB$25-Table3[[#This Row],[scaled control]])*$AB$27,TRUE))*_xlfn.NORM.DIST(1,0,($AB$25-Table3[[#This Row],[scaled control]])*$AB$27,TRUE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="count" dataDxfId="46">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="count" dataDxfId="51">
       <calculatedColumnFormula>$AF$34*$AF$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="hitter discipline bias" dataDxfId="45">
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="hitter discipline bias" dataDxfId="50">
       <calculatedColumnFormula>$AG$25*($AG$34*Table3[[#This Row],[offense]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="bases loaded" dataDxfId="44">
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="bases loaded" dataDxfId="49">
       <calculatedColumnFormula>$AH$25*$AH$34</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="number of outs" dataDxfId="43">
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="number of outs" dataDxfId="48">
       <calculatedColumnFormula>$AI$34*$AI$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="current hitter vs next hitter" dataDxfId="42">
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="current hitter vs next hitter" dataDxfId="47">
       <calculatedColumnFormula>$AJ$25*(Table3[[#This Row],[offense]]-$AJ$27)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="calling modifier" dataDxfId="41">
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="calling modifier" dataDxfId="46">
       <calculatedColumnFormula array="1">SUM(Table3[[#This Row],[count]:[current hitter vs next hitter]]*MIN(1, Table3[[#This Row],[defense]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="sigmoid strike percent" dataDxfId="40" dataCellStyle="Percent">
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="sigmoid strike percent" dataDxfId="45" dataCellStyle="Percent">
       <calculatedColumnFormula>$AL$25-(Table3[[#This Row],[calling modifier]]/(ABS(Table3[[#This Row],[calling modifier]])+$AL$29)*$AL$27)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="tanh strike percent" dataDxfId="39" dataCellStyle="Percent">
+    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="tanh strike percent" dataDxfId="44" dataCellStyle="Percent">
       <calculatedColumnFormula>$AL$25-$AL$27*TANH(Table3[[#This Row],[calling modifier]]/$AM$29)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="called position" dataDxfId="38" dataCellStyle="Percent">
+    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="called position" dataDxfId="43" dataCellStyle="Percent">
       <calculatedColumnFormula>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-Table3[[#This Row],[defense]])))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="called pos 0.2 pitch" dataDxfId="37">
+    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="called pos 0.2 pitch" dataDxfId="42">
       <calculatedColumnFormula>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-0.2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="called pos 2 pitch" dataDxfId="36">
+    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="called pos 2 pitch" dataDxfId="41">
       <calculatedColumnFormula>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="location -1  stdv" dataDxfId="33">
+    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="location -1  stdv" dataDxfId="38">
       <calculatedColumnFormula>Table3[[#This Row],[called position]]-pitchmod*(pitchstdv-Table3[[#This Row],[defense]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="location +1 stdv" dataDxfId="34">
+    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="location +1 stdv" dataDxfId="39">
       <calculatedColumnFormula>ABS(Table3[[#This Row],[called position]]+pitchmod*(pitchstdv-Table3[[#This Row],[defense]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="min dist to sz 1stdv" dataDxfId="32">
+    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="min dist to sz 1stdv" dataDxfId="37">
       <calculatedColumnFormula>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;1, Table3[[#This Row],[location +1 stdv]]&gt;1),0, MIN(Table3[[#This Row],[location -1  stdv]]+1, 1-Table3[[#This Row],[location +1 stdv]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="max dist to sz 1stdv" dataDxfId="31">
+    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="max dist to sz 1stdv" dataDxfId="36">
       <calculatedColumnFormula>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;0, Table3[[#This Row],[location +1 stdv]]&gt;0),1, MAX(1-ABS(Table3[[#This Row],[location -1  stdv]]), Table3[[#This Row],[location +1 stdv]]-1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="ave obscurity" dataDxfId="30">
+    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="ave obscurity" dataDxfId="35">
       <calculatedColumnFormula>$AU$30/(ABS(Table3[[#This Row],[called position]]-1)+$AU$27)+$AU$32*Table3[[#This Row],[defense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="obscurity at _x000a_0.5" dataDxfId="29">
+    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="obscurity at _x000a_0.5" dataDxfId="34">
       <calculatedColumnFormula>$AU$30/(ABS(0.5-1)+$AU$27)+$AU$32*Table3[[#This Row],[defense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="obscurity at  0.9" dataDxfId="28">
+    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="obscurity at  0.9" dataDxfId="33">
       <calculatedColumnFormula>$AU$30/(ABS(0.9-1)+$AU$27)+$AU$32*Table3[[#This Row],[defense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="average difficulty" dataDxfId="18">
+    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="average difficulty" dataDxfId="23">
       <calculatedColumnFormula>Table3[[#This Row],[defense]]*$AX$30+MAX(0, Table3[[#This Row],[called position]]-$AX$27)^$AX$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" name="+1stdv difficulty" dataDxfId="17">
+    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" name="+1stdv difficulty" dataDxfId="22">
       <calculatedColumnFormula>Table3[[#This Row],[defense]]*$AX$30 + MAX(0, Table3[[#This Row],[location +1 stdv]]-$AX$27)^$AX$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0000-000037000000}" name="difficulty at 1" dataDxfId="16">
+    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0000-000037000000}" name="difficulty at 1" dataDxfId="21">
       <calculatedColumnFormula>Table3[[#This Row],[defense]]*$AX$30+MAX(0, 1-$AX$27)^$AX$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="62" xr3:uid="{6513900D-2CAC-4022-A6B3-8A00EE6C566B}" name="reduction" dataDxfId="27">
+    <tableColumn id="62" xr3:uid="{6513900D-2CAC-4022-A6B3-8A00EE6C566B}" name="reduction" dataDxfId="32">
       <calculatedColumnFormula>MAX(0, 0.1*(1-Table3[[#This Row],[defense]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="63" xr3:uid="{12464915-1D8C-4EB5-9BBD-0FF526658E5B}" name="Location" dataDxfId="26">
+    <tableColumn id="63" xr3:uid="{12464915-1D8C-4EB5-9BBD-0FF526658E5B}" name="Location" dataDxfId="31">
       <calculatedColumnFormula>$BB$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="64" xr3:uid="{5F0F19BE-6D04-4E9E-81B2-B324AB353F5C}" name="obscurity" dataDxfId="25">
+    <tableColumn id="64" xr3:uid="{5F0F19BE-6D04-4E9E-81B2-B324AB353F5C}" name="obscurity" dataDxfId="30">
       <calculatedColumnFormula>$AU$30/(ABS(Table3[[#This Row],[Location]]-1)+$AU$27)+$AU$32*Table3[[#This Row],[defense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="65" xr3:uid="{EA3D32E7-A2E2-482C-B6E9-2E17651C5F77}" name="Strike?" dataDxfId="22">
+    <tableColumn id="65" xr3:uid="{EA3D32E7-A2E2-482C-B6E9-2E17651C5F77}" name="Strike?" dataDxfId="27">
       <calculatedColumnFormula>Table3[[#This Row],[Location]]&lt;= (1+MAX(0, (Table3[[#This Row],[defense]]-1)*0.1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="66" xr3:uid="{0C7E9B06-240B-481E-B495-54026E2F00AA}" name="discipline modifier" dataDxfId="24">
+    <tableColumn id="66" xr3:uid="{0C7E9B06-240B-481E-B495-54026E2F00AA}" name="discipline modifier" dataDxfId="29">
       <calculatedColumnFormula>1/(1+Table3[[#This Row],[offense]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="67" xr3:uid="{D3B0837D-02D4-4F62-A2E2-876739E497B0}" name="effective obscurity" dataDxfId="23">
+    <tableColumn id="67" xr3:uid="{D3B0837D-02D4-4F62-A2E2-876739E497B0}" name="effective obscurity" dataDxfId="28">
       <calculatedColumnFormula>Table3[[#This Row],[obscurity]]*Table3[[#This Row],[discipline modifier]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="69" xr3:uid="{39822A5F-1791-48DC-BA9F-A066931C0292}" name="odds of read" dataCellStyle="Percent">
@@ -8094,43 +8109,43 @@
     <tableColumn id="72" xr3:uid="{3E21C76F-F55B-4E49-9BE2-FEE046008C15}" name="adjusted swing %" dataCellStyle="Percent">
       <calculatedColumnFormula>Table3[[#This Row],[desperation echo]]*Table3[[#This Row],[unadjusted swing %]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="130" xr3:uid="{827C9303-3867-43F7-A79B-BC2EAB3F896D}" name="pitch carry forward obsc" dataDxfId="20">
+    <tableColumn id="130" xr3:uid="{827C9303-3867-43F7-A79B-BC2EAB3F896D}" name="pitch carry forward obsc" dataDxfId="25">
       <calculatedColumnFormula>Table3[[#This Row],[ave obscurity]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="131" xr3:uid="{F26B1E2C-89D5-4F6D-877A-1BEA7F7DF5A9}" name="CF odds of read" dataCellStyle="Percent">
       <calculatedColumnFormula>1/(1+Table3[[#This Row],[ave obscurity]]*Table3[[#This Row],[discipline modifier]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="73" xr3:uid="{77BBE784-030D-4E46-9A29-8783B89762BC}" name="contact echo" dataDxfId="21">
+    <tableColumn id="73" xr3:uid="{77BBE784-030D-4E46-9A29-8783B89762BC}" name="contact echo" dataDxfId="26">
       <calculatedColumnFormula>Table3[[#This Row],[offense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="75" xr3:uid="{074A9F48-3941-4E36-90C2-7710217D32C8}" name="pitch carry forward diff" dataDxfId="19">
+    <tableColumn id="75" xr3:uid="{074A9F48-3941-4E36-90C2-7710217D32C8}" name="pitch carry forward diff" dataDxfId="24">
       <calculatedColumnFormula>Table3[[#This Row],[average difficulty]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="76" xr3:uid="{628DDA60-D380-4EE8-AA7D-7EF6C4AAD8A5}" name="CF contact readiness" dataDxfId="15">
+    <tableColumn id="76" xr3:uid="{628DDA60-D380-4EE8-AA7D-7EF6C4AAD8A5}" name="CF contact readiness" dataDxfId="20">
       <calculatedColumnFormula>Table3[[#This Row],[contact echo]]-Table3[[#This Row],[pitch carry forward diff]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="77" xr3:uid="{DBF18AD6-8593-42C7-9058-D19737088E6D}" name="foul %" dataDxfId="13" dataCellStyle="Percent">
+    <tableColumn id="77" xr3:uid="{DBF18AD6-8593-42C7-9058-D19737088E6D}" name="foul %" dataDxfId="18" dataCellStyle="Percent">
       <calculatedColumnFormula>1-_xlfn.NORM.DIST($BP$27,Table3[[#This Row],[CF contact readiness]], $BP$30,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="78" xr3:uid="{6354951A-151E-4E04-9897-9CB39D6098C8}" name="clean %" dataDxfId="14" dataCellStyle="Percent">
+    <tableColumn id="78" xr3:uid="{6354951A-151E-4E04-9897-9CB39D6098C8}" name="clean %" dataDxfId="19" dataCellStyle="Percent">
       <calculatedColumnFormula>1-_xlfn.NORM.DIST($BP$25,Table3[[#This Row],[CF contact readiness]], $BP$30,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="79" xr3:uid="{0070F673-D13C-467D-95AC-FF8413A02F3F}" name="strike swinging %" dataDxfId="12" dataCellStyle="Percent">
+    <tableColumn id="79" xr3:uid="{0070F673-D13C-467D-95AC-FF8413A02F3F}" name="strike swinging %" dataDxfId="17" dataCellStyle="Percent">
       <calculatedColumnFormula>1-Table3[[#This Row],[foul %]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="80" xr3:uid="{9504D0CF-7CD0-472F-8289-44B30538D80C}" name="ave. hit quality" dataDxfId="11">
+    <tableColumn id="80" xr3:uid="{9504D0CF-7CD0-472F-8289-44B30538D80C}" name="ave. hit quality" dataDxfId="16">
       <calculatedColumnFormula>(Table3[[#This Row],[CF contact readiness]]-$BP$27)/$BP$30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="132" xr3:uid="{0BB169E4-F345-4B7D-A549-DE28DC5FB113}" name="hit quality +1stdv" dataDxfId="9">
+    <tableColumn id="132" xr3:uid="{0BB169E4-F345-4B7D-A549-DE28DC5FB113}" name="hit quality +1stdv" dataDxfId="14">
       <calculatedColumnFormula>(Table3[[#This Row],[CF contact readiness]]+$BP$30-$BP$27)/$BP$30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="81" xr3:uid="{37438EAA-344A-486C-A4C2-68EE17D67C60}" name="hit quality remainder" dataDxfId="8">
+    <tableColumn id="81" xr3:uid="{37438EAA-344A-486C-A4C2-68EE17D67C60}" name="hit quality remainder" dataDxfId="13">
       <calculatedColumnFormula>MAX(0, IF(ISBLANK($BU$28), Table3[[#This Row],[hit quality +1stdv]], $BU$28)-1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="82" xr3:uid="{CBA11BEE-0412-44C3-979C-1888629B3C7A}" name="adjusted launch angle" dataDxfId="7">
+    <tableColumn id="82" xr3:uid="{CBA11BEE-0412-44C3-979C-1888629B3C7A}" name="adjusted launch angle" dataDxfId="12">
       <calculatedColumnFormula>$BV$25+Table3[[#This Row],[offense]]*$BV$28</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="83" xr3:uid="{8DC0E209-2987-40FE-9521-B3339A7D8E1F}" name="angle stdev" dataDxfId="10">
+    <tableColumn id="83" xr3:uid="{8DC0E209-2987-40FE-9521-B3339A7D8E1F}" name="angle stdev" dataDxfId="15">
       <calculatedColumnFormula>$BW$25*$BW$28/($BW$28+Table3[[#This Row],[hit quality remainder]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="84" xr3:uid="{F8EB7F4C-5D31-472E-A363-210E62A7E683}" name="grounder % (&lt;10 deg)" dataCellStyle="Percent">
@@ -8139,29 +8154,39 @@
     <tableColumn id="85" xr3:uid="{56DD6E0A-39C0-4DF0-B1CB-47EB71B71306}" name="pop up % (&gt;50 deg)" dataCellStyle="Percent">
       <calculatedColumnFormula>1-_xlfn.NORM.DIST(50, Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="86" xr3:uid="{6ED971D4-0303-4AEB-B7CD-9516517F447E}" name="odds of 3B" dataDxfId="5" dataCellStyle="Percent">
+    <tableColumn id="86" xr3:uid="{6ED971D4-0303-4AEB-B7CD-9516517F447E}" name="odds of 3B" dataDxfId="11" dataCellStyle="Percent">
       <calculatedColumnFormula>1-_xlfn.NORM.DIST(70, $BZ$28,$BZ$25,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="87" xr3:uid="{E9F9DFB6-4A26-4CA7-9318-6ECA478690D6}" name="exit velocity mean" dataDxfId="4">
+    <tableColumn id="87" xr3:uid="{E9F9DFB6-4A26-4CA7-9318-6ECA478690D6}" name="exit velocity mean" dataDxfId="10">
       <calculatedColumnFormula>$CA$25+Table3[[#This Row],[offense]]*($CA$27-$CA$25)/2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="88" xr3:uid="{EB865A5D-CC1D-49FA-9709-DC5F30F55DD8}" name="after reduction" dataDxfId="3">
+    <tableColumn id="88" xr3:uid="{EB865A5D-CC1D-49FA-9709-DC5F30F55DD8}" name="after reduction" dataDxfId="9">
       <calculatedColumnFormula>Table3[[#This Row],[exit velocity mean]]-Table3[[#This Row],[reduction]]*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="89" xr3:uid="{949E8C38-C424-4A4E-9A6F-FCA93496D192}" name="theoretical distance" dataDxfId="2">
+    <tableColumn id="89" xr3:uid="{949E8C38-C424-4A4E-9A6F-FCA93496D192}" name="theoretical distance" dataDxfId="8">
       <calculatedColumnFormula>Table3[[#This Row],[exit velocity mean]]^2*2*SIN(RADIANS(Table3[[#This Row],[adjusted launch angle]]))/$CC$28*5280</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="90" xr3:uid="{9FD0A88A-D0D9-4369-8D70-6C7485CA1509}" name="flight time" dataDxfId="1">
+    <tableColumn id="90" xr3:uid="{9FD0A88A-D0D9-4369-8D70-6C7485CA1509}" name="flight time" dataDxfId="7">
       <calculatedColumnFormula>2*Table3[[#This Row],[exit velocity mean]]*SIN(RADIANS(Table3[[#This Row],[adjusted launch angle]]))/$CC$28*60*60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="91" xr3:uid="{D9D5DFED-BD09-4CB6-A82E-D289D2DAB08D}" name="actual distance" dataDxfId="0">
+    <tableColumn id="91" xr3:uid="{D9D5DFED-BD09-4CB6-A82E-D289D2DAB08D}" name="actual distance" dataDxfId="6">
       <calculatedColumnFormula>Table3[[#This Row],[theoretical distance]]-Table3[[#This Row],[flight time]]^2*$CE$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="92" xr3:uid="{3D80331E-564D-462D-81B5-E5CE730D1EE5}" name="Column90"/>
-    <tableColumn id="93" xr3:uid="{211123A1-65C0-4F59-AB86-C344CFF47F70}" name="Column91"/>
-    <tableColumn id="94" xr3:uid="{C8736D16-AF27-436D-BF61-CA3E58298CD3}" name="Column92"/>
-    <tableColumn id="95" xr3:uid="{C9967388-9755-4293-82E9-4E43A4770599}" name="Column93"/>
-    <tableColumn id="96" xr3:uid="{52B6BA3A-87F7-49FD-BFE7-811EA76B03FD}" name="Column94"/>
+    <tableColumn id="92" xr3:uid="{3D80331E-564D-462D-81B5-E5CE730D1EE5}" name="+1stdv EV" dataDxfId="5">
+      <calculatedColumnFormula>Table3[[#This Row],[exit velocity mean]]+$CC$25-Table3[[#This Row],[reduction]]*100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="93" xr3:uid="{211123A1-65C0-4F59-AB86-C344CFF47F70}" name="+1stdv LA" dataDxfId="0">
+      <calculatedColumnFormula>MIN(Table3[[#This Row],[adjusted launch angle]]+Table3[[#This Row],[angle stdev]], 30)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="94" xr3:uid="{C8736D16-AF27-436D-BF61-CA3E58298CD3}" name="+1stdv flight time" dataDxfId="4">
+      <calculatedColumnFormula>2*Table3[[#This Row],[+1stdv EV]]*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*60*60</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="95" xr3:uid="{C9967388-9755-4293-82E9-4E43A4770599}" name="+1stdev distance" dataDxfId="3">
+      <calculatedColumnFormula>Table3[[#This Row],[+1stdv EV]]^2*2*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*5280-Table3[[#This Row],[+1stdv flight time]]^2*$CE$25</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="96" xr3:uid="{52B6BA3A-87F7-49FD-BFE7-811EA76B03FD}" name="+1stdev delta" dataDxfId="2">
+      <calculatedColumnFormula>Table3[[#This Row],[+1stdev distance]]-Table3[[#This Row],[actual distance]]</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="97" xr3:uid="{50EEB2EF-C836-4BBC-A8B3-EAD31BF29B54}" name="Column95"/>
     <tableColumn id="98" xr3:uid="{823DCE3F-2A43-4BFF-AFF7-BC15E601D901}" name="Column96"/>
     <tableColumn id="99" xr3:uid="{28288627-7AF0-454A-B8A1-A3BC42ECE940}" name="Column97"/>
@@ -8463,8 +8488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DO41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BS1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CD29" sqref="CD29"/>
+    <sheetView tabSelected="1" topLeftCell="CA1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="CI28" sqref="CI28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8595,7 +8620,7 @@
       <c r="AZ5" s="75"/>
       <c r="BA5" s="76"/>
       <c r="BB5" s="74" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="BC5" s="75"/>
       <c r="BD5" s="75"/>
@@ -8608,7 +8633,7 @@
       <c r="BK5" s="74"/>
       <c r="BL5" s="76"/>
       <c r="BM5" s="74" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="BN5" s="75"/>
       <c r="BO5" s="75"/>
@@ -8618,7 +8643,7 @@
       <c r="BS5" s="76"/>
       <c r="BT5" s="167"/>
       <c r="BU5" s="74" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="BV5" s="75"/>
       <c r="BW5" s="75"/>
@@ -8774,220 +8799,220 @@
         <v>208</v>
       </c>
       <c r="AV6" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="AW6" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="AX6" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="AY6" s="153" t="s">
         <v>223</v>
       </c>
-      <c r="AW6" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="AX6" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="AY6" s="153" t="s">
-        <v>228</v>
-      </c>
       <c r="AZ6" s="2" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="BA6" s="2" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="BB6" s="2" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="BC6" s="2" t="s">
         <v>201</v>
       </c>
       <c r="BD6" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="BE6" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="BF6" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="BG6" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="BH6" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="BI6" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="BJ6" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="BE6" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="BF6" s="2" t="s">
+      <c r="BK6" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="BL6" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="BM6" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="BG6" s="2" t="s">
+      <c r="BN6" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="BH6" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="BI6" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="BJ6" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="BK6" s="2" t="s">
+      <c r="BO6" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="BP6" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="BQ6" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="BR6" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="BL6" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="BM6" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="BN6" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="BO6" s="2" t="s">
+      <c r="BS6" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="BT6" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="BU6" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="BP6" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="BQ6" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="BR6" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="BS6" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="BT6" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="BU6" s="2" t="s">
+      <c r="BV6" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="BW6" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="BX6" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="BV6" s="2" t="s">
+      <c r="BY6" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="BW6" s="2" t="s">
+      <c r="BZ6" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="CA6" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="BX6" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="BY6" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="BZ6" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="CA6" s="2" t="s">
+      <c r="CB6" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="CC6" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="CB6" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="CC6" s="2" t="s">
+      <c r="CD6" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="CE6" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="CF6" s="153" t="s">
         <v>297</v>
       </c>
-      <c r="CD6" s="2" t="s">
+      <c r="CG6" s="153" t="s">
+        <v>298</v>
+      </c>
+      <c r="CH6" s="153" t="s">
         <v>299</v>
       </c>
-      <c r="CE6" s="2" t="s">
+      <c r="CI6" s="153" t="s">
+        <v>300</v>
+      </c>
+      <c r="CJ6" s="153" t="s">
         <v>301</v>
       </c>
-      <c r="CF6" s="2" t="s">
+      <c r="CK6" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="CG6" s="2" t="s">
+      <c r="CL6" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="CH6" s="2" t="s">
+      <c r="CM6" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="CI6" s="2" t="s">
+      <c r="CN6" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="CJ6" s="2" t="s">
+      <c r="CO6" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="CK6" s="2" t="s">
+      <c r="CP6" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="CL6" s="2" t="s">
+      <c r="CQ6" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="CM6" s="2" t="s">
+      <c r="CR6" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="CN6" s="2" t="s">
+      <c r="CS6" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="CO6" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="CP6" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="CQ6" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="CR6" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="CS6" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="CT6" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="CU6" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="CV6" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="CW6" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="CX6" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="CY6" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="CU6" s="2" t="s">
+      <c r="CZ6" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="CV6" s="2" t="s">
+      <c r="DA6" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="CW6" s="2" t="s">
+      <c r="DB6" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="CX6" s="2" t="s">
+      <c r="DC6" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="CY6" s="2" t="s">
+      <c r="DD6" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="CZ6" s="2" t="s">
+      <c r="DE6" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="DA6" s="2" t="s">
+      <c r="DF6" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="DB6" s="2" t="s">
+      <c r="DG6" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="DC6" s="2" t="s">
+      <c r="DH6" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="DD6" s="2" t="s">
+      <c r="DI6" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="DE6" s="2" t="s">
+      <c r="DJ6" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="DF6" s="2" t="s">
+      <c r="DK6" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="DG6" s="2" t="s">
+      <c r="DL6" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="DH6" s="2" t="s">
+      <c r="DM6" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="DI6" s="2" t="s">
+      <c r="DN6" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="DJ6" s="2" t="s">
+      <c r="DO6" s="2" t="s">
         <v>245</v>
-      </c>
-      <c r="DK6" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="DL6" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="DM6" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="DN6" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="DO6" s="2" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:119" s="29" customFormat="1" x14ac:dyDescent="0.25">
@@ -9321,7 +9346,27 @@
       </c>
       <c r="CE7" s="155">
         <f>Table3[[#This Row],[theoretical distance]]-Table3[[#This Row],[flight time]]^2*$CE$25</f>
-        <v>96.811738675851615</v>
+        <v>102.38970759427541</v>
+      </c>
+      <c r="CF7" s="29">
+        <f>Table3[[#This Row],[exit velocity mean]]+$CC$25-Table3[[#This Row],[reduction]]*100</f>
+        <v>75.5</v>
+      </c>
+      <c r="CG7" s="29">
+        <f>MIN(Table3[[#This Row],[adjusted launch angle]]+Table3[[#This Row],[angle stdev]], 30)</f>
+        <v>30</v>
+      </c>
+      <c r="CH7" s="117">
+        <f>2*Table3[[#This Row],[+1stdv EV]]*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*60*60</f>
+        <v>3.3974999999999991</v>
+      </c>
+      <c r="CI7" s="155">
+        <f>Table3[[#This Row],[+1stdv EV]]^2*2*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*5280-Table3[[#This Row],[+1stdv flight time]]^2*$CE$25</f>
+        <v>191.52840000000003</v>
+      </c>
+      <c r="CJ7" s="155">
+        <f>Table3[[#This Row],[+1stdev distance]]-Table3[[#This Row],[actual distance]]</f>
+        <v>89.138692405724626</v>
       </c>
     </row>
     <row r="8" spans="1:119" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -9655,7 +9700,27 @@
       </c>
       <c r="CE8" s="156">
         <f>Table3[[#This Row],[theoretical distance]]-Table3[[#This Row],[flight time]]^2*$CE$25</f>
-        <v>134.27814265470863</v>
+        <v>143.99215129474877</v>
+      </c>
+      <c r="CF8" s="3">
+        <f>Table3[[#This Row],[exit velocity mean]]+$CC$25-Table3[[#This Row],[reduction]]*100</f>
+        <v>83.5</v>
+      </c>
+      <c r="CG8" s="3">
+        <f>MIN(Table3[[#This Row],[adjusted launch angle]]+Table3[[#This Row],[angle stdev]], 30)</f>
+        <v>30</v>
+      </c>
+      <c r="CH8" s="118">
+        <f>2*Table3[[#This Row],[+1stdv EV]]*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*60*60</f>
+        <v>3.7574999999999994</v>
+      </c>
+      <c r="CI8" s="156">
+        <f>Table3[[#This Row],[+1stdv EV]]^2*2*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*5280-Table3[[#This Row],[+1stdv flight time]]^2*$CE$25</f>
+        <v>234.26760000000002</v>
+      </c>
+      <c r="CJ8" s="156">
+        <f>Table3[[#This Row],[+1stdev distance]]-Table3[[#This Row],[actual distance]]</f>
+        <v>90.27544870525125</v>
       </c>
     </row>
     <row r="9" spans="1:119" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -9989,7 +10054,27 @@
       </c>
       <c r="CE9" s="157">
         <f>Table3[[#This Row],[theoretical distance]]-Table3[[#This Row],[flight time]]^2*$CE$25</f>
-        <v>188.82859044658542</v>
+        <v>206.40873696199137</v>
+      </c>
+      <c r="CF9" s="4">
+        <f>Table3[[#This Row],[exit velocity mean]]+$CC$25-Table3[[#This Row],[reduction]]*100</f>
+        <v>93.5</v>
+      </c>
+      <c r="CG9" s="4">
+        <f>MIN(Table3[[#This Row],[adjusted launch angle]]+Table3[[#This Row],[angle stdev]], 30)</f>
+        <v>30</v>
+      </c>
+      <c r="CH9" s="119">
+        <f>2*Table3[[#This Row],[+1stdv EV]]*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*60*60</f>
+        <v>4.2074999999999996</v>
+      </c>
+      <c r="CI9" s="157">
+        <f>Table3[[#This Row],[+1stdv EV]]^2*2*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*5280-Table3[[#This Row],[+1stdv flight time]]^2*$CE$25</f>
+        <v>293.73959999999988</v>
+      </c>
+      <c r="CJ9" s="157">
+        <f>Table3[[#This Row],[+1stdev distance]]-Table3[[#This Row],[actual distance]]</f>
+        <v>87.330863038008516</v>
       </c>
     </row>
     <row r="10" spans="1:119" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -10323,7 +10408,27 @@
       </c>
       <c r="CE10" s="156">
         <f>Table3[[#This Row],[theoretical distance]]-Table3[[#This Row],[flight time]]^2*$CE$25</f>
-        <v>316.97473162066836</v>
+        <v>362.83469988048631</v>
+      </c>
+      <c r="CF10" s="3">
+        <f>Table3[[#This Row],[exit velocity mean]]+$CC$25-Table3[[#This Row],[reduction]]*100</f>
+        <v>113.5</v>
+      </c>
+      <c r="CG10" s="3">
+        <f>MIN(Table3[[#This Row],[adjusted launch angle]]+Table3[[#This Row],[angle stdev]], 30)</f>
+        <v>30</v>
+      </c>
+      <c r="CH10" s="118">
+        <f>2*Table3[[#This Row],[+1stdv EV]]*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*60*60</f>
+        <v>5.1074999999999999</v>
+      </c>
+      <c r="CI10" s="156">
+        <f>Table3[[#This Row],[+1stdv EV]]^2*2*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*5280-Table3[[#This Row],[+1stdv flight time]]^2*$CE$25</f>
+        <v>432.84359999999981</v>
+      </c>
+      <c r="CJ10" s="156">
+        <f>Table3[[#This Row],[+1stdev distance]]-Table3[[#This Row],[actual distance]]</f>
+        <v>70.008900119513498</v>
       </c>
     </row>
     <row r="11" spans="1:119" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -10657,7 +10762,27 @@
       </c>
       <c r="CE11" s="158">
         <f>Table3[[#This Row],[theoretical distance]]-Table3[[#This Row],[flight time]]^2*$CE$25</f>
-        <v>96.811738675851615</v>
+        <v>102.38970759427541</v>
+      </c>
+      <c r="CF11" s="13">
+        <f>Table3[[#This Row],[exit velocity mean]]+$CC$25-Table3[[#This Row],[reduction]]*100</f>
+        <v>79.5</v>
+      </c>
+      <c r="CG11" s="13">
+        <f>MIN(Table3[[#This Row],[adjusted launch angle]]+Table3[[#This Row],[angle stdev]], 30)</f>
+        <v>30</v>
+      </c>
+      <c r="CH11" s="120">
+        <f>2*Table3[[#This Row],[+1stdv EV]]*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*60*60</f>
+        <v>3.5774999999999992</v>
+      </c>
+      <c r="CI11" s="158">
+        <f>Table3[[#This Row],[+1stdv EV]]^2*2*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*5280-Table3[[#This Row],[+1stdv flight time]]^2*$CE$25</f>
+        <v>212.36040000000006</v>
+      </c>
+      <c r="CJ11" s="158">
+        <f>Table3[[#This Row],[+1stdev distance]]-Table3[[#This Row],[actual distance]]</f>
+        <v>109.97069240572465</v>
       </c>
     </row>
     <row r="12" spans="1:119" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -10991,7 +11116,27 @@
       </c>
       <c r="CE12" s="159">
         <f>Table3[[#This Row],[theoretical distance]]-Table3[[#This Row],[flight time]]^2*$CE$25</f>
-        <v>134.27814265470863</v>
+        <v>143.99215129474877</v>
+      </c>
+      <c r="CF12" s="26">
+        <f>Table3[[#This Row],[exit velocity mean]]+$CC$25-Table3[[#This Row],[reduction]]*100</f>
+        <v>87.5</v>
+      </c>
+      <c r="CG12" s="26">
+        <f>MIN(Table3[[#This Row],[adjusted launch angle]]+Table3[[#This Row],[angle stdev]], 30)</f>
+        <v>30</v>
+      </c>
+      <c r="CH12" s="121">
+        <f>2*Table3[[#This Row],[+1stdv EV]]*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*60*60</f>
+        <v>3.9374999999999991</v>
+      </c>
+      <c r="CI12" s="159">
+        <f>Table3[[#This Row],[+1stdv EV]]^2*2*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*5280-Table3[[#This Row],[+1stdv flight time]]^2*$CE$25</f>
+        <v>257.25000000000006</v>
+      </c>
+      <c r="CJ12" s="159">
+        <f>Table3[[#This Row],[+1stdev distance]]-Table3[[#This Row],[actual distance]]</f>
+        <v>113.25784870525129</v>
       </c>
     </row>
     <row r="13" spans="1:119" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -11325,7 +11470,27 @@
       </c>
       <c r="CE13" s="158">
         <f>Table3[[#This Row],[theoretical distance]]-Table3[[#This Row],[flight time]]^2*$CE$25</f>
-        <v>188.82859044658542</v>
+        <v>206.40873696199137</v>
+      </c>
+      <c r="CF13" s="13">
+        <f>Table3[[#This Row],[exit velocity mean]]+$CC$25-Table3[[#This Row],[reduction]]*100</f>
+        <v>97.5</v>
+      </c>
+      <c r="CG13" s="13">
+        <f>MIN(Table3[[#This Row],[adjusted launch angle]]+Table3[[#This Row],[angle stdev]], 30)</f>
+        <v>30</v>
+      </c>
+      <c r="CH13" s="120">
+        <f>2*Table3[[#This Row],[+1stdv EV]]*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*60*60</f>
+        <v>4.3874999999999993</v>
+      </c>
+      <c r="CI13" s="158">
+        <f>Table3[[#This Row],[+1stdv EV]]^2*2*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*5280-Table3[[#This Row],[+1stdv flight time]]^2*$CE$25</f>
+        <v>319.41000000000003</v>
+      </c>
+      <c r="CJ13" s="158">
+        <f>Table3[[#This Row],[+1stdev distance]]-Table3[[#This Row],[actual distance]]</f>
+        <v>113.00126303800866</v>
       </c>
     </row>
     <row r="14" spans="1:119" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -11659,7 +11824,27 @@
       </c>
       <c r="CE14" s="160">
         <f>Table3[[#This Row],[theoretical distance]]-Table3[[#This Row],[flight time]]^2*$CE$25</f>
-        <v>316.97473162066836</v>
+        <v>362.83469988048631</v>
+      </c>
+      <c r="CF14" s="5">
+        <f>Table3[[#This Row],[exit velocity mean]]+$CC$25-Table3[[#This Row],[reduction]]*100</f>
+        <v>117.5</v>
+      </c>
+      <c r="CG14" s="5">
+        <f>MIN(Table3[[#This Row],[adjusted launch angle]]+Table3[[#This Row],[angle stdev]], 30)</f>
+        <v>30</v>
+      </c>
+      <c r="CH14" s="122">
+        <f>2*Table3[[#This Row],[+1stdv EV]]*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*60*60</f>
+        <v>5.2874999999999988</v>
+      </c>
+      <c r="CI14" s="160">
+        <f>Table3[[#This Row],[+1stdv EV]]^2*2*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*5280-Table3[[#This Row],[+1stdv flight time]]^2*$CE$25</f>
+        <v>463.8900000000001</v>
+      </c>
+      <c r="CJ14" s="160">
+        <f>Table3[[#This Row],[+1stdev distance]]-Table3[[#This Row],[actual distance]]</f>
+        <v>101.05530011951379</v>
       </c>
     </row>
     <row r="15" spans="1:119" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -11993,7 +12178,27 @@
       </c>
       <c r="CE15" s="161">
         <f>Table3[[#This Row],[theoretical distance]]-Table3[[#This Row],[flight time]]^2*$CE$25</f>
-        <v>96.811738675851615</v>
+        <v>102.38970759427541</v>
+      </c>
+      <c r="CF15" s="17">
+        <f>Table3[[#This Row],[exit velocity mean]]+$CC$25-Table3[[#This Row],[reduction]]*100</f>
+        <v>84.5</v>
+      </c>
+      <c r="CG15" s="17">
+        <f>MIN(Table3[[#This Row],[adjusted launch angle]]+Table3[[#This Row],[angle stdev]], 30)</f>
+        <v>30</v>
+      </c>
+      <c r="CH15" s="123">
+        <f>2*Table3[[#This Row],[+1stdv EV]]*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*60*60</f>
+        <v>3.8024999999999993</v>
+      </c>
+      <c r="CI15" s="161">
+        <f>Table3[[#This Row],[+1stdv EV]]^2*2*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*5280-Table3[[#This Row],[+1stdv flight time]]^2*$CE$25</f>
+        <v>239.91240000000005</v>
+      </c>
+      <c r="CJ15" s="161">
+        <f>Table3[[#This Row],[+1stdev distance]]-Table3[[#This Row],[actual distance]]</f>
+        <v>137.52269240572463</v>
       </c>
     </row>
     <row r="16" spans="1:119" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -12327,10 +12532,30 @@
       </c>
       <c r="CE16" s="162">
         <f>Table3[[#This Row],[theoretical distance]]-Table3[[#This Row],[flight time]]^2*$CE$25</f>
-        <v>134.27814265470863</v>
+        <v>143.99215129474877</v>
+      </c>
+      <c r="CF16" s="6">
+        <f>Table3[[#This Row],[exit velocity mean]]+$CC$25-Table3[[#This Row],[reduction]]*100</f>
+        <v>92.5</v>
+      </c>
+      <c r="CG16" s="6">
+        <f>MIN(Table3[[#This Row],[adjusted launch angle]]+Table3[[#This Row],[angle stdev]], 30)</f>
+        <v>30</v>
+      </c>
+      <c r="CH16" s="124">
+        <f>2*Table3[[#This Row],[+1stdv EV]]*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*60*60</f>
+        <v>4.1624999999999988</v>
+      </c>
+      <c r="CI16" s="162">
+        <f>Table3[[#This Row],[+1stdv EV]]^2*2*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*5280-Table3[[#This Row],[+1stdv flight time]]^2*$CE$25</f>
+        <v>287.49</v>
+      </c>
+      <c r="CJ16" s="162">
+        <f>Table3[[#This Row],[+1stdev distance]]-Table3[[#This Row],[actual distance]]</f>
+        <v>143.49784870525124</v>
       </c>
     </row>
-    <row r="17" spans="1:83" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:88" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -12661,10 +12886,30 @@
       </c>
       <c r="CE17" s="163">
         <f>Table3[[#This Row],[theoretical distance]]-Table3[[#This Row],[flight time]]^2*$CE$25</f>
-        <v>188.82859044658542</v>
+        <v>206.40873696199137</v>
+      </c>
+      <c r="CF17" s="23">
+        <f>Table3[[#This Row],[exit velocity mean]]+$CC$25-Table3[[#This Row],[reduction]]*100</f>
+        <v>102.5</v>
+      </c>
+      <c r="CG17" s="23">
+        <f>MIN(Table3[[#This Row],[adjusted launch angle]]+Table3[[#This Row],[angle stdev]], 30)</f>
+        <v>30</v>
+      </c>
+      <c r="CH17" s="125">
+        <f>2*Table3[[#This Row],[+1stdv EV]]*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*60*60</f>
+        <v>4.6124999999999989</v>
+      </c>
+      <c r="CI17" s="163">
+        <f>Table3[[#This Row],[+1stdv EV]]^2*2*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*5280-Table3[[#This Row],[+1stdv flight time]]^2*$CE$25</f>
+        <v>353.01000000000005</v>
+      </c>
+      <c r="CJ17" s="163">
+        <f>Table3[[#This Row],[+1stdev distance]]-Table3[[#This Row],[actual distance]]</f>
+        <v>146.60126303800868</v>
       </c>
     </row>
-    <row r="18" spans="1:83" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:88" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -12995,10 +13240,30 @@
       </c>
       <c r="CE18" s="162">
         <f>Table3[[#This Row],[theoretical distance]]-Table3[[#This Row],[flight time]]^2*$CE$25</f>
-        <v>316.97473162066836</v>
+        <v>362.83469988048631</v>
+      </c>
+      <c r="CF18" s="6">
+        <f>Table3[[#This Row],[exit velocity mean]]+$CC$25-Table3[[#This Row],[reduction]]*100</f>
+        <v>122.5</v>
+      </c>
+      <c r="CG18" s="6">
+        <f>MIN(Table3[[#This Row],[adjusted launch angle]]+Table3[[#This Row],[angle stdev]], 30)</f>
+        <v>30</v>
+      </c>
+      <c r="CH18" s="124">
+        <f>2*Table3[[#This Row],[+1stdv EV]]*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*60*60</f>
+        <v>5.5124999999999993</v>
+      </c>
+      <c r="CI18" s="162">
+        <f>Table3[[#This Row],[+1stdv EV]]^2*2*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*5280-Table3[[#This Row],[+1stdv flight time]]^2*$CE$25</f>
+        <v>504.21000000000004</v>
+      </c>
+      <c r="CJ18" s="162">
+        <f>Table3[[#This Row],[+1stdev distance]]-Table3[[#This Row],[actual distance]]</f>
+        <v>141.37530011951372</v>
       </c>
     </row>
-    <row r="19" spans="1:83" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:88" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -13329,10 +13594,30 @@
       </c>
       <c r="CE19" s="164">
         <f>Table3[[#This Row],[theoretical distance]]-Table3[[#This Row],[flight time]]^2*$CE$25</f>
-        <v>96.811738675851615</v>
+        <v>102.38970759427541</v>
+      </c>
+      <c r="CF19" s="15">
+        <f>Table3[[#This Row],[exit velocity mean]]+$CC$25-Table3[[#This Row],[reduction]]*100</f>
+        <v>84.5</v>
+      </c>
+      <c r="CG19" s="15">
+        <f>MIN(Table3[[#This Row],[adjusted launch angle]]+Table3[[#This Row],[angle stdev]], 30)</f>
+        <v>30</v>
+      </c>
+      <c r="CH19" s="126">
+        <f>2*Table3[[#This Row],[+1stdv EV]]*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*60*60</f>
+        <v>3.8024999999999993</v>
+      </c>
+      <c r="CI19" s="164">
+        <f>Table3[[#This Row],[+1stdv EV]]^2*2*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*5280-Table3[[#This Row],[+1stdv flight time]]^2*$CE$25</f>
+        <v>239.91240000000005</v>
+      </c>
+      <c r="CJ19" s="164">
+        <f>Table3[[#This Row],[+1stdev distance]]-Table3[[#This Row],[actual distance]]</f>
+        <v>137.52269240572463</v>
       </c>
     </row>
-    <row r="20" spans="1:83" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:88" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -13663,10 +13948,30 @@
       </c>
       <c r="CE20" s="165">
         <f>Table3[[#This Row],[theoretical distance]]-Table3[[#This Row],[flight time]]^2*$CE$25</f>
-        <v>134.27814265470863</v>
+        <v>143.99215129474877</v>
+      </c>
+      <c r="CF20" s="11">
+        <f>Table3[[#This Row],[exit velocity mean]]+$CC$25-Table3[[#This Row],[reduction]]*100</f>
+        <v>92.5</v>
+      </c>
+      <c r="CG20" s="11">
+        <f>MIN(Table3[[#This Row],[adjusted launch angle]]+Table3[[#This Row],[angle stdev]], 30)</f>
+        <v>30</v>
+      </c>
+      <c r="CH20" s="127">
+        <f>2*Table3[[#This Row],[+1stdv EV]]*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*60*60</f>
+        <v>4.1624999999999988</v>
+      </c>
+      <c r="CI20" s="165">
+        <f>Table3[[#This Row],[+1stdv EV]]^2*2*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*5280-Table3[[#This Row],[+1stdv flight time]]^2*$CE$25</f>
+        <v>287.49</v>
+      </c>
+      <c r="CJ20" s="165">
+        <f>Table3[[#This Row],[+1stdev distance]]-Table3[[#This Row],[actual distance]]</f>
+        <v>143.49784870525124</v>
       </c>
     </row>
-    <row r="21" spans="1:83" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:88" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -13997,10 +14302,30 @@
       </c>
       <c r="CE21" s="164">
         <f>Table3[[#This Row],[theoretical distance]]-Table3[[#This Row],[flight time]]^2*$CE$25</f>
-        <v>188.82859044658542</v>
+        <v>206.40873696199137</v>
+      </c>
+      <c r="CF21" s="15">
+        <f>Table3[[#This Row],[exit velocity mean]]+$CC$25-Table3[[#This Row],[reduction]]*100</f>
+        <v>102.5</v>
+      </c>
+      <c r="CG21" s="15">
+        <f>MIN(Table3[[#This Row],[adjusted launch angle]]+Table3[[#This Row],[angle stdev]], 30)</f>
+        <v>30</v>
+      </c>
+      <c r="CH21" s="126">
+        <f>2*Table3[[#This Row],[+1stdv EV]]*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*60*60</f>
+        <v>4.6124999999999989</v>
+      </c>
+      <c r="CI21" s="164">
+        <f>Table3[[#This Row],[+1stdv EV]]^2*2*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*5280-Table3[[#This Row],[+1stdv flight time]]^2*$CE$25</f>
+        <v>353.01000000000005</v>
+      </c>
+      <c r="CJ21" s="164">
+        <f>Table3[[#This Row],[+1stdev distance]]-Table3[[#This Row],[actual distance]]</f>
+        <v>146.60126303800868</v>
       </c>
     </row>
-    <row r="22" spans="1:83" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:88" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -14331,15 +14656,35 @@
       </c>
       <c r="CE22" s="166">
         <f>Table3[[#This Row],[theoretical distance]]-Table3[[#This Row],[flight time]]^2*$CE$25</f>
-        <v>316.97473162066836</v>
+        <v>362.83469988048631</v>
+      </c>
+      <c r="CF22" s="20">
+        <f>Table3[[#This Row],[exit velocity mean]]+$CC$25-Table3[[#This Row],[reduction]]*100</f>
+        <v>122.5</v>
+      </c>
+      <c r="CG22" s="20">
+        <f>MIN(Table3[[#This Row],[adjusted launch angle]]+Table3[[#This Row],[angle stdev]], 30)</f>
+        <v>30</v>
+      </c>
+      <c r="CH22" s="128">
+        <f>2*Table3[[#This Row],[+1stdv EV]]*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*60*60</f>
+        <v>5.5124999999999993</v>
+      </c>
+      <c r="CI22" s="166">
+        <f>Table3[[#This Row],[+1stdv EV]]^2*2*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*5280-Table3[[#This Row],[+1stdv flight time]]^2*$CE$25</f>
+        <v>504.21000000000004</v>
+      </c>
+      <c r="CJ22" s="166">
+        <f>Table3[[#This Row],[+1stdev distance]]-Table3[[#This Row],[actual distance]]</f>
+        <v>141.37530011951372</v>
       </c>
     </row>
-    <row r="23" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:88" x14ac:dyDescent="0.25">
       <c r="AW23" s="154"/>
       <c r="BK23" s="73"/>
       <c r="BL23" s="73"/>
     </row>
-    <row r="24" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:88" x14ac:dyDescent="0.25">
       <c r="Y24" s="63" t="s">
         <v>141</v>
       </c>
@@ -14367,37 +14712,37 @@
         <v>204</v>
       </c>
       <c r="AX24" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="BA24" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="BB24" t="s">
         <v>199</v>
       </c>
       <c r="BP24" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="BV24" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="BW24" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="BZ24" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="CA24" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="CC24" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="CE24" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
     </row>
-    <row r="25" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:88" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
         <v>89</v>
       </c>
@@ -14492,10 +14837,10 @@
         <v>12.5</v>
       </c>
       <c r="CE25">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:88" x14ac:dyDescent="0.25">
       <c r="D26">
         <v>0.1</v>
       </c>
@@ -14564,16 +14909,16 @@
         <v>205</v>
       </c>
       <c r="AX26" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="BP26" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="CA26" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
     </row>
-    <row r="27" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:88" x14ac:dyDescent="0.25">
       <c r="K27" t="s">
         <v>91</v>
       </c>
@@ -14628,29 +14973,29 @@
         <v>-2</v>
       </c>
       <c r="BU27" t="s">
+        <v>276</v>
+      </c>
+      <c r="BV27" t="s">
+        <v>246</v>
+      </c>
+      <c r="BW27" t="s">
         <v>281</v>
       </c>
-      <c r="BV27" t="s">
-        <v>251</v>
-      </c>
-      <c r="BW27" t="s">
-        <v>286</v>
-      </c>
       <c r="BZ27" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="CA27">
         <v>110</v>
       </c>
       <c r="CC27" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="CE27">
         <f>CE10/CE9</f>
-        <v>1.6786373868015081</v>
+        <v>1.7578456475284747</v>
       </c>
     </row>
-    <row r="28" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:88" x14ac:dyDescent="0.25">
       <c r="K28">
         <v>0.9</v>
       </c>
@@ -14685,7 +15030,7 @@
         <v>189</v>
       </c>
       <c r="AU28" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="BB28" t="s">
         <v>136</v>
@@ -14707,7 +15052,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="29" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:88" x14ac:dyDescent="0.25">
       <c r="W29" t="s">
         <v>130</v>
       </c>
@@ -14743,16 +15088,16 @@
         <v>5</v>
       </c>
       <c r="AX29" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="BB29">
         <v>1</v>
       </c>
       <c r="BP29" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
-    <row r="30" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:88" x14ac:dyDescent="0.25">
       <c r="W30">
         <f xml:space="preserve"> W28/2 - W26/3</f>
         <v>-1</v>
@@ -14787,7 +15132,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:88" x14ac:dyDescent="0.25">
       <c r="W31" t="s">
         <v>133</v>
       </c>
@@ -14820,7 +15165,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="32" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:88" x14ac:dyDescent="0.25">
       <c r="W32">
         <f>MAX(0, ((W26+X26)/(3+X26))-(W28/2))</f>
         <v>1</v>
@@ -14970,7 +15315,7 @@
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
   <conditionalFormatting sqref="O7:O22">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added swing decisions, extra support to help pitch, some other misc. cleanup that was missed in previous commits.
</commit_message>
<xml_diff>
--- a/plans/baseball stats.xlsx
+++ b/plans/baseball stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcgiffenk\Desktop\newpy\xtreemblaseball99\plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304D5927-64A9-4B4E-9984-8600057850EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{709F8AF3-4DB8-4CBE-B657-C56076EF0FBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,6 @@
     <definedName name="zeros">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1456,7 +1455,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="174" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -2043,18 +2042,18 @@
     <xf numFmtId="9" fontId="0" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="7" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="174" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="174" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="174" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="174" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="174" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="174" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="174" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="174" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="174" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="174" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="174" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="174" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -2104,26 +2103,16 @@
   </cellStyles>
   <dxfs count="82">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="174" formatCode="0.000"/>
+      <numFmt numFmtId="165" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -2132,7 +2121,7 @@
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="174" formatCode="0.000"/>
+      <numFmt numFmtId="165" formatCode="0.000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -2153,10 +2142,10 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -2177,7 +2166,7 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -2186,19 +2175,10 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="165" formatCode="0.000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="174" formatCode="0.000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -2231,7 +2211,13 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -2451,7 +2437,20 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -7920,181 +7919,181 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A6:DO22" totalsRowShown="0" headerRowDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A6:DO22" totalsRowShown="0" headerRowDxfId="80">
   <autoFilter ref="A6:DO22" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="119">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Rep #">
       <calculatedColumnFormula>ROW()-ROW(home)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="offense" dataDxfId="80">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="offense" dataDxfId="79">
       <calculatedColumnFormula>INDEX(oratings, 1, 1+MOD(Table3[[#This Row],[Rep '#]]-1, COUNT(oratings)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="defense" dataDxfId="79">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="defense" dataDxfId="78">
       <calculatedColumnFormula>INDEX(dratings, 1, MOD(FLOOR( (Table3[[#This Row],[Rep '#]]-1) / COUNT(oratings), 1), COUNT(dratings))+1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="base leadoff" dataDxfId="78">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="base leadoff" dataDxfId="77">
       <calculatedColumnFormula>Table3[[#This Row],[offense]]*$D$26+0.05</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="leadoff modifier" dataDxfId="40">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="leadoff modifier" dataDxfId="76">
       <calculatedColumnFormula>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*$E$26</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="total leadoff (ft)" dataDxfId="77">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="total leadoff (ft)" dataDxfId="75">
       <calculatedColumnFormula>MAX(Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90, 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="pickoff manuver (s)" dataDxfId="76">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="pickoff manuver (s)" dataDxfId="74">
       <calculatedColumnFormula>1.1 - Table3[[#This Row],[defense]]*0.1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="throw speed (s/ft)" dataDxfId="75">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="throw speed (s/ft)" dataDxfId="73">
       <calculatedColumnFormula xml:space="preserve"> 0.01 - 0.0025 *  Table3[[#This Row],[defense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="throw speed (mph)" dataDxfId="74">
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="throw speed (mph)" dataDxfId="72">
       <calculatedColumnFormula>1 / Table3[[#This Row],[throw speed (s/ft)]] * ((60 * 60)/5280)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="pickoff time" dataDxfId="73">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="pickoff time" dataDxfId="71">
       <calculatedColumnFormula>Table3[[#This Row],[pickoff manuver (s)]]+60*Table3[[#This Row],[throw speed (s/ft)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="runner reaction" dataDxfId="72">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="runner reaction" dataDxfId="70">
       <calculatedColumnFormula>$K$28-$K$26*Table3[[#This Row],[offense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="runner speed (s/ft)" dataDxfId="71">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="runner speed (s/ft)" dataDxfId="69">
       <calculatedColumnFormula>0.05 - Table3[[#This Row],[offense]]*$L$26</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="runner speed (mph)" dataDxfId="70">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="runner speed (mph)" dataDxfId="68">
       <calculatedColumnFormula>1 / Table3[[#This Row],[runner speed (s/ft)]] * ((60 * 60)/5280)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="pickoff evade time" dataDxfId="69">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="pickoff evade time" dataDxfId="67">
       <calculatedColumnFormula>Table3[[#This Row],[runner reaction]]+Table3[[#This Row],[runner speed (s/ft)]]*Table3[[#This Row],[total leadoff (ft)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="pickoff probability" dataDxfId="68" dataCellStyle="Percent">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="pickoff probability" dataDxfId="66" dataCellStyle="Percent">
       <calculatedColumnFormula>1 - _xlfn.NORM.DIST(Table3[[#This Row],[pickoff time]], Table3[[#This Row],[pickoff evade time]], $O$4, TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Fielding Odds" dataDxfId="67" dataCellStyle="Percent">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Fielding Odds" dataDxfId="65" dataCellStyle="Percent">
       <calculatedColumnFormula>_xlfn.NORM.DIST(Table3[[#This Row],[defense]], $P$26, $P$27, TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="pickoff worth it?" dataDxfId="66">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="pickoff worth it?" dataDxfId="64">
       <calculatedColumnFormula>Table3[[#This Row],[pickoff probability]] &gt; 1-Table3[[#This Row],[Fielding Odds]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Error %" dataDxfId="65" dataCellStyle="Percent">
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Error %" dataDxfId="63" dataCellStyle="Percent">
       <calculatedColumnFormula>1-Table3[[#This Row],[Fielding Odds]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Blatant steal time" dataDxfId="64">
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Blatant steal time" dataDxfId="62">
       <calculatedColumnFormula>(90-Table3[[#This Row],[total leadoff (ft)]])*Table3[[#This Row],[runner speed (s/ft)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Response speed" dataDxfId="63">
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Response speed" dataDxfId="61">
       <calculatedColumnFormula>$T$26*(2-Table3[[#This Row],[defense]]) + Table3[[#This Row],[pickoff time]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="blatant steal probability" dataDxfId="62" dataCellStyle="Percent">
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="blatant steal probability" dataDxfId="60" dataCellStyle="Percent">
       <calculatedColumnFormula>_xlfn.NORM.DIST(Table3[[#This Row],[Response speed]], Table3[[#This Row],[Blatant steal time]], $U$4, TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="defense fear" dataDxfId="61">
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="defense fear" dataDxfId="59">
       <calculatedColumnFormula>Table3[[#This Row],[defense]]+Table3[[#This Row],[defense]]*Table3[[#This Row],[offense]]*$E$26</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="ball factor" dataDxfId="60">
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="ball factor" dataDxfId="58">
       <calculatedColumnFormula>(1-$W$32)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="desperation" dataDxfId="59" dataCellStyle="Percent">
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="desperation" dataDxfId="57" dataCellStyle="Percent">
       <calculatedColumnFormula>Table3[[#This Row],[ball factor]]/$X$32*(1-$X$34)+$X$34</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="player control" dataDxfId="58">
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="player control" dataDxfId="56">
       <calculatedColumnFormula>Table3[[#This Row],[offense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="ideal steer" dataDxfId="57">
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="ideal steer" dataDxfId="55">
       <calculatedColumnFormula>$AA$33</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="scaled control" dataDxfId="56">
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="scaled control" dataDxfId="54">
       <calculatedColumnFormula>IF(Table3[[#This Row],[player control]]&gt;1,Table3[[#This Row],[player control]]*$AA$41+$AA$40,Table3[[#This Row],[player control]]*$AA$39+$AA$38)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="unmod foul percent 3rd" dataDxfId="55" dataCellStyle="Percent">
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="unmod foul percent 3rd" dataDxfId="53" dataCellStyle="Percent">
       <calculatedColumnFormula>_xlfn.NORM.DIST(-1,Table3[[#This Row],[ideal steer]],($AB$25-Table3[[#This Row],[scaled control]])*$AB$27,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="unmod foul percent 1st" dataDxfId="54" dataCellStyle="Percent">
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="unmod foul percent 1st" dataDxfId="52" dataCellStyle="Percent">
       <calculatedColumnFormula>1-_xlfn.NORM.DIST(1,Table3[[#This Row],[ideal steer]],($AB$25-Table3[[#This Row],[scaled control]])*$AB$27,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="total unmod foul percent" dataDxfId="53" dataCellStyle="Percent">
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="total unmod foul percent" dataDxfId="51" dataCellStyle="Percent">
       <calculatedColumnFormula>1-(1-Table3[[#This Row],[unmod foul percent 3rd]])*(1-Table3[[#This Row],[unmod foul percent 1st]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="unmod dead center foul%" dataDxfId="52" dataCellStyle="Percent">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="unmod dead center foul%" dataDxfId="50" dataCellStyle="Percent">
       <calculatedColumnFormula>1-((1-_xlfn.NORM.DIST(-1,0,($AB$25-Table3[[#This Row],[scaled control]])*$AB$27,TRUE))*_xlfn.NORM.DIST(1,0,($AB$25-Table3[[#This Row],[scaled control]])*$AB$27,TRUE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="count" dataDxfId="51">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="count" dataDxfId="49">
       <calculatedColumnFormula>$AF$34*$AF$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="hitter discipline bias" dataDxfId="50">
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="hitter discipline bias" dataDxfId="48">
       <calculatedColumnFormula>$AG$25*($AG$34*Table3[[#This Row],[offense]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="bases loaded" dataDxfId="49">
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="bases loaded" dataDxfId="47">
       <calculatedColumnFormula>$AH$25*$AH$34</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="number of outs" dataDxfId="48">
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="number of outs" dataDxfId="46">
       <calculatedColumnFormula>$AI$34*$AI$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="current hitter vs next hitter" dataDxfId="47">
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="current hitter vs next hitter" dataDxfId="45">
       <calculatedColumnFormula>$AJ$25*(Table3[[#This Row],[offense]]-$AJ$27)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="calling modifier" dataDxfId="46">
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="calling modifier" dataDxfId="44">
       <calculatedColumnFormula array="1">SUM(Table3[[#This Row],[count]:[current hitter vs next hitter]]*MIN(1, Table3[[#This Row],[defense]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="sigmoid strike percent" dataDxfId="45" dataCellStyle="Percent">
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="sigmoid strike percent" dataDxfId="43" dataCellStyle="Percent">
       <calculatedColumnFormula>$AL$25-(Table3[[#This Row],[calling modifier]]/(ABS(Table3[[#This Row],[calling modifier]])+$AL$29)*$AL$27)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="tanh strike percent" dataDxfId="44" dataCellStyle="Percent">
+    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="tanh strike percent" dataDxfId="42" dataCellStyle="Percent">
       <calculatedColumnFormula>$AL$25-$AL$27*TANH(Table3[[#This Row],[calling modifier]]/$AM$29)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="called position" dataDxfId="43" dataCellStyle="Percent">
+    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="called position" dataDxfId="41" dataCellStyle="Percent">
       <calculatedColumnFormula>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-Table3[[#This Row],[defense]])))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="called pos 0.2 pitch" dataDxfId="42">
+    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="called pos 0.2 pitch" dataDxfId="40">
       <calculatedColumnFormula>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-0.2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="called pos 2 pitch" dataDxfId="41">
+    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="called pos 2 pitch" dataDxfId="39">
       <calculatedColumnFormula>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-2)))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="location -1  stdv" dataDxfId="38">
       <calculatedColumnFormula>Table3[[#This Row],[called position]]-pitchmod*(pitchstdv-Table3[[#This Row],[defense]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="location +1 stdv" dataDxfId="39">
+    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="location +1 stdv" dataDxfId="37">
       <calculatedColumnFormula>ABS(Table3[[#This Row],[called position]]+pitchmod*(pitchstdv-Table3[[#This Row],[defense]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="min dist to sz 1stdv" dataDxfId="37">
+    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="min dist to sz 1stdv" dataDxfId="36">
       <calculatedColumnFormula>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;1, Table3[[#This Row],[location +1 stdv]]&gt;1),0, MIN(Table3[[#This Row],[location -1  stdv]]+1, 1-Table3[[#This Row],[location +1 stdv]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="max dist to sz 1stdv" dataDxfId="36">
+    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="max dist to sz 1stdv" dataDxfId="35">
       <calculatedColumnFormula>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;0, Table3[[#This Row],[location +1 stdv]]&gt;0),1, MAX(1-ABS(Table3[[#This Row],[location -1  stdv]]), Table3[[#This Row],[location +1 stdv]]-1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="ave obscurity" dataDxfId="35">
+    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="ave obscurity" dataDxfId="34">
       <calculatedColumnFormula>$AU$30/(ABS(Table3[[#This Row],[called position]]-1)+$AU$27)+$AU$32*Table3[[#This Row],[defense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="obscurity at _x000a_0.5" dataDxfId="34">
+    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="obscurity at _x000a_0.5" dataDxfId="33">
       <calculatedColumnFormula>$AU$30/(ABS(0.5-1)+$AU$27)+$AU$32*Table3[[#This Row],[defense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="obscurity at  0.9" dataDxfId="33">
+    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="obscurity at  0.9" dataDxfId="32">
       <calculatedColumnFormula>$AU$30/(ABS(0.9-1)+$AU$27)+$AU$32*Table3[[#This Row],[defense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="average difficulty" dataDxfId="23">
+    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="average difficulty" dataDxfId="31">
       <calculatedColumnFormula>Table3[[#This Row],[defense]]*$AX$30+MAX(0, Table3[[#This Row],[called position]]-$AX$27)^$AX$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" name="+1stdv difficulty" dataDxfId="22">
+    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" name="+1stdv difficulty" dataDxfId="30">
       <calculatedColumnFormula>Table3[[#This Row],[defense]]*$AX$30 + MAX(0, Table3[[#This Row],[location +1 stdv]]-$AX$27)^$AX$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0000-000037000000}" name="difficulty at 1" dataDxfId="21">
+    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0000-000037000000}" name="difficulty at 1" dataDxfId="29">
       <calculatedColumnFormula>Table3[[#This Row],[defense]]*$AX$30+MAX(0, 1-$AX$27)^$AX$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="62" xr3:uid="{6513900D-2CAC-4022-A6B3-8A00EE6C566B}" name="reduction" dataDxfId="32">
+    <tableColumn id="62" xr3:uid="{6513900D-2CAC-4022-A6B3-8A00EE6C566B}" name="reduction" dataDxfId="28">
       <calculatedColumnFormula>MAX(0, 0.1*(1-Table3[[#This Row],[defense]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="63" xr3:uid="{12464915-1D8C-4EB5-9BBD-0FF526658E5B}" name="Location" dataDxfId="31">
+    <tableColumn id="63" xr3:uid="{12464915-1D8C-4EB5-9BBD-0FF526658E5B}" name="Location" dataDxfId="27">
       <calculatedColumnFormula>$BB$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="64" xr3:uid="{5F0F19BE-6D04-4E9E-81B2-B324AB353F5C}" name="obscurity" dataDxfId="30">
+    <tableColumn id="64" xr3:uid="{5F0F19BE-6D04-4E9E-81B2-B324AB353F5C}" name="obscurity" dataDxfId="26">
       <calculatedColumnFormula>$AU$30/(ABS(Table3[[#This Row],[Location]]-1)+$AU$27)+$AU$32*Table3[[#This Row],[defense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="65" xr3:uid="{EA3D32E7-A2E2-482C-B6E9-2E17651C5F77}" name="Strike?" dataDxfId="27">
+    <tableColumn id="65" xr3:uid="{EA3D32E7-A2E2-482C-B6E9-2E17651C5F77}" name="Strike?" dataDxfId="25">
       <calculatedColumnFormula>Table3[[#This Row],[Location]]&lt;= (1+MAX(0, (Table3[[#This Row],[defense]]-1)*0.1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="66" xr3:uid="{0C7E9B06-240B-481E-B495-54026E2F00AA}" name="discipline modifier" dataDxfId="29">
+    <tableColumn id="66" xr3:uid="{0C7E9B06-240B-481E-B495-54026E2F00AA}" name="discipline modifier" dataDxfId="24">
       <calculatedColumnFormula>1/(1+Table3[[#This Row],[offense]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="67" xr3:uid="{D3B0837D-02D4-4F62-A2E2-876739E497B0}" name="effective obscurity" dataDxfId="28">
+    <tableColumn id="67" xr3:uid="{D3B0837D-02D4-4F62-A2E2-876739E497B0}" name="effective obscurity" dataDxfId="23">
       <calculatedColumnFormula>Table3[[#This Row],[obscurity]]*Table3[[#This Row],[discipline modifier]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="69" xr3:uid="{39822A5F-1791-48DC-BA9F-A066931C0292}" name="odds of read" dataCellStyle="Percent">
@@ -8109,31 +8108,31 @@
     <tableColumn id="72" xr3:uid="{3E21C76F-F55B-4E49-9BE2-FEE046008C15}" name="adjusted swing %" dataCellStyle="Percent">
       <calculatedColumnFormula>Table3[[#This Row],[desperation echo]]*Table3[[#This Row],[unadjusted swing %]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="130" xr3:uid="{827C9303-3867-43F7-A79B-BC2EAB3F896D}" name="pitch carry forward obsc" dataDxfId="25">
+    <tableColumn id="130" xr3:uid="{827C9303-3867-43F7-A79B-BC2EAB3F896D}" name="pitch carry forward obsc" dataDxfId="22">
       <calculatedColumnFormula>Table3[[#This Row],[ave obscurity]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="131" xr3:uid="{F26B1E2C-89D5-4F6D-877A-1BEA7F7DF5A9}" name="CF odds of read" dataCellStyle="Percent">
       <calculatedColumnFormula>1/(1+Table3[[#This Row],[ave obscurity]]*Table3[[#This Row],[discipline modifier]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="73" xr3:uid="{77BBE784-030D-4E46-9A29-8783B89762BC}" name="contact echo" dataDxfId="26">
+    <tableColumn id="73" xr3:uid="{77BBE784-030D-4E46-9A29-8783B89762BC}" name="contact echo" dataDxfId="21">
       <calculatedColumnFormula>Table3[[#This Row],[offense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="75" xr3:uid="{074A9F48-3941-4E36-90C2-7710217D32C8}" name="pitch carry forward diff" dataDxfId="24">
+    <tableColumn id="75" xr3:uid="{074A9F48-3941-4E36-90C2-7710217D32C8}" name="pitch carry forward diff" dataDxfId="20">
       <calculatedColumnFormula>Table3[[#This Row],[average difficulty]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="76" xr3:uid="{628DDA60-D380-4EE8-AA7D-7EF6C4AAD8A5}" name="CF contact readiness" dataDxfId="20">
+    <tableColumn id="76" xr3:uid="{628DDA60-D380-4EE8-AA7D-7EF6C4AAD8A5}" name="CF contact readiness" dataDxfId="19">
       <calculatedColumnFormula>Table3[[#This Row],[contact echo]]-Table3[[#This Row],[pitch carry forward diff]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="77" xr3:uid="{DBF18AD6-8593-42C7-9058-D19737088E6D}" name="foul %" dataDxfId="18" dataCellStyle="Percent">
       <calculatedColumnFormula>1-_xlfn.NORM.DIST($BP$27,Table3[[#This Row],[CF contact readiness]], $BP$30,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="78" xr3:uid="{6354951A-151E-4E04-9897-9CB39D6098C8}" name="clean %" dataDxfId="19" dataCellStyle="Percent">
+    <tableColumn id="78" xr3:uid="{6354951A-151E-4E04-9897-9CB39D6098C8}" name="clean %" dataDxfId="17" dataCellStyle="Percent">
       <calculatedColumnFormula>1-_xlfn.NORM.DIST($BP$25,Table3[[#This Row],[CF contact readiness]], $BP$30,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="79" xr3:uid="{0070F673-D13C-467D-95AC-FF8413A02F3F}" name="strike swinging %" dataDxfId="17" dataCellStyle="Percent">
+    <tableColumn id="79" xr3:uid="{0070F673-D13C-467D-95AC-FF8413A02F3F}" name="strike swinging %" dataDxfId="16" dataCellStyle="Percent">
       <calculatedColumnFormula>1-Table3[[#This Row],[foul %]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="80" xr3:uid="{9504D0CF-7CD0-472F-8289-44B30538D80C}" name="ave. hit quality" dataDxfId="16">
+    <tableColumn id="80" xr3:uid="{9504D0CF-7CD0-472F-8289-44B30538D80C}" name="ave. hit quality" dataDxfId="15">
       <calculatedColumnFormula>(Table3[[#This Row],[CF contact readiness]]-$BP$27)/$BP$30</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="132" xr3:uid="{0BB169E4-F345-4B7D-A549-DE28DC5FB113}" name="hit quality +1stdv" dataDxfId="14">
@@ -8145,7 +8144,7 @@
     <tableColumn id="82" xr3:uid="{CBA11BEE-0412-44C3-979C-1888629B3C7A}" name="adjusted launch angle" dataDxfId="12">
       <calculatedColumnFormula>$BV$25+Table3[[#This Row],[offense]]*$BV$28</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="83" xr3:uid="{8DC0E209-2987-40FE-9521-B3339A7D8E1F}" name="angle stdev" dataDxfId="15">
+    <tableColumn id="83" xr3:uid="{8DC0E209-2987-40FE-9521-B3339A7D8E1F}" name="angle stdev" dataDxfId="11">
       <calculatedColumnFormula>$BW$25*$BW$28/($BW$28+Table3[[#This Row],[hit quality remainder]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="84" xr3:uid="{F8EB7F4C-5D31-472E-A363-210E62A7E683}" name="grounder % (&lt;10 deg)" dataCellStyle="Percent">
@@ -8154,37 +8153,37 @@
     <tableColumn id="85" xr3:uid="{56DD6E0A-39C0-4DF0-B1CB-47EB71B71306}" name="pop up % (&gt;50 deg)" dataCellStyle="Percent">
       <calculatedColumnFormula>1-_xlfn.NORM.DIST(50, Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="86" xr3:uid="{6ED971D4-0303-4AEB-B7CD-9516517F447E}" name="odds of 3B" dataDxfId="11" dataCellStyle="Percent">
+    <tableColumn id="86" xr3:uid="{6ED971D4-0303-4AEB-B7CD-9516517F447E}" name="odds of 3B" dataDxfId="10" dataCellStyle="Percent">
       <calculatedColumnFormula>1-_xlfn.NORM.DIST(70, $BZ$28,$BZ$25,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="87" xr3:uid="{E9F9DFB6-4A26-4CA7-9318-6ECA478690D6}" name="exit velocity mean" dataDxfId="10">
+    <tableColumn id="87" xr3:uid="{E9F9DFB6-4A26-4CA7-9318-6ECA478690D6}" name="exit velocity mean" dataDxfId="9">
       <calculatedColumnFormula>$CA$25+Table3[[#This Row],[offense]]*($CA$27-$CA$25)/2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="88" xr3:uid="{EB865A5D-CC1D-49FA-9709-DC5F30F55DD8}" name="after reduction" dataDxfId="9">
+    <tableColumn id="88" xr3:uid="{EB865A5D-CC1D-49FA-9709-DC5F30F55DD8}" name="after reduction" dataDxfId="8">
       <calculatedColumnFormula>Table3[[#This Row],[exit velocity mean]]-Table3[[#This Row],[reduction]]*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="89" xr3:uid="{949E8C38-C424-4A4E-9A6F-FCA93496D192}" name="theoretical distance" dataDxfId="8">
+    <tableColumn id="89" xr3:uid="{949E8C38-C424-4A4E-9A6F-FCA93496D192}" name="theoretical distance" dataDxfId="7">
       <calculatedColumnFormula>Table3[[#This Row],[exit velocity mean]]^2*2*SIN(RADIANS(Table3[[#This Row],[adjusted launch angle]]))/$CC$28*5280</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="90" xr3:uid="{9FD0A88A-D0D9-4369-8D70-6C7485CA1509}" name="flight time" dataDxfId="7">
+    <tableColumn id="90" xr3:uid="{9FD0A88A-D0D9-4369-8D70-6C7485CA1509}" name="flight time" dataDxfId="6">
       <calculatedColumnFormula>2*Table3[[#This Row],[exit velocity mean]]*SIN(RADIANS(Table3[[#This Row],[adjusted launch angle]]))/$CC$28*60*60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="91" xr3:uid="{D9D5DFED-BD09-4CB6-A82E-D289D2DAB08D}" name="actual distance" dataDxfId="6">
+    <tableColumn id="91" xr3:uid="{D9D5DFED-BD09-4CB6-A82E-D289D2DAB08D}" name="actual distance" dataDxfId="5">
       <calculatedColumnFormula>Table3[[#This Row],[theoretical distance]]-Table3[[#This Row],[flight time]]^2*$CE$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="92" xr3:uid="{3D80331E-564D-462D-81B5-E5CE730D1EE5}" name="+1stdv EV" dataDxfId="5">
+    <tableColumn id="92" xr3:uid="{3D80331E-564D-462D-81B5-E5CE730D1EE5}" name="+1stdv EV" dataDxfId="4">
       <calculatedColumnFormula>Table3[[#This Row],[exit velocity mean]]+$CC$25-Table3[[#This Row],[reduction]]*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="93" xr3:uid="{211123A1-65C0-4F59-AB86-C344CFF47F70}" name="+1stdv LA" dataDxfId="0">
+    <tableColumn id="93" xr3:uid="{211123A1-65C0-4F59-AB86-C344CFF47F70}" name="+1stdv LA" dataDxfId="3">
       <calculatedColumnFormula>MIN(Table3[[#This Row],[adjusted launch angle]]+Table3[[#This Row],[angle stdev]], 30)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="94" xr3:uid="{C8736D16-AF27-436D-BF61-CA3E58298CD3}" name="+1stdv flight time" dataDxfId="4">
+    <tableColumn id="94" xr3:uid="{C8736D16-AF27-436D-BF61-CA3E58298CD3}" name="+1stdv flight time" dataDxfId="2">
       <calculatedColumnFormula>2*Table3[[#This Row],[+1stdv EV]]*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*60*60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="95" xr3:uid="{C9967388-9755-4293-82E9-4E43A4770599}" name="+1stdev distance" dataDxfId="3">
+    <tableColumn id="95" xr3:uid="{C9967388-9755-4293-82E9-4E43A4770599}" name="+1stdev distance" dataDxfId="1">
       <calculatedColumnFormula>Table3[[#This Row],[+1stdv EV]]^2*2*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*5280-Table3[[#This Row],[+1stdv flight time]]^2*$CE$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="96" xr3:uid="{52B6BA3A-87F7-49FD-BFE7-811EA76B03FD}" name="+1stdev delta" dataDxfId="2">
+    <tableColumn id="96" xr3:uid="{52B6BA3A-87F7-49FD-BFE7-811EA76B03FD}" name="+1stdev delta" dataDxfId="0">
       <calculatedColumnFormula>Table3[[#This Row],[+1stdev distance]]-Table3[[#This Row],[actual distance]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="97" xr3:uid="{50EEB2EF-C836-4BBC-A8B3-EAD31BF29B54}" name="Column95"/>
@@ -8488,8 +8487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DO41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CA1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CI28" sqref="CI28"/>
+    <sheetView tabSelected="1" topLeftCell="AX4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BG9" sqref="BG9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9141,7 +9140,7 @@
         <v>1.5653650964326582E-2</v>
       </c>
       <c r="AF7" s="29">
-        <f>$AF$34*$AF$25</f>
+        <f t="shared" ref="AF7:AF22" si="2">$AF$34*$AF$25</f>
         <v>-4</v>
       </c>
       <c r="AG7" s="29">
@@ -9149,11 +9148,11 @@
         <v>0</v>
       </c>
       <c r="AH7" s="29">
-        <f t="shared" ref="AH7:AH22" si="2">$AH$25*$AH$34</f>
+        <f t="shared" ref="AH7:AH22" si="3">$AH$25*$AH$34</f>
         <v>0</v>
       </c>
       <c r="AI7" s="29">
-        <f>$AI$34*$AI$25</f>
+        <f t="shared" ref="AI7:AI22" si="4">$AI$34*$AI$25</f>
         <v>0</v>
       </c>
       <c r="AJ7" s="29">
@@ -9229,7 +9228,7 @@
         <v>9.0000000000000011E-2</v>
       </c>
       <c r="BB7" s="29">
-        <f t="shared" ref="BB7:BB22" si="3">$BB$25</f>
+        <f t="shared" ref="BB7:BB22" si="5">$BB$25</f>
         <v>0.5</v>
       </c>
       <c r="BC7" s="130">
@@ -9257,7 +9256,7 @@
         <v>0.74157303370786509</v>
       </c>
       <c r="BI7" s="29">
-        <f t="shared" ref="BI7:BI22" si="4">$BB$29</f>
+        <f t="shared" ref="BI7:BI22" si="6">$BB$29</f>
         <v>1</v>
       </c>
       <c r="BJ7" s="105">
@@ -9325,7 +9324,7 @@
         <v>2.4134074004724781E-2</v>
       </c>
       <c r="BZ7" s="105">
-        <f t="shared" ref="BZ7:BZ22" si="5">1-_xlfn.NORM.DIST(70, $BZ$28,$BZ$25,TRUE)</f>
+        <f t="shared" ref="BZ7:BZ22" si="7">1-_xlfn.NORM.DIST(70, $BZ$28,$BZ$25,TRUE)</f>
         <v>0.42944875004736094</v>
       </c>
       <c r="CA7" s="29">
@@ -9459,7 +9458,7 @@
         <v>0.10500000000000001</v>
       </c>
       <c r="W8" s="3">
-        <f t="shared" ref="W8:W22" si="6">(1-$W$32)</f>
+        <f t="shared" ref="W8:W22" si="8">(1-$W$32)</f>
         <v>0</v>
       </c>
       <c r="X8" s="49">
@@ -9495,7 +9494,7 @@
         <v>1.0317546081842099E-2</v>
       </c>
       <c r="AF8" s="3">
-        <f>$AF$34*$AF$25</f>
+        <f t="shared" si="2"/>
         <v>-4</v>
       </c>
       <c r="AG8" s="3">
@@ -9503,11 +9502,11 @@
         <v>0</v>
       </c>
       <c r="AH8" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AI8" s="3">
-        <f>$AI$34*$AI$25</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AJ8" s="3">
@@ -9583,7 +9582,7 @@
         <v>9.0000000000000011E-2</v>
       </c>
       <c r="BB8" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="BC8" s="132">
@@ -9611,7 +9610,7 @@
         <v>0.79646017699115046</v>
       </c>
       <c r="BI8" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="BJ8" s="106">
@@ -9679,7 +9678,7 @@
         <v>3.0396361765261393E-2</v>
       </c>
       <c r="BZ8" s="106">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.42944875004736094</v>
       </c>
       <c r="CA8" s="3">
@@ -9813,7 +9812,7 @@
         <v>0.11000000000000001</v>
       </c>
       <c r="W9" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="X9" s="50">
@@ -9849,7 +9848,7 @@
         <v>5.465714583151815E-3</v>
       </c>
       <c r="AF9" s="4">
-        <f>$AF$34*$AF$25</f>
+        <f t="shared" si="2"/>
         <v>-4</v>
       </c>
       <c r="AG9" s="4">
@@ -9857,11 +9856,11 @@
         <v>0</v>
       </c>
       <c r="AH9" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AI9" s="4">
-        <f>$AI$34*$AI$25</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AJ9" s="4">
@@ -9937,7 +9936,7 @@
         <v>9.0000000000000011E-2</v>
       </c>
       <c r="BB9" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="BC9" s="134">
@@ -9965,7 +9964,7 @@
         <v>0.83916083916083917</v>
       </c>
       <c r="BI9" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="BJ9" s="107">
@@ -10033,7 +10032,7 @@
         <v>4.0059156863817114E-2</v>
       </c>
       <c r="BZ9" s="107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.42944875004736094</v>
       </c>
       <c r="CA9" s="4">
@@ -10167,7 +10166,7 @@
         <v>0.12000000000000001</v>
       </c>
       <c r="W10" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="X10" s="49">
@@ -10203,7 +10202,7 @@
         <v>5.7330306169056655E-7</v>
       </c>
       <c r="AF10" s="3">
-        <f>$AF$34*$AF$25</f>
+        <f t="shared" si="2"/>
         <v>-4</v>
       </c>
       <c r="AG10" s="3">
@@ -10211,11 +10210,11 @@
         <v>0</v>
       </c>
       <c r="AH10" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AI10" s="3">
-        <f>$AI$34*$AI$25</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AJ10" s="3">
@@ -10291,7 +10290,7 @@
         <v>9.0000000000000011E-2</v>
       </c>
       <c r="BB10" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="BC10" s="132">
@@ -10319,7 +10318,7 @@
         <v>0.88669950738916259</v>
       </c>
       <c r="BI10" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="BJ10" s="106">
@@ -10387,7 +10386,7 @@
         <v>6.6807201268858085E-2</v>
       </c>
       <c r="BZ10" s="106">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.42944875004736094</v>
       </c>
       <c r="CA10" s="3">
@@ -10521,7 +10520,7 @@
         <v>0.505</v>
       </c>
       <c r="W11" s="13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="X11" s="51">
@@ -10557,7 +10556,7 @@
         <v>1.5653650964326582E-2</v>
       </c>
       <c r="AF11" s="13">
-        <f>$AF$34*$AF$25</f>
+        <f t="shared" si="2"/>
         <v>-4</v>
       </c>
       <c r="AG11" s="13">
@@ -10565,11 +10564,11 @@
         <v>0</v>
       </c>
       <c r="AH11" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AI11" s="13">
-        <f>$AI$34*$AI$25</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AJ11" s="13">
@@ -10645,7 +10644,7 @@
         <v>0.05</v>
       </c>
       <c r="BB11" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="BC11" s="136">
@@ -10673,7 +10672,7 @@
         <v>0.65346534653465349</v>
       </c>
       <c r="BI11" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="BJ11" s="108">
@@ -10741,7 +10740,7 @@
         <v>2.4134074004724781E-2</v>
       </c>
       <c r="BZ11" s="108">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.42944875004736094</v>
       </c>
       <c r="CA11" s="13">
@@ -10875,7 +10874,7 @@
         <v>0.52500000000000002</v>
       </c>
       <c r="W12" s="26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="X12" s="52">
@@ -10911,7 +10910,7 @@
         <v>1.0317546081842099E-2</v>
       </c>
       <c r="AF12" s="26">
-        <f>$AF$34*$AF$25</f>
+        <f t="shared" si="2"/>
         <v>-4</v>
       </c>
       <c r="AG12" s="26">
@@ -10919,11 +10918,11 @@
         <v>0</v>
       </c>
       <c r="AH12" s="26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AI12" s="26">
-        <f>$AI$34*$AI$25</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AJ12" s="26">
@@ -10999,7 +10998,7 @@
         <v>0.05</v>
       </c>
       <c r="BB12" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="BC12" s="138">
@@ -11027,7 +11026,7 @@
         <v>0.72</v>
       </c>
       <c r="BI12" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="BJ12" s="109">
@@ -11095,7 +11094,7 @@
         <v>3.0396361765261393E-2</v>
       </c>
       <c r="BZ12" s="109">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.42944875004736094</v>
       </c>
       <c r="CA12" s="26">
@@ -11229,7 +11228,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="W13" s="13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="X13" s="51">
@@ -11265,7 +11264,7 @@
         <v>5.465714583151815E-3</v>
       </c>
       <c r="AF13" s="13">
-        <f>$AF$34*$AF$25</f>
+        <f t="shared" si="2"/>
         <v>-4</v>
       </c>
       <c r="AG13" s="13">
@@ -11273,11 +11272,11 @@
         <v>0</v>
       </c>
       <c r="AH13" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AI13" s="13">
-        <f>$AI$34*$AI$25</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AJ13" s="13">
@@ -11353,7 +11352,7 @@
         <v>0.05</v>
       </c>
       <c r="BB13" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="BC13" s="136">
@@ -11381,7 +11380,7 @@
         <v>0.77419354838709675</v>
       </c>
       <c r="BI13" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="BJ13" s="108">
@@ -11449,7 +11448,7 @@
         <v>4.0059156863817114E-2</v>
       </c>
       <c r="BZ13" s="108">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.42944875004736094</v>
       </c>
       <c r="CA13" s="13">
@@ -11583,7 +11582,7 @@
         <v>0.6</v>
       </c>
       <c r="W14" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="X14" s="53">
@@ -11619,7 +11618,7 @@
         <v>5.7330306169056655E-7</v>
       </c>
       <c r="AF14" s="5">
-        <f>$AF$34*$AF$25</f>
+        <f t="shared" si="2"/>
         <v>-4</v>
       </c>
       <c r="AG14" s="5">
@@ -11627,11 +11626,11 @@
         <v>0</v>
       </c>
       <c r="AH14" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AI14" s="5">
-        <f>$AI$34*$AI$25</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AJ14" s="5">
@@ -11707,7 +11706,7 @@
         <v>0.05</v>
       </c>
       <c r="BB14" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="BC14" s="140">
@@ -11735,7 +11734,7 @@
         <v>0.83720930232558144</v>
       </c>
       <c r="BI14" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="BJ14" s="110">
@@ -11803,7 +11802,7 @@
         <v>6.6807201268858085E-2</v>
       </c>
       <c r="BZ14" s="110">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.42944875004736094</v>
       </c>
       <c r="CA14" s="5">
@@ -11937,7 +11936,7 @@
         <v>1.01</v>
       </c>
       <c r="W15" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="X15" s="54">
@@ -11973,7 +11972,7 @@
         <v>1.5653650964326582E-2</v>
       </c>
       <c r="AF15" s="17">
-        <f>$AF$34*$AF$25</f>
+        <f t="shared" si="2"/>
         <v>-4</v>
       </c>
       <c r="AG15" s="17">
@@ -11981,11 +11980,11 @@
         <v>0</v>
       </c>
       <c r="AH15" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AI15" s="17">
-        <f>$AI$34*$AI$25</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AJ15" s="17">
@@ -12061,7 +12060,7 @@
         <v>0</v>
       </c>
       <c r="BB15" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="BC15" s="142">
@@ -12089,7 +12088,7 @@
         <v>0.56896551724137934</v>
       </c>
       <c r="BI15" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="BJ15" s="111">
@@ -12157,7 +12156,7 @@
         <v>2.4134074004724781E-2</v>
       </c>
       <c r="BZ15" s="111">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.42944875004736094</v>
       </c>
       <c r="CA15" s="17">
@@ -12291,7 +12290,7 @@
         <v>1.05</v>
       </c>
       <c r="W16" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="X16" s="55">
@@ -12327,7 +12326,7 @@
         <v>1.0317546081842099E-2</v>
       </c>
       <c r="AF16" s="6">
-        <f>$AF$34*$AF$25</f>
+        <f t="shared" si="2"/>
         <v>-4</v>
       </c>
       <c r="AG16" s="6">
@@ -12335,11 +12334,11 @@
         <v>0</v>
       </c>
       <c r="AH16" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AI16" s="6">
-        <f>$AI$34*$AI$25</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AJ16" s="6">
@@ -12415,7 +12414,7 @@
         <v>0</v>
       </c>
       <c r="BB16" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="BC16" s="144">
@@ -12443,7 +12442,7 @@
         <v>0.64285714285714279</v>
       </c>
       <c r="BI16" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="BJ16" s="112">
@@ -12511,7 +12510,7 @@
         <v>3.0396361765261393E-2</v>
       </c>
       <c r="BZ16" s="112">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.42944875004736094</v>
       </c>
       <c r="CA16" s="6">
@@ -12645,7 +12644,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="W17" s="23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="X17" s="56">
@@ -12681,7 +12680,7 @@
         <v>5.465714583151815E-3</v>
       </c>
       <c r="AF17" s="23">
-        <f>$AF$34*$AF$25</f>
+        <f t="shared" si="2"/>
         <v>-4</v>
       </c>
       <c r="AG17" s="23">
@@ -12689,11 +12688,11 @@
         <v>0</v>
       </c>
       <c r="AH17" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AI17" s="23">
-        <f>$AI$34*$AI$25</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AJ17" s="23">
@@ -12769,7 +12768,7 @@
         <v>0</v>
       </c>
       <c r="BB17" s="23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="BC17" s="146">
@@ -12797,7 +12796,7 @@
         <v>0.70588235294117641</v>
       </c>
       <c r="BI17" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="BJ17" s="113">
@@ -12865,7 +12864,7 @@
         <v>4.0059156863817114E-2</v>
       </c>
       <c r="BZ17" s="113">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.42944875004736094</v>
       </c>
       <c r="CA17" s="23">
@@ -12999,7 +12998,7 @@
         <v>1.2</v>
       </c>
       <c r="W18" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="X18" s="55">
@@ -13035,7 +13034,7 @@
         <v>5.7330306169056655E-7</v>
       </c>
       <c r="AF18" s="6">
-        <f>$AF$34*$AF$25</f>
+        <f t="shared" si="2"/>
         <v>-4</v>
       </c>
       <c r="AG18" s="6">
@@ -13043,11 +13042,11 @@
         <v>0</v>
       </c>
       <c r="AH18" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AI18" s="6">
-        <f>$AI$34*$AI$25</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AJ18" s="6">
@@ -13123,7 +13122,7 @@
         <v>0</v>
       </c>
       <c r="BB18" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="BC18" s="144">
@@ -13151,7 +13150,7 @@
         <v>0.78260869565217395</v>
       </c>
       <c r="BI18" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="BJ18" s="112">
@@ -13219,7 +13218,7 @@
         <v>6.6807201268858085E-2</v>
       </c>
       <c r="BZ18" s="112">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.42944875004736094</v>
       </c>
       <c r="CA18" s="6">
@@ -13353,7 +13352,7 @@
         <v>2.02</v>
       </c>
       <c r="W19" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="X19" s="57">
@@ -13389,7 +13388,7 @@
         <v>1.5653650964326582E-2</v>
       </c>
       <c r="AF19" s="15">
-        <f>$AF$34*$AF$25</f>
+        <f t="shared" si="2"/>
         <v>-4</v>
       </c>
       <c r="AG19" s="15">
@@ -13397,11 +13396,11 @@
         <v>0</v>
       </c>
       <c r="AH19" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AI19" s="15">
-        <f>$AI$34*$AI$25</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AJ19" s="15">
@@ -13477,7 +13476,7 @@
         <v>0</v>
       </c>
       <c r="BB19" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="BC19" s="148">
@@ -13505,7 +13504,7 @@
         <v>0.45205479452054798</v>
       </c>
       <c r="BI19" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="BJ19" s="114">
@@ -13573,7 +13572,7 @@
         <v>2.4134074004724781E-2</v>
       </c>
       <c r="BZ19" s="114">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.42944875004736094</v>
       </c>
       <c r="CA19" s="15">
@@ -13707,7 +13706,7 @@
         <v>2.1</v>
       </c>
       <c r="W20" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="X20" s="58">
@@ -13743,7 +13742,7 @@
         <v>1.0317546081842099E-2</v>
       </c>
       <c r="AF20" s="11">
-        <f>$AF$34*$AF$25</f>
+        <f t="shared" si="2"/>
         <v>-4</v>
       </c>
       <c r="AG20" s="11">
@@ -13751,11 +13750,11 @@
         <v>0</v>
       </c>
       <c r="AH20" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AI20" s="11">
-        <f>$AI$34*$AI$25</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AJ20" s="11">
@@ -13831,7 +13830,7 @@
         <v>0</v>
       </c>
       <c r="BB20" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="BC20" s="150">
@@ -13859,7 +13858,7 @@
         <v>0.52941176470588236</v>
       </c>
       <c r="BI20" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="BJ20" s="115">
@@ -13927,7 +13926,7 @@
         <v>3.0396361765261393E-2</v>
       </c>
       <c r="BZ20" s="115">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.42944875004736094</v>
       </c>
       <c r="CA20" s="11">
@@ -14061,7 +14060,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="W21" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="X21" s="57">
@@ -14097,7 +14096,7 @@
         <v>5.465714583151815E-3</v>
       </c>
       <c r="AF21" s="15">
-        <f>$AF$34*$AF$25</f>
+        <f t="shared" si="2"/>
         <v>-4</v>
       </c>
       <c r="AG21" s="15">
@@ -14105,11 +14104,11 @@
         <v>0</v>
       </c>
       <c r="AH21" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AI21" s="15">
-        <f>$AI$34*$AI$25</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AJ21" s="15">
@@ -14185,7 +14184,7 @@
         <v>0</v>
       </c>
       <c r="BB21" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="BC21" s="148">
@@ -14213,7 +14212,7 @@
         <v>0.6</v>
       </c>
       <c r="BI21" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="BJ21" s="114">
@@ -14281,7 +14280,7 @@
         <v>4.0059156863817114E-2</v>
       </c>
       <c r="BZ21" s="114">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.42944875004736094</v>
       </c>
       <c r="CA21" s="15">
@@ -14415,7 +14414,7 @@
         <v>2.4</v>
       </c>
       <c r="W22" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="X22" s="59">
@@ -14451,7 +14450,7 @@
         <v>5.7330306169056655E-7</v>
       </c>
       <c r="AF22" s="20">
-        <f>$AF$34*$AF$25</f>
+        <f t="shared" si="2"/>
         <v>-4</v>
       </c>
       <c r="AG22" s="20">
@@ -14459,11 +14458,11 @@
         <v>0</v>
       </c>
       <c r="AH22" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AI22" s="20">
-        <f>$AI$34*$AI$25</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AJ22" s="20">
@@ -14539,7 +14538,7 @@
         <v>0</v>
       </c>
       <c r="BB22" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="BC22" s="152">
@@ -14567,7 +14566,7 @@
         <v>0.69230769230769229</v>
       </c>
       <c r="BI22" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="BJ22" s="116">
@@ -14635,7 +14634,7 @@
         <v>6.6807201268858085E-2</v>
       </c>
       <c r="BZ22" s="116">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.42944875004736094</v>
       </c>
       <c r="CA22" s="20">
@@ -15315,7 +15314,7 @@
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
   <conditionalFormatting sqref="O7:O22">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Implemented hitting, did a bunch of architecture work to plan out and support fielding and eventually roll all this into a game.
Players are currently batting 0.025 though so something is broken lol - will fix later.
</commit_message>
<xml_diff>
--- a/plans/baseball stats.xlsx
+++ b/plans/baseball stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcgiffenk\Desktop\newpy\xtreemblaseball99\plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{709F8AF3-4DB8-4CBE-B657-C56076EF0FBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1B85F9-D9E3-460D-BD3B-452D22A73EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8487,8 +8487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DO41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AX4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BG9" sqref="BG9"/>
+    <sheetView tabSelected="1" topLeftCell="AD4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BJ31" sqref="BJ31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15332,7 +15332,7 @@
   <dimension ref="C2:S9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
wrangling with starting fielding.
</commit_message>
<xml_diff>
--- a/plans/baseball stats.xlsx
+++ b/plans/baseball stats.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcgiffenk\Desktop\newpy\xtreemblaseball99\plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1B85F9-D9E3-460D-BD3B-452D22A73EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495A7E3F-942D-439D-903D-CAF26CA8A0B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="iterative" sheetId="2" r:id="rId1"/>
-    <sheet name="gauss cruncher" sheetId="5" r:id="rId2"/>
-    <sheet name="run speed" sheetId="3" r:id="rId3"/>
-    <sheet name="pitch outcomes" sheetId="1" r:id="rId4"/>
-    <sheet name="hit quality truth table" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId2"/>
+    <sheet name="gauss cruncher" sheetId="5" r:id="rId3"/>
+    <sheet name="run speed" sheetId="3" r:id="rId4"/>
+    <sheet name="pitch outcomes" sheetId="1" r:id="rId5"/>
+    <sheet name="hit quality truth table" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="basis">#REF!</definedName>
@@ -540,7 +541,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="304">
   <si>
     <t>Ball</t>
   </si>
@@ -1447,6 +1448,12 @@
   </si>
   <si>
     <t>+1stdev delta</t>
+  </si>
+  <si>
+    <t>net</t>
+  </si>
+  <si>
+    <t>form</t>
   </si>
 </sst>
 </file>
@@ -2101,7 +2108,10 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="82">
+  <dxfs count="83">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -2518,6 +2528,469 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>net</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$13:$J$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$13:$K$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-75D4-4E4F-95C9-DA0E719BFEDE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>form</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$13:$J$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$13:$L$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.66874030497642201</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.91469121922869445</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0466351393921056</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2178832856309068</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4315691227432645</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2636739857523107</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-75D4-4E4F-95C9-DA0E719BFEDE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="447991871"/>
+        <c:axId val="447989375"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="447991871"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="447989375"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="447989375"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="447991871"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -4929,7 +5402,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -5850,7 +6323,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -6223,6 +6696,46 @@
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -6779,6 +7292,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7281,7 +8310,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7804,6 +8833,47 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F29DAB7-FE10-4932-9272-279881F0B584}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>47624</xdr:colOff>
       <xdr:row>18</xdr:row>
@@ -7841,7 +8911,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -7919,181 +8989,181 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A6:DO22" totalsRowShown="0" headerRowDxfId="80">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A6:DO22" totalsRowShown="0" headerRowDxfId="81">
   <autoFilter ref="A6:DO22" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="119">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Rep #">
       <calculatedColumnFormula>ROW()-ROW(home)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="offense" dataDxfId="79">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="offense" dataDxfId="80">
       <calculatedColumnFormula>INDEX(oratings, 1, 1+MOD(Table3[[#This Row],[Rep '#]]-1, COUNT(oratings)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="defense" dataDxfId="78">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="defense" dataDxfId="79">
       <calculatedColumnFormula>INDEX(dratings, 1, MOD(FLOOR( (Table3[[#This Row],[Rep '#]]-1) / COUNT(oratings), 1), COUNT(dratings))+1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="base leadoff" dataDxfId="77">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="base leadoff" dataDxfId="78">
       <calculatedColumnFormula>Table3[[#This Row],[offense]]*$D$26+0.05</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="leadoff modifier" dataDxfId="76">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="leadoff modifier" dataDxfId="77">
       <calculatedColumnFormula>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*$E$26</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="total leadoff (ft)" dataDxfId="75">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="total leadoff (ft)" dataDxfId="76">
       <calculatedColumnFormula>MAX(Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90, 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="pickoff manuver (s)" dataDxfId="74">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="pickoff manuver (s)" dataDxfId="75">
       <calculatedColumnFormula>1.1 - Table3[[#This Row],[defense]]*0.1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="throw speed (s/ft)" dataDxfId="73">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="throw speed (s/ft)" dataDxfId="74">
       <calculatedColumnFormula xml:space="preserve"> 0.01 - 0.0025 *  Table3[[#This Row],[defense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="throw speed (mph)" dataDxfId="72">
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="throw speed (mph)" dataDxfId="73">
       <calculatedColumnFormula>1 / Table3[[#This Row],[throw speed (s/ft)]] * ((60 * 60)/5280)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="pickoff time" dataDxfId="71">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="pickoff time" dataDxfId="72">
       <calculatedColumnFormula>Table3[[#This Row],[pickoff manuver (s)]]+60*Table3[[#This Row],[throw speed (s/ft)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="runner reaction" dataDxfId="70">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="runner reaction" dataDxfId="71">
       <calculatedColumnFormula>$K$28-$K$26*Table3[[#This Row],[offense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="runner speed (s/ft)" dataDxfId="69">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="runner speed (s/ft)" dataDxfId="70">
       <calculatedColumnFormula>0.05 - Table3[[#This Row],[offense]]*$L$26</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="runner speed (mph)" dataDxfId="68">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="runner speed (mph)" dataDxfId="69">
       <calculatedColumnFormula>1 / Table3[[#This Row],[runner speed (s/ft)]] * ((60 * 60)/5280)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="pickoff evade time" dataDxfId="67">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="pickoff evade time" dataDxfId="68">
       <calculatedColumnFormula>Table3[[#This Row],[runner reaction]]+Table3[[#This Row],[runner speed (s/ft)]]*Table3[[#This Row],[total leadoff (ft)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="pickoff probability" dataDxfId="66" dataCellStyle="Percent">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="pickoff probability" dataDxfId="67" dataCellStyle="Percent">
       <calculatedColumnFormula>1 - _xlfn.NORM.DIST(Table3[[#This Row],[pickoff time]], Table3[[#This Row],[pickoff evade time]], $O$4, TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Fielding Odds" dataDxfId="65" dataCellStyle="Percent">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Fielding Odds" dataDxfId="66" dataCellStyle="Percent">
       <calculatedColumnFormula>_xlfn.NORM.DIST(Table3[[#This Row],[defense]], $P$26, $P$27, TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="pickoff worth it?" dataDxfId="64">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="pickoff worth it?" dataDxfId="65">
       <calculatedColumnFormula>Table3[[#This Row],[pickoff probability]] &gt; 1-Table3[[#This Row],[Fielding Odds]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Error %" dataDxfId="63" dataCellStyle="Percent">
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Error %" dataDxfId="64" dataCellStyle="Percent">
       <calculatedColumnFormula>1-Table3[[#This Row],[Fielding Odds]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Blatant steal time" dataDxfId="62">
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Blatant steal time" dataDxfId="63">
       <calculatedColumnFormula>(90-Table3[[#This Row],[total leadoff (ft)]])*Table3[[#This Row],[runner speed (s/ft)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Response speed" dataDxfId="61">
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Response speed" dataDxfId="62">
       <calculatedColumnFormula>$T$26*(2-Table3[[#This Row],[defense]]) + Table3[[#This Row],[pickoff time]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="blatant steal probability" dataDxfId="60" dataCellStyle="Percent">
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="blatant steal probability" dataDxfId="61" dataCellStyle="Percent">
       <calculatedColumnFormula>_xlfn.NORM.DIST(Table3[[#This Row],[Response speed]], Table3[[#This Row],[Blatant steal time]], $U$4, TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="defense fear" dataDxfId="59">
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="defense fear" dataDxfId="60">
       <calculatedColumnFormula>Table3[[#This Row],[defense]]+Table3[[#This Row],[defense]]*Table3[[#This Row],[offense]]*$E$26</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="ball factor" dataDxfId="58">
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="ball factor" dataDxfId="59">
       <calculatedColumnFormula>(1-$W$32)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="desperation" dataDxfId="57" dataCellStyle="Percent">
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="desperation" dataDxfId="58" dataCellStyle="Percent">
       <calculatedColumnFormula>Table3[[#This Row],[ball factor]]/$X$32*(1-$X$34)+$X$34</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="player control" dataDxfId="56">
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="player control" dataDxfId="57">
       <calculatedColumnFormula>Table3[[#This Row],[offense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="ideal steer" dataDxfId="55">
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="ideal steer" dataDxfId="56">
       <calculatedColumnFormula>$AA$33</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="scaled control" dataDxfId="54">
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="scaled control" dataDxfId="55">
       <calculatedColumnFormula>IF(Table3[[#This Row],[player control]]&gt;1,Table3[[#This Row],[player control]]*$AA$41+$AA$40,Table3[[#This Row],[player control]]*$AA$39+$AA$38)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="unmod foul percent 3rd" dataDxfId="53" dataCellStyle="Percent">
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="unmod foul percent 3rd" dataDxfId="54" dataCellStyle="Percent">
       <calculatedColumnFormula>_xlfn.NORM.DIST(-1,Table3[[#This Row],[ideal steer]],($AB$25-Table3[[#This Row],[scaled control]])*$AB$27,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="unmod foul percent 1st" dataDxfId="52" dataCellStyle="Percent">
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="unmod foul percent 1st" dataDxfId="53" dataCellStyle="Percent">
       <calculatedColumnFormula>1-_xlfn.NORM.DIST(1,Table3[[#This Row],[ideal steer]],($AB$25-Table3[[#This Row],[scaled control]])*$AB$27,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="total unmod foul percent" dataDxfId="51" dataCellStyle="Percent">
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="total unmod foul percent" dataDxfId="52" dataCellStyle="Percent">
       <calculatedColumnFormula>1-(1-Table3[[#This Row],[unmod foul percent 3rd]])*(1-Table3[[#This Row],[unmod foul percent 1st]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="unmod dead center foul%" dataDxfId="50" dataCellStyle="Percent">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="unmod dead center foul%" dataDxfId="51" dataCellStyle="Percent">
       <calculatedColumnFormula>1-((1-_xlfn.NORM.DIST(-1,0,($AB$25-Table3[[#This Row],[scaled control]])*$AB$27,TRUE))*_xlfn.NORM.DIST(1,0,($AB$25-Table3[[#This Row],[scaled control]])*$AB$27,TRUE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="count" dataDxfId="49">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="count" dataDxfId="50">
       <calculatedColumnFormula>$AF$34*$AF$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="hitter discipline bias" dataDxfId="48">
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="hitter discipline bias" dataDxfId="49">
       <calculatedColumnFormula>$AG$25*($AG$34*Table3[[#This Row],[offense]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="bases loaded" dataDxfId="47">
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="bases loaded" dataDxfId="48">
       <calculatedColumnFormula>$AH$25*$AH$34</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="number of outs" dataDxfId="46">
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="number of outs" dataDxfId="47">
       <calculatedColumnFormula>$AI$34*$AI$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="current hitter vs next hitter" dataDxfId="45">
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="current hitter vs next hitter" dataDxfId="46">
       <calculatedColumnFormula>$AJ$25*(Table3[[#This Row],[offense]]-$AJ$27)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="calling modifier" dataDxfId="44">
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="calling modifier" dataDxfId="45">
       <calculatedColumnFormula array="1">SUM(Table3[[#This Row],[count]:[current hitter vs next hitter]]*MIN(1, Table3[[#This Row],[defense]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="sigmoid strike percent" dataDxfId="43" dataCellStyle="Percent">
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="sigmoid strike percent" dataDxfId="44" dataCellStyle="Percent">
       <calculatedColumnFormula>$AL$25-(Table3[[#This Row],[calling modifier]]/(ABS(Table3[[#This Row],[calling modifier]])+$AL$29)*$AL$27)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="tanh strike percent" dataDxfId="42" dataCellStyle="Percent">
+    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="tanh strike percent" dataDxfId="43" dataCellStyle="Percent">
       <calculatedColumnFormula>$AL$25-$AL$27*TANH(Table3[[#This Row],[calling modifier]]/$AM$29)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="called position" dataDxfId="41" dataCellStyle="Percent">
+    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="called position" dataDxfId="42" dataCellStyle="Percent">
       <calculatedColumnFormula>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-Table3[[#This Row],[defense]])))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="called pos 0.2 pitch" dataDxfId="40">
+    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="called pos 0.2 pitch" dataDxfId="41">
       <calculatedColumnFormula>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-0.2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="called pos 2 pitch" dataDxfId="39">
+    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="called pos 2 pitch" dataDxfId="40">
       <calculatedColumnFormula>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="location -1  stdv" dataDxfId="38">
+    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="location -1  stdv" dataDxfId="39">
       <calculatedColumnFormula>Table3[[#This Row],[called position]]-pitchmod*(pitchstdv-Table3[[#This Row],[defense]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="location +1 stdv" dataDxfId="37">
+    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="location +1 stdv" dataDxfId="38">
       <calculatedColumnFormula>ABS(Table3[[#This Row],[called position]]+pitchmod*(pitchstdv-Table3[[#This Row],[defense]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="min dist to sz 1stdv" dataDxfId="36">
+    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="min dist to sz 1stdv" dataDxfId="37">
       <calculatedColumnFormula>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;1, Table3[[#This Row],[location +1 stdv]]&gt;1),0, MIN(Table3[[#This Row],[location -1  stdv]]+1, 1-Table3[[#This Row],[location +1 stdv]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="max dist to sz 1stdv" dataDxfId="35">
+    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="max dist to sz 1stdv" dataDxfId="36">
       <calculatedColumnFormula>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;0, Table3[[#This Row],[location +1 stdv]]&gt;0),1, MAX(1-ABS(Table3[[#This Row],[location -1  stdv]]), Table3[[#This Row],[location +1 stdv]]-1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="ave obscurity" dataDxfId="34">
+    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="ave obscurity" dataDxfId="35">
       <calculatedColumnFormula>$AU$30/(ABS(Table3[[#This Row],[called position]]-1)+$AU$27)+$AU$32*Table3[[#This Row],[defense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="obscurity at _x000a_0.5" dataDxfId="33">
+    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="obscurity at _x000a_0.5" dataDxfId="34">
       <calculatedColumnFormula>$AU$30/(ABS(0.5-1)+$AU$27)+$AU$32*Table3[[#This Row],[defense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="obscurity at  0.9" dataDxfId="32">
+    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="obscurity at  0.9" dataDxfId="33">
       <calculatedColumnFormula>$AU$30/(ABS(0.9-1)+$AU$27)+$AU$32*Table3[[#This Row],[defense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="average difficulty" dataDxfId="31">
+    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="average difficulty" dataDxfId="32">
       <calculatedColumnFormula>Table3[[#This Row],[defense]]*$AX$30+MAX(0, Table3[[#This Row],[called position]]-$AX$27)^$AX$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" name="+1stdv difficulty" dataDxfId="30">
+    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" name="+1stdv difficulty" dataDxfId="31">
       <calculatedColumnFormula>Table3[[#This Row],[defense]]*$AX$30 + MAX(0, Table3[[#This Row],[location +1 stdv]]-$AX$27)^$AX$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0000-000037000000}" name="difficulty at 1" dataDxfId="29">
+    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0000-000037000000}" name="difficulty at 1" dataDxfId="30">
       <calculatedColumnFormula>Table3[[#This Row],[defense]]*$AX$30+MAX(0, 1-$AX$27)^$AX$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="62" xr3:uid="{6513900D-2CAC-4022-A6B3-8A00EE6C566B}" name="reduction" dataDxfId="28">
+    <tableColumn id="62" xr3:uid="{6513900D-2CAC-4022-A6B3-8A00EE6C566B}" name="reduction" dataDxfId="29">
       <calculatedColumnFormula>MAX(0, 0.1*(1-Table3[[#This Row],[defense]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="63" xr3:uid="{12464915-1D8C-4EB5-9BBD-0FF526658E5B}" name="Location" dataDxfId="27">
+    <tableColumn id="63" xr3:uid="{12464915-1D8C-4EB5-9BBD-0FF526658E5B}" name="Location" dataDxfId="28">
       <calculatedColumnFormula>$BB$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="64" xr3:uid="{5F0F19BE-6D04-4E9E-81B2-B324AB353F5C}" name="obscurity" dataDxfId="26">
+    <tableColumn id="64" xr3:uid="{5F0F19BE-6D04-4E9E-81B2-B324AB353F5C}" name="obscurity" dataDxfId="27">
       <calculatedColumnFormula>$AU$30/(ABS(Table3[[#This Row],[Location]]-1)+$AU$27)+$AU$32*Table3[[#This Row],[defense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="65" xr3:uid="{EA3D32E7-A2E2-482C-B6E9-2E17651C5F77}" name="Strike?" dataDxfId="25">
+    <tableColumn id="65" xr3:uid="{EA3D32E7-A2E2-482C-B6E9-2E17651C5F77}" name="Strike?" dataDxfId="26">
       <calculatedColumnFormula>Table3[[#This Row],[Location]]&lt;= (1+MAX(0, (Table3[[#This Row],[defense]]-1)*0.1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="66" xr3:uid="{0C7E9B06-240B-481E-B495-54026E2F00AA}" name="discipline modifier" dataDxfId="24">
+    <tableColumn id="66" xr3:uid="{0C7E9B06-240B-481E-B495-54026E2F00AA}" name="discipline modifier" dataDxfId="25">
       <calculatedColumnFormula>1/(1+Table3[[#This Row],[offense]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="67" xr3:uid="{D3B0837D-02D4-4F62-A2E2-876739E497B0}" name="effective obscurity" dataDxfId="23">
+    <tableColumn id="67" xr3:uid="{D3B0837D-02D4-4F62-A2E2-876739E497B0}" name="effective obscurity" dataDxfId="24">
       <calculatedColumnFormula>Table3[[#This Row],[obscurity]]*Table3[[#This Row],[discipline modifier]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="69" xr3:uid="{39822A5F-1791-48DC-BA9F-A066931C0292}" name="odds of read" dataCellStyle="Percent">
@@ -8108,43 +9178,43 @@
     <tableColumn id="72" xr3:uid="{3E21C76F-F55B-4E49-9BE2-FEE046008C15}" name="adjusted swing %" dataCellStyle="Percent">
       <calculatedColumnFormula>Table3[[#This Row],[desperation echo]]*Table3[[#This Row],[unadjusted swing %]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="130" xr3:uid="{827C9303-3867-43F7-A79B-BC2EAB3F896D}" name="pitch carry forward obsc" dataDxfId="22">
+    <tableColumn id="130" xr3:uid="{827C9303-3867-43F7-A79B-BC2EAB3F896D}" name="pitch carry forward obsc" dataDxfId="23">
       <calculatedColumnFormula>Table3[[#This Row],[ave obscurity]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="131" xr3:uid="{F26B1E2C-89D5-4F6D-877A-1BEA7F7DF5A9}" name="CF odds of read" dataCellStyle="Percent">
       <calculatedColumnFormula>1/(1+Table3[[#This Row],[ave obscurity]]*Table3[[#This Row],[discipline modifier]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="73" xr3:uid="{77BBE784-030D-4E46-9A29-8783B89762BC}" name="contact echo" dataDxfId="21">
+    <tableColumn id="73" xr3:uid="{77BBE784-030D-4E46-9A29-8783B89762BC}" name="contact echo" dataDxfId="22">
       <calculatedColumnFormula>Table3[[#This Row],[offense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="75" xr3:uid="{074A9F48-3941-4E36-90C2-7710217D32C8}" name="pitch carry forward diff" dataDxfId="20">
+    <tableColumn id="75" xr3:uid="{074A9F48-3941-4E36-90C2-7710217D32C8}" name="pitch carry forward diff" dataDxfId="21">
       <calculatedColumnFormula>Table3[[#This Row],[average difficulty]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="76" xr3:uid="{628DDA60-D380-4EE8-AA7D-7EF6C4AAD8A5}" name="CF contact readiness" dataDxfId="19">
+    <tableColumn id="76" xr3:uid="{628DDA60-D380-4EE8-AA7D-7EF6C4AAD8A5}" name="CF contact readiness" dataDxfId="20">
       <calculatedColumnFormula>Table3[[#This Row],[contact echo]]-Table3[[#This Row],[pitch carry forward diff]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="77" xr3:uid="{DBF18AD6-8593-42C7-9058-D19737088E6D}" name="foul %" dataDxfId="18" dataCellStyle="Percent">
+    <tableColumn id="77" xr3:uid="{DBF18AD6-8593-42C7-9058-D19737088E6D}" name="foul %" dataDxfId="19" dataCellStyle="Percent">
       <calculatedColumnFormula>1-_xlfn.NORM.DIST($BP$27,Table3[[#This Row],[CF contact readiness]], $BP$30,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="78" xr3:uid="{6354951A-151E-4E04-9897-9CB39D6098C8}" name="clean %" dataDxfId="17" dataCellStyle="Percent">
+    <tableColumn id="78" xr3:uid="{6354951A-151E-4E04-9897-9CB39D6098C8}" name="clean %" dataDxfId="18" dataCellStyle="Percent">
       <calculatedColumnFormula>1-_xlfn.NORM.DIST($BP$25,Table3[[#This Row],[CF contact readiness]], $BP$30,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="79" xr3:uid="{0070F673-D13C-467D-95AC-FF8413A02F3F}" name="strike swinging %" dataDxfId="16" dataCellStyle="Percent">
+    <tableColumn id="79" xr3:uid="{0070F673-D13C-467D-95AC-FF8413A02F3F}" name="strike swinging %" dataDxfId="17" dataCellStyle="Percent">
       <calculatedColumnFormula>1-Table3[[#This Row],[foul %]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="80" xr3:uid="{9504D0CF-7CD0-472F-8289-44B30538D80C}" name="ave. hit quality" dataDxfId="15">
+    <tableColumn id="80" xr3:uid="{9504D0CF-7CD0-472F-8289-44B30538D80C}" name="ave. hit quality" dataDxfId="16">
       <calculatedColumnFormula>(Table3[[#This Row],[CF contact readiness]]-$BP$27)/$BP$30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="132" xr3:uid="{0BB169E4-F345-4B7D-A549-DE28DC5FB113}" name="hit quality +1stdv" dataDxfId="14">
+    <tableColumn id="132" xr3:uid="{0BB169E4-F345-4B7D-A549-DE28DC5FB113}" name="hit quality +1stdv" dataDxfId="15">
       <calculatedColumnFormula>(Table3[[#This Row],[CF contact readiness]]+$BP$30-$BP$27)/$BP$30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="81" xr3:uid="{37438EAA-344A-486C-A4C2-68EE17D67C60}" name="hit quality remainder" dataDxfId="13">
+    <tableColumn id="81" xr3:uid="{37438EAA-344A-486C-A4C2-68EE17D67C60}" name="hit quality remainder" dataDxfId="14">
       <calculatedColumnFormula>MAX(0, IF(ISBLANK($BU$28), Table3[[#This Row],[hit quality +1stdv]], $BU$28)-1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="82" xr3:uid="{CBA11BEE-0412-44C3-979C-1888629B3C7A}" name="adjusted launch angle" dataDxfId="12">
+    <tableColumn id="82" xr3:uid="{CBA11BEE-0412-44C3-979C-1888629B3C7A}" name="adjusted launch angle" dataDxfId="13">
       <calculatedColumnFormula>$BV$25+Table3[[#This Row],[offense]]*$BV$28</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="83" xr3:uid="{8DC0E209-2987-40FE-9521-B3339A7D8E1F}" name="angle stdev" dataDxfId="11">
+    <tableColumn id="83" xr3:uid="{8DC0E209-2987-40FE-9521-B3339A7D8E1F}" name="angle stdev" dataDxfId="12">
       <calculatedColumnFormula>$BW$25*$BW$28/($BW$28+Table3[[#This Row],[hit quality remainder]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="84" xr3:uid="{F8EB7F4C-5D31-472E-A363-210E62A7E683}" name="grounder % (&lt;10 deg)" dataCellStyle="Percent">
@@ -8153,37 +9223,37 @@
     <tableColumn id="85" xr3:uid="{56DD6E0A-39C0-4DF0-B1CB-47EB71B71306}" name="pop up % (&gt;50 deg)" dataCellStyle="Percent">
       <calculatedColumnFormula>1-_xlfn.NORM.DIST(50, Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="86" xr3:uid="{6ED971D4-0303-4AEB-B7CD-9516517F447E}" name="odds of 3B" dataDxfId="10" dataCellStyle="Percent">
+    <tableColumn id="86" xr3:uid="{6ED971D4-0303-4AEB-B7CD-9516517F447E}" name="odds of 3B" dataDxfId="11" dataCellStyle="Percent">
       <calculatedColumnFormula>1-_xlfn.NORM.DIST(70, $BZ$28,$BZ$25,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="87" xr3:uid="{E9F9DFB6-4A26-4CA7-9318-6ECA478690D6}" name="exit velocity mean" dataDxfId="9">
+    <tableColumn id="87" xr3:uid="{E9F9DFB6-4A26-4CA7-9318-6ECA478690D6}" name="exit velocity mean" dataDxfId="10">
       <calculatedColumnFormula>$CA$25+Table3[[#This Row],[offense]]*($CA$27-$CA$25)/2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="88" xr3:uid="{EB865A5D-CC1D-49FA-9709-DC5F30F55DD8}" name="after reduction" dataDxfId="8">
+    <tableColumn id="88" xr3:uid="{EB865A5D-CC1D-49FA-9709-DC5F30F55DD8}" name="after reduction" dataDxfId="9">
       <calculatedColumnFormula>Table3[[#This Row],[exit velocity mean]]-Table3[[#This Row],[reduction]]*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="89" xr3:uid="{949E8C38-C424-4A4E-9A6F-FCA93496D192}" name="theoretical distance" dataDxfId="7">
+    <tableColumn id="89" xr3:uid="{949E8C38-C424-4A4E-9A6F-FCA93496D192}" name="theoretical distance" dataDxfId="8">
       <calculatedColumnFormula>Table3[[#This Row],[exit velocity mean]]^2*2*SIN(RADIANS(Table3[[#This Row],[adjusted launch angle]]))/$CC$28*5280</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="90" xr3:uid="{9FD0A88A-D0D9-4369-8D70-6C7485CA1509}" name="flight time" dataDxfId="6">
+    <tableColumn id="90" xr3:uid="{9FD0A88A-D0D9-4369-8D70-6C7485CA1509}" name="flight time" dataDxfId="7">
       <calculatedColumnFormula>2*Table3[[#This Row],[exit velocity mean]]*SIN(RADIANS(Table3[[#This Row],[adjusted launch angle]]))/$CC$28*60*60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="91" xr3:uid="{D9D5DFED-BD09-4CB6-A82E-D289D2DAB08D}" name="actual distance" dataDxfId="5">
+    <tableColumn id="91" xr3:uid="{D9D5DFED-BD09-4CB6-A82E-D289D2DAB08D}" name="actual distance" dataDxfId="6">
       <calculatedColumnFormula>Table3[[#This Row],[theoretical distance]]-Table3[[#This Row],[flight time]]^2*$CE$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="92" xr3:uid="{3D80331E-564D-462D-81B5-E5CE730D1EE5}" name="+1stdv EV" dataDxfId="4">
+    <tableColumn id="92" xr3:uid="{3D80331E-564D-462D-81B5-E5CE730D1EE5}" name="+1stdv EV" dataDxfId="5">
       <calculatedColumnFormula>Table3[[#This Row],[exit velocity mean]]+$CC$25-Table3[[#This Row],[reduction]]*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="93" xr3:uid="{211123A1-65C0-4F59-AB86-C344CFF47F70}" name="+1stdv LA" dataDxfId="3">
+    <tableColumn id="93" xr3:uid="{211123A1-65C0-4F59-AB86-C344CFF47F70}" name="+1stdv LA" dataDxfId="4">
       <calculatedColumnFormula>MIN(Table3[[#This Row],[adjusted launch angle]]+Table3[[#This Row],[angle stdev]], 30)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="94" xr3:uid="{C8736D16-AF27-436D-BF61-CA3E58298CD3}" name="+1stdv flight time" dataDxfId="2">
+    <tableColumn id="94" xr3:uid="{C8736D16-AF27-436D-BF61-CA3E58298CD3}" name="+1stdv flight time" dataDxfId="3">
       <calculatedColumnFormula>2*Table3[[#This Row],[+1stdv EV]]*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*60*60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="95" xr3:uid="{C9967388-9755-4293-82E9-4E43A4770599}" name="+1stdev distance" dataDxfId="1">
+    <tableColumn id="95" xr3:uid="{C9967388-9755-4293-82E9-4E43A4770599}" name="+1stdev distance" dataDxfId="2">
       <calculatedColumnFormula>Table3[[#This Row],[+1stdv EV]]^2*2*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*5280-Table3[[#This Row],[+1stdv flight time]]^2*$CE$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="96" xr3:uid="{52B6BA3A-87F7-49FD-BFE7-811EA76B03FD}" name="+1stdev delta" dataDxfId="0">
+    <tableColumn id="96" xr3:uid="{52B6BA3A-87F7-49FD-BFE7-811EA76B03FD}" name="+1stdev delta" dataDxfId="1">
       <calculatedColumnFormula>Table3[[#This Row],[+1stdev distance]]-Table3[[#This Row],[actual distance]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="97" xr3:uid="{50EEB2EF-C836-4BBC-A8B3-EAD31BF29B54}" name="Column95"/>
@@ -8217,6 +9287,20 @@
     <tableColumn id="125" xr3:uid="{5EC4C442-B4E7-410B-8F1C-684A18D55779}" name="Column123"/>
     <tableColumn id="126" xr3:uid="{38BD33B3-15CD-47C0-8334-87CB7F96C30E}" name="Column124"/>
     <tableColumn id="127" xr3:uid="{69A8AE3A-0213-42AF-9FC7-17D03726B015}" name="Column125"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{727DBF5C-F1E0-410B-9FAD-D2E7399866B7}" name="Table1" displayName="Table1" ref="J12:L18" totalsRowShown="0">
+  <autoFilter ref="J12:L18" xr:uid="{727DBF5C-F1E0-410B-9FAD-D2E7399866B7}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{23FB116D-6CB4-49F6-A874-F1C610DEF5E1}" name="quality"/>
+    <tableColumn id="2" xr3:uid="{6204ECDD-C980-4BE0-AFC7-9F83BF472BE8}" name="net"/>
+    <tableColumn id="3" xr3:uid="{E9208F79-490A-4A40-B3B7-0914BA16AC90}" name="form" dataDxfId="0">
+      <calculatedColumnFormula>POWER(Table1[[#This Row],[quality]]-0.8, 1/4)</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8487,8 +9571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DO41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BJ31" sqref="BJ31"/>
+    <sheetView topLeftCell="BJ4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BW14" sqref="BW14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9305,7 +10389,7 @@
       </c>
       <c r="BU7" s="29">
         <f>MAX(0, IF(ISBLANK($BU$28), Table3[[#This Row],[hit quality +1stdv]], $BU$28)-1)</f>
-        <v>0.5</v>
+        <v>0.64192855525320414</v>
       </c>
       <c r="BV7" s="29">
         <f>$BV$25+Table3[[#This Row],[offense]]*$BV$28</f>
@@ -9313,15 +10397,15 @@
       </c>
       <c r="BW7" s="29">
         <f>$BW$25*$BW$28/($BW$28+Table3[[#This Row],[hit quality remainder]])</f>
-        <v>20</v>
+        <v>17.514230560216898</v>
       </c>
       <c r="BX7" s="105">
         <f>_xlfn.NORM.DIST(10,Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</f>
-        <v>0.49002748180476197</v>
+        <v>0.48861245728266545</v>
       </c>
       <c r="BY7" s="105">
         <f>1-_xlfn.NORM.DIST(50, Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</f>
-        <v>2.4134074004724781E-2</v>
+        <v>1.2056973296676654E-2</v>
       </c>
       <c r="BZ7" s="105">
         <f t="shared" ref="BZ7:BZ22" si="7">1-_xlfn.NORM.DIST(70, $BZ$28,$BZ$25,TRUE)</f>
@@ -9353,19 +10437,19 @@
       </c>
       <c r="CG7" s="29">
         <f>MIN(Table3[[#This Row],[adjusted launch angle]]+Table3[[#This Row],[angle stdev]], 30)</f>
-        <v>30</v>
+        <v>28.014230560216898</v>
       </c>
       <c r="CH7" s="117">
         <f>2*Table3[[#This Row],[+1stdv EV]]*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*60*60</f>
-        <v>3.3974999999999991</v>
+        <v>3.1915492993304175</v>
       </c>
       <c r="CI7" s="155">
         <f>Table3[[#This Row],[+1stdv EV]]^2*2*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*5280-Table3[[#This Row],[+1stdv flight time]]^2*$CE$25</f>
-        <v>191.52840000000003</v>
+        <v>190.43510153161782</v>
       </c>
       <c r="CJ7" s="155">
         <f>Table3[[#This Row],[+1stdev distance]]-Table3[[#This Row],[actual distance]]</f>
-        <v>89.138692405724626</v>
+        <v>88.045393937342411</v>
       </c>
     </row>
     <row r="8" spans="1:119" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -9659,7 +10743,7 @@
       </c>
       <c r="BU8" s="3">
         <f>MAX(0, IF(ISBLANK($BU$28), Table3[[#This Row],[hit quality +1stdv]], $BU$28)-1)</f>
-        <v>0.5</v>
+        <v>0.77475244561117029</v>
       </c>
       <c r="BV8" s="3">
         <f>$BV$25+Table3[[#This Row],[offense]]*$BV$28</f>
@@ -9667,15 +10751,15 @@
       </c>
       <c r="BW8" s="3">
         <f>$BW$25*$BW$28/($BW$28+Table3[[#This Row],[hit quality remainder]])</f>
-        <v>20</v>
+        <v>15.689320753106029</v>
       </c>
       <c r="BX8" s="106">
         <f>_xlfn.NORM.DIST(10,Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</f>
-        <v>0.45026177516988708</v>
+        <v>0.43669890635404063</v>
       </c>
       <c r="BY8" s="106">
         <f>1-_xlfn.NORM.DIST(50, Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</f>
-        <v>3.0396361765261393E-2</v>
+        <v>8.4204979670932101E-3</v>
       </c>
       <c r="BZ8" s="106">
         <f t="shared" si="7"/>
@@ -9707,19 +10791,19 @@
       </c>
       <c r="CG8" s="3">
         <f>MIN(Table3[[#This Row],[adjusted launch angle]]+Table3[[#This Row],[angle stdev]], 30)</f>
-        <v>30</v>
+        <v>28.189320753106031</v>
       </c>
       <c r="CH8" s="118">
         <f>2*Table3[[#This Row],[+1stdv EV]]*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*60*60</f>
-        <v>3.7574999999999994</v>
+        <v>3.5499844893060266</v>
       </c>
       <c r="CI8" s="156">
         <f>Table3[[#This Row],[+1stdv EV]]^2*2*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*5280-Table3[[#This Row],[+1stdv flight time]]^2*$CE$25</f>
-        <v>234.26760000000002</v>
+        <v>233.11652913466412</v>
       </c>
       <c r="CJ8" s="156">
         <f>Table3[[#This Row],[+1stdev distance]]-Table3[[#This Row],[actual distance]]</f>
-        <v>90.27544870525125</v>
+        <v>89.124377839915354</v>
       </c>
     </row>
     <row r="9" spans="1:119" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -10013,7 +11097,7 @@
       </c>
       <c r="BU9" s="4">
         <f>MAX(0, IF(ISBLANK($BU$28), Table3[[#This Row],[hit quality +1stdv]], $BU$28)-1)</f>
-        <v>0.5</v>
+        <v>0.94077781252657178</v>
       </c>
       <c r="BV9" s="4">
         <f>$BV$25+Table3[[#This Row],[offense]]*$BV$28</f>
@@ -10021,15 +11105,15 @@
       </c>
       <c r="BW9" s="4">
         <f>$BW$25*$BW$28/($BW$28+Table3[[#This Row],[hit quality remainder]])</f>
-        <v>20</v>
+        <v>13.881390889083494</v>
       </c>
       <c r="BX9" s="107">
         <f>_xlfn.NORM.DIST(10,Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</f>
-        <v>0.4012936743170763</v>
+        <v>0.35935086123913501</v>
       </c>
       <c r="BY9" s="107">
         <f>1-_xlfn.NORM.DIST(50, Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</f>
-        <v>4.0059156863817114E-2</v>
+        <v>5.8450897212606323E-3</v>
       </c>
       <c r="BZ9" s="107">
         <f t="shared" si="7"/>
@@ -10061,19 +11145,19 @@
       </c>
       <c r="CG9" s="4">
         <f>MIN(Table3[[#This Row],[adjusted launch angle]]+Table3[[#This Row],[angle stdev]], 30)</f>
-        <v>30</v>
+        <v>28.881390889083494</v>
       </c>
       <c r="CH9" s="119">
         <f>2*Table3[[#This Row],[+1stdv EV]]*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*60*60</f>
-        <v>4.2074999999999996</v>
+        <v>4.0644282997712828</v>
       </c>
       <c r="CI9" s="157">
         <f>Table3[[#This Row],[+1stdv EV]]^2*2*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*5280-Table3[[#This Row],[+1stdv flight time]]^2*$CE$25</f>
-        <v>293.73959999999988</v>
+        <v>293.05536237826169</v>
       </c>
       <c r="CJ9" s="157">
         <f>Table3[[#This Row],[+1stdev distance]]-Table3[[#This Row],[actual distance]]</f>
-        <v>87.330863038008516</v>
+        <v>86.646625416270325</v>
       </c>
     </row>
     <row r="10" spans="1:119" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -10367,7 +11451,7 @@
       </c>
       <c r="BU10" s="3">
         <f>MAX(0, IF(ISBLANK($BU$28), Table3[[#This Row],[hit quality +1stdv]], $BU$28)-1)</f>
-        <v>0.5</v>
+        <v>1.2728137779146098</v>
       </c>
       <c r="BV10" s="3">
         <f>$BV$25+Table3[[#This Row],[offense]]*$BV$28</f>
@@ -10375,15 +11459,15 @@
       </c>
       <c r="BW10" s="3">
         <f>$BW$25*$BW$28/($BW$28+Table3[[#This Row],[hit quality remainder]])</f>
-        <v>20</v>
+        <v>11.281500769655757</v>
       </c>
       <c r="BX10" s="106">
         <f>_xlfn.NORM.DIST(10,Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</f>
-        <v>0.30853753872598688</v>
+        <v>0.18769915416172575</v>
       </c>
       <c r="BY10" s="106">
         <f>1-_xlfn.NORM.DIST(50, Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</f>
-        <v>6.6807201268858085E-2</v>
+        <v>3.9160823204601458E-3</v>
       </c>
       <c r="BZ10" s="106">
         <f t="shared" si="7"/>
@@ -10721,7 +11805,7 @@
       </c>
       <c r="BU11" s="13">
         <f>MAX(0, IF(ISBLANK($BU$28), Table3[[#This Row],[hit quality +1stdv]], $BU$28)-1)</f>
-        <v>0.5</v>
+        <v>0.51981588845550086</v>
       </c>
       <c r="BV11" s="13">
         <f>$BV$25+Table3[[#This Row],[offense]]*$BV$28</f>
@@ -10729,15 +11813,15 @@
       </c>
       <c r="BW11" s="13">
         <f>$BW$25*$BW$28/($BW$28+Table3[[#This Row],[hit quality remainder]])</f>
-        <v>20</v>
+        <v>19.611383021586146</v>
       </c>
       <c r="BX11" s="108">
         <f>_xlfn.NORM.DIST(10,Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</f>
-        <v>0.49002748180476197</v>
+        <v>0.4898299098943425</v>
       </c>
       <c r="BY11" s="108">
         <f>1-_xlfn.NORM.DIST(50, Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</f>
-        <v>2.4134074004724781E-2</v>
+        <v>2.1997608469818908E-2</v>
       </c>
       <c r="BZ11" s="108">
         <f t="shared" si="7"/>
@@ -11075,7 +12159,7 @@
       </c>
       <c r="BU12" s="26">
         <f>MAX(0, IF(ISBLANK($BU$28), Table3[[#This Row],[hit quality +1stdv]], $BU$28)-1)</f>
-        <v>0.5</v>
+        <v>0.65128513288121859</v>
       </c>
       <c r="BV12" s="26">
         <f>$BV$25+Table3[[#This Row],[offense]]*$BV$28</f>
@@ -11083,15 +12167,15 @@
       </c>
       <c r="BW12" s="26">
         <f>$BW$25*$BW$28/($BW$28+Table3[[#This Row],[hit quality remainder]])</f>
-        <v>20</v>
+        <v>17.371891140423038</v>
       </c>
       <c r="BX12" s="109">
         <f>_xlfn.NORM.DIST(10,Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</f>
-        <v>0.45026177516988708</v>
+        <v>0.44278551618726236</v>
       </c>
       <c r="BY12" s="109">
         <f>1-_xlfn.NORM.DIST(50, Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</f>
-        <v>3.0396361765261393E-2</v>
+        <v>1.5438291680317628E-2</v>
       </c>
       <c r="BZ12" s="109">
         <f t="shared" si="7"/>
@@ -11123,19 +12207,19 @@
       </c>
       <c r="CG12" s="26">
         <f>MIN(Table3[[#This Row],[adjusted launch angle]]+Table3[[#This Row],[angle stdev]], 30)</f>
-        <v>30</v>
+        <v>29.871891140423038</v>
       </c>
       <c r="CH12" s="121">
         <f>2*Table3[[#This Row],[+1stdv EV]]*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*60*60</f>
-        <v>3.9374999999999991</v>
+        <v>3.9222412979718122</v>
       </c>
       <c r="CI12" s="159">
         <f>Table3[[#This Row],[+1stdv EV]]^2*2*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*5280-Table3[[#This Row],[+1stdv flight time]]^2*$CE$25</f>
-        <v>257.25000000000006</v>
+        <v>257.21067111413299</v>
       </c>
       <c r="CJ12" s="159">
         <f>Table3[[#This Row],[+1stdev distance]]-Table3[[#This Row],[actual distance]]</f>
-        <v>113.25784870525129</v>
+        <v>113.21851981938423</v>
       </c>
     </row>
     <row r="13" spans="1:119" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -11429,7 +12513,7 @@
       </c>
       <c r="BU13" s="13">
         <f>MAX(0, IF(ISBLANK($BU$28), Table3[[#This Row],[hit quality +1stdv]], $BU$28)-1)</f>
-        <v>0.5</v>
+        <v>0.81551632831883869</v>
       </c>
       <c r="BV13" s="13">
         <f>$BV$25+Table3[[#This Row],[offense]]*$BV$28</f>
@@ -11437,15 +12521,15 @@
       </c>
       <c r="BW13" s="13">
         <f>$BW$25*$BW$28/($BW$28+Table3[[#This Row],[hit quality remainder]])</f>
-        <v>20</v>
+        <v>15.203156030422639</v>
       </c>
       <c r="BX13" s="108">
         <f>_xlfn.NORM.DIST(10,Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</f>
-        <v>0.4012936743170763</v>
+        <v>0.37112354285281923</v>
       </c>
       <c r="BY13" s="108">
         <f>1-_xlfn.NORM.DIST(50, Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</f>
-        <v>4.0059156863817114E-2</v>
+        <v>1.066325651585287E-2</v>
       </c>
       <c r="BZ13" s="108">
         <f t="shared" si="7"/>
@@ -11783,7 +12867,7 @@
       </c>
       <c r="BU14" s="5">
         <f>MAX(0, IF(ISBLANK($BU$28), Table3[[#This Row],[hit quality +1stdv]], $BU$28)-1)</f>
-        <v>0.5</v>
+        <v>1.1436529529332398</v>
       </c>
       <c r="BV14" s="5">
         <f>$BV$25+Table3[[#This Row],[offense]]*$BV$28</f>
@@ -11791,15 +12875,15 @@
       </c>
       <c r="BW14" s="5">
         <f>$BW$25*$BW$28/($BW$28+Table3[[#This Row],[hit quality remainder]])</f>
-        <v>20</v>
+        <v>12.16801878055114</v>
       </c>
       <c r="BX14" s="110">
         <f>_xlfn.NORM.DIST(10,Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</f>
-        <v>0.30853753872598688</v>
+        <v>0.20558783134270991</v>
       </c>
       <c r="BY14" s="110">
         <f>1-_xlfn.NORM.DIST(50, Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</f>
-        <v>6.6807201268858085E-2</v>
+        <v>6.8415015827276715E-3</v>
       </c>
       <c r="BZ14" s="110">
         <f t="shared" si="7"/>
@@ -12137,7 +13221,7 @@
       </c>
       <c r="BU15" s="17">
         <f>MAX(0, IF(ISBLANK($BU$28), Table3[[#This Row],[hit quality +1stdv]], $BU$28)-1)</f>
-        <v>0.5</v>
+        <v>0.35774740885014045</v>
       </c>
       <c r="BV15" s="17">
         <f>$BV$25+Table3[[#This Row],[offense]]*$BV$28</f>
@@ -12145,15 +13229,15 @@
       </c>
       <c r="BW15" s="17">
         <f>$BW$25*$BW$28/($BW$28+Table3[[#This Row],[hit quality remainder]])</f>
-        <v>20</v>
+        <v>23.316887691693697</v>
       </c>
       <c r="BX15" s="111">
         <f>_xlfn.NORM.DIST(10,Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</f>
-        <v>0.49002748180476197</v>
+        <v>0.49144586289978898</v>
       </c>
       <c r="BY15" s="111">
         <f>1-_xlfn.NORM.DIST(50, Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</f>
-        <v>2.4134074004724781E-2</v>
+        <v>4.512778355562419E-2</v>
       </c>
       <c r="BZ15" s="111">
         <f t="shared" si="7"/>
@@ -12491,7 +13575,7 @@
       </c>
       <c r="BU16" s="6">
         <f>MAX(0, IF(ISBLANK($BU$28), Table3[[#This Row],[hit quality +1stdv]], $BU$28)-1)</f>
-        <v>0.5</v>
+        <v>0.48838349853526819</v>
       </c>
       <c r="BV16" s="6">
         <f>$BV$25+Table3[[#This Row],[offense]]*$BV$28</f>
@@ -12499,15 +13583,15 @@
       </c>
       <c r="BW16" s="6">
         <f>$BW$25*$BW$28/($BW$28+Table3[[#This Row],[hit quality remainder]])</f>
-        <v>20</v>
+        <v>20.235060611229283</v>
       </c>
       <c r="BX16" s="112">
         <f>_xlfn.NORM.DIST(10,Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</f>
-        <v>0.45026177516988708</v>
+        <v>0.45083660826844291</v>
       </c>
       <c r="BY16" s="112">
         <f>1-_xlfn.NORM.DIST(50, Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</f>
-        <v>3.0396361765261393E-2</v>
+        <v>3.1925483442733937E-2</v>
       </c>
       <c r="BZ16" s="112">
         <f t="shared" si="7"/>
@@ -12845,7 +13929,7 @@
       </c>
       <c r="BU17" s="23">
         <f>MAX(0, IF(ISBLANK($BU$28), Table3[[#This Row],[hit quality +1stdv]], $BU$28)-1)</f>
-        <v>0.5</v>
+        <v>0.65136813528909987</v>
       </c>
       <c r="BV17" s="23">
         <f>$BV$25+Table3[[#This Row],[offense]]*$BV$28</f>
@@ -12853,15 +13937,15 @@
       </c>
       <c r="BW17" s="23">
         <f>$BW$25*$BW$28/($BW$28+Table3[[#This Row],[hit quality remainder]])</f>
-        <v>20</v>
+        <v>17.370638796581034</v>
       </c>
       <c r="BX17" s="113">
         <f>_xlfn.NORM.DIST(10,Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</f>
-        <v>0.4012936743170763</v>
+        <v>0.3867338300086321</v>
       </c>
       <c r="BY17" s="113">
         <f>1-_xlfn.NORM.DIST(50, Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</f>
-        <v>4.0059156863817114E-2</v>
+        <v>2.1957866000810844E-2</v>
       </c>
       <c r="BZ17" s="113">
         <f t="shared" si="7"/>
@@ -13199,7 +14283,7 @@
       </c>
       <c r="BU18" s="6">
         <f>MAX(0, IF(ISBLANK($BU$28), Table3[[#This Row],[hit quality +1stdv]], $BU$28)-1)</f>
-        <v>0.5</v>
+        <v>0.97642865745633256</v>
       </c>
       <c r="BV18" s="6">
         <f>$BV$25+Table3[[#This Row],[offense]]*$BV$28</f>
@@ -13207,15 +14291,15 @@
       </c>
       <c r="BW18" s="6">
         <f>$BW$25*$BW$28/($BW$28+Table3[[#This Row],[hit quality remainder]])</f>
-        <v>20</v>
+        <v>13.546201436144589</v>
       </c>
       <c r="BX18" s="112">
         <f>_xlfn.NORM.DIST(10,Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</f>
-        <v>0.30853753872598688</v>
+        <v>0.23019210849816696</v>
       </c>
       <c r="BY18" s="112">
         <f>1-_xlfn.NORM.DIST(50, Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</f>
-        <v>6.6807201268858085E-2</v>
+        <v>1.3392289526165668E-2</v>
       </c>
       <c r="BZ18" s="112">
         <f t="shared" si="7"/>
@@ -13553,7 +14637,7 @@
       </c>
       <c r="BU19" s="15">
         <f>MAX(0, IF(ISBLANK($BU$28), Table3[[#This Row],[hit quality +1stdv]], $BU$28)-1)</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="BV19" s="15">
         <f>$BV$25+Table3[[#This Row],[offense]]*$BV$28</f>
@@ -13561,15 +14645,15 @@
       </c>
       <c r="BW19" s="15">
         <f>$BW$25*$BW$28/($BW$28+Table3[[#This Row],[hit quality remainder]])</f>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="BX19" s="114">
         <f>_xlfn.NORM.DIST(10,Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</f>
-        <v>0.49002748180476197</v>
+        <v>0.49501335135596203</v>
       </c>
       <c r="BY19" s="114">
         <f>1-_xlfn.NORM.DIST(50, Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</f>
-        <v>2.4134074004724781E-2</v>
+        <v>0.16169879145728561</v>
       </c>
       <c r="BZ19" s="114">
         <f t="shared" si="7"/>
@@ -13907,7 +14991,7 @@
       </c>
       <c r="BU20" s="11">
         <f>MAX(0, IF(ISBLANK($BU$28), Table3[[#This Row],[hit quality +1stdv]], $BU$28)-1)</f>
-        <v>0.5</v>
+        <v>0.11097554731590242</v>
       </c>
       <c r="BV20" s="11">
         <f>$BV$25+Table3[[#This Row],[offense]]*$BV$28</f>
@@ -13915,15 +14999,15 @@
       </c>
       <c r="BW20" s="11">
         <f>$BW$25*$BW$28/($BW$28+Table3[[#This Row],[hit quality remainder]])</f>
-        <v>20</v>
+        <v>32.73453428351214</v>
       </c>
       <c r="BX20" s="115">
         <f>_xlfn.NORM.DIST(10,Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</f>
-        <v>0.45026177516988708</v>
+        <v>0.46956159515502022</v>
       </c>
       <c r="BY20" s="115">
         <f>1-_xlfn.NORM.DIST(50, Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</f>
-        <v>3.0396361765261393E-2</v>
+        <v>0.12598466394930252</v>
       </c>
       <c r="BZ20" s="115">
         <f t="shared" si="7"/>
@@ -14261,7 +15345,7 @@
       </c>
       <c r="BU21" s="15">
         <f>MAX(0, IF(ISBLANK($BU$28), Table3[[#This Row],[hit quality +1stdv]], $BU$28)-1)</f>
-        <v>0.5</v>
+        <v>0.27465629389675161</v>
       </c>
       <c r="BV21" s="15">
         <f>$BV$25+Table3[[#This Row],[offense]]*$BV$28</f>
@@ -14269,15 +15353,15 @@
       </c>
       <c r="BW21" s="15">
         <f>$BW$25*$BW$28/($BW$28+Table3[[#This Row],[hit quality remainder]])</f>
-        <v>20</v>
+        <v>25.817901639182519</v>
       </c>
       <c r="BX21" s="114">
         <f>_xlfn.NORM.DIST(10,Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</f>
-        <v>0.4012936743170763</v>
+        <v>0.42321946220952417</v>
       </c>
       <c r="BY21" s="114">
         <f>1-_xlfn.NORM.DIST(50, Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</f>
-        <v>4.0059156863817114E-2</v>
+        <v>8.7605514015848596E-2</v>
       </c>
       <c r="BZ21" s="114">
         <f t="shared" si="7"/>
@@ -14615,7 +15699,7 @@
       </c>
       <c r="BU22" s="20">
         <f>MAX(0, IF(ISBLANK($BU$28), Table3[[#This Row],[hit quality +1stdv]], $BU$28)-1)</f>
-        <v>0.5</v>
+        <v>0.60188972504376359</v>
       </c>
       <c r="BV22" s="20">
         <f>$BV$25+Table3[[#This Row],[offense]]*$BV$28</f>
@@ -14623,15 +15707,15 @@
       </c>
       <c r="BW22" s="20">
         <f>$BW$25*$BW$28/($BW$28+Table3[[#This Row],[hit quality remainder]])</f>
-        <v>20</v>
+        <v>18.150636624917855</v>
       </c>
       <c r="BX22" s="116">
         <f>_xlfn.NORM.DIST(10,Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</f>
-        <v>0.30853753872598688</v>
+        <v>0.29083573622253345</v>
       </c>
       <c r="BY22" s="116">
         <f>1-_xlfn.NORM.DIST(50, Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</f>
-        <v>6.6807201268858085E-2</v>
+        <v>4.9182266373134054E-2</v>
       </c>
       <c r="BZ22" s="116">
         <f t="shared" si="7"/>
@@ -15034,9 +16118,6 @@
       <c r="BB28" t="s">
         <v>136</v>
       </c>
-      <c r="BU28">
-        <v>1.5</v>
-      </c>
       <c r="BV28">
         <v>5</v>
       </c>
@@ -15314,7 +16395,7 @@
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
   <conditionalFormatting sqref="O7:O22">
-    <cfRule type="cellIs" dxfId="81" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15328,6 +16409,108 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF285913-BB23-45EF-B183-28069296EF50}">
+  <dimension ref="J12:L18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X6" sqref="X6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="9.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="12" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>112</v>
+      </c>
+      <c r="K12" t="s">
+        <v>302</v>
+      </c>
+      <c r="L12" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="13" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>0.5</v>
+      </c>
+      <c r="L13">
+        <f>POWER(Table1[[#This Row],[quality]]-0.8, 1/4)</f>
+        <v>0.66874030497642201</v>
+      </c>
+    </row>
+    <row r="14" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <v>1.5</v>
+      </c>
+      <c r="K14">
+        <v>0.75</v>
+      </c>
+      <c r="L14">
+        <f>POWER(Table1[[#This Row],[quality]]-0.8, 1/4)</f>
+        <v>0.91469121922869445</v>
+      </c>
+    </row>
+    <row r="15" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <v>2</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <f>POWER(Table1[[#This Row],[quality]]-0.8, 1/4)</f>
+        <v>1.0466351393921056</v>
+      </c>
+    </row>
+    <row r="16" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <v>3</v>
+      </c>
+      <c r="K16">
+        <v>1.4</v>
+      </c>
+      <c r="L16">
+        <f>POWER(Table1[[#This Row],[quality]]-0.8, 1/4)</f>
+        <v>1.2178832856309068</v>
+      </c>
+    </row>
+    <row r="17" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <v>5</v>
+      </c>
+      <c r="K17">
+        <v>2</v>
+      </c>
+      <c r="L17">
+        <f>POWER(Table1[[#This Row],[quality]]-0.8, 1/4)</f>
+        <v>1.4315691227432645</v>
+      </c>
+    </row>
+    <row r="18" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J18">
+        <v>3.35</v>
+      </c>
+      <c r="L18" s="73">
+        <f>POWER(Table1[[#This Row],[quality]]-0.8, 1/4)</f>
+        <v>1.2636739857523107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C2:S9"/>
   <sheetViews>
@@ -15566,7 +16749,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AB18"/>
   <sheetViews>
@@ -17017,7 +18200,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
@@ -17313,7 +18496,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E19"/>
   <sheetViews>

</xml_diff>

<commit_message>
A ton of refactoring work to add and use Updates for single lines of action. Beginning work on fielding.
</commit_message>
<xml_diff>
--- a/plans/baseball stats.xlsx
+++ b/plans/baseball stats.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcgiffenk\Desktop\newpy\xtreemblaseball99\plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495A7E3F-942D-439D-903D-CAF26CA8A0B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778496F6-5405-4E3A-8828-1D89E1F316CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="iterative" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="7" r:id="rId2"/>
-    <sheet name="gauss cruncher" sheetId="5" r:id="rId3"/>
-    <sheet name="run speed" sheetId="3" r:id="rId4"/>
-    <sheet name="pitch outcomes" sheetId="1" r:id="rId5"/>
-    <sheet name="hit quality truth table" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="8" r:id="rId3"/>
+    <sheet name="gauss cruncher" sheetId="5" r:id="rId4"/>
+    <sheet name="run speed" sheetId="3" r:id="rId5"/>
+    <sheet name="pitch outcomes" sheetId="1" r:id="rId6"/>
+    <sheet name="hit quality truth table" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="basis">#REF!</definedName>
@@ -32,6 +33,9 @@
     <definedName name="pitchmod">iterative!$AN$25</definedName>
     <definedName name="pitchstdv">iterative!$AN$27</definedName>
     <definedName name="stratfactor">iterative!$E$26</definedName>
+    <definedName name="throwingfactor">Sheet2!$F$1</definedName>
+    <definedName name="throwingmean">Sheet2!$B$1</definedName>
+    <definedName name="throwingstdv">Sheet2!$D$1</definedName>
     <definedName name="total">#REF!</definedName>
     <definedName name="values">#REF!</definedName>
     <definedName name="weightedvalues">#REF!</definedName>
@@ -409,6 +413,19 @@
         </r>
       </text>
     </comment>
+    <comment ref="CL24" authorId="0" shapeId="0" xr:uid="{64760257-3A41-434E-A0A3-17AAC2BB181B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>worst case infielder distance is probably 45 feet; worst case outfielder distance is probably like 120 feet</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="AH26" authorId="0" shapeId="0" xr:uid="{246EB7CA-2F63-49E7-863F-0B68F2A116B9}">
       <text>
         <r>
@@ -541,7 +558,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="309">
   <si>
     <t>Ball</t>
   </si>
@@ -1171,9 +1188,6 @@
   </si>
   <si>
     <t>Column95</t>
-  </si>
-  <si>
-    <t>Column96</t>
   </si>
   <si>
     <t>Column97</t>
@@ -1454,6 +1468,24 @@
   </si>
   <si>
     <t>form</t>
+  </si>
+  <si>
+    <t>grabbiness</t>
+  </si>
+  <si>
+    <t>throwing</t>
+  </si>
+  <si>
+    <t>factor:</t>
+  </si>
+  <si>
+    <t>catching</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>ball speed:</t>
   </si>
 </sst>
 </file>
@@ -2110,6 +2142,16 @@
   </cellStyles>
   <dxfs count="83">
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -2451,16 +2493,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -8989,181 +9021,181 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A6:DO22" totalsRowShown="0" headerRowDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A6:DO22" totalsRowShown="0" headerRowDxfId="82">
   <autoFilter ref="A6:DO22" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="119">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Rep #">
       <calculatedColumnFormula>ROW()-ROW(home)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="offense" dataDxfId="80">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="offense" dataDxfId="81">
       <calculatedColumnFormula>INDEX(oratings, 1, 1+MOD(Table3[[#This Row],[Rep '#]]-1, COUNT(oratings)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="defense" dataDxfId="79">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="defense" dataDxfId="80">
       <calculatedColumnFormula>INDEX(dratings, 1, MOD(FLOOR( (Table3[[#This Row],[Rep '#]]-1) / COUNT(oratings), 1), COUNT(dratings))+1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="base leadoff" dataDxfId="78">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="base leadoff" dataDxfId="79">
       <calculatedColumnFormula>Table3[[#This Row],[offense]]*$D$26+0.05</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="leadoff modifier" dataDxfId="77">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="leadoff modifier" dataDxfId="78">
       <calculatedColumnFormula>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*$E$26</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="total leadoff (ft)" dataDxfId="76">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="total leadoff (ft)" dataDxfId="77">
       <calculatedColumnFormula>MAX(Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90, 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="pickoff manuver (s)" dataDxfId="75">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="pickoff manuver (s)" dataDxfId="76">
       <calculatedColumnFormula>1.1 - Table3[[#This Row],[defense]]*0.1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="throw speed (s/ft)" dataDxfId="74">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="throw speed (s/ft)" dataDxfId="75">
       <calculatedColumnFormula xml:space="preserve"> 0.01 - 0.0025 *  Table3[[#This Row],[defense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="throw speed (mph)" dataDxfId="73">
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="throw speed (mph)" dataDxfId="74">
       <calculatedColumnFormula>1 / Table3[[#This Row],[throw speed (s/ft)]] * ((60 * 60)/5280)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="pickoff time" dataDxfId="72">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="pickoff time" dataDxfId="73">
       <calculatedColumnFormula>Table3[[#This Row],[pickoff manuver (s)]]+60*Table3[[#This Row],[throw speed (s/ft)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="runner reaction" dataDxfId="71">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="runner reaction" dataDxfId="72">
       <calculatedColumnFormula>$K$28-$K$26*Table3[[#This Row],[offense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="runner speed (s/ft)" dataDxfId="70">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="runner speed (s/ft)" dataDxfId="71">
       <calculatedColumnFormula>0.05 - Table3[[#This Row],[offense]]*$L$26</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="runner speed (mph)" dataDxfId="69">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="runner speed (mph)" dataDxfId="70">
       <calculatedColumnFormula>1 / Table3[[#This Row],[runner speed (s/ft)]] * ((60 * 60)/5280)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="pickoff evade time" dataDxfId="68">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="pickoff evade time" dataDxfId="69">
       <calculatedColumnFormula>Table3[[#This Row],[runner reaction]]+Table3[[#This Row],[runner speed (s/ft)]]*Table3[[#This Row],[total leadoff (ft)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="pickoff probability" dataDxfId="67" dataCellStyle="Percent">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="pickoff probability" dataDxfId="68" dataCellStyle="Percent">
       <calculatedColumnFormula>1 - _xlfn.NORM.DIST(Table3[[#This Row],[pickoff time]], Table3[[#This Row],[pickoff evade time]], $O$4, TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Fielding Odds" dataDxfId="66" dataCellStyle="Percent">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Fielding Odds" dataDxfId="67" dataCellStyle="Percent">
       <calculatedColumnFormula>_xlfn.NORM.DIST(Table3[[#This Row],[defense]], $P$26, $P$27, TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="pickoff worth it?" dataDxfId="65">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="pickoff worth it?" dataDxfId="66">
       <calculatedColumnFormula>Table3[[#This Row],[pickoff probability]] &gt; 1-Table3[[#This Row],[Fielding Odds]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Error %" dataDxfId="64" dataCellStyle="Percent">
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Error %" dataDxfId="65" dataCellStyle="Percent">
       <calculatedColumnFormula>1-Table3[[#This Row],[Fielding Odds]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Blatant steal time" dataDxfId="63">
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Blatant steal time" dataDxfId="64">
       <calculatedColumnFormula>(90-Table3[[#This Row],[total leadoff (ft)]])*Table3[[#This Row],[runner speed (s/ft)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Response speed" dataDxfId="62">
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Response speed" dataDxfId="63">
       <calculatedColumnFormula>$T$26*(2-Table3[[#This Row],[defense]]) + Table3[[#This Row],[pickoff time]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="blatant steal probability" dataDxfId="61" dataCellStyle="Percent">
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="blatant steal probability" dataDxfId="62" dataCellStyle="Percent">
       <calculatedColumnFormula>_xlfn.NORM.DIST(Table3[[#This Row],[Response speed]], Table3[[#This Row],[Blatant steal time]], $U$4, TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="defense fear" dataDxfId="60">
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="defense fear" dataDxfId="61">
       <calculatedColumnFormula>Table3[[#This Row],[defense]]+Table3[[#This Row],[defense]]*Table3[[#This Row],[offense]]*$E$26</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="ball factor" dataDxfId="59">
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="ball factor" dataDxfId="60">
       <calculatedColumnFormula>(1-$W$32)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="desperation" dataDxfId="58" dataCellStyle="Percent">
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="desperation" dataDxfId="59" dataCellStyle="Percent">
       <calculatedColumnFormula>Table3[[#This Row],[ball factor]]/$X$32*(1-$X$34)+$X$34</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="player control" dataDxfId="57">
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="player control" dataDxfId="58">
       <calculatedColumnFormula>Table3[[#This Row],[offense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="ideal steer" dataDxfId="56">
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="ideal steer" dataDxfId="57">
       <calculatedColumnFormula>$AA$33</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="scaled control" dataDxfId="55">
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="scaled control" dataDxfId="56">
       <calculatedColumnFormula>IF(Table3[[#This Row],[player control]]&gt;1,Table3[[#This Row],[player control]]*$AA$41+$AA$40,Table3[[#This Row],[player control]]*$AA$39+$AA$38)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="unmod foul percent 3rd" dataDxfId="54" dataCellStyle="Percent">
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="unmod foul percent 3rd" dataDxfId="55" dataCellStyle="Percent">
       <calculatedColumnFormula>_xlfn.NORM.DIST(-1,Table3[[#This Row],[ideal steer]],($AB$25-Table3[[#This Row],[scaled control]])*$AB$27,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="unmod foul percent 1st" dataDxfId="53" dataCellStyle="Percent">
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="unmod foul percent 1st" dataDxfId="54" dataCellStyle="Percent">
       <calculatedColumnFormula>1-_xlfn.NORM.DIST(1,Table3[[#This Row],[ideal steer]],($AB$25-Table3[[#This Row],[scaled control]])*$AB$27,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="total unmod foul percent" dataDxfId="52" dataCellStyle="Percent">
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="total unmod foul percent" dataDxfId="53" dataCellStyle="Percent">
       <calculatedColumnFormula>1-(1-Table3[[#This Row],[unmod foul percent 3rd]])*(1-Table3[[#This Row],[unmod foul percent 1st]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="unmod dead center foul%" dataDxfId="51" dataCellStyle="Percent">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="unmod dead center foul%" dataDxfId="52" dataCellStyle="Percent">
       <calculatedColumnFormula>1-((1-_xlfn.NORM.DIST(-1,0,($AB$25-Table3[[#This Row],[scaled control]])*$AB$27,TRUE))*_xlfn.NORM.DIST(1,0,($AB$25-Table3[[#This Row],[scaled control]])*$AB$27,TRUE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="count" dataDxfId="50">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="count" dataDxfId="51">
       <calculatedColumnFormula>$AF$34*$AF$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="hitter discipline bias" dataDxfId="49">
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="hitter discipline bias" dataDxfId="50">
       <calculatedColumnFormula>$AG$25*($AG$34*Table3[[#This Row],[offense]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="bases loaded" dataDxfId="48">
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="bases loaded" dataDxfId="49">
       <calculatedColumnFormula>$AH$25*$AH$34</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="number of outs" dataDxfId="47">
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="number of outs" dataDxfId="48">
       <calculatedColumnFormula>$AI$34*$AI$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="current hitter vs next hitter" dataDxfId="46">
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="current hitter vs next hitter" dataDxfId="47">
       <calculatedColumnFormula>$AJ$25*(Table3[[#This Row],[offense]]-$AJ$27)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="calling modifier" dataDxfId="45">
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="calling modifier" dataDxfId="46">
       <calculatedColumnFormula array="1">SUM(Table3[[#This Row],[count]:[current hitter vs next hitter]]*MIN(1, Table3[[#This Row],[defense]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="sigmoid strike percent" dataDxfId="44" dataCellStyle="Percent">
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="sigmoid strike percent" dataDxfId="45" dataCellStyle="Percent">
       <calculatedColumnFormula>$AL$25-(Table3[[#This Row],[calling modifier]]/(ABS(Table3[[#This Row],[calling modifier]])+$AL$29)*$AL$27)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="tanh strike percent" dataDxfId="43" dataCellStyle="Percent">
+    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="tanh strike percent" dataDxfId="44" dataCellStyle="Percent">
       <calculatedColumnFormula>$AL$25-$AL$27*TANH(Table3[[#This Row],[calling modifier]]/$AM$29)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="called position" dataDxfId="42" dataCellStyle="Percent">
+    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="called position" dataDxfId="43" dataCellStyle="Percent">
       <calculatedColumnFormula>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-Table3[[#This Row],[defense]])))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="called pos 0.2 pitch" dataDxfId="41">
+    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="called pos 0.2 pitch" dataDxfId="42">
       <calculatedColumnFormula>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-0.2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="called pos 2 pitch" dataDxfId="40">
+    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="called pos 2 pitch" dataDxfId="41">
       <calculatedColumnFormula>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="location -1  stdv" dataDxfId="39">
+    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="location -1  stdv" dataDxfId="40">
       <calculatedColumnFormula>Table3[[#This Row],[called position]]-pitchmod*(pitchstdv-Table3[[#This Row],[defense]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="location +1 stdv" dataDxfId="38">
+    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="location +1 stdv" dataDxfId="39">
       <calculatedColumnFormula>ABS(Table3[[#This Row],[called position]]+pitchmod*(pitchstdv-Table3[[#This Row],[defense]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="min dist to sz 1stdv" dataDxfId="37">
+    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="min dist to sz 1stdv" dataDxfId="38">
       <calculatedColumnFormula>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;1, Table3[[#This Row],[location +1 stdv]]&gt;1),0, MIN(Table3[[#This Row],[location -1  stdv]]+1, 1-Table3[[#This Row],[location +1 stdv]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="max dist to sz 1stdv" dataDxfId="36">
+    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="max dist to sz 1stdv" dataDxfId="37">
       <calculatedColumnFormula>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;0, Table3[[#This Row],[location +1 stdv]]&gt;0),1, MAX(1-ABS(Table3[[#This Row],[location -1  stdv]]), Table3[[#This Row],[location +1 stdv]]-1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="ave obscurity" dataDxfId="35">
+    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="ave obscurity" dataDxfId="36">
       <calculatedColumnFormula>$AU$30/(ABS(Table3[[#This Row],[called position]]-1)+$AU$27)+$AU$32*Table3[[#This Row],[defense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="obscurity at _x000a_0.5" dataDxfId="34">
+    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="obscurity at _x000a_0.5" dataDxfId="35">
       <calculatedColumnFormula>$AU$30/(ABS(0.5-1)+$AU$27)+$AU$32*Table3[[#This Row],[defense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="obscurity at  0.9" dataDxfId="33">
+    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="obscurity at  0.9" dataDxfId="34">
       <calculatedColumnFormula>$AU$30/(ABS(0.9-1)+$AU$27)+$AU$32*Table3[[#This Row],[defense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="average difficulty" dataDxfId="32">
+    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="average difficulty" dataDxfId="33">
       <calculatedColumnFormula>Table3[[#This Row],[defense]]*$AX$30+MAX(0, Table3[[#This Row],[called position]]-$AX$27)^$AX$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" name="+1stdv difficulty" dataDxfId="31">
+    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" name="+1stdv difficulty" dataDxfId="32">
       <calculatedColumnFormula>Table3[[#This Row],[defense]]*$AX$30 + MAX(0, Table3[[#This Row],[location +1 stdv]]-$AX$27)^$AX$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0000-000037000000}" name="difficulty at 1" dataDxfId="30">
+    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0000-000037000000}" name="difficulty at 1" dataDxfId="31">
       <calculatedColumnFormula>Table3[[#This Row],[defense]]*$AX$30+MAX(0, 1-$AX$27)^$AX$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="62" xr3:uid="{6513900D-2CAC-4022-A6B3-8A00EE6C566B}" name="reduction" dataDxfId="29">
+    <tableColumn id="62" xr3:uid="{6513900D-2CAC-4022-A6B3-8A00EE6C566B}" name="reduction" dataDxfId="30">
       <calculatedColumnFormula>MAX(0, 0.1*(1-Table3[[#This Row],[defense]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="63" xr3:uid="{12464915-1D8C-4EB5-9BBD-0FF526658E5B}" name="Location" dataDxfId="28">
+    <tableColumn id="63" xr3:uid="{12464915-1D8C-4EB5-9BBD-0FF526658E5B}" name="Location" dataDxfId="29">
       <calculatedColumnFormula>$BB$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="64" xr3:uid="{5F0F19BE-6D04-4E9E-81B2-B324AB353F5C}" name="obscurity" dataDxfId="27">
+    <tableColumn id="64" xr3:uid="{5F0F19BE-6D04-4E9E-81B2-B324AB353F5C}" name="obscurity" dataDxfId="28">
       <calculatedColumnFormula>$AU$30/(ABS(Table3[[#This Row],[Location]]-1)+$AU$27)+$AU$32*Table3[[#This Row],[defense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="65" xr3:uid="{EA3D32E7-A2E2-482C-B6E9-2E17651C5F77}" name="Strike?" dataDxfId="26">
+    <tableColumn id="65" xr3:uid="{EA3D32E7-A2E2-482C-B6E9-2E17651C5F77}" name="Strike?" dataDxfId="27">
       <calculatedColumnFormula>Table3[[#This Row],[Location]]&lt;= (1+MAX(0, (Table3[[#This Row],[defense]]-1)*0.1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="66" xr3:uid="{0C7E9B06-240B-481E-B495-54026E2F00AA}" name="discipline modifier" dataDxfId="25">
+    <tableColumn id="66" xr3:uid="{0C7E9B06-240B-481E-B495-54026E2F00AA}" name="discipline modifier" dataDxfId="26">
       <calculatedColumnFormula>1/(1+Table3[[#This Row],[offense]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="67" xr3:uid="{D3B0837D-02D4-4F62-A2E2-876739E497B0}" name="effective obscurity" dataDxfId="24">
+    <tableColumn id="67" xr3:uid="{D3B0837D-02D4-4F62-A2E2-876739E497B0}" name="effective obscurity" dataDxfId="25">
       <calculatedColumnFormula>Table3[[#This Row],[obscurity]]*Table3[[#This Row],[discipline modifier]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="69" xr3:uid="{39822A5F-1791-48DC-BA9F-A066931C0292}" name="odds of read" dataCellStyle="Percent">
@@ -9178,43 +9210,43 @@
     <tableColumn id="72" xr3:uid="{3E21C76F-F55B-4E49-9BE2-FEE046008C15}" name="adjusted swing %" dataCellStyle="Percent">
       <calculatedColumnFormula>Table3[[#This Row],[desperation echo]]*Table3[[#This Row],[unadjusted swing %]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="130" xr3:uid="{827C9303-3867-43F7-A79B-BC2EAB3F896D}" name="pitch carry forward obsc" dataDxfId="23">
+    <tableColumn id="130" xr3:uid="{827C9303-3867-43F7-A79B-BC2EAB3F896D}" name="pitch carry forward obsc" dataDxfId="24">
       <calculatedColumnFormula>Table3[[#This Row],[ave obscurity]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="131" xr3:uid="{F26B1E2C-89D5-4F6D-877A-1BEA7F7DF5A9}" name="CF odds of read" dataCellStyle="Percent">
       <calculatedColumnFormula>1/(1+Table3[[#This Row],[ave obscurity]]*Table3[[#This Row],[discipline modifier]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="73" xr3:uid="{77BBE784-030D-4E46-9A29-8783B89762BC}" name="contact echo" dataDxfId="22">
+    <tableColumn id="73" xr3:uid="{77BBE784-030D-4E46-9A29-8783B89762BC}" name="contact echo" dataDxfId="23">
       <calculatedColumnFormula>Table3[[#This Row],[offense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="75" xr3:uid="{074A9F48-3941-4E36-90C2-7710217D32C8}" name="pitch carry forward diff" dataDxfId="21">
+    <tableColumn id="75" xr3:uid="{074A9F48-3941-4E36-90C2-7710217D32C8}" name="pitch carry forward diff" dataDxfId="22">
       <calculatedColumnFormula>Table3[[#This Row],[average difficulty]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="76" xr3:uid="{628DDA60-D380-4EE8-AA7D-7EF6C4AAD8A5}" name="CF contact readiness" dataDxfId="20">
+    <tableColumn id="76" xr3:uid="{628DDA60-D380-4EE8-AA7D-7EF6C4AAD8A5}" name="CF contact readiness" dataDxfId="21">
       <calculatedColumnFormula>Table3[[#This Row],[contact echo]]-Table3[[#This Row],[pitch carry forward diff]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="77" xr3:uid="{DBF18AD6-8593-42C7-9058-D19737088E6D}" name="foul %" dataDxfId="19" dataCellStyle="Percent">
+    <tableColumn id="77" xr3:uid="{DBF18AD6-8593-42C7-9058-D19737088E6D}" name="foul %" dataDxfId="20" dataCellStyle="Percent">
       <calculatedColumnFormula>1-_xlfn.NORM.DIST($BP$27,Table3[[#This Row],[CF contact readiness]], $BP$30,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="78" xr3:uid="{6354951A-151E-4E04-9897-9CB39D6098C8}" name="clean %" dataDxfId="18" dataCellStyle="Percent">
+    <tableColumn id="78" xr3:uid="{6354951A-151E-4E04-9897-9CB39D6098C8}" name="clean %" dataDxfId="19" dataCellStyle="Percent">
       <calculatedColumnFormula>1-_xlfn.NORM.DIST($BP$25,Table3[[#This Row],[CF contact readiness]], $BP$30,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="79" xr3:uid="{0070F673-D13C-467D-95AC-FF8413A02F3F}" name="strike swinging %" dataDxfId="17" dataCellStyle="Percent">
+    <tableColumn id="79" xr3:uid="{0070F673-D13C-467D-95AC-FF8413A02F3F}" name="strike swinging %" dataDxfId="18" dataCellStyle="Percent">
       <calculatedColumnFormula>1-Table3[[#This Row],[foul %]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="80" xr3:uid="{9504D0CF-7CD0-472F-8289-44B30538D80C}" name="ave. hit quality" dataDxfId="16">
+    <tableColumn id="80" xr3:uid="{9504D0CF-7CD0-472F-8289-44B30538D80C}" name="ave. hit quality" dataDxfId="17">
       <calculatedColumnFormula>(Table3[[#This Row],[CF contact readiness]]-$BP$27)/$BP$30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="132" xr3:uid="{0BB169E4-F345-4B7D-A549-DE28DC5FB113}" name="hit quality +1stdv" dataDxfId="15">
+    <tableColumn id="132" xr3:uid="{0BB169E4-F345-4B7D-A549-DE28DC5FB113}" name="hit quality +1stdv" dataDxfId="16">
       <calculatedColumnFormula>(Table3[[#This Row],[CF contact readiness]]+$BP$30-$BP$27)/$BP$30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="81" xr3:uid="{37438EAA-344A-486C-A4C2-68EE17D67C60}" name="hit quality remainder" dataDxfId="14">
+    <tableColumn id="81" xr3:uid="{37438EAA-344A-486C-A4C2-68EE17D67C60}" name="hit quality remainder" dataDxfId="15">
       <calculatedColumnFormula>MAX(0, IF(ISBLANK($BU$28), Table3[[#This Row],[hit quality +1stdv]], $BU$28)-1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="82" xr3:uid="{CBA11BEE-0412-44C3-979C-1888629B3C7A}" name="adjusted launch angle" dataDxfId="13">
+    <tableColumn id="82" xr3:uid="{CBA11BEE-0412-44C3-979C-1888629B3C7A}" name="adjusted launch angle" dataDxfId="14">
       <calculatedColumnFormula>$BV$25+Table3[[#This Row],[offense]]*$BV$28</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="83" xr3:uid="{8DC0E209-2987-40FE-9521-B3339A7D8E1F}" name="angle stdev" dataDxfId="12">
+    <tableColumn id="83" xr3:uid="{8DC0E209-2987-40FE-9521-B3339A7D8E1F}" name="angle stdev" dataDxfId="13">
       <calculatedColumnFormula>$BW$25*$BW$28/($BW$28+Table3[[#This Row],[hit quality remainder]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="84" xr3:uid="{F8EB7F4C-5D31-472E-A363-210E62A7E683}" name="grounder % (&lt;10 deg)" dataCellStyle="Percent">
@@ -9223,41 +9255,41 @@
     <tableColumn id="85" xr3:uid="{56DD6E0A-39C0-4DF0-B1CB-47EB71B71306}" name="pop up % (&gt;50 deg)" dataCellStyle="Percent">
       <calculatedColumnFormula>1-_xlfn.NORM.DIST(50, Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="86" xr3:uid="{6ED971D4-0303-4AEB-B7CD-9516517F447E}" name="odds of 3B" dataDxfId="11" dataCellStyle="Percent">
+    <tableColumn id="86" xr3:uid="{6ED971D4-0303-4AEB-B7CD-9516517F447E}" name="odds of 3B" dataDxfId="12" dataCellStyle="Percent">
       <calculatedColumnFormula>1-_xlfn.NORM.DIST(70, $BZ$28,$BZ$25,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="87" xr3:uid="{E9F9DFB6-4A26-4CA7-9318-6ECA478690D6}" name="exit velocity mean" dataDxfId="10">
+    <tableColumn id="87" xr3:uid="{E9F9DFB6-4A26-4CA7-9318-6ECA478690D6}" name="exit velocity mean" dataDxfId="11">
       <calculatedColumnFormula>$CA$25+Table3[[#This Row],[offense]]*($CA$27-$CA$25)/2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="88" xr3:uid="{EB865A5D-CC1D-49FA-9709-DC5F30F55DD8}" name="after reduction" dataDxfId="9">
+    <tableColumn id="88" xr3:uid="{EB865A5D-CC1D-49FA-9709-DC5F30F55DD8}" name="after reduction" dataDxfId="10">
       <calculatedColumnFormula>Table3[[#This Row],[exit velocity mean]]-Table3[[#This Row],[reduction]]*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="89" xr3:uid="{949E8C38-C424-4A4E-9A6F-FCA93496D192}" name="theoretical distance" dataDxfId="8">
+    <tableColumn id="89" xr3:uid="{949E8C38-C424-4A4E-9A6F-FCA93496D192}" name="theoretical distance" dataDxfId="9">
       <calculatedColumnFormula>Table3[[#This Row],[exit velocity mean]]^2*2*SIN(RADIANS(Table3[[#This Row],[adjusted launch angle]]))/$CC$28*5280</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="90" xr3:uid="{9FD0A88A-D0D9-4369-8D70-6C7485CA1509}" name="flight time" dataDxfId="7">
+    <tableColumn id="90" xr3:uid="{9FD0A88A-D0D9-4369-8D70-6C7485CA1509}" name="flight time" dataDxfId="8">
       <calculatedColumnFormula>2*Table3[[#This Row],[exit velocity mean]]*SIN(RADIANS(Table3[[#This Row],[adjusted launch angle]]))/$CC$28*60*60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="91" xr3:uid="{D9D5DFED-BD09-4CB6-A82E-D289D2DAB08D}" name="actual distance" dataDxfId="6">
+    <tableColumn id="91" xr3:uid="{D9D5DFED-BD09-4CB6-A82E-D289D2DAB08D}" name="actual distance" dataDxfId="7">
       <calculatedColumnFormula>Table3[[#This Row],[theoretical distance]]-Table3[[#This Row],[flight time]]^2*$CE$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="92" xr3:uid="{3D80331E-564D-462D-81B5-E5CE730D1EE5}" name="+1stdv EV" dataDxfId="5">
+    <tableColumn id="92" xr3:uid="{3D80331E-564D-462D-81B5-E5CE730D1EE5}" name="+1stdv EV" dataDxfId="6">
       <calculatedColumnFormula>Table3[[#This Row],[exit velocity mean]]+$CC$25-Table3[[#This Row],[reduction]]*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="93" xr3:uid="{211123A1-65C0-4F59-AB86-C344CFF47F70}" name="+1stdv LA" dataDxfId="4">
+    <tableColumn id="93" xr3:uid="{211123A1-65C0-4F59-AB86-C344CFF47F70}" name="+1stdv LA" dataDxfId="5">
       <calculatedColumnFormula>MIN(Table3[[#This Row],[adjusted launch angle]]+Table3[[#This Row],[angle stdev]], 30)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="94" xr3:uid="{C8736D16-AF27-436D-BF61-CA3E58298CD3}" name="+1stdv flight time" dataDxfId="3">
+    <tableColumn id="94" xr3:uid="{C8736D16-AF27-436D-BF61-CA3E58298CD3}" name="+1stdv flight time" dataDxfId="4">
       <calculatedColumnFormula>2*Table3[[#This Row],[+1stdv EV]]*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*60*60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="95" xr3:uid="{C9967388-9755-4293-82E9-4E43A4770599}" name="+1stdev distance" dataDxfId="2">
+    <tableColumn id="95" xr3:uid="{C9967388-9755-4293-82E9-4E43A4770599}" name="+1stdev distance" dataDxfId="3">
       <calculatedColumnFormula>Table3[[#This Row],[+1stdv EV]]^2*2*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*5280-Table3[[#This Row],[+1stdv flight time]]^2*$CE$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="96" xr3:uid="{52B6BA3A-87F7-49FD-BFE7-811EA76B03FD}" name="+1stdev delta" dataDxfId="1">
+    <tableColumn id="96" xr3:uid="{52B6BA3A-87F7-49FD-BFE7-811EA76B03FD}" name="+1stdev delta" dataDxfId="2">
       <calculatedColumnFormula>Table3[[#This Row],[+1stdev distance]]-Table3[[#This Row],[actual distance]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="97" xr3:uid="{50EEB2EF-C836-4BBC-A8B3-EAD31BF29B54}" name="Column95"/>
-    <tableColumn id="98" xr3:uid="{823DCE3F-2A43-4BFF-AFF7-BC15E601D901}" name="Column96"/>
+    <tableColumn id="98" xr3:uid="{823DCE3F-2A43-4BFF-AFF7-BC15E601D901}" name="Column1"/>
     <tableColumn id="99" xr3:uid="{28288627-7AF0-454A-B8A1-A3BC42ECE940}" name="Column97"/>
     <tableColumn id="100" xr3:uid="{575103B5-2CCC-44DD-BB88-FB18F1E23A08}" name="Column98"/>
     <tableColumn id="101" xr3:uid="{C55306D8-624E-4BCE-834B-AF49B8202CED}" name="Column99"/>
@@ -9298,7 +9330,7 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{23FB116D-6CB4-49F6-A874-F1C610DEF5E1}" name="quality"/>
     <tableColumn id="2" xr3:uid="{6204ECDD-C980-4BE0-AFC7-9F83BF472BE8}" name="net"/>
-    <tableColumn id="3" xr3:uid="{E9208F79-490A-4A40-B3B7-0914BA16AC90}" name="form" dataDxfId="0">
+    <tableColumn id="3" xr3:uid="{E9208F79-490A-4A40-B3B7-0914BA16AC90}" name="form" dataDxfId="1">
       <calculatedColumnFormula>POWER(Table1[[#This Row],[quality]]-0.8, 1/4)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9571,8 +9603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DO41"/>
   <sheetViews>
-    <sheetView topLeftCell="BJ4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BW14" sqref="BW14"/>
+    <sheetView topLeftCell="CH1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="CL30" sqref="CL30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9703,7 +9735,7 @@
       <c r="AZ5" s="75"/>
       <c r="BA5" s="76"/>
       <c r="BB5" s="74" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="BC5" s="75"/>
       <c r="BD5" s="75"/>
@@ -9716,7 +9748,7 @@
       <c r="BK5" s="74"/>
       <c r="BL5" s="76"/>
       <c r="BM5" s="74" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="BN5" s="75"/>
       <c r="BO5" s="75"/>
@@ -9726,7 +9758,7 @@
       <c r="BS5" s="76"/>
       <c r="BT5" s="167"/>
       <c r="BU5" s="74" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="BV5" s="75"/>
       <c r="BW5" s="75"/>
@@ -9738,6 +9770,9 @@
       <c r="CC5" s="75"/>
       <c r="CD5" s="75"/>
       <c r="CE5" s="76"/>
+      <c r="CL5" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="6" spans="1:119" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -9882,220 +9917,220 @@
         <v>208</v>
       </c>
       <c r="AV6" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="AW6" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="AW6" s="2" t="s">
-        <v>219</v>
-      </c>
       <c r="AX6" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AY6" s="153" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AZ6" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="BA6" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="BB6" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="BC6" s="2" t="s">
         <v>201</v>
       </c>
       <c r="BD6" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="BE6" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="BE6" s="2" t="s">
+      <c r="BF6" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="BF6" s="2" t="s">
+      <c r="BG6" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="BG6" s="2" t="s">
+      <c r="BH6" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="BH6" s="2" t="s">
+      <c r="BI6" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="BJ6" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="BI6" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="BJ6" s="2" t="s">
-        <v>257</v>
-      </c>
       <c r="BK6" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="BL6" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="BL6" s="2" t="s">
-        <v>262</v>
-      </c>
       <c r="BM6" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="BN6" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="BN6" s="2" t="s">
-        <v>260</v>
-      </c>
       <c r="BO6" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="BP6" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="BQ6" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="BQ6" s="2" t="s">
-        <v>269</v>
-      </c>
       <c r="BR6" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="BS6" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="BT6" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="BU6" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="BV6" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="BW6" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="BX6" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="BY6" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="BU6" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="BV6" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="BW6" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="BX6" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="BY6" s="2" t="s">
-        <v>284</v>
-      </c>
       <c r="BZ6" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="CA6" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="CA6" s="2" t="s">
-        <v>287</v>
-      </c>
       <c r="CB6" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="CC6" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="CD6" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="CE6" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="CF6" s="153" t="s">
         <v>296</v>
       </c>
-      <c r="CF6" s="153" t="s">
+      <c r="CG6" s="153" t="s">
         <v>297</v>
       </c>
-      <c r="CG6" s="153" t="s">
+      <c r="CH6" s="153" t="s">
         <v>298</v>
       </c>
-      <c r="CH6" s="153" t="s">
+      <c r="CI6" s="153" t="s">
         <v>299</v>
       </c>
-      <c r="CI6" s="153" t="s">
+      <c r="CJ6" s="153" t="s">
         <v>300</v>
-      </c>
-      <c r="CJ6" s="153" t="s">
-        <v>301</v>
       </c>
       <c r="CK6" s="2" t="s">
         <v>209</v>
       </c>
       <c r="CL6" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="CM6" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="CM6" s="2" t="s">
+      <c r="CN6" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="CN6" s="2" t="s">
+      <c r="CO6" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="CO6" s="2" t="s">
+      <c r="CP6" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="CP6" s="2" t="s">
+      <c r="CQ6" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="CQ6" s="2" t="s">
+      <c r="CR6" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="CR6" s="2" t="s">
+      <c r="CS6" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="CS6" s="2" t="s">
-        <v>217</v>
-      </c>
       <c r="CT6" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="CU6" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="CU6" s="2" t="s">
+      <c r="CV6" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="CV6" s="2" t="s">
+      <c r="CW6" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="CW6" s="2" t="s">
+      <c r="CX6" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="CX6" s="2" t="s">
+      <c r="CY6" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="CY6" s="2" t="s">
+      <c r="CZ6" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="CZ6" s="2" t="s">
+      <c r="DA6" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="DA6" s="2" t="s">
+      <c r="DB6" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="DB6" s="2" t="s">
+      <c r="DC6" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="DC6" s="2" t="s">
+      <c r="DD6" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="DD6" s="2" t="s">
+      <c r="DE6" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="DE6" s="2" t="s">
+      <c r="DF6" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="DF6" s="2" t="s">
+      <c r="DG6" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="DG6" s="2" t="s">
+      <c r="DH6" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="DH6" s="2" t="s">
+      <c r="DI6" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="DI6" s="2" t="s">
+      <c r="DJ6" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="DJ6" s="2" t="s">
+      <c r="DK6" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="DK6" s="2" t="s">
+      <c r="DL6" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="DL6" s="2" t="s">
+      <c r="DM6" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="DM6" s="2" t="s">
+      <c r="DN6" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="DN6" s="2" t="s">
+      <c r="DO6" s="2" t="s">
         <v>244</v>
-      </c>
-      <c r="DO6" s="2" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:119" s="29" customFormat="1" x14ac:dyDescent="0.25">
@@ -13638,7 +13673,7 @@
         <v>143.49784870525124</v>
       </c>
     </row>
-    <row r="17" spans="1:88" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:90" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -13992,7 +14027,7 @@
         <v>146.60126303800868</v>
       </c>
     </row>
-    <row r="18" spans="1:88" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:90" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -14346,7 +14381,7 @@
         <v>141.37530011951372</v>
       </c>
     </row>
-    <row r="19" spans="1:88" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:90" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -14700,7 +14735,7 @@
         <v>137.52269240572463</v>
       </c>
     </row>
-    <row r="20" spans="1:88" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:90" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -15054,7 +15089,7 @@
         <v>143.49784870525124</v>
       </c>
     </row>
-    <row r="21" spans="1:88" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:90" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -15408,7 +15443,7 @@
         <v>146.60126303800868</v>
       </c>
     </row>
-    <row r="22" spans="1:88" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:90" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -15762,12 +15797,12 @@
         <v>141.37530011951372</v>
       </c>
     </row>
-    <row r="23" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:90" x14ac:dyDescent="0.25">
       <c r="AW23" s="154"/>
       <c r="BK23" s="73"/>
       <c r="BL23" s="73"/>
     </row>
-    <row r="24" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:90" x14ac:dyDescent="0.25">
       <c r="Y24" s="63" t="s">
         <v>141</v>
       </c>
@@ -15795,37 +15830,40 @@
         <v>204</v>
       </c>
       <c r="AX24" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="BA24" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="BB24" t="s">
         <v>199</v>
       </c>
       <c r="BP24" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="BV24" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="BW24" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="BZ24" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="CA24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="CC24" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="CE24" t="s">
-        <v>295</v>
+        <v>294</v>
+      </c>
+      <c r="CL24" t="s">
+        <v>113</v>
       </c>
     </row>
-    <row r="25" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:90" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
         <v>89</v>
       </c>
@@ -15922,8 +15960,11 @@
       <c r="CE25">
         <v>16</v>
       </c>
+      <c r="CL25">
+        <v>80</v>
+      </c>
     </row>
-    <row r="26" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:90" x14ac:dyDescent="0.25">
       <c r="D26">
         <v>0.1</v>
       </c>
@@ -15992,16 +16033,16 @@
         <v>205</v>
       </c>
       <c r="AX26" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="BP26" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="CA26" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
-    <row r="27" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:90" x14ac:dyDescent="0.25">
       <c r="K27" t="s">
         <v>91</v>
       </c>
@@ -16056,29 +16097,32 @@
         <v>-2</v>
       </c>
       <c r="BU27" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="BV27" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="BW27" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="BZ27" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="CA27">
         <v>110</v>
       </c>
       <c r="CC27" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="CE27">
         <f>CE10/CE9</f>
         <v>1.7578456475284747</v>
       </c>
+      <c r="CL27" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="28" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:90" x14ac:dyDescent="0.25">
       <c r="K28">
         <v>0.9</v>
       </c>
@@ -16113,7 +16157,7 @@
         <v>189</v>
       </c>
       <c r="AU28" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="BB28" t="s">
         <v>136</v>
@@ -16131,8 +16175,11 @@
       <c r="CC28">
         <v>80000</v>
       </c>
+      <c r="CL28">
+        <v>90</v>
+      </c>
     </row>
-    <row r="29" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:90" x14ac:dyDescent="0.25">
       <c r="W29" t="s">
         <v>130</v>
       </c>
@@ -16168,16 +16215,16 @@
         <v>5</v>
       </c>
       <c r="AX29" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="BB29">
         <v>1</v>
       </c>
       <c r="BP29" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
-    <row r="30" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:90" x14ac:dyDescent="0.25">
       <c r="W30">
         <f xml:space="preserve"> W28/2 - W26/3</f>
         <v>-1</v>
@@ -16212,7 +16259,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:90" x14ac:dyDescent="0.25">
       <c r="W31" t="s">
         <v>133</v>
       </c>
@@ -16245,7 +16292,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="32" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:90" x14ac:dyDescent="0.25">
       <c r="W32">
         <f>MAX(0, ((W26+X26)/(3+X26))-(W28/2))</f>
         <v>1</v>
@@ -16395,7 +16442,7 @@
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
   <conditionalFormatting sqref="O7:O22">
-    <cfRule type="cellIs" dxfId="82" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16412,7 +16459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF285913-BB23-45EF-B183-28069296EF50}">
   <dimension ref="J12:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
@@ -16426,10 +16473,10 @@
         <v>112</v>
       </c>
       <c r="K12" t="s">
+        <v>301</v>
+      </c>
+      <c r="L12" t="s">
         <v>302</v>
-      </c>
-      <c r="L12" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="13" spans="10:12" x14ac:dyDescent="0.25">
@@ -16511,11 +16558,1998 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23DCCA5A-0B13-43BB-84FB-82799C654ACD}">
+  <dimension ref="A1:W23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1">
+        <v>-3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>305</v>
+      </c>
+      <c r="F1">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0.1</v>
+      </c>
+      <c r="E2">
+        <v>0.2</v>
+      </c>
+      <c r="F2">
+        <v>0.3</v>
+      </c>
+      <c r="G2">
+        <v>0.4</v>
+      </c>
+      <c r="H2">
+        <v>0.5</v>
+      </c>
+      <c r="I2">
+        <v>0.6</v>
+      </c>
+      <c r="J2">
+        <v>0.7</v>
+      </c>
+      <c r="K2">
+        <v>0.8</v>
+      </c>
+      <c r="L2">
+        <v>0.9</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O2">
+        <v>1.2</v>
+      </c>
+      <c r="P2">
+        <v>1.3</v>
+      </c>
+      <c r="Q2">
+        <v>1.4</v>
+      </c>
+      <c r="R2">
+        <v>1.5</v>
+      </c>
+      <c r="S2">
+        <v>1.6</v>
+      </c>
+      <c r="T2">
+        <v>1.7</v>
+      </c>
+      <c r="U2">
+        <v>1.8</v>
+      </c>
+      <c r="V2">
+        <v>1.9</v>
+      </c>
+      <c r="W2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>303</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <v>0.93319279873114191</v>
+      </c>
+      <c r="D3">
+        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <v>0.93610096034524259</v>
+      </c>
+      <c r="E3">
+        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <v>0.93899500761383359</v>
+      </c>
+      <c r="F3">
+        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <v>0.941871574470311</v>
+      </c>
+      <c r="G3">
+        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <v>0.94472709570688829</v>
+      </c>
+      <c r="H3">
+        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <v>0.94755780490616992</v>
+      </c>
+      <c r="I3">
+        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <v>0.95035973404319185</v>
+      </c>
+      <c r="J3">
+        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <v>0.95312871510773034</v>
+      </c>
+      <c r="K3">
+        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <v>0.95586038414193264</v>
+      </c>
+      <c r="L3">
+        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <v>0.95855018813574422</v>
+      </c>
+      <c r="M3">
+        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <v>0.96119339527114878</v>
+      </c>
+      <c r="N3">
+        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <v>0.96378510905435966</v>
+      </c>
+      <c r="O3">
+        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <v>0.96632028692061955</v>
+      </c>
+      <c r="P3">
+        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <v>0.96879376393622496</v>
+      </c>
+      <c r="Q3">
+        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <v>0.97120028225284716</v>
+      </c>
+      <c r="R3">
+        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <v>0.97353452698506504</v>
+      </c>
+      <c r="S3">
+        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <v>0.97579116917672093</v>
+      </c>
+      <c r="T3">
+        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <v>0.97796491648714601</v>
+      </c>
+      <c r="U3">
+        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <v>0.98005057215450919</v>
+      </c>
+      <c r="V3">
+        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <v>0.98204310266867123</v>
+      </c>
+      <c r="W3">
+        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <v>0.98393771439617173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>0.1</v>
+      </c>
+      <c r="C4">
+        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <v>0.93942924199794098</v>
+      </c>
+      <c r="D4">
+        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <v>0.94221049307757543</v>
+      </c>
+      <c r="E4">
+        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <v>0.94497162805414114</v>
+      </c>
+      <c r="F4">
+        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <v>0.94770921469607072</v>
+      </c>
+      <c r="G4">
+        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <v>0.95041964397531165</v>
+      </c>
+      <c r="H4">
+        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <v>0.95309913157177895</v>
+      </c>
+      <c r="I4">
+        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <v>0.95574372137968222</v>
+      </c>
+      <c r="J4">
+        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <v>0.9583492913688767</v>
+      </c>
+      <c r="K4">
+        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <v>0.96091156219176899</v>
+      </c>
+      <c r="L4">
+        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <v>0.96342610896336511</v>
+      </c>
+      <c r="M4">
+        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <v>0.96588837667724492</v>
+      </c>
+      <c r="N4">
+        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <v>0.96829369975146407</v>
+      </c>
+      <c r="O4">
+        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <v>0.97063732622285248</v>
+      </c>
+      <c r="P4">
+        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <v>0.97291444712231223</v>
+      </c>
+      <c r="Q4">
+        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <v>0.97512023156297545</v>
+      </c>
+      <c r="R4">
+        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <v>0.97724986805182079</v>
+      </c>
+      <c r="S4">
+        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <v>0.97929861248667271</v>
+      </c>
+      <c r="T4">
+        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <v>0.98126184321621246</v>
+      </c>
+      <c r="U4">
+        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <v>0.98313512341112752</v>
+      </c>
+      <c r="V4">
+        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <v>0.98491427080899996</v>
+      </c>
+      <c r="W4">
+        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <v>0.98659543464220212</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>0.2</v>
+      </c>
+      <c r="C5">
+        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <v>0.94520070830044201</v>
+      </c>
+      <c r="D5">
+        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <v>0.94785108530229123</v>
+      </c>
+      <c r="E5">
+        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <v>0.95047579566670537</v>
+      </c>
+      <c r="F5">
+        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <v>0.95307139309539912</v>
+      </c>
+      <c r="G5">
+        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <v>0.9556342800557962</v>
+      </c>
+      <c r="H5">
+        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <v>0.95816071278906079</v>
+      </c>
+      <c r="I5">
+        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <v>0.96064680858347651</v>
+      </c>
+      <c r="J5">
+        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <v>0.96308855565481921</v>
+      </c>
+      <c r="K5">
+        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <v>0.96548182600279242</v>
+      </c>
+      <c r="L5">
+        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <v>0.96782239163714201</v>
+      </c>
+      <c r="M5">
+        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <v>0.97010594458676791</v>
+      </c>
+      <c r="N5">
+        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <v>0.97232812111745404</v>
+      </c>
+      <c r="O5">
+        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <v>0.97448453058555684</v>
+      </c>
+      <c r="P5">
+        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <v>0.97657078934214148</v>
+      </c>
+      <c r="Q5">
+        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <v>0.97858256006982691</v>
+      </c>
+      <c r="R5">
+        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <v>0.98051559687722489</v>
+      </c>
+      <c r="S5">
+        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <v>0.98236579638662769</v>
+      </c>
+      <c r="T5">
+        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <v>0.98412925492187275</v>
+      </c>
+      <c r="U5">
+        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <v>0.98580233172670073</v>
+      </c>
+      <c r="V5">
+        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <v>0.98738171791059692</v>
+      </c>
+      <c r="W5">
+        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <v>0.9888645105203836</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>0.3</v>
+      </c>
+      <c r="C6">
+        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <v>0.9505285319663519</v>
+      </c>
+      <c r="D6">
+        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <v>0.95304533229487931</v>
+      </c>
+      <c r="E6">
+        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <v>0.95553141012261578</v>
+      </c>
+      <c r="F6">
+        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <v>0.95798335506905641</v>
+      </c>
+      <c r="G6">
+        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <v>0.96039763356816699</v>
+      </c>
+      <c r="H6">
+        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <v>0.96277059720355673</v>
+      </c>
+      <c r="I6">
+        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <v>0.96509849349527255</v>
+      </c>
+      <c r="J6">
+        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <v>0.96737747945404673</v>
+      </c>
+      <c r="K6">
+        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <v>0.96960363823473861</v>
+      </c>
+      <c r="L6">
+        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <v>0.97177299923126637</v>
+      </c>
+      <c r="M6">
+        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <v>0.97388156195825992</v>
+      </c>
+      <c r="N6">
+        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <v>0.97592532405714871</v>
+      </c>
+      <c r="O6">
+        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <v>0.97790031374301589</v>
+      </c>
+      <c r="P6">
+        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <v>0.97980262696922982</v>
+      </c>
+      <c r="Q6">
+        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <v>0.98162846952483385</v>
+      </c>
+      <c r="R6">
+        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <v>0.98337420418952204</v>
+      </c>
+      <c r="S6">
+        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <v>0.98503640294671146</v>
+      </c>
+      <c r="T6">
+        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <v>0.98661190409033794</v>
+      </c>
+      <c r="U6">
+        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <v>0.98809787384903192</v>
+      </c>
+      <c r="V6">
+        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <v>0.98949187188624066</v>
+      </c>
+      <c r="W6">
+        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <v>0.99079191971184799</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>0.4</v>
+      </c>
+      <c r="C7">
+        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <v>0.95543453724145699</v>
+      </c>
+      <c r="D7">
+        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <v>0.95781624723514713</v>
+      </c>
+      <c r="E7">
+        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <v>0.96016270640197721</v>
+      </c>
+      <c r="F7">
+        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <v>0.96247058720650747</v>
+      </c>
+      <c r="G7">
+        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <v>0.96473646869703567</v>
+      </c>
+      <c r="H7">
+        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <v>0.96695684789416148</v>
+      </c>
+      <c r="I7">
+        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <v>0.96912815373421313</v>
+      </c>
+      <c r="J7">
+        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <v>0.97124676384449027</v>
+      </c>
+      <c r="K7">
+        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <v>0.9733090244307121</v>
+      </c>
+      <c r="L7">
+        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <v>0.97531127355290825</v>
+      </c>
+      <c r="M7">
+        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <v>0.97724986805182079</v>
+      </c>
+      <c r="N7">
+        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <v>0.9791212143607767</v>
+      </c>
+      <c r="O7">
+        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <v>0.98092180339453061</v>
+      </c>
+      <c r="P7">
+        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <v>0.98264824964288278</v>
+      </c>
+      <c r="Q7">
+        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <v>0.98429733450858192</v>
+      </c>
+      <c r="R7">
+        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <v>0.98586605381145986</v>
+      </c>
+      <c r="S7">
+        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <v>0.98735166922903572</v>
+      </c>
+      <c r="T7">
+        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <v>0.98875176325331959</v>
+      </c>
+      <c r="U7">
+        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <v>0.99006429701015009</v>
+      </c>
+      <c r="V7">
+        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <v>0.99128767000840101</v>
+      </c>
+      <c r="W7">
+        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <v>0.99242078056128025</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>0.5</v>
+      </c>
+      <c r="C8">
+        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <v>0.95994084313618289</v>
+      </c>
+      <c r="D8">
+        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <v>0.9621870572995479</v>
+      </c>
+      <c r="E8">
+        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <v>0.96439404232427384</v>
+      </c>
+      <c r="F8">
+        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <v>0.96655859658087928</v>
+      </c>
+      <c r="G8">
+        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <v>0.96867745573741471</v>
+      </c>
+      <c r="H8">
+        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <v>0.97074730684334809</v>
+      </c>
+      <c r="I8">
+        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <v>0.97276480498626128</v>
+      </c>
+      <c r="J8">
+        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <v>0.97472659274822582</v>
+      </c>
+      <c r="K8">
+        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <v>0.97662932267937719</v>
+      </c>
+      <c r="L8">
+        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <v>0.97846968298743109</v>
+      </c>
+      <c r="M8">
+        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <v>0.98024442661121902</v>
+      </c>
+      <c r="N8">
+        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <v>0.98195040380095566</v>
+      </c>
+      <c r="O8">
+        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <v>0.98358459826471212</v>
+      </c>
+      <c r="P8">
+        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <v>0.98514416685602335</v>
+      </c>
+      <c r="Q8">
+        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <v>0.98662648266809205</v>
+      </c>
+      <c r="R8">
+        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <v>0.98802918126206773</v>
+      </c>
+      <c r="S8">
+        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <v>0.98935020958708397</v>
+      </c>
+      <c r="T8">
+        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <v>0.99058787694556816</v>
+      </c>
+      <c r="U8">
+        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <v>0.99174090711751128</v>
+      </c>
+      <c r="V8">
+        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <v>0.99280849048270048</v>
+      </c>
+      <c r="W8">
+        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <v>0.99379033467422384</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>0.6</v>
+      </c>
+      <c r="C9">
+        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <v>0.96406968088707423</v>
+      </c>
+      <c r="D9">
+        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <v>0.96618101424832259</v>
+      </c>
+      <c r="E9">
+        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <v>0.96824970264897547</v>
+      </c>
+      <c r="F9">
+        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <v>0.97027270889703676</v>
+      </c>
+      <c r="G9">
+        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <v>0.97224696399442845</v>
+      </c>
+      <c r="H9">
+        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <v>0.97416938348928472</v>
+      </c>
+      <c r="I9">
+        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <v>0.97603688633498631</v>
+      </c>
+      <c r="J9">
+        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <v>0.97784641642385983</v>
+      </c>
+      <c r="K9">
+        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <v>0.9795949669416939</v>
+      </c>
+      <c r="L9">
+        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <v>0.98127960765667077</v>
+      </c>
+      <c r="M9">
+        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <v>0.98289751521066271</v>
+      </c>
+      <c r="N9">
+        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <v>0.98444600641955393</v>
+      </c>
+      <c r="O9">
+        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <v>0.98592257450963416</v>
+      </c>
+      <c r="P9">
+        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <v>0.98732492811641093</v>
+      </c>
+      <c r="Q9">
+        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <v>0.98865103274781108</v>
+      </c>
+      <c r="R9">
+        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <v>0.98989915426344599</v>
+      </c>
+      <c r="S9">
+        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <v>0.99106790374392784</v>
+      </c>
+      <c r="T9">
+        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <v>0.99215628291889535</v>
+      </c>
+      <c r="U9">
+        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <v>0.99316372909104689</v>
+      </c>
+      <c r="V9">
+        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <v>0.99409015824032565</v>
+      </c>
+      <c r="W9">
+        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <v>0.99493600472530463</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>0.7</v>
+      </c>
+      <c r="C10">
+        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <v>0.96784322520438626</v>
+      </c>
+      <c r="D10">
+        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <v>0.96982122064229781</v>
+      </c>
+      <c r="E10">
+        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <v>0.97175372082062006</v>
+      </c>
+      <c r="F10">
+        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <v>0.97363788647703964</v>
+      </c>
+      <c r="G10">
+        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <v>0.97547087689619361</v>
+      </c>
+      <c r="H10">
+        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <v>0.97724986805182079</v>
+      </c>
+      <c r="I10">
+        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <v>0.97897207311016909</v>
+      </c>
+      <c r="J10">
+        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <v>0.98063476539748684</v>
+      </c>
+      <c r="K10">
+        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <v>0.98223530390123148</v>
+      </c>
+      <c r="L10">
+        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <v>0.98377116132986453</v>
+      </c>
+      <c r="M10">
+        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <v>0.98523995469775305</v>
+      </c>
+      <c r="N10">
+        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <v>0.98663947832768129</v>
+      </c>
+      <c r="O10">
+        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <v>0.98796773907173285</v>
+      </c>
+      <c r="P10">
+        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <v>0.98922299344000109</v>
+      </c>
+      <c r="Q10">
+        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <v>0.99040378619428515</v>
+      </c>
+      <c r="R10">
+        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <v>0.9915089898099565</v>
+      </c>
+      <c r="S10">
+        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <v>0.99253784403396828</v>
+      </c>
+      <c r="T10">
+        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <v>0.993489994572619</v>
+      </c>
+      <c r="U10">
+        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <v>0.99436552973351766</v>
+      </c>
+      <c r="V10">
+        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <v>0.9951650136295519</v>
+      </c>
+      <c r="W10">
+        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <v>0.99588951433965567</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>0.8</v>
+      </c>
+      <c r="C11">
+        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <v>0.97128344018399815</v>
+      </c>
+      <c r="D11">
+        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <v>0.97313047249844897</v>
+      </c>
+      <c r="E11">
+        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <v>0.97492971907180315</v>
+      </c>
+      <c r="F11">
+        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <v>0.9766785666692418</v>
+      </c>
+      <c r="G11">
+        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <v>0.97837442974191546</v>
+      </c>
+      <c r="H11">
+        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <v>0.98001476984692537</v>
+      </c>
+      <c r="I11">
+        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <v>0.9815971172112371</v>
+      </c>
+      <c r="J11">
+        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <v>0.98311909447403878</v>
+      </c>
+      <c r="K11">
+        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <v>0.98457844259899263</v>
+      </c>
+      <c r="L11">
+        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <v>0.98597304889303117</v>
+      </c>
+      <c r="M11">
+        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <v>0.98730097700023178</v>
+      </c>
+      <c r="N11">
+        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <v>0.98856049865636386</v>
+      </c>
+      <c r="O11">
+        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <v>0.98975012689068897</v>
+      </c>
+      <c r="P11">
+        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <v>0.99086865024566873</v>
+      </c>
+      <c r="Q11">
+        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <v>0.99191516745228692</v>
+      </c>
+      <c r="R11">
+        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <v>0.99288912184959954</v>
+      </c>
+      <c r="S11">
+        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <v>0.99379033467422384</v>
+      </c>
+      <c r="T11">
+        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <v>0.99461903617301051</v>
+      </c>
+      <c r="U11">
+        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <v>0.9953758933168243</v>
+      </c>
+      <c r="V11">
+        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <v>0.99606203272497285</v>
+      </c>
+      <c r="W11">
+        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <v>0.99667905726178674</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>0.9</v>
+      </c>
+      <c r="C12">
+        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <v>0.97441194047836144</v>
+      </c>
+      <c r="D12">
+        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <v>0.97613111888135196</v>
+      </c>
+      <c r="E12">
+        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <v>0.9778007672556237</v>
+      </c>
+      <c r="F12">
+        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <v>0.9794185208944417</v>
+      </c>
+      <c r="G12">
+        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <v>0.98098207010284577</v>
+      </c>
+      <c r="H12">
+        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <v>0.98248918036829402</v>
+      </c>
+      <c r="I12">
+        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <v>0.98393771439617173</v>
+      </c>
+      <c r="J12">
+        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <v>0.98532565597611843</v>
+      </c>
+      <c r="K12">
+        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <v>0.98665113559422191</v>
+      </c>
+      <c r="L12">
+        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <v>0.98791245764394509</v>
+      </c>
+      <c r="M12">
+        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <v>0.98910812901414658</v>
+      </c>
+      <c r="N12">
+        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <v>0.99023688874489857</v>
+      </c>
+      <c r="O12">
+        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <v>0.99129773834062174</v>
+      </c>
+      <c r="P12">
+        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <v>0.99228997221560522</v>
+      </c>
+      <c r="Q12">
+        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <v>0.99321320762041643</v>
+      </c>
+      <c r="R12">
+        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <v>0.99406741326145165</v>
+      </c>
+      <c r="S12">
+        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <v>0.99485293568395028</v>
+      </c>
+      <c r="T12">
+        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <v>0.99557052234725518</v>
+      </c>
+      <c r="U12">
+        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <v>0.9962213401885005</v>
+      </c>
+      <c r="V12">
+        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <v>0.99680698835864645</v>
+      </c>
+      <c r="W12">
+        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <v>0.99732950373746643</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <v>0.97724986805182079</v>
+      </c>
+      <c r="D13">
+        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <v>0.97884493863434063</v>
+      </c>
+      <c r="E13">
+        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <v>0.98038926046139385</v>
+      </c>
+      <c r="F13">
+        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <v>0.98188073420027189</v>
+      </c>
+      <c r="G13">
+        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <v>0.98331734052759789</v>
+      </c>
+      <c r="H13">
+        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <v>0.98469716052612621</v>
+      </c>
+      <c r="I13">
+        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <v>0.98601839761764787</v>
+      </c>
+      <c r="J13">
+        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <v>0.98727940093204036</v>
+      </c>
+      <c r="K13">
+        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <v>0.98847868995611909</v>
+      </c>
+      <c r="L13">
+        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <v>0.98961498023936256</v>
+      </c>
+      <c r="M13">
+        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <v>0.99068720985629855</v>
+      </c>
+      <c r="N13">
+        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <v>0.99169456623730734</v>
+      </c>
+      <c r="O13">
+        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <v>0.99263651288131527</v>
+      </c>
+      <c r="P13">
+        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <v>0.99351281535665104</v>
+      </c>
+      <c r="Q13">
+        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <v>0.9943235658825752</v>
+      </c>
+      <c r="R13">
+        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <v>0.99506920566743162</v>
+      </c>
+      <c r="S13">
+        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <v>0.99575054406539887</v>
+      </c>
+      <c r="T13">
+        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <v>0.99636877350986042</v>
+      </c>
+      <c r="U13">
+        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <v>0.99692547909715257</v>
+      </c>
+      <c r="V13">
+        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <v>0.99742264164199901</v>
+      </c>
+      <c r="W13">
+        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <v>0.99786263301991374</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C14">
+        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <v>0.97981778459429558</v>
+      </c>
+      <c r="D14">
+        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <v>0.98129303418367897</v>
+      </c>
+      <c r="E14">
+        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <v>0.98271681517805853</v>
+      </c>
+      <c r="F14">
+        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <v>0.98408730488766094</v>
+      </c>
+      <c r="G14">
+        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <v>0.98540278287955929</v>
+      </c>
+      <c r="H14">
+        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <v>0.9866616510953955</v>
+      </c>
+      <c r="I14">
+        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <v>0.98786245514015714</v>
+      </c>
+      <c r="J14">
+        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <v>0.98900390658142112</v>
+      </c>
+      <c r="K14">
+        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <v>0.9900849060392205</v>
+      </c>
+      <c r="L14">
+        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <v>0.99110456677879533</v>
+      </c>
+      <c r="M14">
+        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <v>0.99206223844209485</v>
+      </c>
+      <c r="N14">
+        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <v>0.99295753046970459</v>
+      </c>
+      <c r="O14">
+        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <v>0.99379033467422384</v>
+      </c>
+      <c r="P14">
+        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <v>0.99456084633132047</v>
+      </c>
+      <c r="Q14">
+        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <v>0.99526958305914193</v>
+      </c>
+      <c r="R14">
+        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <v>0.99591740066526613</v>
+      </c>
+      <c r="S14">
+        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <v>0.99650550505931867</v>
+      </c>
+      <c r="T14">
+        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <v>0.99703545926696446</v>
+      </c>
+      <c r="U14">
+        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <v>0.99750918454727489</v>
+      </c>
+      <c r="V14">
+        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <v>0.99792895462238751</v>
+      </c>
+      <c r="W14">
+        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <v>0.99829738208935259</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>1.2</v>
+      </c>
+      <c r="C15">
+        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <v>0.98213557943718344</v>
+      </c>
+      <c r="D15">
+        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <v>0.98349574210455681</v>
+      </c>
+      <c r="E15">
+        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <v>0.98480418351194976</v>
+      </c>
+      <c r="F15">
+        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <v>0.98605936350374279</v>
+      </c>
+      <c r="G15">
+        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <v>0.98725986335550087</v>
+      </c>
+      <c r="H15">
+        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <v>0.98840440514152805</v>
+      </c>
+      <c r="I15">
+        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <v>0.98949187188624066</v>
+      </c>
+      <c r="J15">
+        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <v>0.99052132828574579</v>
+      </c>
+      <c r="K15">
+        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <v>0.99149204172653183</v>
+      </c>
+      <c r="L15">
+        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <v>0.99240350326205273</v>
+      </c>
+      <c r="M15">
+        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <v>0.99325544813598621</v>
+      </c>
+      <c r="N15">
+        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <v>0.99404787536444239</v>
+      </c>
+      <c r="O15">
+        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <v>0.99478106581052672</v>
+      </c>
+      <c r="P15">
+        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <v>0.99545559810651818</v>
+      </c>
+      <c r="Q15">
+        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <v>0.99607236170571123</v>
+      </c>
+      <c r="R15">
+        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <v>0.99663256628319929</v>
+      </c>
+      <c r="S15">
+        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <v>0.99713774665945876</v>
+      </c>
+      <c r="T15">
+        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <v>0.99758976240089414</v>
+      </c>
+      <c r="U15">
+        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <v>0.99799079126726198</v>
+      </c>
+      <c r="V15">
+        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <v>0.99834331573791169</v>
+      </c>
+      <c r="W15">
+        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <v>0.9986501019683699</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>1.3</v>
+      </c>
+      <c r="C16">
+        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <v>0.98422239260890954</v>
+      </c>
+      <c r="D16">
+        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <v>0.9854725599216041</v>
+      </c>
+      <c r="E16">
+        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <v>0.98667118474140514</v>
+      </c>
+      <c r="F16">
+        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <v>0.98781701026588054</v>
+      </c>
+      <c r="G16">
+        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <v>0.98890891700233552</v>
+      </c>
+      <c r="H16">
+        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <v>0.98994594096094168</v>
+      </c>
+      <c r="I16">
+        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <v>0.99092729223645926</v>
+      </c>
+      <c r="J16">
+        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <v>0.99185237372137502</v>
+      </c>
+      <c r="K16">
+        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <v>0.99272079963615401</v>
+      </c>
+      <c r="L16">
+        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <v>0.99353241350084198</v>
+      </c>
+      <c r="M16">
+        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <v>0.99428730510778573</v>
+      </c>
+      <c r="N16">
+        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <v>0.99498582598973795</v>
+      </c>
+      <c r="O16">
+        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <v>0.99562860281384891</v>
+      </c>
+      <c r="P16">
+        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <v>0.99621654807370474</v>
+      </c>
+      <c r="Q16">
+        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <v>0.99675086740336638</v>
+      </c>
+      <c r="R16">
+        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <v>0.99723306280512991</v>
+      </c>
+      <c r="S16">
+        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <v>0.99766493107341181</v>
+      </c>
+      <c r="T16">
+        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <v>0.9980485567187205</v>
+      </c>
+      <c r="U16">
+        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <v>0.99838629875681095</v>
+      </c>
+      <c r="V16">
+        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <v>0.99868077083778739</v>
+      </c>
+      <c r="W16">
+        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <v>0.99893481435657228</v>
+      </c>
+    </row>
+    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>1.4</v>
+      </c>
+      <c r="C17">
+        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <v>0.98609655248650141</v>
+      </c>
+      <c r="D17">
+        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <v>0.98724208843039174</v>
+      </c>
+      <c r="E17">
+        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <v>0.98833665330160048</v>
+      </c>
+      <c r="F17">
+        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <v>0.98937926979223911</v>
+      </c>
+      <c r="G17">
+        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <v>0.99036911036340736</v>
+      </c>
+      <c r="H17">
+        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <v>0.99130551389665644</v>
+      </c>
+      <c r="I17">
+        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <v>0.99218800234452975</v>
+      </c>
+      <c r="J17">
+        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <v>0.99301629709024808</v>
+      </c>
+      <c r="K17">
+        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <v>0.99379033467422384</v>
+      </c>
+      <c r="L17">
+        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <v>0.99451028149084664</v>
+      </c>
+      <c r="M17">
+        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <v>0.99517654700468294</v>
+      </c>
+      <c r="N17">
+        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <v>0.99578979498334452</v>
+      </c>
+      <c r="O17">
+        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <v>0.99635095219800218</v>
+      </c>
+      <c r="P17">
+        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <v>0.99686121400590511</v>
+      </c>
+      <c r="Q17">
+        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <v>0.99732204620721154</v>
+      </c>
+      <c r="R17">
+        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <v>0.99773518256671845</v>
+      </c>
+      <c r="S17">
+        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <v>0.99810261741620365</v>
+      </c>
+      <c r="T17">
+        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <v>0.99842659281208423</v>
+      </c>
+      <c r="U17">
+        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <v>0.99870957982304531</v>
+      </c>
+      <c r="V17">
+        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <v>0.99895425366976121</v>
+      </c>
+      <c r="W17">
+        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <v>0.99916346263892386</v>
+      </c>
+    </row>
+    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>1.5</v>
+      </c>
+      <c r="C18">
+        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <v>0.98777552734495533</v>
+      </c>
+      <c r="D18">
+        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <v>0.98882198867076931</v>
+      </c>
+      <c r="E18">
+        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <v>0.989818402138959</v>
+      </c>
+      <c r="F18">
+        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <v>0.99076406186531352</v>
+      </c>
+      <c r="G18">
+        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <v>0.99165842074571242</v>
+      </c>
+      <c r="H18">
+        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <v>0.99250110526320356</v>
+      </c>
+      <c r="I18">
+        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <v>0.99329192992302162</v>
+      </c>
+      <c r="J18">
+        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <v>0.99403091100447794</v>
+      </c>
+      <c r="K18">
+        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <v>0.99471827927308554</v>
+      </c>
+      <c r="L18">
+        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <v>0.99535449125135822</v>
+      </c>
+      <c r="M18">
+        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <v>0.99594023860462444</v>
+      </c>
+      <c r="N18">
+        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <v>0.99647645516170658</v>
+      </c>
+      <c r="O18">
+        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <v>0.99696432106288702</v>
+      </c>
+      <c r="P18">
+        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <v>0.99740526351334968</v>
+      </c>
+      <c r="Q18">
+        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <v>0.99780095362404031</v>
+      </c>
+      <c r="R18">
+        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <v>0.9981532988489582</v>
+      </c>
+      <c r="S18">
+        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <v>0.9984644305839443</v>
+      </c>
+      <c r="T18">
+        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <v>0.99873668658270343</v>
+      </c>
+      <c r="U18">
+        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <v>0.99897258797617372</v>
+      </c>
+      <c r="V18">
+        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <v>0.99917481085525794</v>
+      </c>
+      <c r="W18">
+        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <v>0.99934615259594539</v>
+      </c>
+    </row>
+    <row r="19" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>1.6</v>
+      </c>
+      <c r="C19">
+        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <v>0.98927588997832416</v>
+      </c>
+      <c r="D19">
+        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <v>0.99022895255784427</v>
+      </c>
+      <c r="E19">
+        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <v>0.99113320025518947</v>
+      </c>
+      <c r="F19">
+        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <v>0.99198818684480428</v>
+      </c>
+      <c r="G19">
+        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <v>0.99279363050302394</v>
+      </c>
+      <c r="H19">
+        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <v>0.99354942653731249</v>
+      </c>
+      <c r="I19">
+        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <v>0.99425565940188498</v>
+      </c>
+      <c r="J19">
+        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <v>0.99491261367939154</v>
+      </c>
+      <c r="K19">
+        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <v>0.99552078367125296</v>
+      </c>
+      <c r="L19">
+        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <v>0.99608088120520577</v>
+      </c>
+      <c r="M19">
+        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <v>0.99659384124004158</v>
+      </c>
+      <c r="N19">
+        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <v>0.99706082482737046</v>
+      </c>
+      <c r="O19">
+        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <v>0.99748321898197434</v>
+      </c>
+      <c r="P19">
+        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <v>0.99786263301991374</v>
+      </c>
+      <c r="Q19">
+        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <v>0.99820089095140607</v>
+      </c>
+      <c r="R19">
+        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <v>0.9985000195681506</v>
+      </c>
+      <c r="S19">
+        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <v>0.99876223194673974</v>
+      </c>
+      <c r="T19">
+        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <v>0.99898990620501338</v>
+      </c>
+      <c r="U19">
+        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <v>0.9991855594995066</v>
+      </c>
+      <c r="V19">
+        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <v>0.99935181744050361</v>
+      </c>
+      <c r="W19">
+        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <v>0.99949137932483567</v>
+      </c>
+    </row>
+    <row r="20" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>1.7</v>
+      </c>
+      <c r="C20">
+        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <v>0.99061329446516144</v>
+      </c>
+      <c r="D20">
+        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <v>0.9914786860812399</v>
+      </c>
+      <c r="E20">
+        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <v>0.99229676317508175</v>
+      </c>
+      <c r="F20">
+        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <v>0.99306732427326405</v>
+      </c>
+      <c r="G20">
+        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <v>0.99379033467422384</v>
+      </c>
+      <c r="H20">
+        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <v>0.99446593693750274</v>
+      </c>
+      <c r="I20">
+        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <v>0.99509446035679117</v>
+      </c>
+      <c r="J20">
+        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <v>0.99567642909881338</v>
+      </c>
+      <c r="K20">
+        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <v>0.99621256866269048</v>
+      </c>
+      <c r="L20">
+        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <v>0.99670381029225796</v>
+      </c>
+      <c r="M20">
+        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <v>0.99715129295938176</v>
+      </c>
+      <c r="N20">
+        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <v>0.99755636253257118</v>
+      </c>
+      <c r="O20">
+        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <v>0.99792056775540883</v>
+      </c>
+      <c r="P20">
+        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <v>0.99824565268711207</v>
+      </c>
+      <c r="Q20">
+        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <v>0.99853354530660077</v>
+      </c>
+      <c r="R20">
+        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <v>0.99878634205533956</v>
+      </c>
+      <c r="S20">
+        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <v>0.99900628819602255</v>
+      </c>
+      <c r="T20">
+        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <v>0.99919575399596294</v>
+      </c>
+      <c r="U20">
+        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <v>0.99935720690637442</v>
+      </c>
+      <c r="V20">
+        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <v>0.99949318009983712</v>
+      </c>
+      <c r="W20">
+        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <v>0.99960623794332182</v>
+      </c>
+    </row>
+    <row r="21" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>1.8</v>
+      </c>
+      <c r="C21">
+        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <v>0.99180246407540384</v>
+      </c>
+      <c r="D21">
+        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <v>0.9925859039167042</v>
+      </c>
+      <c r="E21">
+        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <v>0.99332375501779535</v>
+      </c>
+      <c r="F21">
+        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <v>0.9940160431794185</v>
+      </c>
+      <c r="G21">
+        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <v>0.99466296029774037</v>
+      </c>
+      <c r="H21">
+        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <v>0.99526487252223783</v>
+      </c>
+      <c r="I21">
+        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <v>0.99582232714110541</v>
+      </c>
+      <c r="J21">
+        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <v>0.99633605788946533</v>
+      </c>
+      <c r="K21">
+        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <v>0.99680698835864645</v>
+      </c>
+      <c r="L21">
+        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <v>0.9972362331748813</v>
+      </c>
+      <c r="M21">
+        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <v>0.99762509661539056</v>
+      </c>
+      <c r="N21">
+        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <v>0.99797506834174698</v>
+      </c>
+      <c r="O21">
+        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <v>0.99828781595757443</v>
+      </c>
+      <c r="P21">
+        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <v>0.99856517414304602</v>
+      </c>
+      <c r="Q21">
+        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <v>0.99880913018513184</v>
+      </c>
+      <c r="R21">
+        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <v>0.99902180581250244</v>
+      </c>
+      <c r="S21">
+        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <v>0.99920543535894968</v>
+      </c>
+      <c r="T21">
+        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <v>0.99936234041936356</v>
+      </c>
+      <c r="U21">
+        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <v>0.99949490132603891</v>
+      </c>
+      <c r="V21">
+        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <v>0.99960552595622765</v>
+      </c>
+      <c r="W21">
+        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <v>0.99969661657718201</v>
+      </c>
+    </row>
+    <row r="22" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>1.9</v>
+      </c>
+      <c r="C22">
+        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <v>0.99285718926472855</v>
+      </c>
+      <c r="D22">
+        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <v>0.99356433425440716</v>
+      </c>
+      <c r="E22">
+        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <v>0.9942278008261155</v>
+      </c>
+      <c r="F22">
+        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <v>0.99484782257686355</v>
+      </c>
+      <c r="G22">
+        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <v>0.995424795737889</v>
+      </c>
+      <c r="H22">
+        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <v>0.99595928497776753</v>
+      </c>
+      <c r="I22">
+        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <v>0.99645202772823449</v>
+      </c>
+      <c r="J22">
+        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <v>0.9969039367509489</v>
+      </c>
+      <c r="K22">
+        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <v>0.99731610065702081</v>
+      </c>
+      <c r="L22">
+        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <v>0.99768978209323977</v>
+      </c>
+      <c r="M22">
+        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <v>0.99802641332185826</v>
+      </c>
+      <c r="N22">
+        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <v>0.99832758894694029</v>
+      </c>
+      <c r="O22">
+        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <v>0.99859505558209449</v>
+      </c>
+      <c r="P22">
+        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <v>0.99883069831415505</v>
+      </c>
+      <c r="Q22">
+        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <v>0.99903652389688324</v>
+      </c>
+      <c r="R22">
+        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <v>0.99921464070916677</v>
+      </c>
+      <c r="S22">
+        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <v>0.99936723563349539</v>
+      </c>
+      <c r="T22">
+        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <v>0.99949654815113109</v>
+      </c>
+      <c r="U22">
+        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <v>0.99960484210678979</v>
+      </c>
+      <c r="V22">
+        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <v>0.99969437576173004</v>
+      </c>
+      <c r="W22">
+        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <v>0.99976737092096446</v>
+      </c>
+    </row>
+    <row r="23" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <v>0.99379033467422384</v>
+      </c>
+      <c r="D23">
+        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <v>0.99442673263320192</v>
+      </c>
+      <c r="E23">
+        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <v>0.99502150780925247</v>
+      </c>
+      <c r="F23">
+        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <v>0.99557508067649803</v>
+      </c>
+      <c r="G23">
+        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <v>0.99608802840283917</v>
+      </c>
+      <c r="H23">
+        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <v>0.99656108833800094</v>
+      </c>
+      <c r="I23">
+        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <v>0.99699515987387455</v>
+      </c>
+      <c r="J23">
+        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <v>0.99739130442657642</v>
+      </c>
+      <c r="K23">
+        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <v>0.99775074329355862</v>
+      </c>
+      <c r="L23">
+        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <v>0.99807485315250621</v>
+      </c>
+      <c r="M23">
+        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <v>0.99836515899365319</v>
+      </c>
+      <c r="N23">
+        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <v>0.99862332431550138</v>
+      </c>
+      <c r="O23">
+        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <v>0.99885113846754769</v>
+      </c>
+      <c r="P23">
+        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <v>0.99905050109394478</v>
+      </c>
+      <c r="Q23">
+        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <v>0.99922340371983398</v>
+      </c>
+      <c r="R23">
+        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <v>0.99937190862726821</v>
+      </c>
+      <c r="S23">
+        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <v>0.99949812528874615</v>
+      </c>
+      <c r="T23">
+        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <v>0.99960418476031487</v>
+      </c>
+      <c r="U23">
+        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <v>0.99969221257784135</v>
+      </c>
+      <c r="V23">
+        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <v>0.9997643008419731</v>
+      </c>
+      <c r="W23">
+        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <v>0.9998224803096265</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C3:W23">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="0.95"/>
+        <cfvo type="num" val="0.98"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C2:S9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16749,12 +18783,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AB18"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Z25" sqref="Z25"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="AC15" sqref="AC15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18200,7 +20234,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
@@ -18496,7 +20530,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E19"/>
   <sheetViews>

</xml_diff>

<commit_message>
hacking away at fielding.
</commit_message>
<xml_diff>
--- a/plans/baseball stats.xlsx
+++ b/plans/baseball stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcgiffenk\Desktop\newpy\xtreemblaseball99\plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778496F6-5405-4E3A-8828-1D89E1F316CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED43DD84-53AB-4218-BCCD-C2D84024B7E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="iterative" sheetId="2" r:id="rId1"/>
@@ -2142,16 +2142,6 @@
   </cellStyles>
   <dxfs count="83">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -2493,6 +2483,16 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -9021,181 +9021,181 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A6:DO22" totalsRowShown="0" headerRowDxfId="82">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A6:DO22" totalsRowShown="0" headerRowDxfId="81">
   <autoFilter ref="A6:DO22" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="119">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Rep #">
       <calculatedColumnFormula>ROW()-ROW(home)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="offense" dataDxfId="81">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="offense" dataDxfId="80">
       <calculatedColumnFormula>INDEX(oratings, 1, 1+MOD(Table3[[#This Row],[Rep '#]]-1, COUNT(oratings)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="defense" dataDxfId="80">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="defense" dataDxfId="79">
       <calculatedColumnFormula>INDEX(dratings, 1, MOD(FLOOR( (Table3[[#This Row],[Rep '#]]-1) / COUNT(oratings), 1), COUNT(dratings))+1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="base leadoff" dataDxfId="79">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="base leadoff" dataDxfId="78">
       <calculatedColumnFormula>Table3[[#This Row],[offense]]*$D$26+0.05</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="leadoff modifier" dataDxfId="78">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="leadoff modifier" dataDxfId="77">
       <calculatedColumnFormula>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*$E$26</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="total leadoff (ft)" dataDxfId="77">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="total leadoff (ft)" dataDxfId="76">
       <calculatedColumnFormula>MAX(Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90, 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="pickoff manuver (s)" dataDxfId="76">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="pickoff manuver (s)" dataDxfId="75">
       <calculatedColumnFormula>1.1 - Table3[[#This Row],[defense]]*0.1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="throw speed (s/ft)" dataDxfId="75">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="throw speed (s/ft)" dataDxfId="74">
       <calculatedColumnFormula xml:space="preserve"> 0.01 - 0.0025 *  Table3[[#This Row],[defense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="throw speed (mph)" dataDxfId="74">
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="throw speed (mph)" dataDxfId="73">
       <calculatedColumnFormula>1 / Table3[[#This Row],[throw speed (s/ft)]] * ((60 * 60)/5280)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="pickoff time" dataDxfId="73">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="pickoff time" dataDxfId="72">
       <calculatedColumnFormula>Table3[[#This Row],[pickoff manuver (s)]]+60*Table3[[#This Row],[throw speed (s/ft)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="runner reaction" dataDxfId="72">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="runner reaction" dataDxfId="71">
       <calculatedColumnFormula>$K$28-$K$26*Table3[[#This Row],[offense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="runner speed (s/ft)" dataDxfId="71">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="runner speed (s/ft)" dataDxfId="70">
       <calculatedColumnFormula>0.05 - Table3[[#This Row],[offense]]*$L$26</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="runner speed (mph)" dataDxfId="70">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="runner speed (mph)" dataDxfId="69">
       <calculatedColumnFormula>1 / Table3[[#This Row],[runner speed (s/ft)]] * ((60 * 60)/5280)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="pickoff evade time" dataDxfId="69">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="pickoff evade time" dataDxfId="68">
       <calculatedColumnFormula>Table3[[#This Row],[runner reaction]]+Table3[[#This Row],[runner speed (s/ft)]]*Table3[[#This Row],[total leadoff (ft)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="pickoff probability" dataDxfId="68" dataCellStyle="Percent">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="pickoff probability" dataDxfId="67" dataCellStyle="Percent">
       <calculatedColumnFormula>1 - _xlfn.NORM.DIST(Table3[[#This Row],[pickoff time]], Table3[[#This Row],[pickoff evade time]], $O$4, TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Fielding Odds" dataDxfId="67" dataCellStyle="Percent">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Fielding Odds" dataDxfId="66" dataCellStyle="Percent">
       <calculatedColumnFormula>_xlfn.NORM.DIST(Table3[[#This Row],[defense]], $P$26, $P$27, TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="pickoff worth it?" dataDxfId="66">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="pickoff worth it?" dataDxfId="65">
       <calculatedColumnFormula>Table3[[#This Row],[pickoff probability]] &gt; 1-Table3[[#This Row],[Fielding Odds]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Error %" dataDxfId="65" dataCellStyle="Percent">
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Error %" dataDxfId="64" dataCellStyle="Percent">
       <calculatedColumnFormula>1-Table3[[#This Row],[Fielding Odds]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Blatant steal time" dataDxfId="64">
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Blatant steal time" dataDxfId="63">
       <calculatedColumnFormula>(90-Table3[[#This Row],[total leadoff (ft)]])*Table3[[#This Row],[runner speed (s/ft)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Response speed" dataDxfId="63">
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Response speed" dataDxfId="62">
       <calculatedColumnFormula>$T$26*(2-Table3[[#This Row],[defense]]) + Table3[[#This Row],[pickoff time]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="blatant steal probability" dataDxfId="62" dataCellStyle="Percent">
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="blatant steal probability" dataDxfId="61" dataCellStyle="Percent">
       <calculatedColumnFormula>_xlfn.NORM.DIST(Table3[[#This Row],[Response speed]], Table3[[#This Row],[Blatant steal time]], $U$4, TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="defense fear" dataDxfId="61">
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="defense fear" dataDxfId="60">
       <calculatedColumnFormula>Table3[[#This Row],[defense]]+Table3[[#This Row],[defense]]*Table3[[#This Row],[offense]]*$E$26</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="ball factor" dataDxfId="60">
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="ball factor" dataDxfId="59">
       <calculatedColumnFormula>(1-$W$32)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="desperation" dataDxfId="59" dataCellStyle="Percent">
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="desperation" dataDxfId="58" dataCellStyle="Percent">
       <calculatedColumnFormula>Table3[[#This Row],[ball factor]]/$X$32*(1-$X$34)+$X$34</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="player control" dataDxfId="58">
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="player control" dataDxfId="57">
       <calculatedColumnFormula>Table3[[#This Row],[offense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="ideal steer" dataDxfId="57">
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="ideal steer" dataDxfId="56">
       <calculatedColumnFormula>$AA$33</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="scaled control" dataDxfId="56">
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="scaled control" dataDxfId="55">
       <calculatedColumnFormula>IF(Table3[[#This Row],[player control]]&gt;1,Table3[[#This Row],[player control]]*$AA$41+$AA$40,Table3[[#This Row],[player control]]*$AA$39+$AA$38)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="unmod foul percent 3rd" dataDxfId="55" dataCellStyle="Percent">
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="unmod foul percent 3rd" dataDxfId="54" dataCellStyle="Percent">
       <calculatedColumnFormula>_xlfn.NORM.DIST(-1,Table3[[#This Row],[ideal steer]],($AB$25-Table3[[#This Row],[scaled control]])*$AB$27,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="unmod foul percent 1st" dataDxfId="54" dataCellStyle="Percent">
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="unmod foul percent 1st" dataDxfId="53" dataCellStyle="Percent">
       <calculatedColumnFormula>1-_xlfn.NORM.DIST(1,Table3[[#This Row],[ideal steer]],($AB$25-Table3[[#This Row],[scaled control]])*$AB$27,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="total unmod foul percent" dataDxfId="53" dataCellStyle="Percent">
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="total unmod foul percent" dataDxfId="52" dataCellStyle="Percent">
       <calculatedColumnFormula>1-(1-Table3[[#This Row],[unmod foul percent 3rd]])*(1-Table3[[#This Row],[unmod foul percent 1st]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="unmod dead center foul%" dataDxfId="52" dataCellStyle="Percent">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="unmod dead center foul%" dataDxfId="51" dataCellStyle="Percent">
       <calculatedColumnFormula>1-((1-_xlfn.NORM.DIST(-1,0,($AB$25-Table3[[#This Row],[scaled control]])*$AB$27,TRUE))*_xlfn.NORM.DIST(1,0,($AB$25-Table3[[#This Row],[scaled control]])*$AB$27,TRUE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="count" dataDxfId="51">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="count" dataDxfId="50">
       <calculatedColumnFormula>$AF$34*$AF$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="hitter discipline bias" dataDxfId="50">
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="hitter discipline bias" dataDxfId="49">
       <calculatedColumnFormula>$AG$25*($AG$34*Table3[[#This Row],[offense]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="bases loaded" dataDxfId="49">
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="bases loaded" dataDxfId="48">
       <calculatedColumnFormula>$AH$25*$AH$34</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="number of outs" dataDxfId="48">
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="number of outs" dataDxfId="47">
       <calculatedColumnFormula>$AI$34*$AI$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="current hitter vs next hitter" dataDxfId="47">
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="current hitter vs next hitter" dataDxfId="46">
       <calculatedColumnFormula>$AJ$25*(Table3[[#This Row],[offense]]-$AJ$27)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="calling modifier" dataDxfId="46">
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="calling modifier" dataDxfId="45">
       <calculatedColumnFormula array="1">SUM(Table3[[#This Row],[count]:[current hitter vs next hitter]]*MIN(1, Table3[[#This Row],[defense]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="sigmoid strike percent" dataDxfId="45" dataCellStyle="Percent">
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="sigmoid strike percent" dataDxfId="44" dataCellStyle="Percent">
       <calculatedColumnFormula>$AL$25-(Table3[[#This Row],[calling modifier]]/(ABS(Table3[[#This Row],[calling modifier]])+$AL$29)*$AL$27)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="tanh strike percent" dataDxfId="44" dataCellStyle="Percent">
+    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="tanh strike percent" dataDxfId="43" dataCellStyle="Percent">
       <calculatedColumnFormula>$AL$25-$AL$27*TANH(Table3[[#This Row],[calling modifier]]/$AM$29)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="called position" dataDxfId="43" dataCellStyle="Percent">
+    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="called position" dataDxfId="42" dataCellStyle="Percent">
       <calculatedColumnFormula>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-Table3[[#This Row],[defense]])))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="called pos 0.2 pitch" dataDxfId="42">
+    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="called pos 0.2 pitch" dataDxfId="41">
       <calculatedColumnFormula>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-0.2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="called pos 2 pitch" dataDxfId="41">
+    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="called pos 2 pitch" dataDxfId="40">
       <calculatedColumnFormula>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="location -1  stdv" dataDxfId="40">
+    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="location -1  stdv" dataDxfId="39">
       <calculatedColumnFormula>Table3[[#This Row],[called position]]-pitchmod*(pitchstdv-Table3[[#This Row],[defense]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="location +1 stdv" dataDxfId="39">
+    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="location +1 stdv" dataDxfId="38">
       <calculatedColumnFormula>ABS(Table3[[#This Row],[called position]]+pitchmod*(pitchstdv-Table3[[#This Row],[defense]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="min dist to sz 1stdv" dataDxfId="38">
+    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="min dist to sz 1stdv" dataDxfId="37">
       <calculatedColumnFormula>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;1, Table3[[#This Row],[location +1 stdv]]&gt;1),0, MIN(Table3[[#This Row],[location -1  stdv]]+1, 1-Table3[[#This Row],[location +1 stdv]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="max dist to sz 1stdv" dataDxfId="37">
+    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="max dist to sz 1stdv" dataDxfId="36">
       <calculatedColumnFormula>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;0, Table3[[#This Row],[location +1 stdv]]&gt;0),1, MAX(1-ABS(Table3[[#This Row],[location -1  stdv]]), Table3[[#This Row],[location +1 stdv]]-1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="ave obscurity" dataDxfId="36">
+    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="ave obscurity" dataDxfId="35">
       <calculatedColumnFormula>$AU$30/(ABS(Table3[[#This Row],[called position]]-1)+$AU$27)+$AU$32*Table3[[#This Row],[defense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="obscurity at _x000a_0.5" dataDxfId="35">
+    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="obscurity at _x000a_0.5" dataDxfId="34">
       <calculatedColumnFormula>$AU$30/(ABS(0.5-1)+$AU$27)+$AU$32*Table3[[#This Row],[defense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="obscurity at  0.9" dataDxfId="34">
+    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="obscurity at  0.9" dataDxfId="33">
       <calculatedColumnFormula>$AU$30/(ABS(0.9-1)+$AU$27)+$AU$32*Table3[[#This Row],[defense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="average difficulty" dataDxfId="33">
+    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="average difficulty" dataDxfId="32">
       <calculatedColumnFormula>Table3[[#This Row],[defense]]*$AX$30+MAX(0, Table3[[#This Row],[called position]]-$AX$27)^$AX$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" name="+1stdv difficulty" dataDxfId="32">
+    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" name="+1stdv difficulty" dataDxfId="31">
       <calculatedColumnFormula>Table3[[#This Row],[defense]]*$AX$30 + MAX(0, Table3[[#This Row],[location +1 stdv]]-$AX$27)^$AX$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0000-000037000000}" name="difficulty at 1" dataDxfId="31">
+    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0000-000037000000}" name="difficulty at 1" dataDxfId="30">
       <calculatedColumnFormula>Table3[[#This Row],[defense]]*$AX$30+MAX(0, 1-$AX$27)^$AX$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="62" xr3:uid="{6513900D-2CAC-4022-A6B3-8A00EE6C566B}" name="reduction" dataDxfId="30">
+    <tableColumn id="62" xr3:uid="{6513900D-2CAC-4022-A6B3-8A00EE6C566B}" name="reduction" dataDxfId="29">
       <calculatedColumnFormula>MAX(0, 0.1*(1-Table3[[#This Row],[defense]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="63" xr3:uid="{12464915-1D8C-4EB5-9BBD-0FF526658E5B}" name="Location" dataDxfId="29">
+    <tableColumn id="63" xr3:uid="{12464915-1D8C-4EB5-9BBD-0FF526658E5B}" name="Location" dataDxfId="28">
       <calculatedColumnFormula>$BB$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="64" xr3:uid="{5F0F19BE-6D04-4E9E-81B2-B324AB353F5C}" name="obscurity" dataDxfId="28">
+    <tableColumn id="64" xr3:uid="{5F0F19BE-6D04-4E9E-81B2-B324AB353F5C}" name="obscurity" dataDxfId="27">
       <calculatedColumnFormula>$AU$30/(ABS(Table3[[#This Row],[Location]]-1)+$AU$27)+$AU$32*Table3[[#This Row],[defense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="65" xr3:uid="{EA3D32E7-A2E2-482C-B6E9-2E17651C5F77}" name="Strike?" dataDxfId="27">
+    <tableColumn id="65" xr3:uid="{EA3D32E7-A2E2-482C-B6E9-2E17651C5F77}" name="Strike?" dataDxfId="26">
       <calculatedColumnFormula>Table3[[#This Row],[Location]]&lt;= (1+MAX(0, (Table3[[#This Row],[defense]]-1)*0.1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="66" xr3:uid="{0C7E9B06-240B-481E-B495-54026E2F00AA}" name="discipline modifier" dataDxfId="26">
+    <tableColumn id="66" xr3:uid="{0C7E9B06-240B-481E-B495-54026E2F00AA}" name="discipline modifier" dataDxfId="25">
       <calculatedColumnFormula>1/(1+Table3[[#This Row],[offense]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="67" xr3:uid="{D3B0837D-02D4-4F62-A2E2-876739E497B0}" name="effective obscurity" dataDxfId="25">
+    <tableColumn id="67" xr3:uid="{D3B0837D-02D4-4F62-A2E2-876739E497B0}" name="effective obscurity" dataDxfId="24">
       <calculatedColumnFormula>Table3[[#This Row],[obscurity]]*Table3[[#This Row],[discipline modifier]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="69" xr3:uid="{39822A5F-1791-48DC-BA9F-A066931C0292}" name="odds of read" dataCellStyle="Percent">
@@ -9210,43 +9210,43 @@
     <tableColumn id="72" xr3:uid="{3E21C76F-F55B-4E49-9BE2-FEE046008C15}" name="adjusted swing %" dataCellStyle="Percent">
       <calculatedColumnFormula>Table3[[#This Row],[desperation echo]]*Table3[[#This Row],[unadjusted swing %]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="130" xr3:uid="{827C9303-3867-43F7-A79B-BC2EAB3F896D}" name="pitch carry forward obsc" dataDxfId="24">
+    <tableColumn id="130" xr3:uid="{827C9303-3867-43F7-A79B-BC2EAB3F896D}" name="pitch carry forward obsc" dataDxfId="23">
       <calculatedColumnFormula>Table3[[#This Row],[ave obscurity]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="131" xr3:uid="{F26B1E2C-89D5-4F6D-877A-1BEA7F7DF5A9}" name="CF odds of read" dataCellStyle="Percent">
       <calculatedColumnFormula>1/(1+Table3[[#This Row],[ave obscurity]]*Table3[[#This Row],[discipline modifier]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="73" xr3:uid="{77BBE784-030D-4E46-9A29-8783B89762BC}" name="contact echo" dataDxfId="23">
+    <tableColumn id="73" xr3:uid="{77BBE784-030D-4E46-9A29-8783B89762BC}" name="contact echo" dataDxfId="22">
       <calculatedColumnFormula>Table3[[#This Row],[offense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="75" xr3:uid="{074A9F48-3941-4E36-90C2-7710217D32C8}" name="pitch carry forward diff" dataDxfId="22">
+    <tableColumn id="75" xr3:uid="{074A9F48-3941-4E36-90C2-7710217D32C8}" name="pitch carry forward diff" dataDxfId="21">
       <calculatedColumnFormula>Table3[[#This Row],[average difficulty]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="76" xr3:uid="{628DDA60-D380-4EE8-AA7D-7EF6C4AAD8A5}" name="CF contact readiness" dataDxfId="21">
+    <tableColumn id="76" xr3:uid="{628DDA60-D380-4EE8-AA7D-7EF6C4AAD8A5}" name="CF contact readiness" dataDxfId="20">
       <calculatedColumnFormula>Table3[[#This Row],[contact echo]]-Table3[[#This Row],[pitch carry forward diff]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="77" xr3:uid="{DBF18AD6-8593-42C7-9058-D19737088E6D}" name="foul %" dataDxfId="20" dataCellStyle="Percent">
+    <tableColumn id="77" xr3:uid="{DBF18AD6-8593-42C7-9058-D19737088E6D}" name="foul %" dataDxfId="19" dataCellStyle="Percent">
       <calculatedColumnFormula>1-_xlfn.NORM.DIST($BP$27,Table3[[#This Row],[CF contact readiness]], $BP$30,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="78" xr3:uid="{6354951A-151E-4E04-9897-9CB39D6098C8}" name="clean %" dataDxfId="19" dataCellStyle="Percent">
+    <tableColumn id="78" xr3:uid="{6354951A-151E-4E04-9897-9CB39D6098C8}" name="clean %" dataDxfId="18" dataCellStyle="Percent">
       <calculatedColumnFormula>1-_xlfn.NORM.DIST($BP$25,Table3[[#This Row],[CF contact readiness]], $BP$30,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="79" xr3:uid="{0070F673-D13C-467D-95AC-FF8413A02F3F}" name="strike swinging %" dataDxfId="18" dataCellStyle="Percent">
+    <tableColumn id="79" xr3:uid="{0070F673-D13C-467D-95AC-FF8413A02F3F}" name="strike swinging %" dataDxfId="17" dataCellStyle="Percent">
       <calculatedColumnFormula>1-Table3[[#This Row],[foul %]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="80" xr3:uid="{9504D0CF-7CD0-472F-8289-44B30538D80C}" name="ave. hit quality" dataDxfId="17">
+    <tableColumn id="80" xr3:uid="{9504D0CF-7CD0-472F-8289-44B30538D80C}" name="ave. hit quality" dataDxfId="16">
       <calculatedColumnFormula>(Table3[[#This Row],[CF contact readiness]]-$BP$27)/$BP$30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="132" xr3:uid="{0BB169E4-F345-4B7D-A549-DE28DC5FB113}" name="hit quality +1stdv" dataDxfId="16">
+    <tableColumn id="132" xr3:uid="{0BB169E4-F345-4B7D-A549-DE28DC5FB113}" name="hit quality +1stdv" dataDxfId="15">
       <calculatedColumnFormula>(Table3[[#This Row],[CF contact readiness]]+$BP$30-$BP$27)/$BP$30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="81" xr3:uid="{37438EAA-344A-486C-A4C2-68EE17D67C60}" name="hit quality remainder" dataDxfId="15">
+    <tableColumn id="81" xr3:uid="{37438EAA-344A-486C-A4C2-68EE17D67C60}" name="hit quality remainder" dataDxfId="14">
       <calculatedColumnFormula>MAX(0, IF(ISBLANK($BU$28), Table3[[#This Row],[hit quality +1stdv]], $BU$28)-1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="82" xr3:uid="{CBA11BEE-0412-44C3-979C-1888629B3C7A}" name="adjusted launch angle" dataDxfId="14">
+    <tableColumn id="82" xr3:uid="{CBA11BEE-0412-44C3-979C-1888629B3C7A}" name="adjusted launch angle" dataDxfId="13">
       <calculatedColumnFormula>$BV$25+Table3[[#This Row],[offense]]*$BV$28</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="83" xr3:uid="{8DC0E209-2987-40FE-9521-B3339A7D8E1F}" name="angle stdev" dataDxfId="13">
+    <tableColumn id="83" xr3:uid="{8DC0E209-2987-40FE-9521-B3339A7D8E1F}" name="angle stdev" dataDxfId="12">
       <calculatedColumnFormula>$BW$25*$BW$28/($BW$28+Table3[[#This Row],[hit quality remainder]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="84" xr3:uid="{F8EB7F4C-5D31-472E-A363-210E62A7E683}" name="grounder % (&lt;10 deg)" dataCellStyle="Percent">
@@ -9255,37 +9255,37 @@
     <tableColumn id="85" xr3:uid="{56DD6E0A-39C0-4DF0-B1CB-47EB71B71306}" name="pop up % (&gt;50 deg)" dataCellStyle="Percent">
       <calculatedColumnFormula>1-_xlfn.NORM.DIST(50, Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="86" xr3:uid="{6ED971D4-0303-4AEB-B7CD-9516517F447E}" name="odds of 3B" dataDxfId="12" dataCellStyle="Percent">
+    <tableColumn id="86" xr3:uid="{6ED971D4-0303-4AEB-B7CD-9516517F447E}" name="odds of 3B" dataDxfId="11" dataCellStyle="Percent">
       <calculatedColumnFormula>1-_xlfn.NORM.DIST(70, $BZ$28,$BZ$25,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="87" xr3:uid="{E9F9DFB6-4A26-4CA7-9318-6ECA478690D6}" name="exit velocity mean" dataDxfId="11">
+    <tableColumn id="87" xr3:uid="{E9F9DFB6-4A26-4CA7-9318-6ECA478690D6}" name="exit velocity mean" dataDxfId="10">
       <calculatedColumnFormula>$CA$25+Table3[[#This Row],[offense]]*($CA$27-$CA$25)/2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="88" xr3:uid="{EB865A5D-CC1D-49FA-9709-DC5F30F55DD8}" name="after reduction" dataDxfId="10">
+    <tableColumn id="88" xr3:uid="{EB865A5D-CC1D-49FA-9709-DC5F30F55DD8}" name="after reduction" dataDxfId="9">
       <calculatedColumnFormula>Table3[[#This Row],[exit velocity mean]]-Table3[[#This Row],[reduction]]*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="89" xr3:uid="{949E8C38-C424-4A4E-9A6F-FCA93496D192}" name="theoretical distance" dataDxfId="9">
+    <tableColumn id="89" xr3:uid="{949E8C38-C424-4A4E-9A6F-FCA93496D192}" name="theoretical distance" dataDxfId="8">
       <calculatedColumnFormula>Table3[[#This Row],[exit velocity mean]]^2*2*SIN(RADIANS(Table3[[#This Row],[adjusted launch angle]]))/$CC$28*5280</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="90" xr3:uid="{9FD0A88A-D0D9-4369-8D70-6C7485CA1509}" name="flight time" dataDxfId="8">
+    <tableColumn id="90" xr3:uid="{9FD0A88A-D0D9-4369-8D70-6C7485CA1509}" name="flight time" dataDxfId="7">
       <calculatedColumnFormula>2*Table3[[#This Row],[exit velocity mean]]*SIN(RADIANS(Table3[[#This Row],[adjusted launch angle]]))/$CC$28*60*60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="91" xr3:uid="{D9D5DFED-BD09-4CB6-A82E-D289D2DAB08D}" name="actual distance" dataDxfId="7">
+    <tableColumn id="91" xr3:uid="{D9D5DFED-BD09-4CB6-A82E-D289D2DAB08D}" name="actual distance" dataDxfId="6">
       <calculatedColumnFormula>Table3[[#This Row],[theoretical distance]]-Table3[[#This Row],[flight time]]^2*$CE$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="92" xr3:uid="{3D80331E-564D-462D-81B5-E5CE730D1EE5}" name="+1stdv EV" dataDxfId="6">
+    <tableColumn id="92" xr3:uid="{3D80331E-564D-462D-81B5-E5CE730D1EE5}" name="+1stdv EV" dataDxfId="5">
       <calculatedColumnFormula>Table3[[#This Row],[exit velocity mean]]+$CC$25-Table3[[#This Row],[reduction]]*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="93" xr3:uid="{211123A1-65C0-4F59-AB86-C344CFF47F70}" name="+1stdv LA" dataDxfId="5">
+    <tableColumn id="93" xr3:uid="{211123A1-65C0-4F59-AB86-C344CFF47F70}" name="+1stdv LA" dataDxfId="4">
       <calculatedColumnFormula>MIN(Table3[[#This Row],[adjusted launch angle]]+Table3[[#This Row],[angle stdev]], 30)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="94" xr3:uid="{C8736D16-AF27-436D-BF61-CA3E58298CD3}" name="+1stdv flight time" dataDxfId="4">
+    <tableColumn id="94" xr3:uid="{C8736D16-AF27-436D-BF61-CA3E58298CD3}" name="+1stdv flight time" dataDxfId="3">
       <calculatedColumnFormula>2*Table3[[#This Row],[+1stdv EV]]*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*60*60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="95" xr3:uid="{C9967388-9755-4293-82E9-4E43A4770599}" name="+1stdev distance" dataDxfId="3">
+    <tableColumn id="95" xr3:uid="{C9967388-9755-4293-82E9-4E43A4770599}" name="+1stdev distance" dataDxfId="2">
       <calculatedColumnFormula>Table3[[#This Row],[+1stdv EV]]^2*2*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*5280-Table3[[#This Row],[+1stdv flight time]]^2*$CE$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="96" xr3:uid="{52B6BA3A-87F7-49FD-BFE7-811EA76B03FD}" name="+1stdev delta" dataDxfId="2">
+    <tableColumn id="96" xr3:uid="{52B6BA3A-87F7-49FD-BFE7-811EA76B03FD}" name="+1stdev delta" dataDxfId="1">
       <calculatedColumnFormula>Table3[[#This Row],[+1stdev distance]]-Table3[[#This Row],[actual distance]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="97" xr3:uid="{50EEB2EF-C836-4BBC-A8B3-EAD31BF29B54}" name="Column95"/>
@@ -9330,7 +9330,7 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{23FB116D-6CB4-49F6-A874-F1C610DEF5E1}" name="quality"/>
     <tableColumn id="2" xr3:uid="{6204ECDD-C980-4BE0-AFC7-9F83BF472BE8}" name="net"/>
-    <tableColumn id="3" xr3:uid="{E9208F79-490A-4A40-B3B7-0914BA16AC90}" name="form" dataDxfId="1">
+    <tableColumn id="3" xr3:uid="{E9208F79-490A-4A40-B3B7-0914BA16AC90}" name="form" dataDxfId="0">
       <calculatedColumnFormula>POWER(Table1[[#This Row],[quality]]-0.8, 1/4)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9603,8 +9603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DO41"/>
   <sheetViews>
-    <sheetView topLeftCell="CH1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CL30" sqref="CL30"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16442,7 +16442,7 @@
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
   <conditionalFormatting sqref="O7:O22">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16663,87 +16663,87 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <f t="shared" ref="C3:L12" si="0">_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
         <v>0.93319279873114191</v>
       </c>
       <c r="D3">
-        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.93610096034524259</v>
       </c>
       <c r="E3">
-        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.93899500761383359</v>
       </c>
       <c r="F3">
-        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.941871574470311</v>
       </c>
       <c r="G3">
-        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.94472709570688829</v>
       </c>
       <c r="H3">
-        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.94755780490616992</v>
       </c>
       <c r="I3">
-        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.95035973404319185</v>
       </c>
       <c r="J3">
-        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.95312871510773034</v>
       </c>
       <c r="K3">
-        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.95586038414193264</v>
       </c>
       <c r="L3">
-        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.95855018813574422</v>
       </c>
       <c r="M3">
-        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <f t="shared" ref="M3:W12" si="1">_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
         <v>0.96119339527114878</v>
       </c>
       <c r="N3">
-        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.96378510905435966</v>
       </c>
       <c r="O3">
-        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.96632028692061955</v>
       </c>
       <c r="P3">
-        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.96879376393622496</v>
       </c>
       <c r="Q3">
-        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.97120028225284716</v>
       </c>
       <c r="R3">
-        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.97353452698506504</v>
       </c>
       <c r="S3">
-        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.97579116917672093</v>
       </c>
       <c r="T3">
-        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.97796491648714601</v>
       </c>
       <c r="U3">
-        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98005057215450919</v>
       </c>
       <c r="V3">
-        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98204310266867123</v>
       </c>
       <c r="W3">
-        <f>_xlfn.NORM.DIST($B3, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98393771439617173</v>
       </c>
     </row>
@@ -16752,87 +16752,87 @@
         <v>0.1</v>
       </c>
       <c r="C4">
-        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.93942924199794098</v>
       </c>
       <c r="D4">
-        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.94221049307757543</v>
       </c>
       <c r="E4">
-        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.94497162805414114</v>
       </c>
       <c r="F4">
-        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.94770921469607072</v>
       </c>
       <c r="G4">
-        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.95041964397531165</v>
       </c>
       <c r="H4">
-        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.95309913157177895</v>
       </c>
       <c r="I4">
-        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.95574372137968222</v>
       </c>
       <c r="J4">
-        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.9583492913688767</v>
       </c>
       <c r="K4">
-        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.96091156219176899</v>
       </c>
       <c r="L4">
-        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.96342610896336511</v>
       </c>
       <c r="M4">
-        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.96588837667724492</v>
       </c>
       <c r="N4">
-        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.96829369975146407</v>
       </c>
       <c r="O4">
-        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.97063732622285248</v>
       </c>
       <c r="P4">
-        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.97291444712231223</v>
       </c>
       <c r="Q4">
-        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.97512023156297545</v>
       </c>
       <c r="R4">
-        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.97724986805182079</v>
       </c>
       <c r="S4">
-        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.97929861248667271</v>
       </c>
       <c r="T4">
-        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98126184321621246</v>
       </c>
       <c r="U4">
-        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98313512341112752</v>
       </c>
       <c r="V4">
-        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98491427080899996</v>
       </c>
       <c r="W4">
-        <f>_xlfn.NORM.DIST($B4, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98659543464220212</v>
       </c>
     </row>
@@ -16841,87 +16841,87 @@
         <v>0.2</v>
       </c>
       <c r="C5">
-        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.94520070830044201</v>
       </c>
       <c r="D5">
-        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.94785108530229123</v>
       </c>
       <c r="E5">
-        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.95047579566670537</v>
       </c>
       <c r="F5">
-        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.95307139309539912</v>
       </c>
       <c r="G5">
-        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.9556342800557962</v>
       </c>
       <c r="H5">
-        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.95816071278906079</v>
       </c>
       <c r="I5">
-        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.96064680858347651</v>
       </c>
       <c r="J5">
-        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.96308855565481921</v>
       </c>
       <c r="K5">
-        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.96548182600279242</v>
       </c>
       <c r="L5">
-        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.96782239163714201</v>
       </c>
       <c r="M5">
-        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.97010594458676791</v>
       </c>
       <c r="N5">
-        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.97232812111745404</v>
       </c>
       <c r="O5">
-        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.97448453058555684</v>
       </c>
       <c r="P5">
-        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.97657078934214148</v>
       </c>
       <c r="Q5">
-        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.97858256006982691</v>
       </c>
       <c r="R5">
-        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98051559687722489</v>
       </c>
       <c r="S5">
-        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98236579638662769</v>
       </c>
       <c r="T5">
-        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98412925492187275</v>
       </c>
       <c r="U5">
-        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98580233172670073</v>
       </c>
       <c r="V5">
-        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98738171791059692</v>
       </c>
       <c r="W5">
-        <f>_xlfn.NORM.DIST($B5, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.9888645105203836</v>
       </c>
     </row>
@@ -16930,87 +16930,87 @@
         <v>0.3</v>
       </c>
       <c r="C6">
-        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.9505285319663519</v>
       </c>
       <c r="D6">
-        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.95304533229487931</v>
       </c>
       <c r="E6">
-        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.95553141012261578</v>
       </c>
       <c r="F6">
-        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.95798335506905641</v>
       </c>
       <c r="G6">
-        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.96039763356816699</v>
       </c>
       <c r="H6">
-        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.96277059720355673</v>
       </c>
       <c r="I6">
-        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.96509849349527255</v>
       </c>
       <c r="J6">
-        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.96737747945404673</v>
       </c>
       <c r="K6">
-        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.96960363823473861</v>
       </c>
       <c r="L6">
-        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.97177299923126637</v>
       </c>
       <c r="M6">
-        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.97388156195825992</v>
       </c>
       <c r="N6">
-        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.97592532405714871</v>
       </c>
       <c r="O6">
-        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.97790031374301589</v>
       </c>
       <c r="P6">
-        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.97980262696922982</v>
       </c>
       <c r="Q6">
-        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98162846952483385</v>
       </c>
       <c r="R6">
-        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98337420418952204</v>
       </c>
       <c r="S6">
-        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98503640294671146</v>
       </c>
       <c r="T6">
-        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98661190409033794</v>
       </c>
       <c r="U6">
-        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98809787384903192</v>
       </c>
       <c r="V6">
-        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98949187188624066</v>
       </c>
       <c r="W6">
-        <f>_xlfn.NORM.DIST($B6, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.99079191971184799</v>
       </c>
     </row>
@@ -17019,87 +17019,87 @@
         <v>0.4</v>
       </c>
       <c r="C7">
-        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.95543453724145699</v>
       </c>
       <c r="D7">
-        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.95781624723514713</v>
       </c>
       <c r="E7">
-        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.96016270640197721</v>
       </c>
       <c r="F7">
-        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.96247058720650747</v>
       </c>
       <c r="G7">
-        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.96473646869703567</v>
       </c>
       <c r="H7">
-        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.96695684789416148</v>
       </c>
       <c r="I7">
-        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.96912815373421313</v>
       </c>
       <c r="J7">
-        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.97124676384449027</v>
       </c>
       <c r="K7">
-        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.9733090244307121</v>
       </c>
       <c r="L7">
-        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.97531127355290825</v>
       </c>
       <c r="M7">
-        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.97724986805182079</v>
       </c>
       <c r="N7">
-        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.9791212143607767</v>
       </c>
       <c r="O7">
-        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98092180339453061</v>
       </c>
       <c r="P7">
-        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98264824964288278</v>
       </c>
       <c r="Q7">
-        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98429733450858192</v>
       </c>
       <c r="R7">
-        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98586605381145986</v>
       </c>
       <c r="S7">
-        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98735166922903572</v>
       </c>
       <c r="T7">
-        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98875176325331959</v>
       </c>
       <c r="U7">
-        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.99006429701015009</v>
       </c>
       <c r="V7">
-        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.99128767000840101</v>
       </c>
       <c r="W7">
-        <f>_xlfn.NORM.DIST($B7, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.99242078056128025</v>
       </c>
     </row>
@@ -17108,87 +17108,87 @@
         <v>0.5</v>
       </c>
       <c r="C8">
-        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.95994084313618289</v>
       </c>
       <c r="D8">
-        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.9621870572995479</v>
       </c>
       <c r="E8">
-        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.96439404232427384</v>
       </c>
       <c r="F8">
-        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.96655859658087928</v>
       </c>
       <c r="G8">
-        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.96867745573741471</v>
       </c>
       <c r="H8">
-        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.97074730684334809</v>
       </c>
       <c r="I8">
-        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.97276480498626128</v>
       </c>
       <c r="J8">
-        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.97472659274822582</v>
       </c>
       <c r="K8">
-        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.97662932267937719</v>
       </c>
       <c r="L8">
-        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.97846968298743109</v>
       </c>
       <c r="M8">
-        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98024442661121902</v>
       </c>
       <c r="N8">
-        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98195040380095566</v>
       </c>
       <c r="O8">
-        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98358459826471212</v>
       </c>
       <c r="P8">
-        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98514416685602335</v>
       </c>
       <c r="Q8">
-        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98662648266809205</v>
       </c>
       <c r="R8">
-        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98802918126206773</v>
       </c>
       <c r="S8">
-        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98935020958708397</v>
       </c>
       <c r="T8">
-        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.99058787694556816</v>
       </c>
       <c r="U8">
-        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.99174090711751128</v>
       </c>
       <c r="V8">
-        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.99280849048270048</v>
       </c>
       <c r="W8">
-        <f>_xlfn.NORM.DIST($B8, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.99379033467422384</v>
       </c>
     </row>
@@ -17197,87 +17197,87 @@
         <v>0.6</v>
       </c>
       <c r="C9">
-        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.96406968088707423</v>
       </c>
       <c r="D9">
-        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.96618101424832259</v>
       </c>
       <c r="E9">
-        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.96824970264897547</v>
       </c>
       <c r="F9">
-        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.97027270889703676</v>
       </c>
       <c r="G9">
-        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.97224696399442845</v>
       </c>
       <c r="H9">
-        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.97416938348928472</v>
       </c>
       <c r="I9">
-        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.97603688633498631</v>
       </c>
       <c r="J9">
-        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.97784641642385983</v>
       </c>
       <c r="K9">
-        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.9795949669416939</v>
       </c>
       <c r="L9">
-        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.98127960765667077</v>
       </c>
       <c r="M9">
-        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98289751521066271</v>
       </c>
       <c r="N9">
-        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98444600641955393</v>
       </c>
       <c r="O9">
-        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98592257450963416</v>
       </c>
       <c r="P9">
-        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98732492811641093</v>
       </c>
       <c r="Q9">
-        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98865103274781108</v>
       </c>
       <c r="R9">
-        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98989915426344599</v>
       </c>
       <c r="S9">
-        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.99106790374392784</v>
       </c>
       <c r="T9">
-        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.99215628291889535</v>
       </c>
       <c r="U9">
-        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.99316372909104689</v>
       </c>
       <c r="V9">
-        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.99409015824032565</v>
       </c>
       <c r="W9">
-        <f>_xlfn.NORM.DIST($B9, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.99493600472530463</v>
       </c>
     </row>
@@ -17286,87 +17286,87 @@
         <v>0.7</v>
       </c>
       <c r="C10">
-        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.96784322520438626</v>
       </c>
       <c r="D10">
-        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.96982122064229781</v>
       </c>
       <c r="E10">
-        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.97175372082062006</v>
       </c>
       <c r="F10">
-        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.97363788647703964</v>
       </c>
       <c r="G10">
-        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.97547087689619361</v>
       </c>
       <c r="H10">
-        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.97724986805182079</v>
       </c>
       <c r="I10">
-        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.97897207311016909</v>
       </c>
       <c r="J10">
-        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.98063476539748684</v>
       </c>
       <c r="K10">
-        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.98223530390123148</v>
       </c>
       <c r="L10">
-        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.98377116132986453</v>
       </c>
       <c r="M10">
-        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98523995469775305</v>
       </c>
       <c r="N10">
-        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98663947832768129</v>
       </c>
       <c r="O10">
-        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98796773907173285</v>
       </c>
       <c r="P10">
-        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98922299344000109</v>
       </c>
       <c r="Q10">
-        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.99040378619428515</v>
       </c>
       <c r="R10">
-        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.9915089898099565</v>
       </c>
       <c r="S10">
-        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.99253784403396828</v>
       </c>
       <c r="T10">
-        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.993489994572619</v>
       </c>
       <c r="U10">
-        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.99436552973351766</v>
       </c>
       <c r="V10">
-        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.9951650136295519</v>
       </c>
       <c r="W10">
-        <f>_xlfn.NORM.DIST($B10, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.99588951433965567</v>
       </c>
     </row>
@@ -17375,87 +17375,87 @@
         <v>0.8</v>
       </c>
       <c r="C11">
-        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.97128344018399815</v>
       </c>
       <c r="D11">
-        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.97313047249844897</v>
       </c>
       <c r="E11">
-        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.97492971907180315</v>
       </c>
       <c r="F11">
-        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.9766785666692418</v>
       </c>
       <c r="G11">
-        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.97837442974191546</v>
       </c>
       <c r="H11">
-        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.98001476984692537</v>
       </c>
       <c r="I11">
-        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.9815971172112371</v>
       </c>
       <c r="J11">
-        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.98311909447403878</v>
       </c>
       <c r="K11">
-        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.98457844259899263</v>
       </c>
       <c r="L11">
-        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.98597304889303117</v>
       </c>
       <c r="M11">
-        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98730097700023178</v>
       </c>
       <c r="N11">
-        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98856049865636386</v>
       </c>
       <c r="O11">
-        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98975012689068897</v>
       </c>
       <c r="P11">
-        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.99086865024566873</v>
       </c>
       <c r="Q11">
-        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.99191516745228692</v>
       </c>
       <c r="R11">
-        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.99288912184959954</v>
       </c>
       <c r="S11">
-        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.99379033467422384</v>
       </c>
       <c r="T11">
-        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.99461903617301051</v>
       </c>
       <c r="U11">
-        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.9953758933168243</v>
       </c>
       <c r="V11">
-        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.99606203272497285</v>
       </c>
       <c r="W11">
-        <f>_xlfn.NORM.DIST($B11, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.99667905726178674</v>
       </c>
     </row>
@@ -17464,87 +17464,87 @@
         <v>0.9</v>
       </c>
       <c r="C12">
-        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.97441194047836144</v>
       </c>
       <c r="D12">
-        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.97613111888135196</v>
       </c>
       <c r="E12">
-        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.9778007672556237</v>
       </c>
       <c r="F12">
-        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.9794185208944417</v>
       </c>
       <c r="G12">
-        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.98098207010284577</v>
       </c>
       <c r="H12">
-        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.98248918036829402</v>
       </c>
       <c r="I12">
-        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.98393771439617173</v>
       </c>
       <c r="J12">
-        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.98532565597611843</v>
       </c>
       <c r="K12">
-        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.98665113559422191</v>
       </c>
       <c r="L12">
-        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <f t="shared" si="0"/>
         <v>0.98791245764394509</v>
       </c>
       <c r="M12">
-        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.98910812901414658</v>
       </c>
       <c r="N12">
-        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.99023688874489857</v>
       </c>
       <c r="O12">
-        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.99129773834062174</v>
       </c>
       <c r="P12">
-        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.99228997221560522</v>
       </c>
       <c r="Q12">
-        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.99321320762041643</v>
       </c>
       <c r="R12">
-        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.99406741326145165</v>
       </c>
       <c r="S12">
-        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.99485293568395028</v>
       </c>
       <c r="T12">
-        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.99557052234725518</v>
       </c>
       <c r="U12">
-        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.9962213401885005</v>
       </c>
       <c r="V12">
-        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.99680698835864645</v>
       </c>
       <c r="W12">
-        <f>_xlfn.NORM.DIST($B12, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <f t="shared" si="1"/>
         <v>0.99732950373746643</v>
       </c>
     </row>
@@ -17553,87 +17553,87 @@
         <v>1</v>
       </c>
       <c r="C13">
-        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <f t="shared" ref="C13:L23" si="2">_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
         <v>0.97724986805182079</v>
       </c>
       <c r="D13">
-        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.97884493863434063</v>
       </c>
       <c r="E13">
-        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.98038926046139385</v>
       </c>
       <c r="F13">
-        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.98188073420027189</v>
       </c>
       <c r="G13">
-        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.98331734052759789</v>
       </c>
       <c r="H13">
-        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.98469716052612621</v>
       </c>
       <c r="I13">
-        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.98601839761764787</v>
       </c>
       <c r="J13">
-        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.98727940093204036</v>
       </c>
       <c r="K13">
-        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.98847868995611909</v>
       </c>
       <c r="L13">
-        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.98961498023936256</v>
       </c>
       <c r="M13">
-        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <f t="shared" ref="M13:W23" si="3">_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
         <v>0.99068720985629855</v>
       </c>
       <c r="N13">
-        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99169456623730734</v>
       </c>
       <c r="O13">
-        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99263651288131527</v>
       </c>
       <c r="P13">
-        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99351281535665104</v>
       </c>
       <c r="Q13">
-        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.9943235658825752</v>
       </c>
       <c r="R13">
-        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99506920566743162</v>
       </c>
       <c r="S13">
-        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99575054406539887</v>
       </c>
       <c r="T13">
-        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99636877350986042</v>
       </c>
       <c r="U13">
-        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99692547909715257</v>
       </c>
       <c r="V13">
-        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99742264164199901</v>
       </c>
       <c r="W13">
-        <f>_xlfn.NORM.DIST($B13, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99786263301991374</v>
       </c>
     </row>
@@ -17642,87 +17642,87 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C14">
-        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.97981778459429558</v>
       </c>
       <c r="D14">
-        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.98129303418367897</v>
       </c>
       <c r="E14">
-        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.98271681517805853</v>
       </c>
       <c r="F14">
-        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.98408730488766094</v>
       </c>
       <c r="G14">
-        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.98540278287955929</v>
       </c>
       <c r="H14">
-        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.9866616510953955</v>
       </c>
       <c r="I14">
-        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.98786245514015714</v>
       </c>
       <c r="J14">
-        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.98900390658142112</v>
       </c>
       <c r="K14">
-        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.9900849060392205</v>
       </c>
       <c r="L14">
-        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99110456677879533</v>
       </c>
       <c r="M14">
-        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99206223844209485</v>
       </c>
       <c r="N14">
-        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99295753046970459</v>
       </c>
       <c r="O14">
-        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99379033467422384</v>
       </c>
       <c r="P14">
-        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99456084633132047</v>
       </c>
       <c r="Q14">
-        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99526958305914193</v>
       </c>
       <c r="R14">
-        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99591740066526613</v>
       </c>
       <c r="S14">
-        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99650550505931867</v>
       </c>
       <c r="T14">
-        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99703545926696446</v>
       </c>
       <c r="U14">
-        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99750918454727489</v>
       </c>
       <c r="V14">
-        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99792895462238751</v>
       </c>
       <c r="W14">
-        <f>_xlfn.NORM.DIST($B14, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99829738208935259</v>
       </c>
     </row>
@@ -17731,87 +17731,87 @@
         <v>1.2</v>
       </c>
       <c r="C15">
-        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.98213557943718344</v>
       </c>
       <c r="D15">
-        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.98349574210455681</v>
       </c>
       <c r="E15">
-        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.98480418351194976</v>
       </c>
       <c r="F15">
-        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.98605936350374279</v>
       </c>
       <c r="G15">
-        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.98725986335550087</v>
       </c>
       <c r="H15">
-        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.98840440514152805</v>
       </c>
       <c r="I15">
-        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.98949187188624066</v>
       </c>
       <c r="J15">
-        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99052132828574579</v>
       </c>
       <c r="K15">
-        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99149204172653183</v>
       </c>
       <c r="L15">
-        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99240350326205273</v>
       </c>
       <c r="M15">
-        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99325544813598621</v>
       </c>
       <c r="N15">
-        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99404787536444239</v>
       </c>
       <c r="O15">
-        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99478106581052672</v>
       </c>
       <c r="P15">
-        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99545559810651818</v>
       </c>
       <c r="Q15">
-        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99607236170571123</v>
       </c>
       <c r="R15">
-        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99663256628319929</v>
       </c>
       <c r="S15">
-        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99713774665945876</v>
       </c>
       <c r="T15">
-        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99758976240089414</v>
       </c>
       <c r="U15">
-        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99799079126726198</v>
       </c>
       <c r="V15">
-        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99834331573791169</v>
       </c>
       <c r="W15">
-        <f>_xlfn.NORM.DIST($B15, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.9986501019683699</v>
       </c>
     </row>
@@ -17820,87 +17820,87 @@
         <v>1.3</v>
       </c>
       <c r="C16">
-        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.98422239260890954</v>
       </c>
       <c r="D16">
-        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.9854725599216041</v>
       </c>
       <c r="E16">
-        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.98667118474140514</v>
       </c>
       <c r="F16">
-        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.98781701026588054</v>
       </c>
       <c r="G16">
-        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.98890891700233552</v>
       </c>
       <c r="H16">
-        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.98994594096094168</v>
       </c>
       <c r="I16">
-        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99092729223645926</v>
       </c>
       <c r="J16">
-        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99185237372137502</v>
       </c>
       <c r="K16">
-        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99272079963615401</v>
       </c>
       <c r="L16">
-        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99353241350084198</v>
       </c>
       <c r="M16">
-        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99428730510778573</v>
       </c>
       <c r="N16">
-        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99498582598973795</v>
       </c>
       <c r="O16">
-        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99562860281384891</v>
       </c>
       <c r="P16">
-        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99621654807370474</v>
       </c>
       <c r="Q16">
-        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99675086740336638</v>
       </c>
       <c r="R16">
-        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99723306280512991</v>
       </c>
       <c r="S16">
-        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99766493107341181</v>
       </c>
       <c r="T16">
-        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.9980485567187205</v>
       </c>
       <c r="U16">
-        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99838629875681095</v>
       </c>
       <c r="V16">
-        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99868077083778739</v>
       </c>
       <c r="W16">
-        <f>_xlfn.NORM.DIST($B16, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99893481435657228</v>
       </c>
     </row>
@@ -17909,87 +17909,87 @@
         <v>1.4</v>
       </c>
       <c r="C17">
-        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.98609655248650141</v>
       </c>
       <c r="D17">
-        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.98724208843039174</v>
       </c>
       <c r="E17">
-        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.98833665330160048</v>
       </c>
       <c r="F17">
-        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.98937926979223911</v>
       </c>
       <c r="G17">
-        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99036911036340736</v>
       </c>
       <c r="H17">
-        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99130551389665644</v>
       </c>
       <c r="I17">
-        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99218800234452975</v>
       </c>
       <c r="J17">
-        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99301629709024808</v>
       </c>
       <c r="K17">
-        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99379033467422384</v>
       </c>
       <c r="L17">
-        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99451028149084664</v>
       </c>
       <c r="M17">
-        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99517654700468294</v>
       </c>
       <c r="N17">
-        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99578979498334452</v>
       </c>
       <c r="O17">
-        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99635095219800218</v>
       </c>
       <c r="P17">
-        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99686121400590511</v>
       </c>
       <c r="Q17">
-        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99732204620721154</v>
       </c>
       <c r="R17">
-        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99773518256671845</v>
       </c>
       <c r="S17">
-        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99810261741620365</v>
       </c>
       <c r="T17">
-        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99842659281208423</v>
       </c>
       <c r="U17">
-        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99870957982304531</v>
       </c>
       <c r="V17">
-        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99895425366976121</v>
       </c>
       <c r="W17">
-        <f>_xlfn.NORM.DIST($B17, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99916346263892386</v>
       </c>
     </row>
@@ -17998,87 +17998,87 @@
         <v>1.5</v>
       </c>
       <c r="C18">
-        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.98777552734495533</v>
       </c>
       <c r="D18">
-        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.98882198867076931</v>
       </c>
       <c r="E18">
-        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.989818402138959</v>
       </c>
       <c r="F18">
-        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99076406186531352</v>
       </c>
       <c r="G18">
-        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99165842074571242</v>
       </c>
       <c r="H18">
-        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99250110526320356</v>
       </c>
       <c r="I18">
-        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99329192992302162</v>
       </c>
       <c r="J18">
-        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99403091100447794</v>
       </c>
       <c r="K18">
-        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99471827927308554</v>
       </c>
       <c r="L18">
-        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99535449125135822</v>
       </c>
       <c r="M18">
-        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99594023860462444</v>
       </c>
       <c r="N18">
-        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99647645516170658</v>
       </c>
       <c r="O18">
-        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99696432106288702</v>
       </c>
       <c r="P18">
-        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99740526351334968</v>
       </c>
       <c r="Q18">
-        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99780095362404031</v>
       </c>
       <c r="R18">
-        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.9981532988489582</v>
       </c>
       <c r="S18">
-        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.9984644305839443</v>
       </c>
       <c r="T18">
-        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99873668658270343</v>
       </c>
       <c r="U18">
-        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99897258797617372</v>
       </c>
       <c r="V18">
-        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99917481085525794</v>
       </c>
       <c r="W18">
-        <f>_xlfn.NORM.DIST($B18, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99934615259594539</v>
       </c>
     </row>
@@ -18087,87 +18087,87 @@
         <v>1.6</v>
       </c>
       <c r="C19">
-        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.98927588997832416</v>
       </c>
       <c r="D19">
-        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99022895255784427</v>
       </c>
       <c r="E19">
-        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99113320025518947</v>
       </c>
       <c r="F19">
-        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99198818684480428</v>
       </c>
       <c r="G19">
-        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99279363050302394</v>
       </c>
       <c r="H19">
-        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99354942653731249</v>
       </c>
       <c r="I19">
-        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99425565940188498</v>
       </c>
       <c r="J19">
-        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99491261367939154</v>
       </c>
       <c r="K19">
-        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99552078367125296</v>
       </c>
       <c r="L19">
-        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99608088120520577</v>
       </c>
       <c r="M19">
-        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99659384124004158</v>
       </c>
       <c r="N19">
-        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99706082482737046</v>
       </c>
       <c r="O19">
-        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99748321898197434</v>
       </c>
       <c r="P19">
-        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99786263301991374</v>
       </c>
       <c r="Q19">
-        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99820089095140607</v>
       </c>
       <c r="R19">
-        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.9985000195681506</v>
       </c>
       <c r="S19">
-        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99876223194673974</v>
       </c>
       <c r="T19">
-        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99898990620501338</v>
       </c>
       <c r="U19">
-        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.9991855594995066</v>
       </c>
       <c r="V19">
-        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99935181744050361</v>
       </c>
       <c r="W19">
-        <f>_xlfn.NORM.DIST($B19, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99949137932483567</v>
       </c>
     </row>
@@ -18176,87 +18176,87 @@
         <v>1.7</v>
       </c>
       <c r="C20">
-        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99061329446516144</v>
       </c>
       <c r="D20">
-        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.9914786860812399</v>
       </c>
       <c r="E20">
-        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99229676317508175</v>
       </c>
       <c r="F20">
-        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99306732427326405</v>
       </c>
       <c r="G20">
-        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99379033467422384</v>
       </c>
       <c r="H20">
-        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99446593693750274</v>
       </c>
       <c r="I20">
-        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99509446035679117</v>
       </c>
       <c r="J20">
-        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99567642909881338</v>
       </c>
       <c r="K20">
-        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99621256866269048</v>
       </c>
       <c r="L20">
-        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99670381029225796</v>
       </c>
       <c r="M20">
-        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99715129295938176</v>
       </c>
       <c r="N20">
-        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99755636253257118</v>
       </c>
       <c r="O20">
-        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99792056775540883</v>
       </c>
       <c r="P20">
-        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99824565268711207</v>
       </c>
       <c r="Q20">
-        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99853354530660077</v>
       </c>
       <c r="R20">
-        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99878634205533956</v>
       </c>
       <c r="S20">
-        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99900628819602255</v>
       </c>
       <c r="T20">
-        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99919575399596294</v>
       </c>
       <c r="U20">
-        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99935720690637442</v>
       </c>
       <c r="V20">
-        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99949318009983712</v>
       </c>
       <c r="W20">
-        <f>_xlfn.NORM.DIST($B20, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99960623794332182</v>
       </c>
     </row>
@@ -18265,87 +18265,87 @@
         <v>1.8</v>
       </c>
       <c r="C21">
-        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99180246407540384</v>
       </c>
       <c r="D21">
-        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.9925859039167042</v>
       </c>
       <c r="E21">
-        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99332375501779535</v>
       </c>
       <c r="F21">
-        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.9940160431794185</v>
       </c>
       <c r="G21">
-        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99466296029774037</v>
       </c>
       <c r="H21">
-        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99526487252223783</v>
       </c>
       <c r="I21">
-        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99582232714110541</v>
       </c>
       <c r="J21">
-        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99633605788946533</v>
       </c>
       <c r="K21">
-        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99680698835864645</v>
       </c>
       <c r="L21">
-        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.9972362331748813</v>
       </c>
       <c r="M21">
-        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99762509661539056</v>
       </c>
       <c r="N21">
-        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99797506834174698</v>
       </c>
       <c r="O21">
-        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99828781595757443</v>
       </c>
       <c r="P21">
-        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99856517414304602</v>
       </c>
       <c r="Q21">
-        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99880913018513184</v>
       </c>
       <c r="R21">
-        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99902180581250244</v>
       </c>
       <c r="S21">
-        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99920543535894968</v>
       </c>
       <c r="T21">
-        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99936234041936356</v>
       </c>
       <c r="U21">
-        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99949490132603891</v>
       </c>
       <c r="V21">
-        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99960552595622765</v>
       </c>
       <c r="W21">
-        <f>_xlfn.NORM.DIST($B21, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99969661657718201</v>
       </c>
     </row>
@@ -18354,87 +18354,87 @@
         <v>1.9</v>
       </c>
       <c r="C22">
-        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99285718926472855</v>
       </c>
       <c r="D22">
-        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99356433425440716</v>
       </c>
       <c r="E22">
-        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.9942278008261155</v>
       </c>
       <c r="F22">
-        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99484782257686355</v>
       </c>
       <c r="G22">
-        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.995424795737889</v>
       </c>
       <c r="H22">
-        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99595928497776753</v>
       </c>
       <c r="I22">
-        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99645202772823449</v>
       </c>
       <c r="J22">
-        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.9969039367509489</v>
       </c>
       <c r="K22">
-        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99731610065702081</v>
       </c>
       <c r="L22">
-        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99768978209323977</v>
       </c>
       <c r="M22">
-        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99802641332185826</v>
       </c>
       <c r="N22">
-        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99832758894694029</v>
       </c>
       <c r="O22">
-        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99859505558209449</v>
       </c>
       <c r="P22">
-        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99883069831415505</v>
       </c>
       <c r="Q22">
-        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99903652389688324</v>
       </c>
       <c r="R22">
-        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99921464070916677</v>
       </c>
       <c r="S22">
-        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99936723563349539</v>
       </c>
       <c r="T22">
-        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99949654815113109</v>
       </c>
       <c r="U22">
-        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99960484210678979</v>
       </c>
       <c r="V22">
-        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99969437576173004</v>
       </c>
       <c r="W22">
-        <f>_xlfn.NORM.DIST($B22, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99976737092096446</v>
       </c>
     </row>
@@ -18443,87 +18443,87 @@
         <v>2</v>
       </c>
       <c r="C23">
-        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *C$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99379033467422384</v>
       </c>
       <c r="D23">
-        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *D$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99442673263320192</v>
       </c>
       <c r="E23">
-        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *E$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99502150780925247</v>
       </c>
       <c r="F23">
-        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *F$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99557508067649803</v>
       </c>
       <c r="G23">
-        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *G$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99608802840283917</v>
       </c>
       <c r="H23">
-        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *H$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99656108833800094</v>
       </c>
       <c r="I23">
-        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *I$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99699515987387455</v>
       </c>
       <c r="J23">
-        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *J$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99739130442657642</v>
       </c>
       <c r="K23">
-        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *K$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99775074329355862</v>
       </c>
       <c r="L23">
-        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *L$2, TRUE)</f>
+        <f t="shared" si="2"/>
         <v>0.99807485315250621</v>
       </c>
       <c r="M23">
-        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *M$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99836515899365319</v>
       </c>
       <c r="N23">
-        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *N$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99862332431550138</v>
       </c>
       <c r="O23">
-        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *O$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99885113846754769</v>
       </c>
       <c r="P23">
-        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *P$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99905050109394478</v>
       </c>
       <c r="Q23">
-        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *Q$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99922340371983398</v>
       </c>
       <c r="R23">
-        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *R$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99937190862726821</v>
       </c>
       <c r="S23">
-        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *S$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99949812528874615</v>
       </c>
       <c r="T23">
-        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *T$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99960418476031487</v>
       </c>
       <c r="U23">
-        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *U$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.99969221257784135</v>
       </c>
       <c r="V23">
-        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *V$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.9997643008419731</v>
       </c>
       <c r="W23">
-        <f>_xlfn.NORM.DIST($B23, throwingmean, throwingstdv + throwingfactor *W$2, TRUE)</f>
+        <f t="shared" si="3"/>
         <v>0.9998224803096265</v>
       </c>
     </row>
@@ -18787,7 +18787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AB18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="AC15" sqref="AC15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Outlined simplefielding in sufficient resolution to (hopefully!) finish it tomorrow!
</commit_message>
<xml_diff>
--- a/plans/baseball stats.xlsx
+++ b/plans/baseball stats.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcgiffenk\Desktop\newpy\xtreemblaseball99\plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED43DD84-53AB-4218-BCCD-C2D84024B7E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0201F8D1-F05F-4035-A2B6-D4ECE5DFC62F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="iterative" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="7" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="8" r:id="rId3"/>
-    <sheet name="gauss cruncher" sheetId="5" r:id="rId4"/>
-    <sheet name="run speed" sheetId="3" r:id="rId5"/>
-    <sheet name="pitch outcomes" sheetId="1" r:id="rId6"/>
-    <sheet name="hit quality truth table" sheetId="6" r:id="rId7"/>
+    <sheet name="Sheet3" sheetId="9" r:id="rId4"/>
+    <sheet name="gauss cruncher" sheetId="5" r:id="rId5"/>
+    <sheet name="run speed" sheetId="3" r:id="rId6"/>
+    <sheet name="pitch outcomes" sheetId="1" r:id="rId7"/>
+    <sheet name="hit quality truth table" sheetId="6" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="basis">#REF!</definedName>
@@ -558,7 +559,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="311">
   <si>
     <t>Ball</t>
   </si>
@@ -1486,6 +1487,12 @@
   </si>
   <si>
     <t>ball speed:</t>
+  </si>
+  <si>
+    <t>timing</t>
+  </si>
+  <si>
+    <t>bravery</t>
   </si>
 </sst>
 </file>
@@ -1629,7 +1636,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -1953,13 +1960,84 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="168">
+  <cellXfs count="176">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2134,6 +2212,14 @@
     <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
@@ -9603,7 +9689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DO41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
@@ -16562,7 +16648,7 @@
   <dimension ref="A1:W23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18545,6 +18631,323 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBA148E4-8960-49BB-84B7-B9F77657BF02}">
+  <dimension ref="A1:W23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA6" sqref="AA6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="23" width="6.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0.1</v>
+      </c>
+      <c r="E2">
+        <v>0.2</v>
+      </c>
+      <c r="F2">
+        <v>0.3</v>
+      </c>
+      <c r="G2">
+        <v>0.4</v>
+      </c>
+      <c r="H2">
+        <v>0.5</v>
+      </c>
+      <c r="I2">
+        <v>0.6</v>
+      </c>
+      <c r="J2">
+        <v>0.7</v>
+      </c>
+      <c r="K2">
+        <v>0.8</v>
+      </c>
+      <c r="L2">
+        <v>0.9</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O2">
+        <v>1.2</v>
+      </c>
+      <c r="P2">
+        <v>1.3</v>
+      </c>
+      <c r="Q2">
+        <v>1.4</v>
+      </c>
+      <c r="R2">
+        <v>1.5</v>
+      </c>
+      <c r="S2">
+        <v>1.6</v>
+      </c>
+      <c r="T2">
+        <v>1.7</v>
+      </c>
+      <c r="U2">
+        <v>1.8</v>
+      </c>
+      <c r="V2">
+        <v>1.9</v>
+      </c>
+      <c r="W2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>310</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="168"/>
+      <c r="D3" s="169"/>
+      <c r="E3" s="169"/>
+      <c r="F3" s="169"/>
+      <c r="G3" s="169"/>
+      <c r="H3" s="169"/>
+      <c r="I3" s="169"/>
+      <c r="J3" s="169"/>
+      <c r="K3" s="169"/>
+      <c r="L3" s="169"/>
+      <c r="M3" s="170"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>0.1</v>
+      </c>
+      <c r="C4" s="171"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="172"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>0.2</v>
+      </c>
+      <c r="C5" s="171"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="172"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>0.3</v>
+      </c>
+      <c r="C6" s="171"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="172"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>0.4</v>
+      </c>
+      <c r="C7" s="171"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="172"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>0.5</v>
+      </c>
+      <c r="C8" s="171"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="32"/>
+      <c r="M8" s="172"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>0.6</v>
+      </c>
+      <c r="C9" s="171"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="172"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>0.7</v>
+      </c>
+      <c r="C10" s="171"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="172"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>0.8</v>
+      </c>
+      <c r="C11" s="171"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="172"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>0.9</v>
+      </c>
+      <c r="C12" s="171"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="172"/>
+    </row>
+    <row r="13" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="173"/>
+      <c r="D13" s="174"/>
+      <c r="E13" s="174"/>
+      <c r="F13" s="174"/>
+      <c r="G13" s="174"/>
+      <c r="H13" s="174"/>
+      <c r="I13" s="174"/>
+      <c r="J13" s="174"/>
+      <c r="K13" s="174"/>
+      <c r="L13" s="174"/>
+      <c r="M13" s="175"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C2:S9"/>
   <sheetViews>
@@ -18783,7 +19186,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AB18"/>
   <sheetViews>
@@ -20234,7 +20637,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
@@ -20530,7 +20933,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E19"/>
   <sheetViews>

</xml_diff>

<commit_message>
Test Hitting is coming together. Documentation + bugfixes also! Next up is moving reduction out to pitches.
</commit_message>
<xml_diff>
--- a/plans/baseball stats.xlsx
+++ b/plans/baseball stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcgiffenk\Desktop\newpy\xtreemblaseball99\plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0201F8D1-F05F-4035-A2B6-D4ECE5DFC62F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA4BED4-D999-4427-BF9D-15FCFDCBB244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="iterative" sheetId="2" r:id="rId1"/>
@@ -9689,8 +9689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DO41"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10310,11 +10310,11 @@
       </c>
       <c r="W7" s="29">
         <f>(1-$W$32)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X7" s="48">
         <f>Table3[[#This Row],[ball factor]]/$X$32*(1-$X$34)+$X$34</f>
-        <v>0.2</v>
+        <v>1.1411764705882355</v>
       </c>
       <c r="Y7" s="29">
         <f>Table3[[#This Row],[offense]]</f>
@@ -10664,11 +10664,11 @@
       </c>
       <c r="W8" s="3">
         <f t="shared" ref="W8:W22" si="8">(1-$W$32)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X8" s="49">
         <f>Table3[[#This Row],[ball factor]]/$X$32*(1-$X$34)+$X$34</f>
-        <v>0.2</v>
+        <v>1.1411764705882355</v>
       </c>
       <c r="Y8" s="3">
         <f>Table3[[#This Row],[offense]]</f>
@@ -11018,11 +11018,11 @@
       </c>
       <c r="W9" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X9" s="50">
         <f>Table3[[#This Row],[ball factor]]/$X$32*(1-$X$34)+$X$34</f>
-        <v>0.2</v>
+        <v>1.1411764705882355</v>
       </c>
       <c r="Y9" s="4">
         <f>Table3[[#This Row],[offense]]</f>
@@ -11372,11 +11372,11 @@
       </c>
       <c r="W10" s="3">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X10" s="49">
         <f>Table3[[#This Row],[ball factor]]/$X$32*(1-$X$34)+$X$34</f>
-        <v>0.2</v>
+        <v>1.1411764705882355</v>
       </c>
       <c r="Y10" s="3">
         <f>Table3[[#This Row],[offense]]</f>
@@ -11726,11 +11726,11 @@
       </c>
       <c r="W11" s="13">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X11" s="51">
         <f>Table3[[#This Row],[ball factor]]/$X$32*(1-$X$34)+$X$34</f>
-        <v>0.2</v>
+        <v>1.1411764705882355</v>
       </c>
       <c r="Y11" s="13">
         <f>Table3[[#This Row],[offense]]</f>
@@ -12080,11 +12080,11 @@
       </c>
       <c r="W12" s="26">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X12" s="52">
         <f>Table3[[#This Row],[ball factor]]/$X$32*(1-$X$34)+$X$34</f>
-        <v>0.2</v>
+        <v>1.1411764705882355</v>
       </c>
       <c r="Y12" s="26">
         <f>Table3[[#This Row],[offense]]</f>
@@ -12434,11 +12434,11 @@
       </c>
       <c r="W13" s="13">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X13" s="51">
         <f>Table3[[#This Row],[ball factor]]/$X$32*(1-$X$34)+$X$34</f>
-        <v>0.2</v>
+        <v>1.1411764705882355</v>
       </c>
       <c r="Y13" s="13">
         <f>Table3[[#This Row],[offense]]</f>
@@ -12788,11 +12788,11 @@
       </c>
       <c r="W14" s="5">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X14" s="53">
         <f>Table3[[#This Row],[ball factor]]/$X$32*(1-$X$34)+$X$34</f>
-        <v>0.2</v>
+        <v>1.1411764705882355</v>
       </c>
       <c r="Y14" s="5">
         <f>Table3[[#This Row],[offense]]</f>
@@ -13142,11 +13142,11 @@
       </c>
       <c r="W15" s="17">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X15" s="54">
         <f>Table3[[#This Row],[ball factor]]/$X$32*(1-$X$34)+$X$34</f>
-        <v>0.2</v>
+        <v>1.1411764705882355</v>
       </c>
       <c r="Y15" s="17">
         <f>Table3[[#This Row],[offense]]</f>
@@ -13496,11 +13496,11 @@
       </c>
       <c r="W16" s="6">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X16" s="55">
         <f>Table3[[#This Row],[ball factor]]/$X$32*(1-$X$34)+$X$34</f>
-        <v>0.2</v>
+        <v>1.1411764705882355</v>
       </c>
       <c r="Y16" s="6">
         <f>Table3[[#This Row],[offense]]</f>
@@ -13850,11 +13850,11 @@
       </c>
       <c r="W17" s="23">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X17" s="56">
         <f>Table3[[#This Row],[ball factor]]/$X$32*(1-$X$34)+$X$34</f>
-        <v>0.2</v>
+        <v>1.1411764705882355</v>
       </c>
       <c r="Y17" s="23">
         <f>Table3[[#This Row],[offense]]</f>
@@ -14204,11 +14204,11 @@
       </c>
       <c r="W18" s="6">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X18" s="55">
         <f>Table3[[#This Row],[ball factor]]/$X$32*(1-$X$34)+$X$34</f>
-        <v>0.2</v>
+        <v>1.1411764705882355</v>
       </c>
       <c r="Y18" s="6">
         <f>Table3[[#This Row],[offense]]</f>
@@ -14558,11 +14558,11 @@
       </c>
       <c r="W19" s="15">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X19" s="57">
         <f>Table3[[#This Row],[ball factor]]/$X$32*(1-$X$34)+$X$34</f>
-        <v>0.2</v>
+        <v>1.1411764705882355</v>
       </c>
       <c r="Y19" s="15">
         <f>Table3[[#This Row],[offense]]</f>
@@ -14912,11 +14912,11 @@
       </c>
       <c r="W20" s="11">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X20" s="58">
         <f>Table3[[#This Row],[ball factor]]/$X$32*(1-$X$34)+$X$34</f>
-        <v>0.2</v>
+        <v>1.1411764705882355</v>
       </c>
       <c r="Y20" s="11">
         <f>Table3[[#This Row],[offense]]</f>
@@ -15266,11 +15266,11 @@
       </c>
       <c r="W21" s="15">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X21" s="57">
         <f>Table3[[#This Row],[ball factor]]/$X$32*(1-$X$34)+$X$34</f>
-        <v>0.2</v>
+        <v>1.1411764705882355</v>
       </c>
       <c r="Y21" s="15">
         <f>Table3[[#This Row],[offense]]</f>
@@ -15620,11 +15620,11 @@
       </c>
       <c r="W22" s="20">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X22" s="59">
         <f>Table3[[#This Row],[ball factor]]/$X$32*(1-$X$34)+$X$34</f>
-        <v>0.2</v>
+        <v>1.1411764705882355</v>
       </c>
       <c r="Y22" s="20">
         <f>Table3[[#This Row],[offense]]</f>
@@ -16079,7 +16079,7 @@
         <v>0.2</v>
       </c>
       <c r="W26">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X26">
         <v>0.5</v>
@@ -16213,7 +16213,7 @@
         <v>0.9</v>
       </c>
       <c r="W28">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y28" s="71" t="s">
         <v>148</v>
@@ -16313,7 +16313,7 @@
     <row r="30" spans="1:90" x14ac:dyDescent="0.25">
       <c r="W30">
         <f xml:space="preserve"> W28/2 - W26/3</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Y30" s="71" t="s">
         <v>146</v>
@@ -16381,7 +16381,7 @@
     <row r="32" spans="1:90" x14ac:dyDescent="0.25">
       <c r="W32">
         <f>MAX(0, ((W26+X26)/(3+X26))-(W28/2))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X32">
         <v>0.85</v>
@@ -18634,7 +18634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBA148E4-8960-49BB-84B7-B9F77657BF02}">
   <dimension ref="A1:W23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Bad reduction scaling formula, checking in so I can revert it so reduction applies directly to quality instead.
</commit_message>
<xml_diff>
--- a/plans/baseball stats.xlsx
+++ b/plans/baseball stats.xlsx
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcgiffenk\Desktop\newpy\xtreemblaseball99\plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA4BED4-D999-4427-BF9D-15FCFDCBB244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17444565-3F8E-45CB-8AD9-ED2F925FD984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="iterative" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="7" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="8" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="9" r:id="rId4"/>
-    <sheet name="gauss cruncher" sheetId="5" r:id="rId5"/>
-    <sheet name="run speed" sheetId="3" r:id="rId6"/>
-    <sheet name="pitch outcomes" sheetId="1" r:id="rId7"/>
-    <sheet name="hit quality truth table" sheetId="6" r:id="rId8"/>
+    <sheet name="as-run reduct" sheetId="11" r:id="rId3"/>
+    <sheet name="reduction" sheetId="10" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="8" r:id="rId5"/>
+    <sheet name="Sheet3" sheetId="9" r:id="rId6"/>
+    <sheet name="gauss cruncher" sheetId="5" r:id="rId7"/>
+    <sheet name="run speed" sheetId="3" r:id="rId8"/>
+    <sheet name="pitch outcomes" sheetId="1" r:id="rId9"/>
+    <sheet name="hit quality truth table" sheetId="6" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="basis">#REF!</definedName>
@@ -559,7 +561,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="314">
   <si>
     <t>Ball</t>
   </si>
@@ -1493,6 +1495,15 @@
   </si>
   <si>
     <t>bravery</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>delta</t>
   </si>
 </sst>
 </file>
@@ -2226,7 +2237,23 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="83">
+  <dxfs count="85">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -2570,16 +2597,6 @@
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3103,6 +3120,1485 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'as-run reduct'!$A$2:$CV$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>42.212801833565102</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42.934887913960999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42.898730355704302</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41.656111618988803</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>38.088802865929203</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>36.283573380573003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>34.977259720042497</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>33.909741670306197</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>32.986494885463202</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32.161158910431297</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>31.4071344909994</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30.707576594918599</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>30.051060991771799</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>29.429437819890701</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>28.836661700422098</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>28.268106510022601</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>27.720140767285901</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>27.189852293771501</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>26.674862864410802</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>26.173199454009101</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>25.6832023704597</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>25.203458172670601</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>24.732749686016099</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24.270018086598199</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>23.8143336787242</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>23.364873047401002</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>22.9209009611025</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>22.4817558651011</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>22.046838123804999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>21.615600392170901</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>21.1875396531895</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>20.7621905712273</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>20.339119893166199</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>20.011713709635799</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>20.071248189251101</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>20.130028834074501</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>20.188124066911701</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>20.245597638021898</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>20.302509224591599</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>20.358914953995999</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>20.414867863754701</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>20.470418308789402</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>20.525614324777099</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>20.5805019549544</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>20.6351255465785</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>20.689528022341101</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>20.7437511313037</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>20.797835683351199</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>20.851821770710799</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>20.905748979740999</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>20.959656595943098</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>21.013583804973401</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>21.067569892333001</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>21.1216544443805</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>21.175877553343</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>21.2302800291056</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>21.2849036207297</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>21.339791250906998</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>21.394987266894699</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>21.4505377119294</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>21.506490621688101</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>21.562896351092501</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>21.619807937662198</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>21.677281508772399</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>21.735376741609599</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>21.794157386433</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>21.853691866048301</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>21.914053967316502</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>21.975323644259301</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>22.037587957135599</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>22.100942178116199</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>22.165491102371799</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>22.231350614215</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>22.298649572394101</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>22.367532098154999</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>22.4381603763584</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>22.510718116853301</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>22.585414875136799</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>22.6624915052126</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>22.742227124704499</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>22.824948130571201</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>22.9110400425233</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>23.000963319756298</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>23.095274880314001</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>23.1946580043324</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>23.299964907415799</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>23.412279082039699</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>23.5330096545689</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>23.664039946016299</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>23.8079728605322</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>23.968561107030599</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>24.151521308655902</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>24.3662394945848</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>24.629895364844899</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>24.979913904377401</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>25.530687395308298</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>27.113167400177701</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>28.370735758753501</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>29.462484375689701</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>30.439551405476202</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-90CC-42DB-815A-DA4C21CE1798}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="92815936"/>
+        <c:axId val="92817600"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="92815936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="92817600"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="92817600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="92815936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>reduction!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>y</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>reduction!$A$2:$A$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>560</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>580</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>reduction!$B$2:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.4444444444444444E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7777777777777778E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0000000000000008E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.1111111111111111E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1111111111111111</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.16000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.21777777777777779</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.28444444444444444</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.44444444444444442</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.53777777777777769</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.64000000000000012</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.75111111111111117</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.87111111111111117</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.0666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.1333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.2666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.3333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.4666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.5333333333333334</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.6666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.7333333333333334</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.8666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.9333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FF7B-4C12-B683-363228E72117}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>reduction!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>target</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>reduction!$A$2:$A$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>560</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>580</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>reduction!$C$2:$C$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FF7B-4C12-B683-363228E72117}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>reduction!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>delta</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>reduction!$A$2:$A$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>560</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>580</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>reduction!$D$2:$D$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.4444444444444444E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3333333333333332E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.222222222222223E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.1111111111111103E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.9999999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.8888888888888926E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.7777777777777761E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.6666666666666652E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.5555555555555542E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.4444444444444433E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.3333333333333268E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.10222222222222244</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.11111111111111105</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.12888888888888883</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.6666666666666652E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.6666666666666652E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.6666666666666652E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.6666666666666652E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6.6666666666666652E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6.6666666666666652E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6.6666666666666652E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6.6666666666666874E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6.6666666666666652E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6.6666666666666652E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6.6666666666666652E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6.6666666666666652E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>6.6666666666666652E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6.6666666666666652E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>6.6666666666666652E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-FF7B-4C12-B683-363228E72117}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2112011648"/>
+        <c:axId val="2112012480"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2112011648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2112012480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2112012480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2112011648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
@@ -5520,7 +7016,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -6441,7 +7937,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -6854,6 +8350,86 @@
 </file>
 
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -7410,6 +8986,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7925,7 +10017,523 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8428,7 +11036,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8992,6 +11600,88 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC51C21A-BA3B-4275-8130-A74F7BAA31F2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C4E4E4C-B340-4675-AA5A-B675624FF28B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>47624</xdr:colOff>
       <xdr:row>18</xdr:row>
@@ -9029,7 +11719,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -9107,181 +11797,181 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A6:DO22" totalsRowShown="0" headerRowDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A6:DO22" totalsRowShown="0" headerRowDxfId="84">
   <autoFilter ref="A6:DO22" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="119">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Rep #">
       <calculatedColumnFormula>ROW()-ROW(home)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="offense" dataDxfId="80">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="offense" dataDxfId="83">
       <calculatedColumnFormula>INDEX(oratings, 1, 1+MOD(Table3[[#This Row],[Rep '#]]-1, COUNT(oratings)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="defense" dataDxfId="79">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="defense" dataDxfId="82">
       <calculatedColumnFormula>INDEX(dratings, 1, MOD(FLOOR( (Table3[[#This Row],[Rep '#]]-1) / COUNT(oratings), 1), COUNT(dratings))+1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="base leadoff" dataDxfId="78">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="base leadoff" dataDxfId="81">
       <calculatedColumnFormula>Table3[[#This Row],[offense]]*$D$26+0.05</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="leadoff modifier" dataDxfId="77">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="leadoff modifier" dataDxfId="80">
       <calculatedColumnFormula>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*$E$26</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="total leadoff (ft)" dataDxfId="76">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="total leadoff (ft)" dataDxfId="79">
       <calculatedColumnFormula>MAX(Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90, 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="pickoff manuver (s)" dataDxfId="75">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="pickoff manuver (s)" dataDxfId="78">
       <calculatedColumnFormula>1.1 - Table3[[#This Row],[defense]]*0.1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="throw speed (s/ft)" dataDxfId="74">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="throw speed (s/ft)" dataDxfId="77">
       <calculatedColumnFormula xml:space="preserve"> 0.01 - 0.0025 *  Table3[[#This Row],[defense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="throw speed (mph)" dataDxfId="73">
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="throw speed (mph)" dataDxfId="76">
       <calculatedColumnFormula>1 / Table3[[#This Row],[throw speed (s/ft)]] * ((60 * 60)/5280)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="pickoff time" dataDxfId="72">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="pickoff time" dataDxfId="75">
       <calculatedColumnFormula>Table3[[#This Row],[pickoff manuver (s)]]+60*Table3[[#This Row],[throw speed (s/ft)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="runner reaction" dataDxfId="71">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="runner reaction" dataDxfId="74">
       <calculatedColumnFormula>$K$28-$K$26*Table3[[#This Row],[offense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="runner speed (s/ft)" dataDxfId="70">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="runner speed (s/ft)" dataDxfId="73">
       <calculatedColumnFormula>0.05 - Table3[[#This Row],[offense]]*$L$26</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="runner speed (mph)" dataDxfId="69">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="runner speed (mph)" dataDxfId="72">
       <calculatedColumnFormula>1 / Table3[[#This Row],[runner speed (s/ft)]] * ((60 * 60)/5280)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="pickoff evade time" dataDxfId="68">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="pickoff evade time" dataDxfId="71">
       <calculatedColumnFormula>Table3[[#This Row],[runner reaction]]+Table3[[#This Row],[runner speed (s/ft)]]*Table3[[#This Row],[total leadoff (ft)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="pickoff probability" dataDxfId="67" dataCellStyle="Percent">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="pickoff probability" dataDxfId="70" dataCellStyle="Percent">
       <calculatedColumnFormula>1 - _xlfn.NORM.DIST(Table3[[#This Row],[pickoff time]], Table3[[#This Row],[pickoff evade time]], $O$4, TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Fielding Odds" dataDxfId="66" dataCellStyle="Percent">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Fielding Odds" dataDxfId="69" dataCellStyle="Percent">
       <calculatedColumnFormula>_xlfn.NORM.DIST(Table3[[#This Row],[defense]], $P$26, $P$27, TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="pickoff worth it?" dataDxfId="65">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="pickoff worth it?" dataDxfId="68">
       <calculatedColumnFormula>Table3[[#This Row],[pickoff probability]] &gt; 1-Table3[[#This Row],[Fielding Odds]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Error %" dataDxfId="64" dataCellStyle="Percent">
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Error %" dataDxfId="67" dataCellStyle="Percent">
       <calculatedColumnFormula>1-Table3[[#This Row],[Fielding Odds]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Blatant steal time" dataDxfId="63">
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Blatant steal time" dataDxfId="66">
       <calculatedColumnFormula>(90-Table3[[#This Row],[total leadoff (ft)]])*Table3[[#This Row],[runner speed (s/ft)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Response speed" dataDxfId="62">
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Response speed" dataDxfId="65">
       <calculatedColumnFormula>$T$26*(2-Table3[[#This Row],[defense]]) + Table3[[#This Row],[pickoff time]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="blatant steal probability" dataDxfId="61" dataCellStyle="Percent">
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="blatant steal probability" dataDxfId="64" dataCellStyle="Percent">
       <calculatedColumnFormula>_xlfn.NORM.DIST(Table3[[#This Row],[Response speed]], Table3[[#This Row],[Blatant steal time]], $U$4, TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="defense fear" dataDxfId="60">
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="defense fear" dataDxfId="63">
       <calculatedColumnFormula>Table3[[#This Row],[defense]]+Table3[[#This Row],[defense]]*Table3[[#This Row],[offense]]*$E$26</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="ball factor" dataDxfId="59">
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="ball factor" dataDxfId="62">
       <calculatedColumnFormula>(1-$W$32)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="desperation" dataDxfId="58" dataCellStyle="Percent">
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="desperation" dataDxfId="61" dataCellStyle="Percent">
       <calculatedColumnFormula>Table3[[#This Row],[ball factor]]/$X$32*(1-$X$34)+$X$34</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="player control" dataDxfId="57">
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="player control" dataDxfId="60">
       <calculatedColumnFormula>Table3[[#This Row],[offense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="ideal steer" dataDxfId="56">
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="ideal steer" dataDxfId="59">
       <calculatedColumnFormula>$AA$33</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="scaled control" dataDxfId="55">
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="scaled control" dataDxfId="58">
       <calculatedColumnFormula>IF(Table3[[#This Row],[player control]]&gt;1,Table3[[#This Row],[player control]]*$AA$41+$AA$40,Table3[[#This Row],[player control]]*$AA$39+$AA$38)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="unmod foul percent 3rd" dataDxfId="54" dataCellStyle="Percent">
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="unmod foul percent 3rd" dataDxfId="57" dataCellStyle="Percent">
       <calculatedColumnFormula>_xlfn.NORM.DIST(-1,Table3[[#This Row],[ideal steer]],($AB$25-Table3[[#This Row],[scaled control]])*$AB$27,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="unmod foul percent 1st" dataDxfId="53" dataCellStyle="Percent">
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="unmod foul percent 1st" dataDxfId="56" dataCellStyle="Percent">
       <calculatedColumnFormula>1-_xlfn.NORM.DIST(1,Table3[[#This Row],[ideal steer]],($AB$25-Table3[[#This Row],[scaled control]])*$AB$27,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="total unmod foul percent" dataDxfId="52" dataCellStyle="Percent">
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="total unmod foul percent" dataDxfId="55" dataCellStyle="Percent">
       <calculatedColumnFormula>1-(1-Table3[[#This Row],[unmod foul percent 3rd]])*(1-Table3[[#This Row],[unmod foul percent 1st]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="unmod dead center foul%" dataDxfId="51" dataCellStyle="Percent">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="unmod dead center foul%" dataDxfId="54" dataCellStyle="Percent">
       <calculatedColumnFormula>1-((1-_xlfn.NORM.DIST(-1,0,($AB$25-Table3[[#This Row],[scaled control]])*$AB$27,TRUE))*_xlfn.NORM.DIST(1,0,($AB$25-Table3[[#This Row],[scaled control]])*$AB$27,TRUE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="count" dataDxfId="50">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="count" dataDxfId="53">
       <calculatedColumnFormula>$AF$34*$AF$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="hitter discipline bias" dataDxfId="49">
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="hitter discipline bias" dataDxfId="52">
       <calculatedColumnFormula>$AG$25*($AG$34*Table3[[#This Row],[offense]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="bases loaded" dataDxfId="48">
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="bases loaded" dataDxfId="51">
       <calculatedColumnFormula>$AH$25*$AH$34</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="number of outs" dataDxfId="47">
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="number of outs" dataDxfId="50">
       <calculatedColumnFormula>$AI$34*$AI$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="current hitter vs next hitter" dataDxfId="46">
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="current hitter vs next hitter" dataDxfId="49">
       <calculatedColumnFormula>$AJ$25*(Table3[[#This Row],[offense]]-$AJ$27)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="calling modifier" dataDxfId="45">
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="calling modifier" dataDxfId="48">
       <calculatedColumnFormula array="1">SUM(Table3[[#This Row],[count]:[current hitter vs next hitter]]*MIN(1, Table3[[#This Row],[defense]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="sigmoid strike percent" dataDxfId="44" dataCellStyle="Percent">
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="sigmoid strike percent" dataDxfId="47" dataCellStyle="Percent">
       <calculatedColumnFormula>$AL$25-(Table3[[#This Row],[calling modifier]]/(ABS(Table3[[#This Row],[calling modifier]])+$AL$29)*$AL$27)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="tanh strike percent" dataDxfId="43" dataCellStyle="Percent">
+    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="tanh strike percent" dataDxfId="46" dataCellStyle="Percent">
       <calculatedColumnFormula>$AL$25-$AL$27*TANH(Table3[[#This Row],[calling modifier]]/$AM$29)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="called position" dataDxfId="42" dataCellStyle="Percent">
+    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="called position" dataDxfId="45" dataCellStyle="Percent">
       <calculatedColumnFormula>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-Table3[[#This Row],[defense]])))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="called pos 0.2 pitch" dataDxfId="41">
+    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="called pos 0.2 pitch" dataDxfId="44">
       <calculatedColumnFormula>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-0.2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="called pos 2 pitch" dataDxfId="40">
+    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="called pos 2 pitch" dataDxfId="43">
       <calculatedColumnFormula>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="location -1  stdv" dataDxfId="39">
+    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="location -1  stdv" dataDxfId="42">
       <calculatedColumnFormula>Table3[[#This Row],[called position]]-pitchmod*(pitchstdv-Table3[[#This Row],[defense]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="location +1 stdv" dataDxfId="38">
+    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="location +1 stdv" dataDxfId="41">
       <calculatedColumnFormula>ABS(Table3[[#This Row],[called position]]+pitchmod*(pitchstdv-Table3[[#This Row],[defense]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="min dist to sz 1stdv" dataDxfId="37">
+    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="min dist to sz 1stdv" dataDxfId="40">
       <calculatedColumnFormula>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;1, Table3[[#This Row],[location +1 stdv]]&gt;1),0, MIN(Table3[[#This Row],[location -1  stdv]]+1, 1-Table3[[#This Row],[location +1 stdv]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="max dist to sz 1stdv" dataDxfId="36">
+    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="max dist to sz 1stdv" dataDxfId="39">
       <calculatedColumnFormula>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;0, Table3[[#This Row],[location +1 stdv]]&gt;0),1, MAX(1-ABS(Table3[[#This Row],[location -1  stdv]]), Table3[[#This Row],[location +1 stdv]]-1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="ave obscurity" dataDxfId="35">
+    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="ave obscurity" dataDxfId="38">
       <calculatedColumnFormula>$AU$30/(ABS(Table3[[#This Row],[called position]]-1)+$AU$27)+$AU$32*Table3[[#This Row],[defense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="obscurity at _x000a_0.5" dataDxfId="34">
+    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="obscurity at _x000a_0.5" dataDxfId="37">
       <calculatedColumnFormula>$AU$30/(ABS(0.5-1)+$AU$27)+$AU$32*Table3[[#This Row],[defense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="obscurity at  0.9" dataDxfId="33">
+    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="obscurity at  0.9" dataDxfId="36">
       <calculatedColumnFormula>$AU$30/(ABS(0.9-1)+$AU$27)+$AU$32*Table3[[#This Row],[defense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="average difficulty" dataDxfId="32">
+    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="average difficulty" dataDxfId="35">
       <calculatedColumnFormula>Table3[[#This Row],[defense]]*$AX$30+MAX(0, Table3[[#This Row],[called position]]-$AX$27)^$AX$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" name="+1stdv difficulty" dataDxfId="31">
+    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" name="+1stdv difficulty" dataDxfId="34">
       <calculatedColumnFormula>Table3[[#This Row],[defense]]*$AX$30 + MAX(0, Table3[[#This Row],[location +1 stdv]]-$AX$27)^$AX$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0000-000037000000}" name="difficulty at 1" dataDxfId="30">
+    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0000-000037000000}" name="difficulty at 1" dataDxfId="33">
       <calculatedColumnFormula>Table3[[#This Row],[defense]]*$AX$30+MAX(0, 1-$AX$27)^$AX$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="62" xr3:uid="{6513900D-2CAC-4022-A6B3-8A00EE6C566B}" name="reduction" dataDxfId="29">
+    <tableColumn id="62" xr3:uid="{6513900D-2CAC-4022-A6B3-8A00EE6C566B}" name="reduction" dataDxfId="32">
       <calculatedColumnFormula>MAX(0, 0.1*(1-Table3[[#This Row],[defense]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="63" xr3:uid="{12464915-1D8C-4EB5-9BBD-0FF526658E5B}" name="Location" dataDxfId="28">
+    <tableColumn id="63" xr3:uid="{12464915-1D8C-4EB5-9BBD-0FF526658E5B}" name="Location" dataDxfId="31">
       <calculatedColumnFormula>$BB$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="64" xr3:uid="{5F0F19BE-6D04-4E9E-81B2-B324AB353F5C}" name="obscurity" dataDxfId="27">
+    <tableColumn id="64" xr3:uid="{5F0F19BE-6D04-4E9E-81B2-B324AB353F5C}" name="obscurity" dataDxfId="30">
       <calculatedColumnFormula>$AU$30/(ABS(Table3[[#This Row],[Location]]-1)+$AU$27)+$AU$32*Table3[[#This Row],[defense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="65" xr3:uid="{EA3D32E7-A2E2-482C-B6E9-2E17651C5F77}" name="Strike?" dataDxfId="26">
+    <tableColumn id="65" xr3:uid="{EA3D32E7-A2E2-482C-B6E9-2E17651C5F77}" name="Strike?" dataDxfId="29">
       <calculatedColumnFormula>Table3[[#This Row],[Location]]&lt;= (1+MAX(0, (Table3[[#This Row],[defense]]-1)*0.1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="66" xr3:uid="{0C7E9B06-240B-481E-B495-54026E2F00AA}" name="discipline modifier" dataDxfId="25">
+    <tableColumn id="66" xr3:uid="{0C7E9B06-240B-481E-B495-54026E2F00AA}" name="discipline modifier" dataDxfId="28">
       <calculatedColumnFormula>1/(1+Table3[[#This Row],[offense]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="67" xr3:uid="{D3B0837D-02D4-4F62-A2E2-876739E497B0}" name="effective obscurity" dataDxfId="24">
+    <tableColumn id="67" xr3:uid="{D3B0837D-02D4-4F62-A2E2-876739E497B0}" name="effective obscurity" dataDxfId="27">
       <calculatedColumnFormula>Table3[[#This Row],[obscurity]]*Table3[[#This Row],[discipline modifier]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="69" xr3:uid="{39822A5F-1791-48DC-BA9F-A066931C0292}" name="odds of read" dataCellStyle="Percent">
@@ -9296,43 +11986,43 @@
     <tableColumn id="72" xr3:uid="{3E21C76F-F55B-4E49-9BE2-FEE046008C15}" name="adjusted swing %" dataCellStyle="Percent">
       <calculatedColumnFormula>Table3[[#This Row],[desperation echo]]*Table3[[#This Row],[unadjusted swing %]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="130" xr3:uid="{827C9303-3867-43F7-A79B-BC2EAB3F896D}" name="pitch carry forward obsc" dataDxfId="23">
+    <tableColumn id="130" xr3:uid="{827C9303-3867-43F7-A79B-BC2EAB3F896D}" name="pitch carry forward obsc" dataDxfId="26">
       <calculatedColumnFormula>Table3[[#This Row],[ave obscurity]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="131" xr3:uid="{F26B1E2C-89D5-4F6D-877A-1BEA7F7DF5A9}" name="CF odds of read" dataCellStyle="Percent">
       <calculatedColumnFormula>1/(1+Table3[[#This Row],[ave obscurity]]*Table3[[#This Row],[discipline modifier]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="73" xr3:uid="{77BBE784-030D-4E46-9A29-8783B89762BC}" name="contact echo" dataDxfId="22">
+    <tableColumn id="73" xr3:uid="{77BBE784-030D-4E46-9A29-8783B89762BC}" name="contact echo" dataDxfId="25">
       <calculatedColumnFormula>Table3[[#This Row],[offense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="75" xr3:uid="{074A9F48-3941-4E36-90C2-7710217D32C8}" name="pitch carry forward diff" dataDxfId="21">
+    <tableColumn id="75" xr3:uid="{074A9F48-3941-4E36-90C2-7710217D32C8}" name="pitch carry forward diff" dataDxfId="24">
       <calculatedColumnFormula>Table3[[#This Row],[average difficulty]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="76" xr3:uid="{628DDA60-D380-4EE8-AA7D-7EF6C4AAD8A5}" name="CF contact readiness" dataDxfId="20">
+    <tableColumn id="76" xr3:uid="{628DDA60-D380-4EE8-AA7D-7EF6C4AAD8A5}" name="CF contact readiness" dataDxfId="23">
       <calculatedColumnFormula>Table3[[#This Row],[contact echo]]-Table3[[#This Row],[pitch carry forward diff]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="77" xr3:uid="{DBF18AD6-8593-42C7-9058-D19737088E6D}" name="foul %" dataDxfId="19" dataCellStyle="Percent">
+    <tableColumn id="77" xr3:uid="{DBF18AD6-8593-42C7-9058-D19737088E6D}" name="foul %" dataDxfId="22" dataCellStyle="Percent">
       <calculatedColumnFormula>1-_xlfn.NORM.DIST($BP$27,Table3[[#This Row],[CF contact readiness]], $BP$30,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="78" xr3:uid="{6354951A-151E-4E04-9897-9CB39D6098C8}" name="clean %" dataDxfId="18" dataCellStyle="Percent">
+    <tableColumn id="78" xr3:uid="{6354951A-151E-4E04-9897-9CB39D6098C8}" name="clean %" dataDxfId="21" dataCellStyle="Percent">
       <calculatedColumnFormula>1-_xlfn.NORM.DIST($BP$25,Table3[[#This Row],[CF contact readiness]], $BP$30,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="79" xr3:uid="{0070F673-D13C-467D-95AC-FF8413A02F3F}" name="strike swinging %" dataDxfId="17" dataCellStyle="Percent">
+    <tableColumn id="79" xr3:uid="{0070F673-D13C-467D-95AC-FF8413A02F3F}" name="strike swinging %" dataDxfId="20" dataCellStyle="Percent">
       <calculatedColumnFormula>1-Table3[[#This Row],[foul %]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="80" xr3:uid="{9504D0CF-7CD0-472F-8289-44B30538D80C}" name="ave. hit quality" dataDxfId="16">
+    <tableColumn id="80" xr3:uid="{9504D0CF-7CD0-472F-8289-44B30538D80C}" name="ave. hit quality" dataDxfId="19">
       <calculatedColumnFormula>(Table3[[#This Row],[CF contact readiness]]-$BP$27)/$BP$30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="132" xr3:uid="{0BB169E4-F345-4B7D-A549-DE28DC5FB113}" name="hit quality +1stdv" dataDxfId="15">
+    <tableColumn id="132" xr3:uid="{0BB169E4-F345-4B7D-A549-DE28DC5FB113}" name="hit quality +1stdv" dataDxfId="18">
       <calculatedColumnFormula>(Table3[[#This Row],[CF contact readiness]]+$BP$30-$BP$27)/$BP$30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="81" xr3:uid="{37438EAA-344A-486C-A4C2-68EE17D67C60}" name="hit quality remainder" dataDxfId="14">
+    <tableColumn id="81" xr3:uid="{37438EAA-344A-486C-A4C2-68EE17D67C60}" name="hit quality remainder" dataDxfId="17">
       <calculatedColumnFormula>MAX(0, IF(ISBLANK($BU$28), Table3[[#This Row],[hit quality +1stdv]], $BU$28)-1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="82" xr3:uid="{CBA11BEE-0412-44C3-979C-1888629B3C7A}" name="adjusted launch angle" dataDxfId="13">
+    <tableColumn id="82" xr3:uid="{CBA11BEE-0412-44C3-979C-1888629B3C7A}" name="adjusted launch angle" dataDxfId="16">
       <calculatedColumnFormula>$BV$25+Table3[[#This Row],[offense]]*$BV$28</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="83" xr3:uid="{8DC0E209-2987-40FE-9521-B3339A7D8E1F}" name="angle stdev" dataDxfId="12">
+    <tableColumn id="83" xr3:uid="{8DC0E209-2987-40FE-9521-B3339A7D8E1F}" name="angle stdev" dataDxfId="15">
       <calculatedColumnFormula>$BW$25*$BW$28/($BW$28+Table3[[#This Row],[hit quality remainder]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="84" xr3:uid="{F8EB7F4C-5D31-472E-A363-210E62A7E683}" name="grounder % (&lt;10 deg)" dataCellStyle="Percent">
@@ -9341,37 +12031,37 @@
     <tableColumn id="85" xr3:uid="{56DD6E0A-39C0-4DF0-B1CB-47EB71B71306}" name="pop up % (&gt;50 deg)" dataCellStyle="Percent">
       <calculatedColumnFormula>1-_xlfn.NORM.DIST(50, Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="86" xr3:uid="{6ED971D4-0303-4AEB-B7CD-9516517F447E}" name="odds of 3B" dataDxfId="11" dataCellStyle="Percent">
+    <tableColumn id="86" xr3:uid="{6ED971D4-0303-4AEB-B7CD-9516517F447E}" name="odds of 3B" dataDxfId="14" dataCellStyle="Percent">
       <calculatedColumnFormula>1-_xlfn.NORM.DIST(70, $BZ$28,$BZ$25,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="87" xr3:uid="{E9F9DFB6-4A26-4CA7-9318-6ECA478690D6}" name="exit velocity mean" dataDxfId="10">
+    <tableColumn id="87" xr3:uid="{E9F9DFB6-4A26-4CA7-9318-6ECA478690D6}" name="exit velocity mean" dataDxfId="13">
       <calculatedColumnFormula>$CA$25+Table3[[#This Row],[offense]]*($CA$27-$CA$25)/2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="88" xr3:uid="{EB865A5D-CC1D-49FA-9709-DC5F30F55DD8}" name="after reduction" dataDxfId="9">
+    <tableColumn id="88" xr3:uid="{EB865A5D-CC1D-49FA-9709-DC5F30F55DD8}" name="after reduction" dataDxfId="12">
       <calculatedColumnFormula>Table3[[#This Row],[exit velocity mean]]-Table3[[#This Row],[reduction]]*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="89" xr3:uid="{949E8C38-C424-4A4E-9A6F-FCA93496D192}" name="theoretical distance" dataDxfId="8">
+    <tableColumn id="89" xr3:uid="{949E8C38-C424-4A4E-9A6F-FCA93496D192}" name="theoretical distance" dataDxfId="11">
       <calculatedColumnFormula>Table3[[#This Row],[exit velocity mean]]^2*2*SIN(RADIANS(Table3[[#This Row],[adjusted launch angle]]))/$CC$28*5280</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="90" xr3:uid="{9FD0A88A-D0D9-4369-8D70-6C7485CA1509}" name="flight time" dataDxfId="7">
+    <tableColumn id="90" xr3:uid="{9FD0A88A-D0D9-4369-8D70-6C7485CA1509}" name="flight time" dataDxfId="10">
       <calculatedColumnFormula>2*Table3[[#This Row],[exit velocity mean]]*SIN(RADIANS(Table3[[#This Row],[adjusted launch angle]]))/$CC$28*60*60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="91" xr3:uid="{D9D5DFED-BD09-4CB6-A82E-D289D2DAB08D}" name="actual distance" dataDxfId="6">
+    <tableColumn id="91" xr3:uid="{D9D5DFED-BD09-4CB6-A82E-D289D2DAB08D}" name="actual distance" dataDxfId="9">
       <calculatedColumnFormula>Table3[[#This Row],[theoretical distance]]-Table3[[#This Row],[flight time]]^2*$CE$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="92" xr3:uid="{3D80331E-564D-462D-81B5-E5CE730D1EE5}" name="+1stdv EV" dataDxfId="5">
+    <tableColumn id="92" xr3:uid="{3D80331E-564D-462D-81B5-E5CE730D1EE5}" name="+1stdv EV" dataDxfId="8">
       <calculatedColumnFormula>Table3[[#This Row],[exit velocity mean]]+$CC$25-Table3[[#This Row],[reduction]]*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="93" xr3:uid="{211123A1-65C0-4F59-AB86-C344CFF47F70}" name="+1stdv LA" dataDxfId="4">
+    <tableColumn id="93" xr3:uid="{211123A1-65C0-4F59-AB86-C344CFF47F70}" name="+1stdv LA" dataDxfId="7">
       <calculatedColumnFormula>MIN(Table3[[#This Row],[adjusted launch angle]]+Table3[[#This Row],[angle stdev]], 30)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="94" xr3:uid="{C8736D16-AF27-436D-BF61-CA3E58298CD3}" name="+1stdv flight time" dataDxfId="3">
+    <tableColumn id="94" xr3:uid="{C8736D16-AF27-436D-BF61-CA3E58298CD3}" name="+1stdv flight time" dataDxfId="6">
       <calculatedColumnFormula>2*Table3[[#This Row],[+1stdv EV]]*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*60*60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="95" xr3:uid="{C9967388-9755-4293-82E9-4E43A4770599}" name="+1stdev distance" dataDxfId="2">
+    <tableColumn id="95" xr3:uid="{C9967388-9755-4293-82E9-4E43A4770599}" name="+1stdev distance" dataDxfId="5">
       <calculatedColumnFormula>Table3[[#This Row],[+1stdv EV]]^2*2*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*5280-Table3[[#This Row],[+1stdv flight time]]^2*$CE$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="96" xr3:uid="{52B6BA3A-87F7-49FD-BFE7-811EA76B03FD}" name="+1stdev delta" dataDxfId="1">
+    <tableColumn id="96" xr3:uid="{52B6BA3A-87F7-49FD-BFE7-811EA76B03FD}" name="+1stdev delta" dataDxfId="4">
       <calculatedColumnFormula>Table3[[#This Row],[+1stdev distance]]-Table3[[#This Row],[actual distance]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="97" xr3:uid="{50EEB2EF-C836-4BBC-A8B3-EAD31BF29B54}" name="Column95"/>
@@ -9416,8 +12106,25 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{23FB116D-6CB4-49F6-A874-F1C610DEF5E1}" name="quality"/>
     <tableColumn id="2" xr3:uid="{6204ECDD-C980-4BE0-AFC7-9F83BF472BE8}" name="net"/>
-    <tableColumn id="3" xr3:uid="{E9208F79-490A-4A40-B3B7-0914BA16AC90}" name="form" dataDxfId="0">
+    <tableColumn id="3" xr3:uid="{E9208F79-490A-4A40-B3B7-0914BA16AC90}" name="form" dataDxfId="3">
       <calculatedColumnFormula>POWER(Table1[[#This Row],[quality]]-0.8, 1/4)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CEC18A43-64FC-4CDC-9CAF-1945616C5259}" name="Table2" displayName="Table2" ref="A1:D32" totalsRowShown="0">
+  <autoFilter ref="A1:D32" xr:uid="{CEC18A43-64FC-4CDC-9CAF-1945616C5259}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{1AE5C4EC-1E31-4AB8-9D00-52347412BAAD}" name="x"/>
+    <tableColumn id="2" xr3:uid="{DE2F5C94-46DF-4FEE-9B65-021E2F22BA8F}" name="y" dataDxfId="1">
+      <calculatedColumnFormula>IF(Table2[[#This Row],[x]]&gt;300, Table2[[#This Row],[x]]/300, (Table2[[#This Row],[x]]/300)^2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{7F7D12A9-EB9C-4F1E-AA19-600982A4A24A}" name="target"/>
+    <tableColumn id="4" xr3:uid="{7C986021-1ABB-4A6F-8B01-CE482AFA0C81}" name="delta" dataDxfId="2">
+      <calculatedColumnFormula>Table2[[#This Row],[y]]-B1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -9689,8 +12396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DO41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+    <sheetView topLeftCell="BQ1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="CB11" sqref="CB11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16528,7 +19235,7 @@
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
   <conditionalFormatting sqref="O7:O22">
-    <cfRule type="cellIs" dxfId="82" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16541,12 +19248,234 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="23.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D7" t="s">
+        <v>118</v>
+      </c>
+      <c r="E7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D8" t="s">
+        <v>117</v>
+      </c>
+      <c r="E8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" t="s">
+        <v>118</v>
+      </c>
+      <c r="D9" t="s">
+        <v>118</v>
+      </c>
+      <c r="E9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF285913-BB23-45EF-B183-28069296EF50}">
   <dimension ref="J12:L18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X6" sqref="X6"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16644,6 +19573,768 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80A4F72A-6EF1-4451-BFA6-39EE9D1AFD85}">
+  <dimension ref="A2:CV2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:100" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>42.212801833565102</v>
+      </c>
+      <c r="B2">
+        <v>42.934887913960999</v>
+      </c>
+      <c r="C2">
+        <v>42.898730355704302</v>
+      </c>
+      <c r="D2">
+        <v>41.656111618988803</v>
+      </c>
+      <c r="E2">
+        <v>38.088802865929203</v>
+      </c>
+      <c r="F2">
+        <v>36.283573380573003</v>
+      </c>
+      <c r="G2">
+        <v>34.977259720042497</v>
+      </c>
+      <c r="H2">
+        <v>33.909741670306197</v>
+      </c>
+      <c r="I2">
+        <v>32.986494885463202</v>
+      </c>
+      <c r="J2">
+        <v>32.161158910431297</v>
+      </c>
+      <c r="K2">
+        <v>31.4071344909994</v>
+      </c>
+      <c r="L2">
+        <v>30.707576594918599</v>
+      </c>
+      <c r="M2">
+        <v>30.051060991771799</v>
+      </c>
+      <c r="N2">
+        <v>29.429437819890701</v>
+      </c>
+      <c r="O2">
+        <v>28.836661700422098</v>
+      </c>
+      <c r="P2">
+        <v>28.268106510022601</v>
+      </c>
+      <c r="Q2">
+        <v>27.720140767285901</v>
+      </c>
+      <c r="R2">
+        <v>27.189852293771501</v>
+      </c>
+      <c r="S2">
+        <v>26.674862864410802</v>
+      </c>
+      <c r="T2">
+        <v>26.173199454009101</v>
+      </c>
+      <c r="U2">
+        <v>25.6832023704597</v>
+      </c>
+      <c r="V2">
+        <v>25.203458172670601</v>
+      </c>
+      <c r="W2">
+        <v>24.732749686016099</v>
+      </c>
+      <c r="X2">
+        <v>24.270018086598199</v>
+      </c>
+      <c r="Y2">
+        <v>23.8143336787242</v>
+      </c>
+      <c r="Z2">
+        <v>23.364873047401002</v>
+      </c>
+      <c r="AA2">
+        <v>22.9209009611025</v>
+      </c>
+      <c r="AB2">
+        <v>22.4817558651011</v>
+      </c>
+      <c r="AC2">
+        <v>22.046838123804999</v>
+      </c>
+      <c r="AD2">
+        <v>21.615600392170901</v>
+      </c>
+      <c r="AE2">
+        <v>21.1875396531895</v>
+      </c>
+      <c r="AF2">
+        <v>20.7621905712273</v>
+      </c>
+      <c r="AG2">
+        <v>20.339119893166199</v>
+      </c>
+      <c r="AH2">
+        <v>20.011713709635799</v>
+      </c>
+      <c r="AI2">
+        <v>20.071248189251101</v>
+      </c>
+      <c r="AJ2">
+        <v>20.130028834074501</v>
+      </c>
+      <c r="AK2">
+        <v>20.188124066911701</v>
+      </c>
+      <c r="AL2">
+        <v>20.245597638021898</v>
+      </c>
+      <c r="AM2">
+        <v>20.302509224591599</v>
+      </c>
+      <c r="AN2">
+        <v>20.358914953995999</v>
+      </c>
+      <c r="AO2">
+        <v>20.414867863754701</v>
+      </c>
+      <c r="AP2">
+        <v>20.470418308789402</v>
+      </c>
+      <c r="AQ2">
+        <v>20.525614324777099</v>
+      </c>
+      <c r="AR2">
+        <v>20.5805019549544</v>
+      </c>
+      <c r="AS2">
+        <v>20.6351255465785</v>
+      </c>
+      <c r="AT2">
+        <v>20.689528022341101</v>
+      </c>
+      <c r="AU2">
+        <v>20.7437511313037</v>
+      </c>
+      <c r="AV2">
+        <v>20.797835683351199</v>
+      </c>
+      <c r="AW2">
+        <v>20.851821770710799</v>
+      </c>
+      <c r="AX2">
+        <v>20.905748979740999</v>
+      </c>
+      <c r="AY2">
+        <v>20.959656595943098</v>
+      </c>
+      <c r="AZ2">
+        <v>21.013583804973401</v>
+      </c>
+      <c r="BA2">
+        <v>21.067569892333001</v>
+      </c>
+      <c r="BB2">
+        <v>21.1216544443805</v>
+      </c>
+      <c r="BC2">
+        <v>21.175877553343</v>
+      </c>
+      <c r="BD2">
+        <v>21.2302800291056</v>
+      </c>
+      <c r="BE2">
+        <v>21.2849036207297</v>
+      </c>
+      <c r="BF2">
+        <v>21.339791250906998</v>
+      </c>
+      <c r="BG2">
+        <v>21.394987266894699</v>
+      </c>
+      <c r="BH2">
+        <v>21.4505377119294</v>
+      </c>
+      <c r="BI2">
+        <v>21.506490621688101</v>
+      </c>
+      <c r="BJ2">
+        <v>21.562896351092501</v>
+      </c>
+      <c r="BK2">
+        <v>21.619807937662198</v>
+      </c>
+      <c r="BL2">
+        <v>21.677281508772399</v>
+      </c>
+      <c r="BM2">
+        <v>21.735376741609599</v>
+      </c>
+      <c r="BN2">
+        <v>21.794157386433</v>
+      </c>
+      <c r="BO2">
+        <v>21.853691866048301</v>
+      </c>
+      <c r="BP2">
+        <v>21.914053967316502</v>
+      </c>
+      <c r="BQ2">
+        <v>21.975323644259301</v>
+      </c>
+      <c r="BR2">
+        <v>22.037587957135599</v>
+      </c>
+      <c r="BS2">
+        <v>22.100942178116199</v>
+      </c>
+      <c r="BT2">
+        <v>22.165491102371799</v>
+      </c>
+      <c r="BU2">
+        <v>22.231350614215</v>
+      </c>
+      <c r="BV2">
+        <v>22.298649572394101</v>
+      </c>
+      <c r="BW2">
+        <v>22.367532098154999</v>
+      </c>
+      <c r="BX2">
+        <v>22.4381603763584</v>
+      </c>
+      <c r="BY2">
+        <v>22.510718116853301</v>
+      </c>
+      <c r="BZ2">
+        <v>22.585414875136799</v>
+      </c>
+      <c r="CA2">
+        <v>22.6624915052126</v>
+      </c>
+      <c r="CB2">
+        <v>22.742227124704499</v>
+      </c>
+      <c r="CC2">
+        <v>22.824948130571201</v>
+      </c>
+      <c r="CD2">
+        <v>22.9110400425233</v>
+      </c>
+      <c r="CE2">
+        <v>23.000963319756298</v>
+      </c>
+      <c r="CF2">
+        <v>23.095274880314001</v>
+      </c>
+      <c r="CG2">
+        <v>23.1946580043324</v>
+      </c>
+      <c r="CH2">
+        <v>23.299964907415799</v>
+      </c>
+      <c r="CI2">
+        <v>23.412279082039699</v>
+      </c>
+      <c r="CJ2">
+        <v>23.5330096545689</v>
+      </c>
+      <c r="CK2">
+        <v>23.664039946016299</v>
+      </c>
+      <c r="CL2">
+        <v>23.8079728605322</v>
+      </c>
+      <c r="CM2">
+        <v>23.968561107030599</v>
+      </c>
+      <c r="CN2">
+        <v>24.151521308655902</v>
+      </c>
+      <c r="CO2">
+        <v>24.3662394945848</v>
+      </c>
+      <c r="CP2">
+        <v>24.629895364844899</v>
+      </c>
+      <c r="CQ2">
+        <v>24.979913904377401</v>
+      </c>
+      <c r="CR2">
+        <v>25.530687395308298</v>
+      </c>
+      <c r="CS2">
+        <v>27.113167400177701</v>
+      </c>
+      <c r="CT2">
+        <v>28.370735758753501</v>
+      </c>
+      <c r="CU2">
+        <v>29.462484375689701</v>
+      </c>
+      <c r="CV2">
+        <v>30.439551405476202</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48AF6B93-1A07-417B-961A-AB8D0F990765}">
+  <dimension ref="A1:D32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <f>IF(Table2[[#This Row],[x]]&gt;300, Table2[[#This Row],[x]]/300, (Table2[[#This Row],[x]]/300)^2)</f>
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="e">
+        <f>Table2[[#This Row],[y]]-B1</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <f>IF(Table2[[#This Row],[x]]&gt;300, Table2[[#This Row],[x]]/300, (Table2[[#This Row],[x]]/300)^2)</f>
+        <v>4.4444444444444444E-3</v>
+      </c>
+      <c r="D3">
+        <f>Table2[[#This Row],[y]]-B2</f>
+        <v>4.4444444444444444E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>40</v>
+      </c>
+      <c r="B4">
+        <f>IF(Table2[[#This Row],[x]]&gt;300, Table2[[#This Row],[x]]/300, (Table2[[#This Row],[x]]/300)^2)</f>
+        <v>1.7777777777777778E-2</v>
+      </c>
+      <c r="D4">
+        <f>Table2[[#This Row],[y]]-B3</f>
+        <v>1.3333333333333332E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>60</v>
+      </c>
+      <c r="B5">
+        <f>IF(Table2[[#This Row],[x]]&gt;300, Table2[[#This Row],[x]]/300, (Table2[[#This Row],[x]]/300)^2)</f>
+        <v>4.0000000000000008E-2</v>
+      </c>
+      <c r="D5">
+        <f>Table2[[#This Row],[y]]-B4</f>
+        <v>2.222222222222223E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>80</v>
+      </c>
+      <c r="B6">
+        <f>IF(Table2[[#This Row],[x]]&gt;300, Table2[[#This Row],[x]]/300, (Table2[[#This Row],[x]]/300)^2)</f>
+        <v>7.1111111111111111E-2</v>
+      </c>
+      <c r="D6">
+        <f>Table2[[#This Row],[y]]-B5</f>
+        <v>3.1111111111111103E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>100</v>
+      </c>
+      <c r="B7">
+        <f>IF(Table2[[#This Row],[x]]&gt;300, Table2[[#This Row],[x]]/300, (Table2[[#This Row],[x]]/300)^2)</f>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="D7">
+        <f>Table2[[#This Row],[y]]-B6</f>
+        <v>3.9999999999999994E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>120</v>
+      </c>
+      <c r="B8">
+        <f>IF(Table2[[#This Row],[x]]&gt;300, Table2[[#This Row],[x]]/300, (Table2[[#This Row],[x]]/300)^2)</f>
+        <v>0.16000000000000003</v>
+      </c>
+      <c r="D8">
+        <f>Table2[[#This Row],[y]]-B7</f>
+        <v>4.8888888888888926E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>140</v>
+      </c>
+      <c r="B9">
+        <f>IF(Table2[[#This Row],[x]]&gt;300, Table2[[#This Row],[x]]/300, (Table2[[#This Row],[x]]/300)^2)</f>
+        <v>0.21777777777777779</v>
+      </c>
+      <c r="D9">
+        <f>Table2[[#This Row],[y]]-B8</f>
+        <v>5.7777777777777761E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>160</v>
+      </c>
+      <c r="B10">
+        <f>IF(Table2[[#This Row],[x]]&gt;300, Table2[[#This Row],[x]]/300, (Table2[[#This Row],[x]]/300)^2)</f>
+        <v>0.28444444444444444</v>
+      </c>
+      <c r="D10">
+        <f>Table2[[#This Row],[y]]-B9</f>
+        <v>6.6666666666666652E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>180</v>
+      </c>
+      <c r="B11">
+        <f>IF(Table2[[#This Row],[x]]&gt;300, Table2[[#This Row],[x]]/300, (Table2[[#This Row],[x]]/300)^2)</f>
+        <v>0.36</v>
+      </c>
+      <c r="D11">
+        <f>Table2[[#This Row],[y]]-B10</f>
+        <v>7.5555555555555542E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>200</v>
+      </c>
+      <c r="B12">
+        <f>IF(Table2[[#This Row],[x]]&gt;300, Table2[[#This Row],[x]]/300, (Table2[[#This Row],[x]]/300)^2)</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D12">
+        <f>Table2[[#This Row],[y]]-B11</f>
+        <v>8.4444444444444433E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>220</v>
+      </c>
+      <c r="B13">
+        <f>IF(Table2[[#This Row],[x]]&gt;300, Table2[[#This Row],[x]]/300, (Table2[[#This Row],[x]]/300)^2)</f>
+        <v>0.53777777777777769</v>
+      </c>
+      <c r="D13">
+        <f>Table2[[#This Row],[y]]-B12</f>
+        <v>9.3333333333333268E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>240</v>
+      </c>
+      <c r="B14">
+        <f>IF(Table2[[#This Row],[x]]&gt;300, Table2[[#This Row],[x]]/300, (Table2[[#This Row],[x]]/300)^2)</f>
+        <v>0.64000000000000012</v>
+      </c>
+      <c r="D14">
+        <f>Table2[[#This Row],[y]]-B13</f>
+        <v>0.10222222222222244</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>260</v>
+      </c>
+      <c r="B15">
+        <f>IF(Table2[[#This Row],[x]]&gt;300, Table2[[#This Row],[x]]/300, (Table2[[#This Row],[x]]/300)^2)</f>
+        <v>0.75111111111111117</v>
+      </c>
+      <c r="D15">
+        <f>Table2[[#This Row],[y]]-B14</f>
+        <v>0.11111111111111105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>280</v>
+      </c>
+      <c r="B16">
+        <f>IF(Table2[[#This Row],[x]]&gt;300, Table2[[#This Row],[x]]/300, (Table2[[#This Row],[x]]/300)^2)</f>
+        <v>0.87111111111111117</v>
+      </c>
+      <c r="D16">
+        <f>Table2[[#This Row],[y]]-B15</f>
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>300</v>
+      </c>
+      <c r="B17">
+        <f>IF(Table2[[#This Row],[x]]&gt;300, Table2[[#This Row],[x]]/300, (Table2[[#This Row],[x]]/300)^2)</f>
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <f>Table2[[#This Row],[y]]-B16</f>
+        <v>0.12888888888888883</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>320</v>
+      </c>
+      <c r="B18">
+        <f>IF(Table2[[#This Row],[x]]&gt;300, Table2[[#This Row],[x]]/300, (Table2[[#This Row],[x]]/300)^2)</f>
+        <v>1.0666666666666667</v>
+      </c>
+      <c r="D18">
+        <f>Table2[[#This Row],[y]]-B17</f>
+        <v>6.6666666666666652E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>340</v>
+      </c>
+      <c r="B19">
+        <f>IF(Table2[[#This Row],[x]]&gt;300, Table2[[#This Row],[x]]/300, (Table2[[#This Row],[x]]/300)^2)</f>
+        <v>1.1333333333333333</v>
+      </c>
+      <c r="D19">
+        <f>Table2[[#This Row],[y]]-B18</f>
+        <v>6.6666666666666652E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>360</v>
+      </c>
+      <c r="B20">
+        <f>IF(Table2[[#This Row],[x]]&gt;300, Table2[[#This Row],[x]]/300, (Table2[[#This Row],[x]]/300)^2)</f>
+        <v>1.2</v>
+      </c>
+      <c r="D20">
+        <f>Table2[[#This Row],[y]]-B19</f>
+        <v>6.6666666666666652E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>380</v>
+      </c>
+      <c r="B21">
+        <f>IF(Table2[[#This Row],[x]]&gt;300, Table2[[#This Row],[x]]/300, (Table2[[#This Row],[x]]/300)^2)</f>
+        <v>1.2666666666666666</v>
+      </c>
+      <c r="D21">
+        <f>Table2[[#This Row],[y]]-B20</f>
+        <v>6.6666666666666652E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>400</v>
+      </c>
+      <c r="B22">
+        <f>IF(Table2[[#This Row],[x]]&gt;300, Table2[[#This Row],[x]]/300, (Table2[[#This Row],[x]]/300)^2)</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="D22">
+        <f>Table2[[#This Row],[y]]-B21</f>
+        <v>6.6666666666666652E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>420</v>
+      </c>
+      <c r="B23">
+        <f>IF(Table2[[#This Row],[x]]&gt;300, Table2[[#This Row],[x]]/300, (Table2[[#This Row],[x]]/300)^2)</f>
+        <v>1.4</v>
+      </c>
+      <c r="D23">
+        <f>Table2[[#This Row],[y]]-B22</f>
+        <v>6.6666666666666652E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>440</v>
+      </c>
+      <c r="B24">
+        <f>IF(Table2[[#This Row],[x]]&gt;300, Table2[[#This Row],[x]]/300, (Table2[[#This Row],[x]]/300)^2)</f>
+        <v>1.4666666666666666</v>
+      </c>
+      <c r="D24">
+        <f>Table2[[#This Row],[y]]-B23</f>
+        <v>6.6666666666666652E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>460</v>
+      </c>
+      <c r="B25">
+        <f>IF(Table2[[#This Row],[x]]&gt;300, Table2[[#This Row],[x]]/300, (Table2[[#This Row],[x]]/300)^2)</f>
+        <v>1.5333333333333334</v>
+      </c>
+      <c r="D25">
+        <f>Table2[[#This Row],[y]]-B24</f>
+        <v>6.6666666666666874E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>480</v>
+      </c>
+      <c r="B26">
+        <f>IF(Table2[[#This Row],[x]]&gt;300, Table2[[#This Row],[x]]/300, (Table2[[#This Row],[x]]/300)^2)</f>
+        <v>1.6</v>
+      </c>
+      <c r="D26">
+        <f>Table2[[#This Row],[y]]-B25</f>
+        <v>6.6666666666666652E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>500</v>
+      </c>
+      <c r="B27">
+        <f>IF(Table2[[#This Row],[x]]&gt;300, Table2[[#This Row],[x]]/300, (Table2[[#This Row],[x]]/300)^2)</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="D27">
+        <f>Table2[[#This Row],[y]]-B26</f>
+        <v>6.6666666666666652E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>520</v>
+      </c>
+      <c r="B28">
+        <f>IF(Table2[[#This Row],[x]]&gt;300, Table2[[#This Row],[x]]/300, (Table2[[#This Row],[x]]/300)^2)</f>
+        <v>1.7333333333333334</v>
+      </c>
+      <c r="D28">
+        <f>Table2[[#This Row],[y]]-B27</f>
+        <v>6.6666666666666652E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>540</v>
+      </c>
+      <c r="B29">
+        <f>IF(Table2[[#This Row],[x]]&gt;300, Table2[[#This Row],[x]]/300, (Table2[[#This Row],[x]]/300)^2)</f>
+        <v>1.8</v>
+      </c>
+      <c r="D29">
+        <f>Table2[[#This Row],[y]]-B28</f>
+        <v>6.6666666666666652E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>560</v>
+      </c>
+      <c r="B30">
+        <f>IF(Table2[[#This Row],[x]]&gt;300, Table2[[#This Row],[x]]/300, (Table2[[#This Row],[x]]/300)^2)</f>
+        <v>1.8666666666666667</v>
+      </c>
+      <c r="D30">
+        <f>Table2[[#This Row],[y]]-B29</f>
+        <v>6.6666666666666652E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>580</v>
+      </c>
+      <c r="B31">
+        <f>IF(Table2[[#This Row],[x]]&gt;300, Table2[[#This Row],[x]]/300, (Table2[[#This Row],[x]]/300)^2)</f>
+        <v>1.9333333333333333</v>
+      </c>
+      <c r="D31">
+        <f>Table2[[#This Row],[y]]-B30</f>
+        <v>6.6666666666666652E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>600</v>
+      </c>
+      <c r="B32">
+        <f>IF(Table2[[#This Row],[x]]&gt;300, Table2[[#This Row],[x]]/300, (Table2[[#This Row],[x]]/300)^2)</f>
+        <v>2</v>
+      </c>
+      <c r="D32">
+        <f>Table2[[#This Row],[y]]-B31</f>
+        <v>6.6666666666666652E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23DCCA5A-0B13-43BB-84FB-82799C654ACD}">
   <dimension ref="A1:W23"/>
   <sheetViews>
@@ -18630,7 +22321,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBA148E4-8960-49BB-84B7-B9F77657BF02}">
   <dimension ref="A1:W23"/>
   <sheetViews>
@@ -18947,7 +22638,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C2:S9"/>
   <sheetViews>
@@ -19186,7 +22877,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AB18"/>
   <sheetViews>
@@ -20637,7 +24328,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
@@ -20931,226 +24622,4 @@
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:E19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="5" max="5" width="23.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D3" t="s">
-        <v>118</v>
-      </c>
-      <c r="E3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C4" t="s">
-        <v>118</v>
-      </c>
-      <c r="D4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C5" t="s">
-        <v>118</v>
-      </c>
-      <c r="D5" t="s">
-        <v>118</v>
-      </c>
-      <c r="E5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>99</v>
-      </c>
-      <c r="B6" t="s">
-        <v>118</v>
-      </c>
-      <c r="C6" t="s">
-        <v>117</v>
-      </c>
-      <c r="D6" t="s">
-        <v>117</v>
-      </c>
-      <c r="E6" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B7" t="s">
-        <v>118</v>
-      </c>
-      <c r="C7" t="s">
-        <v>117</v>
-      </c>
-      <c r="D7" t="s">
-        <v>118</v>
-      </c>
-      <c r="E7" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>99</v>
-      </c>
-      <c r="B8" t="s">
-        <v>118</v>
-      </c>
-      <c r="C8" t="s">
-        <v>118</v>
-      </c>
-      <c r="D8" t="s">
-        <v>117</v>
-      </c>
-      <c r="E8" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>99</v>
-      </c>
-      <c r="B9" t="s">
-        <v>118</v>
-      </c>
-      <c r="C9" t="s">
-        <v>118</v>
-      </c>
-      <c r="D9" t="s">
-        <v>118</v>
-      </c>
-      <c r="E9" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>99</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Hitball testing done! Next: back into fielding!!
</commit_message>
<xml_diff>
--- a/plans/baseball stats.xlsx
+++ b/plans/baseball stats.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcgiffenk\Desktop\newpy\xtreemblaseball99\plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17444565-3F8E-45CB-8AD9-ED2F925FD984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6643C56A-6D0D-465F-80DA-7009DC3F4F24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="iterative" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId2"/>
-    <sheet name="as-run reduct" sheetId="11" r:id="rId3"/>
-    <sheet name="reduction" sheetId="10" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="8" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="9" r:id="rId6"/>
-    <sheet name="gauss cruncher" sheetId="5" r:id="rId7"/>
-    <sheet name="run speed" sheetId="3" r:id="rId8"/>
-    <sheet name="pitch outcomes" sheetId="1" r:id="rId9"/>
-    <sheet name="hit quality truth table" sheetId="6" r:id="rId10"/>
+    <sheet name="quality" sheetId="7" r:id="rId2"/>
+    <sheet name="quality 2" sheetId="12" r:id="rId3"/>
+    <sheet name="as-run reduct" sheetId="11" r:id="rId4"/>
+    <sheet name="reduction" sheetId="10" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="8" r:id="rId6"/>
+    <sheet name="Sheet3" sheetId="9" r:id="rId7"/>
+    <sheet name="gauss cruncher" sheetId="5" r:id="rId8"/>
+    <sheet name="run speed" sheetId="3" r:id="rId9"/>
+    <sheet name="pitch outcomes" sheetId="1" r:id="rId10"/>
+    <sheet name="hit quality truth table" sheetId="6" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="basis">#REF!</definedName>
@@ -30,6 +31,7 @@
     <definedName name="counts">#REF!</definedName>
     <definedName name="dratings">iterative!$B$2:$L$2</definedName>
     <definedName name="factors">#REF!</definedName>
+    <definedName name="home" localSheetId="2">Table3[[#Headers],[Rep '#]]</definedName>
     <definedName name="home">Table3[[#Headers],[Rep '#]]</definedName>
     <definedName name="ms">#REF!</definedName>
     <definedName name="oratings">iterative!$B$1:$L$1</definedName>
@@ -561,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="314">
   <si>
     <t>Ball</t>
   </si>
@@ -2237,16 +2239,12 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="85">
+  <dxfs count="87">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -2597,6 +2595,16 @@
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2665,7 +2673,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$12</c:f>
+              <c:f>quality!$K$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2700,7 +2708,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$J$13:$J$18</c:f>
+              <c:f>quality!$J$13:$J$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2727,7 +2735,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$K$13:$K$18</c:f>
+              <c:f>quality!$K$13:$K$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2761,7 +2769,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$L$12</c:f>
+              <c:f>quality!$L$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2796,7 +2804,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$J$13:$J$18</c:f>
+              <c:f>quality!$J$13:$J$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2823,7 +2831,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$L$13:$L$18</c:f>
+              <c:f>quality!$L$13:$L$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -3120,6 +3128,940 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'quality 2'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>y</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'quality 2'!$A$2:$A$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'quality 2'!$B$2:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>0.66874030497642201</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.74008280449228525</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.79527072876705063</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8408964152537145</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.88011173679339338</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.91469121922869445</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.94574160900317583</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.97400374642529675</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0241136890844451</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0466351393921056</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0677899723724409</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.0877573059372772</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.1066819197003217</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.1246826503806981</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.1418583454354265</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.158292185288269</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.1740548859440185</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.189207115002721</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.2038013435027159</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.2178832856309068</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.2314930323839881</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.2446659545769567</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.2574334296829355</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.2698234324738655</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.2818610191887023</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.2935687276168018</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.3049669101523764</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.3160740129524926</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.3269068114098672</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.337480609952844</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-59AD-4912-8E16-5DFC34BA8A87}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'quality 2'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>target</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'quality 2'!$A$2:$A$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'quality 2'!$C$2:$C$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-59AD-4912-8E16-5DFC34BA8A87}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'quality 2'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>delta</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'quality 2'!$A$2:$A$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'quality 2'!$D$2:$D$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.1342499515863245E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.5187924274765376E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.5625686486663874E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.9215321539678882E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.4579482435301068E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.1050389774481379E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.8262137422120914E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.5996253574703254E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.4113689084445111E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.2521450307660507E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.115483298033527E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.9967333564836265E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.8924613763044551E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.8000730680376442E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.7175695054728379E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.6433839852842524E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.5762700655749473E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.5152229058702504E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.4594228499994921E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.4081942128190805E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.3609746753081353E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.3172922192968617E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.2767475105978754E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.2390002790930055E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.203758671483679E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.1707708428099428E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.1398182535574675E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.1107102800116175E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.0832798457374615E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.0573798542976798E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-59AD-4912-8E16-5DFC34BA8A87}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2112011648"/>
+        <c:axId val="2112012480"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2112011648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2112012480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2112012480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2112011648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -3624,7 +4566,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4552,7 +5494,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -7016,7 +7958,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -7937,7 +8879,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -8430,6 +9372,46 @@
 </file>
 
 <file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -8986,6 +9968,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -9482,522 +10980,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -10534,6 +11516,522 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -11036,7 +12534,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -11601,6 +13099,49 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A3A3AA7-2041-4864-8BA7-3AA6A9019F10}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
@@ -11637,7 +13178,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -11678,7 +13219,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -11719,7 +13260,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -11797,181 +13338,181 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A6:DO22" totalsRowShown="0" headerRowDxfId="84">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A6:DO22" totalsRowShown="0" headerRowDxfId="85">
   <autoFilter ref="A6:DO22" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="119">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Rep #">
       <calculatedColumnFormula>ROW()-ROW(home)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="offense" dataDxfId="83">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="offense" dataDxfId="84">
       <calculatedColumnFormula>INDEX(oratings, 1, 1+MOD(Table3[[#This Row],[Rep '#]]-1, COUNT(oratings)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="defense" dataDxfId="82">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="defense" dataDxfId="83">
       <calculatedColumnFormula>INDEX(dratings, 1, MOD(FLOOR( (Table3[[#This Row],[Rep '#]]-1) / COUNT(oratings), 1), COUNT(dratings))+1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="base leadoff" dataDxfId="81">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="base leadoff" dataDxfId="82">
       <calculatedColumnFormula>Table3[[#This Row],[offense]]*$D$26+0.05</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="leadoff modifier" dataDxfId="80">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="leadoff modifier" dataDxfId="81">
       <calculatedColumnFormula>((2*Table3[[#This Row],[defense]]+1*Table3[[#This Row],[defense]])-1.5)*Table3[[#This Row],[offense]]*$E$26</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="total leadoff (ft)" dataDxfId="79">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="total leadoff (ft)" dataDxfId="80">
       <calculatedColumnFormula>MAX(Table3[[#This Row],[base leadoff]]*(1-Table3[[#This Row],[leadoff modifier]]) * 90, 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="pickoff manuver (s)" dataDxfId="78">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="pickoff manuver (s)" dataDxfId="79">
       <calculatedColumnFormula>1.1 - Table3[[#This Row],[defense]]*0.1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="throw speed (s/ft)" dataDxfId="77">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="throw speed (s/ft)" dataDxfId="78">
       <calculatedColumnFormula xml:space="preserve"> 0.01 - 0.0025 *  Table3[[#This Row],[defense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="throw speed (mph)" dataDxfId="76">
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="throw speed (mph)" dataDxfId="77">
       <calculatedColumnFormula>1 / Table3[[#This Row],[throw speed (s/ft)]] * ((60 * 60)/5280)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="pickoff time" dataDxfId="75">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="pickoff time" dataDxfId="76">
       <calculatedColumnFormula>Table3[[#This Row],[pickoff manuver (s)]]+60*Table3[[#This Row],[throw speed (s/ft)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="runner reaction" dataDxfId="74">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="runner reaction" dataDxfId="75">
       <calculatedColumnFormula>$K$28-$K$26*Table3[[#This Row],[offense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="runner speed (s/ft)" dataDxfId="73">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="runner speed (s/ft)" dataDxfId="74">
       <calculatedColumnFormula>0.05 - Table3[[#This Row],[offense]]*$L$26</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="runner speed (mph)" dataDxfId="72">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="runner speed (mph)" dataDxfId="73">
       <calculatedColumnFormula>1 / Table3[[#This Row],[runner speed (s/ft)]] * ((60 * 60)/5280)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="pickoff evade time" dataDxfId="71">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="pickoff evade time" dataDxfId="72">
       <calculatedColumnFormula>Table3[[#This Row],[runner reaction]]+Table3[[#This Row],[runner speed (s/ft)]]*Table3[[#This Row],[total leadoff (ft)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="pickoff probability" dataDxfId="70" dataCellStyle="Percent">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="pickoff probability" dataDxfId="71" dataCellStyle="Percent">
       <calculatedColumnFormula>1 - _xlfn.NORM.DIST(Table3[[#This Row],[pickoff time]], Table3[[#This Row],[pickoff evade time]], $O$4, TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Fielding Odds" dataDxfId="69" dataCellStyle="Percent">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Fielding Odds" dataDxfId="70" dataCellStyle="Percent">
       <calculatedColumnFormula>_xlfn.NORM.DIST(Table3[[#This Row],[defense]], $P$26, $P$27, TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="pickoff worth it?" dataDxfId="68">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="pickoff worth it?" dataDxfId="69">
       <calculatedColumnFormula>Table3[[#This Row],[pickoff probability]] &gt; 1-Table3[[#This Row],[Fielding Odds]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Error %" dataDxfId="67" dataCellStyle="Percent">
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Error %" dataDxfId="68" dataCellStyle="Percent">
       <calculatedColumnFormula>1-Table3[[#This Row],[Fielding Odds]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Blatant steal time" dataDxfId="66">
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Blatant steal time" dataDxfId="67">
       <calculatedColumnFormula>(90-Table3[[#This Row],[total leadoff (ft)]])*Table3[[#This Row],[runner speed (s/ft)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Response speed" dataDxfId="65">
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Response speed" dataDxfId="66">
       <calculatedColumnFormula>$T$26*(2-Table3[[#This Row],[defense]]) + Table3[[#This Row],[pickoff time]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="blatant steal probability" dataDxfId="64" dataCellStyle="Percent">
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="blatant steal probability" dataDxfId="65" dataCellStyle="Percent">
       <calculatedColumnFormula>_xlfn.NORM.DIST(Table3[[#This Row],[Response speed]], Table3[[#This Row],[Blatant steal time]], $U$4, TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="defense fear" dataDxfId="63">
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="defense fear" dataDxfId="64">
       <calculatedColumnFormula>Table3[[#This Row],[defense]]+Table3[[#This Row],[defense]]*Table3[[#This Row],[offense]]*$E$26</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="ball factor" dataDxfId="62">
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="ball factor" dataDxfId="63">
       <calculatedColumnFormula>(1-$W$32)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="desperation" dataDxfId="61" dataCellStyle="Percent">
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="desperation" dataDxfId="62" dataCellStyle="Percent">
       <calculatedColumnFormula>Table3[[#This Row],[ball factor]]/$X$32*(1-$X$34)+$X$34</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="player control" dataDxfId="60">
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="player control" dataDxfId="61">
       <calculatedColumnFormula>Table3[[#This Row],[offense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="ideal steer" dataDxfId="59">
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="ideal steer" dataDxfId="60">
       <calculatedColumnFormula>$AA$33</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="scaled control" dataDxfId="58">
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="scaled control" dataDxfId="59">
       <calculatedColumnFormula>IF(Table3[[#This Row],[player control]]&gt;1,Table3[[#This Row],[player control]]*$AA$41+$AA$40,Table3[[#This Row],[player control]]*$AA$39+$AA$38)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="unmod foul percent 3rd" dataDxfId="57" dataCellStyle="Percent">
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="unmod foul percent 3rd" dataDxfId="58" dataCellStyle="Percent">
       <calculatedColumnFormula>_xlfn.NORM.DIST(-1,Table3[[#This Row],[ideal steer]],($AB$25-Table3[[#This Row],[scaled control]])*$AB$27,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="unmod foul percent 1st" dataDxfId="56" dataCellStyle="Percent">
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="unmod foul percent 1st" dataDxfId="57" dataCellStyle="Percent">
       <calculatedColumnFormula>1-_xlfn.NORM.DIST(1,Table3[[#This Row],[ideal steer]],($AB$25-Table3[[#This Row],[scaled control]])*$AB$27,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="total unmod foul percent" dataDxfId="55" dataCellStyle="Percent">
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="total unmod foul percent" dataDxfId="56" dataCellStyle="Percent">
       <calculatedColumnFormula>1-(1-Table3[[#This Row],[unmod foul percent 3rd]])*(1-Table3[[#This Row],[unmod foul percent 1st]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="unmod dead center foul%" dataDxfId="54" dataCellStyle="Percent">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="unmod dead center foul%" dataDxfId="55" dataCellStyle="Percent">
       <calculatedColumnFormula>1-((1-_xlfn.NORM.DIST(-1,0,($AB$25-Table3[[#This Row],[scaled control]])*$AB$27,TRUE))*_xlfn.NORM.DIST(1,0,($AB$25-Table3[[#This Row],[scaled control]])*$AB$27,TRUE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="count" dataDxfId="53">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="count" dataDxfId="54">
       <calculatedColumnFormula>$AF$34*$AF$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="hitter discipline bias" dataDxfId="52">
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="hitter discipline bias" dataDxfId="53">
       <calculatedColumnFormula>$AG$25*($AG$34*Table3[[#This Row],[offense]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="bases loaded" dataDxfId="51">
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="bases loaded" dataDxfId="52">
       <calculatedColumnFormula>$AH$25*$AH$34</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="number of outs" dataDxfId="50">
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="number of outs" dataDxfId="51">
       <calculatedColumnFormula>$AI$34*$AI$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="current hitter vs next hitter" dataDxfId="49">
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="current hitter vs next hitter" dataDxfId="50">
       <calculatedColumnFormula>$AJ$25*(Table3[[#This Row],[offense]]-$AJ$27)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="calling modifier" dataDxfId="48">
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="calling modifier" dataDxfId="49">
       <calculatedColumnFormula array="1">SUM(Table3[[#This Row],[count]:[current hitter vs next hitter]]*MIN(1, Table3[[#This Row],[defense]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="sigmoid strike percent" dataDxfId="47" dataCellStyle="Percent">
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="sigmoid strike percent" dataDxfId="48" dataCellStyle="Percent">
       <calculatedColumnFormula>$AL$25-(Table3[[#This Row],[calling modifier]]/(ABS(Table3[[#This Row],[calling modifier]])+$AL$29)*$AL$27)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="tanh strike percent" dataDxfId="46" dataCellStyle="Percent">
+    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="tanh strike percent" dataDxfId="47" dataCellStyle="Percent">
       <calculatedColumnFormula>$AL$25-$AL$27*TANH(Table3[[#This Row],[calling modifier]]/$AM$29)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="called position" dataDxfId="45" dataCellStyle="Percent">
+    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="called position" dataDxfId="46" dataCellStyle="Percent">
       <calculatedColumnFormula>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-Table3[[#This Row],[defense]])))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="called pos 0.2 pitch" dataDxfId="44">
+    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="called pos 0.2 pitch" dataDxfId="45">
       <calculatedColumnFormula>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-0.2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="called pos 2 pitch" dataDxfId="43">
+    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="called pos 2 pitch" dataDxfId="44">
       <calculatedColumnFormula>MAX(0, 1-_xlfn.NORM.S.INV(Table3[[#This Row],[tanh strike percent]])*($AN$25*($AN$27-2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="location -1  stdv" dataDxfId="42">
+    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="location -1  stdv" dataDxfId="43">
       <calculatedColumnFormula>Table3[[#This Row],[called position]]-pitchmod*(pitchstdv-Table3[[#This Row],[defense]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="location +1 stdv" dataDxfId="41">
+    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="location +1 stdv" dataDxfId="42">
       <calculatedColumnFormula>ABS(Table3[[#This Row],[called position]]+pitchmod*(pitchstdv-Table3[[#This Row],[defense]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="min dist to sz 1stdv" dataDxfId="40">
+    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="min dist to sz 1stdv" dataDxfId="41">
       <calculatedColumnFormula>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;1, Table3[[#This Row],[location +1 stdv]]&gt;1),0, MIN(Table3[[#This Row],[location -1  stdv]]+1, 1-Table3[[#This Row],[location +1 stdv]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="max dist to sz 1stdv" dataDxfId="39">
+    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="max dist to sz 1stdv" dataDxfId="40">
       <calculatedColumnFormula>IF(AND(Table3[[#This Row],[location -1  stdv]]&lt;0, Table3[[#This Row],[location +1 stdv]]&gt;0),1, MAX(1-ABS(Table3[[#This Row],[location -1  stdv]]), Table3[[#This Row],[location +1 stdv]]-1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="ave obscurity" dataDxfId="38">
+    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="ave obscurity" dataDxfId="39">
       <calculatedColumnFormula>$AU$30/(ABS(Table3[[#This Row],[called position]]-1)+$AU$27)+$AU$32*Table3[[#This Row],[defense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="obscurity at _x000a_0.5" dataDxfId="37">
+    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="obscurity at _x000a_0.5" dataDxfId="38">
       <calculatedColumnFormula>$AU$30/(ABS(0.5-1)+$AU$27)+$AU$32*Table3[[#This Row],[defense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="obscurity at  0.9" dataDxfId="36">
+    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="obscurity at  0.9" dataDxfId="37">
       <calculatedColumnFormula>$AU$30/(ABS(0.9-1)+$AU$27)+$AU$32*Table3[[#This Row],[defense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="average difficulty" dataDxfId="35">
+    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="average difficulty" dataDxfId="36">
       <calculatedColumnFormula>Table3[[#This Row],[defense]]*$AX$30+MAX(0, Table3[[#This Row],[called position]]-$AX$27)^$AX$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" name="+1stdv difficulty" dataDxfId="34">
+    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" name="+1stdv difficulty" dataDxfId="35">
       <calculatedColumnFormula>Table3[[#This Row],[defense]]*$AX$30 + MAX(0, Table3[[#This Row],[location +1 stdv]]-$AX$27)^$AX$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0000-000037000000}" name="difficulty at 1" dataDxfId="33">
+    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0000-000037000000}" name="difficulty at 1" dataDxfId="34">
       <calculatedColumnFormula>Table3[[#This Row],[defense]]*$AX$30+MAX(0, 1-$AX$27)^$AX$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="62" xr3:uid="{6513900D-2CAC-4022-A6B3-8A00EE6C566B}" name="reduction" dataDxfId="32">
+    <tableColumn id="62" xr3:uid="{6513900D-2CAC-4022-A6B3-8A00EE6C566B}" name="reduction" dataDxfId="33">
       <calculatedColumnFormula>MAX(0, 0.1*(1-Table3[[#This Row],[defense]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="63" xr3:uid="{12464915-1D8C-4EB5-9BBD-0FF526658E5B}" name="Location" dataDxfId="31">
+    <tableColumn id="63" xr3:uid="{12464915-1D8C-4EB5-9BBD-0FF526658E5B}" name="Location" dataDxfId="32">
       <calculatedColumnFormula>$BB$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="64" xr3:uid="{5F0F19BE-6D04-4E9E-81B2-B324AB353F5C}" name="obscurity" dataDxfId="30">
+    <tableColumn id="64" xr3:uid="{5F0F19BE-6D04-4E9E-81B2-B324AB353F5C}" name="obscurity" dataDxfId="31">
       <calculatedColumnFormula>$AU$30/(ABS(Table3[[#This Row],[Location]]-1)+$AU$27)+$AU$32*Table3[[#This Row],[defense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="65" xr3:uid="{EA3D32E7-A2E2-482C-B6E9-2E17651C5F77}" name="Strike?" dataDxfId="29">
+    <tableColumn id="65" xr3:uid="{EA3D32E7-A2E2-482C-B6E9-2E17651C5F77}" name="Strike?" dataDxfId="30">
       <calculatedColumnFormula>Table3[[#This Row],[Location]]&lt;= (1+MAX(0, (Table3[[#This Row],[defense]]-1)*0.1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="66" xr3:uid="{0C7E9B06-240B-481E-B495-54026E2F00AA}" name="discipline modifier" dataDxfId="28">
+    <tableColumn id="66" xr3:uid="{0C7E9B06-240B-481E-B495-54026E2F00AA}" name="discipline modifier" dataDxfId="29">
       <calculatedColumnFormula>1/(1+Table3[[#This Row],[offense]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="67" xr3:uid="{D3B0837D-02D4-4F62-A2E2-876739E497B0}" name="effective obscurity" dataDxfId="27">
+    <tableColumn id="67" xr3:uid="{D3B0837D-02D4-4F62-A2E2-876739E497B0}" name="effective obscurity" dataDxfId="28">
       <calculatedColumnFormula>Table3[[#This Row],[obscurity]]*Table3[[#This Row],[discipline modifier]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="69" xr3:uid="{39822A5F-1791-48DC-BA9F-A066931C0292}" name="odds of read" dataCellStyle="Percent">
@@ -11986,43 +13527,43 @@
     <tableColumn id="72" xr3:uid="{3E21C76F-F55B-4E49-9BE2-FEE046008C15}" name="adjusted swing %" dataCellStyle="Percent">
       <calculatedColumnFormula>Table3[[#This Row],[desperation echo]]*Table3[[#This Row],[unadjusted swing %]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="130" xr3:uid="{827C9303-3867-43F7-A79B-BC2EAB3F896D}" name="pitch carry forward obsc" dataDxfId="26">
+    <tableColumn id="130" xr3:uid="{827C9303-3867-43F7-A79B-BC2EAB3F896D}" name="pitch carry forward obsc" dataDxfId="27">
       <calculatedColumnFormula>Table3[[#This Row],[ave obscurity]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="131" xr3:uid="{F26B1E2C-89D5-4F6D-877A-1BEA7F7DF5A9}" name="CF odds of read" dataCellStyle="Percent">
       <calculatedColumnFormula>1/(1+Table3[[#This Row],[ave obscurity]]*Table3[[#This Row],[discipline modifier]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="73" xr3:uid="{77BBE784-030D-4E46-9A29-8783B89762BC}" name="contact echo" dataDxfId="25">
+    <tableColumn id="73" xr3:uid="{77BBE784-030D-4E46-9A29-8783B89762BC}" name="contact echo" dataDxfId="26">
       <calculatedColumnFormula>Table3[[#This Row],[offense]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="75" xr3:uid="{074A9F48-3941-4E36-90C2-7710217D32C8}" name="pitch carry forward diff" dataDxfId="24">
+    <tableColumn id="75" xr3:uid="{074A9F48-3941-4E36-90C2-7710217D32C8}" name="pitch carry forward diff" dataDxfId="25">
       <calculatedColumnFormula>Table3[[#This Row],[average difficulty]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="76" xr3:uid="{628DDA60-D380-4EE8-AA7D-7EF6C4AAD8A5}" name="CF contact readiness" dataDxfId="23">
+    <tableColumn id="76" xr3:uid="{628DDA60-D380-4EE8-AA7D-7EF6C4AAD8A5}" name="CF contact readiness" dataDxfId="24">
       <calculatedColumnFormula>Table3[[#This Row],[contact echo]]-Table3[[#This Row],[pitch carry forward diff]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="77" xr3:uid="{DBF18AD6-8593-42C7-9058-D19737088E6D}" name="foul %" dataDxfId="22" dataCellStyle="Percent">
+    <tableColumn id="77" xr3:uid="{DBF18AD6-8593-42C7-9058-D19737088E6D}" name="foul %" dataDxfId="23" dataCellStyle="Percent">
       <calculatedColumnFormula>1-_xlfn.NORM.DIST($BP$27,Table3[[#This Row],[CF contact readiness]], $BP$30,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="78" xr3:uid="{6354951A-151E-4E04-9897-9CB39D6098C8}" name="clean %" dataDxfId="21" dataCellStyle="Percent">
+    <tableColumn id="78" xr3:uid="{6354951A-151E-4E04-9897-9CB39D6098C8}" name="clean %" dataDxfId="22" dataCellStyle="Percent">
       <calculatedColumnFormula>1-_xlfn.NORM.DIST($BP$25,Table3[[#This Row],[CF contact readiness]], $BP$30,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="79" xr3:uid="{0070F673-D13C-467D-95AC-FF8413A02F3F}" name="strike swinging %" dataDxfId="20" dataCellStyle="Percent">
+    <tableColumn id="79" xr3:uid="{0070F673-D13C-467D-95AC-FF8413A02F3F}" name="strike swinging %" dataDxfId="21" dataCellStyle="Percent">
       <calculatedColumnFormula>1-Table3[[#This Row],[foul %]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="80" xr3:uid="{9504D0CF-7CD0-472F-8289-44B30538D80C}" name="ave. hit quality" dataDxfId="19">
+    <tableColumn id="80" xr3:uid="{9504D0CF-7CD0-472F-8289-44B30538D80C}" name="ave. hit quality" dataDxfId="20">
       <calculatedColumnFormula>(Table3[[#This Row],[CF contact readiness]]-$BP$27)/$BP$30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="132" xr3:uid="{0BB169E4-F345-4B7D-A549-DE28DC5FB113}" name="hit quality +1stdv" dataDxfId="18">
+    <tableColumn id="132" xr3:uid="{0BB169E4-F345-4B7D-A549-DE28DC5FB113}" name="hit quality +1stdv" dataDxfId="19">
       <calculatedColumnFormula>(Table3[[#This Row],[CF contact readiness]]+$BP$30-$BP$27)/$BP$30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="81" xr3:uid="{37438EAA-344A-486C-A4C2-68EE17D67C60}" name="hit quality remainder" dataDxfId="17">
+    <tableColumn id="81" xr3:uid="{37438EAA-344A-486C-A4C2-68EE17D67C60}" name="hit quality remainder" dataDxfId="18">
       <calculatedColumnFormula>MAX(0, IF(ISBLANK($BU$28), Table3[[#This Row],[hit quality +1stdv]], $BU$28)-1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="82" xr3:uid="{CBA11BEE-0412-44C3-979C-1888629B3C7A}" name="adjusted launch angle" dataDxfId="16">
+    <tableColumn id="82" xr3:uid="{CBA11BEE-0412-44C3-979C-1888629B3C7A}" name="adjusted launch angle" dataDxfId="17">
       <calculatedColumnFormula>$BV$25+Table3[[#This Row],[offense]]*$BV$28</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="83" xr3:uid="{8DC0E209-2987-40FE-9521-B3339A7D8E1F}" name="angle stdev" dataDxfId="15">
+    <tableColumn id="83" xr3:uid="{8DC0E209-2987-40FE-9521-B3339A7D8E1F}" name="angle stdev" dataDxfId="16">
       <calculatedColumnFormula>$BW$25*$BW$28/($BW$28+Table3[[#This Row],[hit quality remainder]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="84" xr3:uid="{F8EB7F4C-5D31-472E-A363-210E62A7E683}" name="grounder % (&lt;10 deg)" dataCellStyle="Percent">
@@ -12031,37 +13572,37 @@
     <tableColumn id="85" xr3:uid="{56DD6E0A-39C0-4DF0-B1CB-47EB71B71306}" name="pop up % (&gt;50 deg)" dataCellStyle="Percent">
       <calculatedColumnFormula>1-_xlfn.NORM.DIST(50, Table3[[#This Row],[adjusted launch angle]],Table3[[#This Row],[angle stdev]],TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="86" xr3:uid="{6ED971D4-0303-4AEB-B7CD-9516517F447E}" name="odds of 3B" dataDxfId="14" dataCellStyle="Percent">
+    <tableColumn id="86" xr3:uid="{6ED971D4-0303-4AEB-B7CD-9516517F447E}" name="odds of 3B" dataDxfId="15" dataCellStyle="Percent">
       <calculatedColumnFormula>1-_xlfn.NORM.DIST(70, $BZ$28,$BZ$25,TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="87" xr3:uid="{E9F9DFB6-4A26-4CA7-9318-6ECA478690D6}" name="exit velocity mean" dataDxfId="13">
+    <tableColumn id="87" xr3:uid="{E9F9DFB6-4A26-4CA7-9318-6ECA478690D6}" name="exit velocity mean" dataDxfId="14">
       <calculatedColumnFormula>$CA$25+Table3[[#This Row],[offense]]*($CA$27-$CA$25)/2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="88" xr3:uid="{EB865A5D-CC1D-49FA-9709-DC5F30F55DD8}" name="after reduction" dataDxfId="12">
+    <tableColumn id="88" xr3:uid="{EB865A5D-CC1D-49FA-9709-DC5F30F55DD8}" name="after reduction" dataDxfId="13">
       <calculatedColumnFormula>Table3[[#This Row],[exit velocity mean]]-Table3[[#This Row],[reduction]]*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="89" xr3:uid="{949E8C38-C424-4A4E-9A6F-FCA93496D192}" name="theoretical distance" dataDxfId="11">
+    <tableColumn id="89" xr3:uid="{949E8C38-C424-4A4E-9A6F-FCA93496D192}" name="theoretical distance" dataDxfId="12">
       <calculatedColumnFormula>Table3[[#This Row],[exit velocity mean]]^2*2*SIN(RADIANS(Table3[[#This Row],[adjusted launch angle]]))/$CC$28*5280</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="90" xr3:uid="{9FD0A88A-D0D9-4369-8D70-6C7485CA1509}" name="flight time" dataDxfId="10">
+    <tableColumn id="90" xr3:uid="{9FD0A88A-D0D9-4369-8D70-6C7485CA1509}" name="flight time" dataDxfId="11">
       <calculatedColumnFormula>2*Table3[[#This Row],[exit velocity mean]]*SIN(RADIANS(Table3[[#This Row],[adjusted launch angle]]))/$CC$28*60*60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="91" xr3:uid="{D9D5DFED-BD09-4CB6-A82E-D289D2DAB08D}" name="actual distance" dataDxfId="9">
+    <tableColumn id="91" xr3:uid="{D9D5DFED-BD09-4CB6-A82E-D289D2DAB08D}" name="actual distance" dataDxfId="10">
       <calculatedColumnFormula>Table3[[#This Row],[theoretical distance]]-Table3[[#This Row],[flight time]]^2*$CE$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="92" xr3:uid="{3D80331E-564D-462D-81B5-E5CE730D1EE5}" name="+1stdv EV" dataDxfId="8">
+    <tableColumn id="92" xr3:uid="{3D80331E-564D-462D-81B5-E5CE730D1EE5}" name="+1stdv EV" dataDxfId="9">
       <calculatedColumnFormula>Table3[[#This Row],[exit velocity mean]]+$CC$25-Table3[[#This Row],[reduction]]*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="93" xr3:uid="{211123A1-65C0-4F59-AB86-C344CFF47F70}" name="+1stdv LA" dataDxfId="7">
+    <tableColumn id="93" xr3:uid="{211123A1-65C0-4F59-AB86-C344CFF47F70}" name="+1stdv LA" dataDxfId="8">
       <calculatedColumnFormula>MIN(Table3[[#This Row],[adjusted launch angle]]+Table3[[#This Row],[angle stdev]], 30)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="94" xr3:uid="{C8736D16-AF27-436D-BF61-CA3E58298CD3}" name="+1stdv flight time" dataDxfId="6">
+    <tableColumn id="94" xr3:uid="{C8736D16-AF27-436D-BF61-CA3E58298CD3}" name="+1stdv flight time" dataDxfId="7">
       <calculatedColumnFormula>2*Table3[[#This Row],[+1stdv EV]]*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*60*60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="95" xr3:uid="{C9967388-9755-4293-82E9-4E43A4770599}" name="+1stdev distance" dataDxfId="5">
+    <tableColumn id="95" xr3:uid="{C9967388-9755-4293-82E9-4E43A4770599}" name="+1stdev distance" dataDxfId="6">
       <calculatedColumnFormula>Table3[[#This Row],[+1stdv EV]]^2*2*SIN(RADIANS(Table3[[#This Row],[+1stdv LA]]))/$CC$28*5280-Table3[[#This Row],[+1stdv flight time]]^2*$CE$25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="96" xr3:uid="{52B6BA3A-87F7-49FD-BFE7-811EA76B03FD}" name="+1stdev delta" dataDxfId="4">
+    <tableColumn id="96" xr3:uid="{52B6BA3A-87F7-49FD-BFE7-811EA76B03FD}" name="+1stdev delta" dataDxfId="5">
       <calculatedColumnFormula>Table3[[#This Row],[+1stdev distance]]-Table3[[#This Row],[actual distance]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="97" xr3:uid="{50EEB2EF-C836-4BBC-A8B3-EAD31BF29B54}" name="Column95"/>
@@ -12106,7 +13647,7 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{23FB116D-6CB4-49F6-A874-F1C610DEF5E1}" name="quality"/>
     <tableColumn id="2" xr3:uid="{6204ECDD-C980-4BE0-AFC7-9F83BF472BE8}" name="net"/>
-    <tableColumn id="3" xr3:uid="{E9208F79-490A-4A40-B3B7-0914BA16AC90}" name="form" dataDxfId="3">
+    <tableColumn id="3" xr3:uid="{E9208F79-490A-4A40-B3B7-0914BA16AC90}" name="form" dataDxfId="4">
       <calculatedColumnFormula>POWER(Table1[[#This Row],[quality]]-0.8, 1/4)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -12115,11 +13656,28 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{95127CA8-91E1-4775-BB6E-505D391365E1}" name="Table25" displayName="Table25" ref="A1:D32" totalsRowShown="0">
+  <autoFilter ref="A1:D32" xr:uid="{CEC18A43-64FC-4CDC-9CAF-1945616C5259}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{1F927288-9DCD-4C9F-99B6-231C93B232BD}" name="x"/>
+    <tableColumn id="2" xr3:uid="{CF4782DD-2BE1-475B-9CA8-67CD24EC8ECA}" name="y" dataDxfId="0">
+      <calculatedColumnFormula>(Table25[[#This Row],[x]]+0.2)^(1/4)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{3EC13FAB-E206-4412-9C6D-B9F2F09BDB60}" name="target"/>
+    <tableColumn id="4" xr3:uid="{31C9552B-0B66-4C6C-8D29-F1BB69F6879E}" name="delta" dataDxfId="1">
+      <calculatedColumnFormula>Table25[[#This Row],[y]]-B1</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CEC18A43-64FC-4CDC-9CAF-1945616C5259}" name="Table2" displayName="Table2" ref="A1:D32" totalsRowShown="0">
   <autoFilter ref="A1:D32" xr:uid="{CEC18A43-64FC-4CDC-9CAF-1945616C5259}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{1AE5C4EC-1E31-4AB8-9D00-52347412BAAD}" name="x"/>
-    <tableColumn id="2" xr3:uid="{DE2F5C94-46DF-4FEE-9B65-021E2F22BA8F}" name="y" dataDxfId="1">
+    <tableColumn id="2" xr3:uid="{DE2F5C94-46DF-4FEE-9B65-021E2F22BA8F}" name="y" dataDxfId="3">
       <calculatedColumnFormula>IF(Table2[[#This Row],[x]]&gt;300, Table2[[#This Row],[x]]/300, (Table2[[#This Row],[x]]/300)^2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{7F7D12A9-EB9C-4F1E-AA19-600982A4A24A}" name="target"/>
@@ -19235,7 +20793,7 @@
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
   <conditionalFormatting sqref="O7:O22">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19249,6 +20807,302 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1988</v>
+      </c>
+      <c r="B2">
+        <v>0.4269</v>
+      </c>
+      <c r="C2">
+        <v>0.28660000000000002</v>
+      </c>
+      <c r="D2">
+        <v>0.1007</v>
+      </c>
+      <c r="E2">
+        <v>5.8200000000000002E-2</v>
+      </c>
+      <c r="F2">
+        <v>0.12759999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1989</v>
+      </c>
+      <c r="B3">
+        <v>0.39779999999999999</v>
+      </c>
+      <c r="C3">
+        <v>0.1666</v>
+      </c>
+      <c r="D3">
+        <v>0.1575</v>
+      </c>
+      <c r="E3">
+        <v>9.0399999999999994E-2</v>
+      </c>
+      <c r="F3">
+        <v>0.18770000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1990</v>
+      </c>
+      <c r="B4">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="C4">
+        <v>0.1285</v>
+      </c>
+      <c r="D4">
+        <v>0.1787</v>
+      </c>
+      <c r="E4">
+        <v>9.9400000000000002E-2</v>
+      </c>
+      <c r="F4">
+        <v>0.20730000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>1991</v>
+      </c>
+      <c r="B5">
+        <v>0.3528</v>
+      </c>
+      <c r="C5">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="D5">
+        <v>0.19789999999999999</v>
+      </c>
+      <c r="E5">
+        <v>0.1057</v>
+      </c>
+      <c r="F5">
+        <v>0.2266</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1992</v>
+      </c>
+      <c r="B6">
+        <v>0.31290000000000001</v>
+      </c>
+      <c r="C6">
+        <v>7.6700000000000004E-2</v>
+      </c>
+      <c r="D6">
+        <v>0.23</v>
+      </c>
+      <c r="E6">
+        <v>0.112</v>
+      </c>
+      <c r="F6">
+        <v>0.26850000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>1993</v>
+      </c>
+      <c r="B7">
+        <v>0.26369999999999999</v>
+      </c>
+      <c r="C7">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="D7">
+        <v>0.26490000000000002</v>
+      </c>
+      <c r="E7">
+        <v>0.1154</v>
+      </c>
+      <c r="F7">
+        <v>0.31190000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>1994</v>
+      </c>
+      <c r="B8">
+        <v>0.2505</v>
+      </c>
+      <c r="C8">
+        <v>4.0500000000000001E-2</v>
+      </c>
+      <c r="D8">
+        <v>0.27650000000000002</v>
+      </c>
+      <c r="E8">
+        <v>0.1104</v>
+      </c>
+      <c r="F8">
+        <v>0.32200000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>1995</v>
+      </c>
+      <c r="B9">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="C9">
+        <v>3.8199999999999998E-2</v>
+      </c>
+      <c r="D9">
+        <v>0.28849999999999998</v>
+      </c>
+      <c r="E9">
+        <v>0.1062</v>
+      </c>
+      <c r="F9">
+        <v>0.3322</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>1996</v>
+      </c>
+      <c r="B10">
+        <v>0.22650000000000001</v>
+      </c>
+      <c r="C10">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="D10">
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="E10">
+        <v>0.1031</v>
+      </c>
+      <c r="F10">
+        <v>0.33739999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>1997</v>
+      </c>
+      <c r="B11">
+        <v>0.21079999999999999</v>
+      </c>
+      <c r="C11">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="D11">
+        <v>0.314</v>
+      </c>
+      <c r="E11">
+        <v>0.1033</v>
+      </c>
+      <c r="F11">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>1998</v>
+      </c>
+      <c r="B12">
+        <v>0.21149999999999999</v>
+      </c>
+      <c r="C12">
+        <v>3.2500000000000001E-2</v>
+      </c>
+      <c r="D12">
+        <v>0.31419999999999998</v>
+      </c>
+      <c r="E12">
+        <v>0.10489999999999999</v>
+      </c>
+      <c r="F12">
+        <v>0.33689999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>1999</v>
+      </c>
+      <c r="B13">
+        <v>0.20449999999999999</v>
+      </c>
+      <c r="C13">
+        <v>3.56E-2</v>
+      </c>
+      <c r="D13">
+        <v>0.31430000000000002</v>
+      </c>
+      <c r="E13">
+        <v>0.10580000000000001</v>
+      </c>
+      <c r="F13">
+        <v>0.33979999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <f>AVERAGE(B2:B13)</f>
+        <v>0.28990833333333332</v>
+      </c>
+      <c r="C17">
+        <f>AVERAGE(C2:C13)</f>
+        <v>8.6183333333333348E-2</v>
+      </c>
+      <c r="D17">
+        <f>AVERAGE(D2:D13)</f>
+        <v>0.24451666666666663</v>
+      </c>
+      <c r="E17">
+        <f>AVERAGE(E2:E13)</f>
+        <v>0.10123333333333333</v>
+      </c>
+      <c r="F17">
+        <f>AVERAGE(F2:F13)</f>
+        <v>0.27815833333333334</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E19"/>
   <sheetViews>
@@ -19475,7 +21329,7 @@
   <dimension ref="J12:L18"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="E35" sqref="A24:E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19573,10 +21427,459 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E520AB81-5C79-4CBA-9F02-17B2DAAECB82}">
+  <dimension ref="A1:D32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <f>(Table25[[#This Row],[x]]+0.2)^(1/4)</f>
+        <v>0.66874030497642201</v>
+      </c>
+      <c r="C2">
+        <v>0.5</v>
+      </c>
+      <c r="D2" t="e">
+        <f>Table25[[#This Row],[y]]-B1</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.1</v>
+      </c>
+      <c r="B3">
+        <f>(Table25[[#This Row],[x]]+0.2)^(1/4)</f>
+        <v>0.74008280449228525</v>
+      </c>
+      <c r="D3">
+        <f>Table25[[#This Row],[y]]-B2</f>
+        <v>7.1342499515863245E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.2</v>
+      </c>
+      <c r="B4">
+        <f>(Table25[[#This Row],[x]]+0.2)^(1/4)</f>
+        <v>0.79527072876705063</v>
+      </c>
+      <c r="D4">
+        <f>Table25[[#This Row],[y]]-B3</f>
+        <v>5.5187924274765376E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.3</v>
+      </c>
+      <c r="B5">
+        <f>(Table25[[#This Row],[x]]+0.2)^(1/4)</f>
+        <v>0.8408964152537145</v>
+      </c>
+      <c r="D5">
+        <f>Table25[[#This Row],[y]]-B4</f>
+        <v>4.5625686486663874E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0.4</v>
+      </c>
+      <c r="B6">
+        <f>(Table25[[#This Row],[x]]+0.2)^(1/4)</f>
+        <v>0.88011173679339338</v>
+      </c>
+      <c r="D6">
+        <f>Table25[[#This Row],[y]]-B5</f>
+        <v>3.9215321539678882E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.5</v>
+      </c>
+      <c r="B7">
+        <f>(Table25[[#This Row],[x]]+0.2)^(1/4)</f>
+        <v>0.91469121922869445</v>
+      </c>
+      <c r="D7">
+        <f>Table25[[#This Row],[y]]-B6</f>
+        <v>3.4579482435301068E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0.6</v>
+      </c>
+      <c r="B8">
+        <f>(Table25[[#This Row],[x]]+0.2)^(1/4)</f>
+        <v>0.94574160900317583</v>
+      </c>
+      <c r="D8">
+        <f>Table25[[#This Row],[y]]-B7</f>
+        <v>3.1050389774481379E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0.7</v>
+      </c>
+      <c r="B9">
+        <f>(Table25[[#This Row],[x]]+0.2)^(1/4)</f>
+        <v>0.97400374642529675</v>
+      </c>
+      <c r="D9">
+        <f>Table25[[#This Row],[y]]-B8</f>
+        <v>2.8262137422120914E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.8</v>
+      </c>
+      <c r="B10">
+        <f>(Table25[[#This Row],[x]]+0.2)^(1/4)</f>
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <f>Table25[[#This Row],[y]]-B9</f>
+        <v>2.5996253574703254E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0.9</v>
+      </c>
+      <c r="B11">
+        <f>(Table25[[#This Row],[x]]+0.2)^(1/4)</f>
+        <v>1.0241136890844451</v>
+      </c>
+      <c r="D11">
+        <f>Table25[[#This Row],[y]]-B10</f>
+        <v>2.4113689084445111E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <f>(Table25[[#This Row],[x]]+0.2)^(1/4)</f>
+        <v>1.0466351393921056</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <f>Table25[[#This Row],[y]]-B11</f>
+        <v>2.2521450307660507E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B13">
+        <f>(Table25[[#This Row],[x]]+0.2)^(1/4)</f>
+        <v>1.0677899723724409</v>
+      </c>
+      <c r="D13">
+        <f>Table25[[#This Row],[y]]-B12</f>
+        <v>2.115483298033527E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1.2</v>
+      </c>
+      <c r="B14">
+        <f>(Table25[[#This Row],[x]]+0.2)^(1/4)</f>
+        <v>1.0877573059372772</v>
+      </c>
+      <c r="D14">
+        <f>Table25[[#This Row],[y]]-B13</f>
+        <v>1.9967333564836265E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1.3</v>
+      </c>
+      <c r="B15">
+        <f>(Table25[[#This Row],[x]]+0.2)^(1/4)</f>
+        <v>1.1066819197003217</v>
+      </c>
+      <c r="D15">
+        <f>Table25[[#This Row],[y]]-B14</f>
+        <v>1.8924613763044551E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1.4</v>
+      </c>
+      <c r="B16">
+        <f>(Table25[[#This Row],[x]]+0.2)^(1/4)</f>
+        <v>1.1246826503806981</v>
+      </c>
+      <c r="D16">
+        <f>Table25[[#This Row],[y]]-B15</f>
+        <v>1.8000730680376442E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1.5</v>
+      </c>
+      <c r="B17">
+        <f>(Table25[[#This Row],[x]]+0.2)^(1/4)</f>
+        <v>1.1418583454354265</v>
+      </c>
+      <c r="D17">
+        <f>Table25[[#This Row],[y]]-B16</f>
+        <v>1.7175695054728379E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1.6</v>
+      </c>
+      <c r="B18">
+        <f>(Table25[[#This Row],[x]]+0.2)^(1/4)</f>
+        <v>1.158292185288269</v>
+      </c>
+      <c r="D18">
+        <f>Table25[[#This Row],[y]]-B17</f>
+        <v>1.6433839852842524E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1.7</v>
+      </c>
+      <c r="B19">
+        <f>(Table25[[#This Row],[x]]+0.2)^(1/4)</f>
+        <v>1.1740548859440185</v>
+      </c>
+      <c r="D19">
+        <f>Table25[[#This Row],[y]]-B18</f>
+        <v>1.5762700655749473E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1.8</v>
+      </c>
+      <c r="B20">
+        <f>(Table25[[#This Row],[x]]+0.2)^(1/4)</f>
+        <v>1.189207115002721</v>
+      </c>
+      <c r="D20">
+        <f>Table25[[#This Row],[y]]-B19</f>
+        <v>1.5152229058702504E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1.9</v>
+      </c>
+      <c r="B21">
+        <f>(Table25[[#This Row],[x]]+0.2)^(1/4)</f>
+        <v>1.2038013435027159</v>
+      </c>
+      <c r="D21">
+        <f>Table25[[#This Row],[y]]-B20</f>
+        <v>1.4594228499994921E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22">
+        <f>(Table25[[#This Row],[x]]+0.2)^(1/4)</f>
+        <v>1.2178832856309068</v>
+      </c>
+      <c r="C22">
+        <v>1.2</v>
+      </c>
+      <c r="D22">
+        <f>Table25[[#This Row],[y]]-B21</f>
+        <v>1.4081942128190805E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2.1</v>
+      </c>
+      <c r="B23">
+        <f>(Table25[[#This Row],[x]]+0.2)^(1/4)</f>
+        <v>1.2314930323839881</v>
+      </c>
+      <c r="D23">
+        <f>Table25[[#This Row],[y]]-B22</f>
+        <v>1.3609746753081353E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B24">
+        <f>(Table25[[#This Row],[x]]+0.2)^(1/4)</f>
+        <v>1.2446659545769567</v>
+      </c>
+      <c r="D24">
+        <f>Table25[[#This Row],[y]]-B23</f>
+        <v>1.3172922192968617E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B25">
+        <f>(Table25[[#This Row],[x]]+0.2)^(1/4)</f>
+        <v>1.2574334296829355</v>
+      </c>
+      <c r="D25">
+        <f>Table25[[#This Row],[y]]-B24</f>
+        <v>1.2767475105978754E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2.4</v>
+      </c>
+      <c r="B26">
+        <f>(Table25[[#This Row],[x]]+0.2)^(1/4)</f>
+        <v>1.2698234324738655</v>
+      </c>
+      <c r="D26">
+        <f>Table25[[#This Row],[y]]-B25</f>
+        <v>1.2390002790930055E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2.5</v>
+      </c>
+      <c r="B27">
+        <f>(Table25[[#This Row],[x]]+0.2)^(1/4)</f>
+        <v>1.2818610191887023</v>
+      </c>
+      <c r="D27">
+        <f>Table25[[#This Row],[y]]-B26</f>
+        <v>1.203758671483679E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2.6</v>
+      </c>
+      <c r="B28">
+        <f>(Table25[[#This Row],[x]]+0.2)^(1/4)</f>
+        <v>1.2935687276168018</v>
+      </c>
+      <c r="D28">
+        <f>Table25[[#This Row],[y]]-B27</f>
+        <v>1.1707708428099428E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2.7</v>
+      </c>
+      <c r="B29">
+        <f>(Table25[[#This Row],[x]]+0.2)^(1/4)</f>
+        <v>1.3049669101523764</v>
+      </c>
+      <c r="D29">
+        <f>Table25[[#This Row],[y]]-B28</f>
+        <v>1.1398182535574675E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2.8</v>
+      </c>
+      <c r="B30">
+        <f>(Table25[[#This Row],[x]]+0.2)^(1/4)</f>
+        <v>1.3160740129524926</v>
+      </c>
+      <c r="D30">
+        <f>Table25[[#This Row],[y]]-B29</f>
+        <v>1.1107102800116175E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>2.9</v>
+      </c>
+      <c r="B31">
+        <f>(Table25[[#This Row],[x]]+0.2)^(1/4)</f>
+        <v>1.3269068114098672</v>
+      </c>
+      <c r="D31">
+        <f>Table25[[#This Row],[y]]-B30</f>
+        <v>1.0832798457374615E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>3</v>
+      </c>
+      <c r="B32">
+        <f>(Table25[[#This Row],[x]]+0.2)^(1/4)</f>
+        <v>1.337480609952844</v>
+      </c>
+      <c r="C32">
+        <v>1.3</v>
+      </c>
+      <c r="D32">
+        <f>Table25[[#This Row],[y]]-B31</f>
+        <v>1.0573798542976798E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80A4F72A-6EF1-4451-BFA6-39EE9D1AFD85}">
   <dimension ref="A2:CV2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
@@ -19891,7 +22194,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48AF6B93-1A07-417B-961A-AB8D0F990765}">
   <dimension ref="A1:D32"/>
   <sheetViews>
@@ -20334,7 +22637,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23DCCA5A-0B13-43BB-84FB-82799C654ACD}">
   <dimension ref="A1:W23"/>
   <sheetViews>
@@ -22321,7 +24624,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBA148E4-8960-49BB-84B7-B9F77657BF02}">
   <dimension ref="A1:W23"/>
   <sheetViews>
@@ -22638,7 +24941,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C2:S9"/>
   <sheetViews>
@@ -22877,7 +25180,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AB18"/>
   <sheetViews>
@@ -24326,300 +26629,4 @@
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:F17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1988</v>
-      </c>
-      <c r="B2">
-        <v>0.4269</v>
-      </c>
-      <c r="C2">
-        <v>0.28660000000000002</v>
-      </c>
-      <c r="D2">
-        <v>0.1007</v>
-      </c>
-      <c r="E2">
-        <v>5.8200000000000002E-2</v>
-      </c>
-      <c r="F2">
-        <v>0.12759999999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1989</v>
-      </c>
-      <c r="B3">
-        <v>0.39779999999999999</v>
-      </c>
-      <c r="C3">
-        <v>0.1666</v>
-      </c>
-      <c r="D3">
-        <v>0.1575</v>
-      </c>
-      <c r="E3">
-        <v>9.0399999999999994E-2</v>
-      </c>
-      <c r="F3">
-        <v>0.18770000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>1990</v>
-      </c>
-      <c r="B4">
-        <v>0.38600000000000001</v>
-      </c>
-      <c r="C4">
-        <v>0.1285</v>
-      </c>
-      <c r="D4">
-        <v>0.1787</v>
-      </c>
-      <c r="E4">
-        <v>9.9400000000000002E-2</v>
-      </c>
-      <c r="F4">
-        <v>0.20730000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>1991</v>
-      </c>
-      <c r="B5">
-        <v>0.3528</v>
-      </c>
-      <c r="C5">
-        <v>0.11700000000000001</v>
-      </c>
-      <c r="D5">
-        <v>0.19789999999999999</v>
-      </c>
-      <c r="E5">
-        <v>0.1057</v>
-      </c>
-      <c r="F5">
-        <v>0.2266</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>1992</v>
-      </c>
-      <c r="B6">
-        <v>0.31290000000000001</v>
-      </c>
-      <c r="C6">
-        <v>7.6700000000000004E-2</v>
-      </c>
-      <c r="D6">
-        <v>0.23</v>
-      </c>
-      <c r="E6">
-        <v>0.112</v>
-      </c>
-      <c r="F6">
-        <v>0.26850000000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>1993</v>
-      </c>
-      <c r="B7">
-        <v>0.26369999999999999</v>
-      </c>
-      <c r="C7">
-        <v>4.3999999999999997E-2</v>
-      </c>
-      <c r="D7">
-        <v>0.26490000000000002</v>
-      </c>
-      <c r="E7">
-        <v>0.1154</v>
-      </c>
-      <c r="F7">
-        <v>0.31190000000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>1994</v>
-      </c>
-      <c r="B8">
-        <v>0.2505</v>
-      </c>
-      <c r="C8">
-        <v>4.0500000000000001E-2</v>
-      </c>
-      <c r="D8">
-        <v>0.27650000000000002</v>
-      </c>
-      <c r="E8">
-        <v>0.1104</v>
-      </c>
-      <c r="F8">
-        <v>0.32200000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>1995</v>
-      </c>
-      <c r="B9">
-        <v>0.23499999999999999</v>
-      </c>
-      <c r="C9">
-        <v>3.8199999999999998E-2</v>
-      </c>
-      <c r="D9">
-        <v>0.28849999999999998</v>
-      </c>
-      <c r="E9">
-        <v>0.1062</v>
-      </c>
-      <c r="F9">
-        <v>0.3322</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>1996</v>
-      </c>
-      <c r="B10">
-        <v>0.22650000000000001</v>
-      </c>
-      <c r="C10">
-        <v>3.5999999999999997E-2</v>
-      </c>
-      <c r="D10">
-        <v>0.29699999999999999</v>
-      </c>
-      <c r="E10">
-        <v>0.1031</v>
-      </c>
-      <c r="F10">
-        <v>0.33739999999999998</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>1997</v>
-      </c>
-      <c r="B11">
-        <v>0.21079999999999999</v>
-      </c>
-      <c r="C11">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="D11">
-        <v>0.314</v>
-      </c>
-      <c r="E11">
-        <v>0.1033</v>
-      </c>
-      <c r="F11">
-        <v>0.34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>1998</v>
-      </c>
-      <c r="B12">
-        <v>0.21149999999999999</v>
-      </c>
-      <c r="C12">
-        <v>3.2500000000000001E-2</v>
-      </c>
-      <c r="D12">
-        <v>0.31419999999999998</v>
-      </c>
-      <c r="E12">
-        <v>0.10489999999999999</v>
-      </c>
-      <c r="F12">
-        <v>0.33689999999999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>1999</v>
-      </c>
-      <c r="B13">
-        <v>0.20449999999999999</v>
-      </c>
-      <c r="C13">
-        <v>3.56E-2</v>
-      </c>
-      <c r="D13">
-        <v>0.31430000000000002</v>
-      </c>
-      <c r="E13">
-        <v>0.10580000000000001</v>
-      </c>
-      <c r="F13">
-        <v>0.33979999999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17">
-        <f>AVERAGE(B2:B13)</f>
-        <v>0.28990833333333332</v>
-      </c>
-      <c r="C17">
-        <f>AVERAGE(C2:C13)</f>
-        <v>8.6183333333333348E-2</v>
-      </c>
-      <c r="D17">
-        <f>AVERAGE(D2:D13)</f>
-        <v>0.24451666666666663</v>
-      </c>
-      <c r="E17">
-        <f>AVERAGE(E2:E13)</f>
-        <v>0.10123333333333333</v>
-      </c>
-      <c r="F17">
-        <f>AVERAGE(F2:F13)</f>
-        <v>0.27815833333333334</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Initial tests for Runner, although advance is still a work in progress.
</commit_message>
<xml_diff>
--- a/plans/baseball stats.xlsx
+++ b/plans/baseball stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcgiffenk\Desktop\newpy\xtreemblaseball99\plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11A98AB-E16C-4714-BBE0-A99320D995D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{526131DD-361A-439E-872E-C7C329EDD611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="iterative" sheetId="2" r:id="rId1"/>
@@ -18274,11 +18274,11 @@
   <autoFilter ref="A6:D37" xr:uid="{3C9452C2-1B9C-4FCE-B409-4884E378E31E}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{E97B6F5F-BE7F-4DF9-A62D-3BC2F5D86680}" name="x"/>
-    <tableColumn id="2" xr3:uid="{9CB09BE8-C9BA-4368-B0DB-0AD29E193C50}" name="y" dataDxfId="4">
+    <tableColumn id="2" xr3:uid="{9CB09BE8-C9BA-4368-B0DB-0AD29E193C50}" name="y" dataDxfId="5">
       <calculatedColumnFormula>MIN(1, (60-Table26[[#This Row],[x]])/55)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{4DDBDF87-9C1A-43F4-B622-C0601C5607F2}" name="target"/>
-    <tableColumn id="4" xr3:uid="{11802B18-9820-45B9-917A-3656CD9F5F68}" name="delta" dataDxfId="5">
+    <tableColumn id="4" xr3:uid="{11802B18-9820-45B9-917A-3656CD9F5F68}" name="delta" dataDxfId="4">
       <calculatedColumnFormula>Table26[[#This Row],[y]]-B6</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -18291,11 +18291,11 @@
   <autoFilter ref="A6:D34" xr:uid="{3C9452C2-1B9C-4FCE-B409-4884E378E31E}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{ECE87426-CDD8-4F88-955D-273C4875C76B}" name="x"/>
-    <tableColumn id="2" xr3:uid="{64C04DF3-8FF3-4EDC-BAB9-1747A6E337C1}" name="y" dataDxfId="2">
+    <tableColumn id="2" xr3:uid="{64C04DF3-8FF3-4EDC-BAB9-1747A6E337C1}" name="y" dataDxfId="3">
       <calculatedColumnFormula>(1-Table267[[#This Row],[x]])^(1/2)*4+1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{138B8243-9FBD-42BD-A0C9-144AFECE0829}" name="target"/>
-    <tableColumn id="4" xr3:uid="{7BE3DD3B-38A7-4C75-8DF8-9186EA9833DB}" name="delta" dataDxfId="3">
+    <tableColumn id="4" xr3:uid="{7BE3DD3B-38A7-4C75-8DF8-9186EA9833DB}" name="delta" dataDxfId="2">
       <calculatedColumnFormula>Table267[[#This Row],[y]]-B6</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -18308,11 +18308,11 @@
   <autoFilter ref="A6:D34" xr:uid="{3C9452C2-1B9C-4FCE-B409-4884E378E31E}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{DEF0F7AA-22F9-4C1A-8BD9-7B0C7CCAC9DD}" name="x"/>
-    <tableColumn id="2" xr3:uid="{1F507D1A-B2AA-480E-B3CC-DAEF443615EA}" name="y" dataDxfId="0">
+    <tableColumn id="2" xr3:uid="{1F507D1A-B2AA-480E-B3CC-DAEF443615EA}" name="y" dataDxfId="1">
       <calculatedColumnFormula>MIN(5, 10 * (1-Table2678[[#This Row],[x]]) + 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{6B702C2A-0C06-40D4-A2C3-567604E36C4A}" name="target"/>
-    <tableColumn id="4" xr3:uid="{7F46F515-7326-4DFA-A053-D585C5F92EA5}" name="delta" dataDxfId="1">
+    <tableColumn id="4" xr3:uid="{7F46F515-7326-4DFA-A053-D585C5F92EA5}" name="delta" dataDxfId="0">
       <calculatedColumnFormula>Table2678[[#This Row],[y]]-B6</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -18585,7 +18585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DO41"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
@@ -30867,7 +30867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C2:S9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>

</xml_diff>